<commit_message>
Fixed APWorld to properly represent Strawberries and handle bad option values
</commit_message>
<xml_diff>
--- a/worlds/celeste/data/items.xlsx
+++ b/worlds/celeste/data/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Archipelago\worlds\celeste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E63551-B6AD-4112-8845-00A129DF3D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D73B774-C4CE-42B9-80B0-DD5C3012104C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="0" windowWidth="30936" windowHeight="16896" xr2:uid="{C0CD6F56-D694-4BE6-8516-FA8CA6FB3D5E}"/>
+    <workbookView xWindow="-30828" yWindow="0" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{C0CD6F56-D694-4BE6-8516-FA8CA6FB3D5E}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="37">
   <si>
     <t>level</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>strawberry</t>
-  </si>
-  <si>
-    <t>Prologue</t>
   </si>
   <si>
     <t>Epilogue</t>
@@ -535,9 +532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A95FA-F51A-42F8-84DA-309114F88AAA}">
   <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,13 +556,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -583,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="str" cm="1">
-        <f t="array" ref="E2">_xlfn.CONCAT(IF(A2="completion", "Completion", IF(A2="cassette", "Cassette", IF(A2="gemheart", "Crystal Heart", IF(A2="strawberry", _xlfn.CONCAT("Strawberry ", D2+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B2)*(regions!$B$2:$B$28=C2), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E2">_xlfn.CONCAT(IF(A2="completion", "Completion", IF(A2="cassette", "Cassette", IF(A2="gemheart", "Crystal Heart", IF(A2="strawberry", _xlfn.CONCAT("Strawberry ", D2+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B2)*(regions!$B$2:$B$27=C2), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F2" t="str">
@@ -606,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="str" cm="1">
-        <f t="array" ref="E3">_xlfn.CONCAT(IF(A3="completion", "Completion", IF(A3="cassette", "Cassette", IF(A3="gemheart", "Crystal Heart", IF(A3="strawberry", _xlfn.CONCAT("Strawberry ", D3+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B3)*(regions!$B$2:$B$28=C3), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E3">_xlfn.CONCAT(IF(A3="completion", "Completion", IF(A3="cassette", "Cassette", IF(A3="gemheart", "Crystal Heart", IF(A3="strawberry", _xlfn.CONCAT("Strawberry ", D3+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B3)*(regions!$B$2:$B$27=C3), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F3" t="str">
@@ -629,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="str" cm="1">
-        <f t="array" ref="E4">_xlfn.CONCAT(IF(A4="completion", "Completion", IF(A4="cassette", "Cassette", IF(A4="gemheart", "Crystal Heart", IF(A4="strawberry", _xlfn.CONCAT("Strawberry ", D4+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B4)*(regions!$B$2:$B$28=C4), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E4">_xlfn.CONCAT(IF(A4="completion", "Completion", IF(A4="cassette", "Cassette", IF(A4="gemheart", "Crystal Heart", IF(A4="strawberry", _xlfn.CONCAT("Strawberry ", D4+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B4)*(regions!$B$2:$B$27=C4), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F4" t="str">
@@ -652,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="str" cm="1">
-        <f t="array" ref="E5">_xlfn.CONCAT(IF(A5="completion", "Completion", IF(A5="cassette", "Cassette", IF(A5="gemheart", "Crystal Heart", IF(A5="strawberry", _xlfn.CONCAT("Strawberry ", D5+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B5)*(regions!$B$2:$B$28=C5), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E5">_xlfn.CONCAT(IF(A5="completion", "Completion", IF(A5="cassette", "Cassette", IF(A5="gemheart", "Crystal Heart", IF(A5="strawberry", _xlfn.CONCAT("Strawberry ", D5+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B5)*(regions!$B$2:$B$27=C5), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F5" t="str">
@@ -675,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="str" cm="1">
-        <f t="array" ref="E6">_xlfn.CONCAT(IF(A6="completion", "Completion", IF(A6="cassette", "Cassette", IF(A6="gemheart", "Crystal Heart", IF(A6="strawberry", _xlfn.CONCAT("Strawberry ", D6+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B6)*(regions!$B$2:$B$28=C6), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E6">_xlfn.CONCAT(IF(A6="completion", "Completion", IF(A6="cassette", "Cassette", IF(A6="gemheart", "Crystal Heart", IF(A6="strawberry", _xlfn.CONCAT("Strawberry ", D6+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B6)*(regions!$B$2:$B$27=C6), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F6" t="str">
@@ -698,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="str" cm="1">
-        <f t="array" ref="E7">_xlfn.CONCAT(IF(A7="completion", "Completion", IF(A7="cassette", "Cassette", IF(A7="gemheart", "Crystal Heart", IF(A7="strawberry", _xlfn.CONCAT("Strawberry ", D7+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B7)*(regions!$B$2:$B$28=C7), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E7">_xlfn.CONCAT(IF(A7="completion", "Completion", IF(A7="cassette", "Cassette", IF(A7="gemheart", "Crystal Heart", IF(A7="strawberry", _xlfn.CONCAT("Strawberry ", D7+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B7)*(regions!$B$2:$B$27=C7), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F7" t="str">
@@ -721,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="str" cm="1">
-        <f t="array" ref="E8">_xlfn.CONCAT(IF(A8="completion", "Completion", IF(A8="cassette", "Cassette", IF(A8="gemheart", "Crystal Heart", IF(A8="strawberry", _xlfn.CONCAT("Strawberry ", D8+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B8)*(regions!$B$2:$B$28=C8), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E8">_xlfn.CONCAT(IF(A8="completion", "Completion", IF(A8="cassette", "Cassette", IF(A8="gemheart", "Crystal Heart", IF(A8="strawberry", _xlfn.CONCAT("Strawberry ", D8+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B8)*(regions!$B$2:$B$27=C8), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F8" t="str">
@@ -744,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="str" cm="1">
-        <f t="array" ref="E9">_xlfn.CONCAT(IF(A9="completion", "Completion", IF(A9="cassette", "Cassette", IF(A9="gemheart", "Crystal Heart", IF(A9="strawberry", _xlfn.CONCAT("Strawberry ", D9+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B9)*(regions!$B$2:$B$28=C9), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E9">_xlfn.CONCAT(IF(A9="completion", "Completion", IF(A9="cassette", "Cassette", IF(A9="gemheart", "Crystal Heart", IF(A9="strawberry", _xlfn.CONCAT("Strawberry ", D9+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B9)*(regions!$B$2:$B$27=C9), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Cassette (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F9" t="str">
@@ -767,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="str" cm="1">
-        <f t="array" ref="E10">_xlfn.CONCAT(IF(A10="completion", "Completion", IF(A10="cassette", "Cassette", IF(A10="gemheart", "Crystal Heart", IF(A10="strawberry", _xlfn.CONCAT("Strawberry ", D10+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B10)*(regions!$B$2:$B$28=C10), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E10">_xlfn.CONCAT(IF(A10="completion", "Completion", IF(A10="cassette", "Cassette", IF(A10="gemheart", "Crystal Heart", IF(A10="strawberry", _xlfn.CONCAT("Strawberry ", D10+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B10)*(regions!$B$2:$B$27=C10), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F10" t="str">
@@ -790,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="str" cm="1">
-        <f t="array" ref="E11">_xlfn.CONCAT(IF(A11="completion", "Completion", IF(A11="cassette", "Cassette", IF(A11="gemheart", "Crystal Heart", IF(A11="strawberry", _xlfn.CONCAT("Strawberry ", D11+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B11)*(regions!$B$2:$B$28=C11), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E11">_xlfn.CONCAT(IF(A11="completion", "Completion", IF(A11="cassette", "Cassette", IF(A11="gemheart", "Crystal Heart", IF(A11="strawberry", _xlfn.CONCAT("Strawberry ", D11+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B11)*(regions!$B$2:$B$27=C11), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F11" t="str">
@@ -813,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="str" cm="1">
-        <f t="array" ref="E12">_xlfn.CONCAT(IF(A12="completion", "Completion", IF(A12="cassette", "Cassette", IF(A12="gemheart", "Crystal Heart", IF(A12="strawberry", _xlfn.CONCAT("Strawberry ", D12+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B12)*(regions!$B$2:$B$28=C12), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E12">_xlfn.CONCAT(IF(A12="completion", "Completion", IF(A12="cassette", "Cassette", IF(A12="gemheart", "Crystal Heart", IF(A12="strawberry", _xlfn.CONCAT("Strawberry ", D12+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B12)*(regions!$B$2:$B$27=C12), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F12" t="str">
@@ -836,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="str" cm="1">
-        <f t="array" ref="E13">_xlfn.CONCAT(IF(A13="completion", "Completion", IF(A13="cassette", "Cassette", IF(A13="gemheart", "Crystal Heart", IF(A13="strawberry", _xlfn.CONCAT("Strawberry ", D13+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B13)*(regions!$B$2:$B$28=C13), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E13">_xlfn.CONCAT(IF(A13="completion", "Completion", IF(A13="cassette", "Cassette", IF(A13="gemheart", "Crystal Heart", IF(A13="strawberry", _xlfn.CONCAT("Strawberry ", D13+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B13)*(regions!$B$2:$B$27=C13), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F13" t="str">
@@ -859,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="str" cm="1">
-        <f t="array" ref="E14">_xlfn.CONCAT(IF(A14="completion", "Completion", IF(A14="cassette", "Cassette", IF(A14="gemheart", "Crystal Heart", IF(A14="strawberry", _xlfn.CONCAT("Strawberry ", D14+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B14)*(regions!$B$2:$B$28=C14), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E14">_xlfn.CONCAT(IF(A14="completion", "Completion", IF(A14="cassette", "Cassette", IF(A14="gemheart", "Crystal Heart", IF(A14="strawberry", _xlfn.CONCAT("Strawberry ", D14+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B14)*(regions!$B$2:$B$27=C14), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F14" t="str">
@@ -882,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="str" cm="1">
-        <f t="array" ref="E15">_xlfn.CONCAT(IF(A15="completion", "Completion", IF(A15="cassette", "Cassette", IF(A15="gemheart", "Crystal Heart", IF(A15="strawberry", _xlfn.CONCAT("Strawberry ", D15+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B15)*(regions!$B$2:$B$28=C15), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E15">_xlfn.CONCAT(IF(A15="completion", "Completion", IF(A15="cassette", "Cassette", IF(A15="gemheart", "Crystal Heart", IF(A15="strawberry", _xlfn.CONCAT("Strawberry ", D15+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B15)*(regions!$B$2:$B$27=C15), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F15" t="str">
@@ -905,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="str" cm="1">
-        <f t="array" ref="E16">_xlfn.CONCAT(IF(A16="completion", "Completion", IF(A16="cassette", "Cassette", IF(A16="gemheart", "Crystal Heart", IF(A16="strawberry", _xlfn.CONCAT("Strawberry ", D16+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B16)*(regions!$B$2:$B$28=C16), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E16">_xlfn.CONCAT(IF(A16="completion", "Completion", IF(A16="cassette", "Cassette", IF(A16="gemheart", "Crystal Heart", IF(A16="strawberry", _xlfn.CONCAT("Strawberry ", D16+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B16)*(regions!$B$2:$B$27=C16), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F16" t="str">
@@ -928,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="str" cm="1">
-        <f t="array" ref="E17">_xlfn.CONCAT(IF(A17="completion", "Completion", IF(A17="cassette", "Cassette", IF(A17="gemheart", "Crystal Heart", IF(A17="strawberry", _xlfn.CONCAT("Strawberry ", D17+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B17)*(regions!$B$2:$B$28=C17), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E17">_xlfn.CONCAT(IF(A17="completion", "Completion", IF(A17="cassette", "Cassette", IF(A17="gemheart", "Crystal Heart", IF(A17="strawberry", _xlfn.CONCAT("Strawberry ", D17+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B17)*(regions!$B$2:$B$27=C17), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Epilogue)</v>
       </c>
       <c r="F17" t="str">
@@ -951,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="str" cm="1">
-        <f t="array" ref="E18">_xlfn.CONCAT(IF(A18="completion", "Completion", IF(A18="cassette", "Cassette", IF(A18="gemheart", "Crystal Heart", IF(A18="strawberry", _xlfn.CONCAT("Strawberry ", D18+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B18)*(regions!$B$2:$B$28=C18), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E18">_xlfn.CONCAT(IF(A18="completion", "Completion", IF(A18="cassette", "Cassette", IF(A18="gemheart", "Crystal Heart", IF(A18="strawberry", _xlfn.CONCAT("Strawberry ", D18+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B18)*(regions!$B$2:$B$27=C18), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F18" t="str">
@@ -974,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="str" cm="1">
-        <f t="array" ref="E19">_xlfn.CONCAT(IF(A19="completion", "Completion", IF(A19="cassette", "Cassette", IF(A19="gemheart", "Crystal Heart", IF(A19="strawberry", _xlfn.CONCAT("Strawberry ", D19+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B19)*(regions!$B$2:$B$28=C19), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E19">_xlfn.CONCAT(IF(A19="completion", "Completion", IF(A19="cassette", "Cassette", IF(A19="gemheart", "Crystal Heart", IF(A19="strawberry", _xlfn.CONCAT("Strawberry ", D19+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B19)*(regions!$B$2:$B$27=C19), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 9: Farewell A-Side)</v>
       </c>
       <c r="F19" t="str">
@@ -997,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="str" cm="1">
-        <f t="array" ref="E20">_xlfn.CONCAT(IF(A20="completion", "Completion", IF(A20="cassette", "Cassette", IF(A20="gemheart", "Crystal Heart", IF(A20="strawberry", _xlfn.CONCAT("Strawberry ", D20+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B20)*(regions!$B$2:$B$28=C20), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E20">_xlfn.CONCAT(IF(A20="completion", "Completion", IF(A20="cassette", "Cassette", IF(A20="gemheart", "Crystal Heart", IF(A20="strawberry", _xlfn.CONCAT("Strawberry ", D20+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B20)*(regions!$B$2:$B$27=C20), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 1: Forsaken City B-Side)</v>
       </c>
       <c r="F20" t="str">
@@ -1020,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="str" cm="1">
-        <f t="array" ref="E21">_xlfn.CONCAT(IF(A21="completion", "Completion", IF(A21="cassette", "Cassette", IF(A21="gemheart", "Crystal Heart", IF(A21="strawberry", _xlfn.CONCAT("Strawberry ", D21+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B21)*(regions!$B$2:$B$28=C21), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E21">_xlfn.CONCAT(IF(A21="completion", "Completion", IF(A21="cassette", "Cassette", IF(A21="gemheart", "Crystal Heart", IF(A21="strawberry", _xlfn.CONCAT("Strawberry ", D21+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B21)*(regions!$B$2:$B$27=C21), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 2: Old Site B-Side)</v>
       </c>
       <c r="F21" t="str">
@@ -1043,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="str" cm="1">
-        <f t="array" ref="E22">_xlfn.CONCAT(IF(A22="completion", "Completion", IF(A22="cassette", "Cassette", IF(A22="gemheart", "Crystal Heart", IF(A22="strawberry", _xlfn.CONCAT("Strawberry ", D22+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B22)*(regions!$B$2:$B$28=C22), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E22">_xlfn.CONCAT(IF(A22="completion", "Completion", IF(A22="cassette", "Cassette", IF(A22="gemheart", "Crystal Heart", IF(A22="strawberry", _xlfn.CONCAT("Strawberry ", D22+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B22)*(regions!$B$2:$B$27=C22), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
       </c>
       <c r="F22" t="str">
@@ -1066,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="str" cm="1">
-        <f t="array" ref="E23">_xlfn.CONCAT(IF(A23="completion", "Completion", IF(A23="cassette", "Cassette", IF(A23="gemheart", "Crystal Heart", IF(A23="strawberry", _xlfn.CONCAT("Strawberry ", D23+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B23)*(regions!$B$2:$B$28=C23), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E23">_xlfn.CONCAT(IF(A23="completion", "Completion", IF(A23="cassette", "Cassette", IF(A23="gemheart", "Crystal Heart", IF(A23="strawberry", _xlfn.CONCAT("Strawberry ", D23+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B23)*(regions!$B$2:$B$27=C23), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
       </c>
       <c r="F23" t="str">
@@ -1089,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="str" cm="1">
-        <f t="array" ref="E24">_xlfn.CONCAT(IF(A24="completion", "Completion", IF(A24="cassette", "Cassette", IF(A24="gemheart", "Crystal Heart", IF(A24="strawberry", _xlfn.CONCAT("Strawberry ", D24+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B24)*(regions!$B$2:$B$28=C24), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E24">_xlfn.CONCAT(IF(A24="completion", "Completion", IF(A24="cassette", "Cassette", IF(A24="gemheart", "Crystal Heart", IF(A24="strawberry", _xlfn.CONCAT("Strawberry ", D24+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B24)*(regions!$B$2:$B$27=C24), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
       </c>
       <c r="F24" t="str">
@@ -1112,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="str" cm="1">
-        <f t="array" ref="E25">_xlfn.CONCAT(IF(A25="completion", "Completion", IF(A25="cassette", "Cassette", IF(A25="gemheart", "Crystal Heart", IF(A25="strawberry", _xlfn.CONCAT("Strawberry ", D25+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B25)*(regions!$B$2:$B$28=C25), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E25">_xlfn.CONCAT(IF(A25="completion", "Completion", IF(A25="cassette", "Cassette", IF(A25="gemheart", "Crystal Heart", IF(A25="strawberry", _xlfn.CONCAT("Strawberry ", D25+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B25)*(regions!$B$2:$B$27=C25), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 6: Reflection B-Side)</v>
       </c>
       <c r="F25" t="str">
@@ -1135,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="str" cm="1">
-        <f t="array" ref="E26">_xlfn.CONCAT(IF(A26="completion", "Completion", IF(A26="cassette", "Cassette", IF(A26="gemheart", "Crystal Heart", IF(A26="strawberry", _xlfn.CONCAT("Strawberry ", D26+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B26)*(regions!$B$2:$B$28=C26), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E26">_xlfn.CONCAT(IF(A26="completion", "Completion", IF(A26="cassette", "Cassette", IF(A26="gemheart", "Crystal Heart", IF(A26="strawberry", _xlfn.CONCAT("Strawberry ", D26+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B26)*(regions!$B$2:$B$27=C26), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 7: The Summit B-Side)</v>
       </c>
       <c r="F26" t="str">
@@ -1158,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="str" cm="1">
-        <f t="array" ref="E27">_xlfn.CONCAT(IF(A27="completion", "Completion", IF(A27="cassette", "Cassette", IF(A27="gemheart", "Crystal Heart", IF(A27="strawberry", _xlfn.CONCAT("Strawberry ", D27+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B27)*(regions!$B$2:$B$28=C27), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E27">_xlfn.CONCAT(IF(A27="completion", "Completion", IF(A27="cassette", "Cassette", IF(A27="gemheart", "Crystal Heart", IF(A27="strawberry", _xlfn.CONCAT("Strawberry ", D27+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B27)*(regions!$B$2:$B$27=C27), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 8: Core B-Side)</v>
       </c>
       <c r="F27" t="str">
@@ -1181,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="str" cm="1">
-        <f t="array" ref="E28">_xlfn.CONCAT(IF(A28="completion", "Completion", IF(A28="cassette", "Cassette", IF(A28="gemheart", "Crystal Heart", IF(A28="strawberry", _xlfn.CONCAT("Strawberry ", D28+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B28)*(regions!$B$2:$B$28=C28), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E28">_xlfn.CONCAT(IF(A28="completion", "Completion", IF(A28="cassette", "Cassette", IF(A28="gemheart", "Crystal Heart", IF(A28="strawberry", _xlfn.CONCAT("Strawberry ", D28+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B28)*(regions!$B$2:$B$27=C28), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 1: Forsaken City C-Side)</v>
       </c>
       <c r="F28" t="str">
@@ -1204,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="str" cm="1">
-        <f t="array" ref="E29">_xlfn.CONCAT(IF(A29="completion", "Completion", IF(A29="cassette", "Cassette", IF(A29="gemheart", "Crystal Heart", IF(A29="strawberry", _xlfn.CONCAT("Strawberry ", D29+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B29)*(regions!$B$2:$B$28=C29), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E29">_xlfn.CONCAT(IF(A29="completion", "Completion", IF(A29="cassette", "Cassette", IF(A29="gemheart", "Crystal Heart", IF(A29="strawberry", _xlfn.CONCAT("Strawberry ", D29+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B29)*(regions!$B$2:$B$27=C29), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 2: Old Site C-Side)</v>
       </c>
       <c r="F29" t="str">
@@ -1227,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="str" cm="1">
-        <f t="array" ref="E30">_xlfn.CONCAT(IF(A30="completion", "Completion", IF(A30="cassette", "Cassette", IF(A30="gemheart", "Crystal Heart", IF(A30="strawberry", _xlfn.CONCAT("Strawberry ", D30+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B30)*(regions!$B$2:$B$28=C30), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E30">_xlfn.CONCAT(IF(A30="completion", "Completion", IF(A30="cassette", "Cassette", IF(A30="gemheart", "Crystal Heart", IF(A30="strawberry", _xlfn.CONCAT("Strawberry ", D30+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B30)*(regions!$B$2:$B$27=C30), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
       </c>
       <c r="F30" t="str">
@@ -1250,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="str" cm="1">
-        <f t="array" ref="E31">_xlfn.CONCAT(IF(A31="completion", "Completion", IF(A31="cassette", "Cassette", IF(A31="gemheart", "Crystal Heart", IF(A31="strawberry", _xlfn.CONCAT("Strawberry ", D31+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B31)*(regions!$B$2:$B$28=C31), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E31">_xlfn.CONCAT(IF(A31="completion", "Completion", IF(A31="cassette", "Cassette", IF(A31="gemheart", "Crystal Heart", IF(A31="strawberry", _xlfn.CONCAT("Strawberry ", D31+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B31)*(regions!$B$2:$B$27=C31), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
       </c>
       <c r="F31" t="str">
@@ -1273,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="str" cm="1">
-        <f t="array" ref="E32">_xlfn.CONCAT(IF(A32="completion", "Completion", IF(A32="cassette", "Cassette", IF(A32="gemheart", "Crystal Heart", IF(A32="strawberry", _xlfn.CONCAT("Strawberry ", D32+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B32)*(regions!$B$2:$B$28=C32), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E32">_xlfn.CONCAT(IF(A32="completion", "Completion", IF(A32="cassette", "Cassette", IF(A32="gemheart", "Crystal Heart", IF(A32="strawberry", _xlfn.CONCAT("Strawberry ", D32+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B32)*(regions!$B$2:$B$27=C32), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
       </c>
       <c r="F32" t="str">
@@ -1296,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="str" cm="1">
-        <f t="array" ref="E33">_xlfn.CONCAT(IF(A33="completion", "Completion", IF(A33="cassette", "Cassette", IF(A33="gemheart", "Crystal Heart", IF(A33="strawberry", _xlfn.CONCAT("Strawberry ", D33+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B33)*(regions!$B$2:$B$28=C33), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E33">_xlfn.CONCAT(IF(A33="completion", "Completion", IF(A33="cassette", "Cassette", IF(A33="gemheart", "Crystal Heart", IF(A33="strawberry", _xlfn.CONCAT("Strawberry ", D33+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B33)*(regions!$B$2:$B$27=C33), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 6: Reflection C-Side)</v>
       </c>
       <c r="F33" t="str">
@@ -1319,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="str" cm="1">
-        <f t="array" ref="E34">_xlfn.CONCAT(IF(A34="completion", "Completion", IF(A34="cassette", "Cassette", IF(A34="gemheart", "Crystal Heart", IF(A34="strawberry", _xlfn.CONCAT("Strawberry ", D34+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B34)*(regions!$B$2:$B$28=C34), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E34">_xlfn.CONCAT(IF(A34="completion", "Completion", IF(A34="cassette", "Cassette", IF(A34="gemheart", "Crystal Heart", IF(A34="strawberry", _xlfn.CONCAT("Strawberry ", D34+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B34)*(regions!$B$2:$B$27=C34), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 7: The Summit C-Side)</v>
       </c>
       <c r="F34" t="str">
@@ -1342,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="str" cm="1">
-        <f t="array" ref="E35">_xlfn.CONCAT(IF(A35="completion", "Completion", IF(A35="cassette", "Cassette", IF(A35="gemheart", "Crystal Heart", IF(A35="strawberry", _xlfn.CONCAT("Strawberry ", D35+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B35)*(regions!$B$2:$B$28=C35), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E35">_xlfn.CONCAT(IF(A35="completion", "Completion", IF(A35="cassette", "Cassette", IF(A35="gemheart", "Crystal Heart", IF(A35="strawberry", _xlfn.CONCAT("Strawberry ", D35+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B35)*(regions!$B$2:$B$27=C35), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Completion (Chapter 8: Core C-Side)</v>
       </c>
       <c r="F35" t="str">
@@ -1365,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="str" cm="1">
-        <f t="array" ref="E36">_xlfn.CONCAT(IF(A36="completion", "Completion", IF(A36="cassette", "Cassette", IF(A36="gemheart", "Crystal Heart", IF(A36="strawberry", _xlfn.CONCAT("Strawberry ", D36+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B36)*(regions!$B$2:$B$28=C36), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E36">_xlfn.CONCAT(IF(A36="completion", "Completion", IF(A36="cassette", "Cassette", IF(A36="gemheart", "Crystal Heart", IF(A36="strawberry", _xlfn.CONCAT("Strawberry ", D36+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B36)*(regions!$B$2:$B$27=C36), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F36" t="str">
@@ -1388,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="str" cm="1">
-        <f t="array" ref="E37">_xlfn.CONCAT(IF(A37="completion", "Completion", IF(A37="cassette", "Cassette", IF(A37="gemheart", "Crystal Heart", IF(A37="strawberry", _xlfn.CONCAT("Strawberry ", D37+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B37)*(regions!$B$2:$B$28=C37), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E37">_xlfn.CONCAT(IF(A37="completion", "Completion", IF(A37="cassette", "Cassette", IF(A37="gemheart", "Crystal Heart", IF(A37="strawberry", _xlfn.CONCAT("Strawberry ", D37+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B37)*(regions!$B$2:$B$27=C37), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F37" t="str">
@@ -1411,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="str" cm="1">
-        <f t="array" ref="E38">_xlfn.CONCAT(IF(A38="completion", "Completion", IF(A38="cassette", "Cassette", IF(A38="gemheart", "Crystal Heart", IF(A38="strawberry", _xlfn.CONCAT("Strawberry ", D38+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B38)*(regions!$B$2:$B$28=C38), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E38">_xlfn.CONCAT(IF(A38="completion", "Completion", IF(A38="cassette", "Cassette", IF(A38="gemheart", "Crystal Heart", IF(A38="strawberry", _xlfn.CONCAT("Strawberry ", D38+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B38)*(regions!$B$2:$B$27=C38), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F38" t="str">
@@ -1434,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="str" cm="1">
-        <f t="array" ref="E39">_xlfn.CONCAT(IF(A39="completion", "Completion", IF(A39="cassette", "Cassette", IF(A39="gemheart", "Crystal Heart", IF(A39="strawberry", _xlfn.CONCAT("Strawberry ", D39+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B39)*(regions!$B$2:$B$28=C39), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E39">_xlfn.CONCAT(IF(A39="completion", "Completion", IF(A39="cassette", "Cassette", IF(A39="gemheart", "Crystal Heart", IF(A39="strawberry", _xlfn.CONCAT("Strawberry ", D39+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B39)*(regions!$B$2:$B$27=C39), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F39" t="str">
@@ -1457,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="str" cm="1">
-        <f t="array" ref="E40">_xlfn.CONCAT(IF(A40="completion", "Completion", IF(A40="cassette", "Cassette", IF(A40="gemheart", "Crystal Heart", IF(A40="strawberry", _xlfn.CONCAT("Strawberry ", D40+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B40)*(regions!$B$2:$B$28=C40), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E40">_xlfn.CONCAT(IF(A40="completion", "Completion", IF(A40="cassette", "Cassette", IF(A40="gemheart", "Crystal Heart", IF(A40="strawberry", _xlfn.CONCAT("Strawberry ", D40+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B40)*(regions!$B$2:$B$27=C40), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F40" t="str">
@@ -1480,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="str" cm="1">
-        <f t="array" ref="E41">_xlfn.CONCAT(IF(A41="completion", "Completion", IF(A41="cassette", "Cassette", IF(A41="gemheart", "Crystal Heart", IF(A41="strawberry", _xlfn.CONCAT("Strawberry ", D41+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B41)*(regions!$B$2:$B$28=C41), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E41">_xlfn.CONCAT(IF(A41="completion", "Completion", IF(A41="cassette", "Cassette", IF(A41="gemheart", "Crystal Heart", IF(A41="strawberry", _xlfn.CONCAT("Strawberry ", D41+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B41)*(regions!$B$2:$B$27=C41), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F41" t="str">
@@ -1503,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="str" cm="1">
-        <f t="array" ref="E42">_xlfn.CONCAT(IF(A42="completion", "Completion", IF(A42="cassette", "Cassette", IF(A42="gemheart", "Crystal Heart", IF(A42="strawberry", _xlfn.CONCAT("Strawberry ", D42+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B42)*(regions!$B$2:$B$28=C42), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E42">_xlfn.CONCAT(IF(A42="completion", "Completion", IF(A42="cassette", "Cassette", IF(A42="gemheart", "Crystal Heart", IF(A42="strawberry", _xlfn.CONCAT("Strawberry ", D42+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B42)*(regions!$B$2:$B$27=C42), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F42" t="str">
@@ -1526,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="str" cm="1">
-        <f t="array" ref="E43">_xlfn.CONCAT(IF(A43="completion", "Completion", IF(A43="cassette", "Cassette", IF(A43="gemheart", "Crystal Heart", IF(A43="strawberry", _xlfn.CONCAT("Strawberry ", D43+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B43)*(regions!$B$2:$B$28=C43), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E43">_xlfn.CONCAT(IF(A43="completion", "Completion", IF(A43="cassette", "Cassette", IF(A43="gemheart", "Crystal Heart", IF(A43="strawberry", _xlfn.CONCAT("Strawberry ", D43+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B43)*(regions!$B$2:$B$27=C43), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F43" t="str">
@@ -1549,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="str" cm="1">
-        <f t="array" ref="E44">_xlfn.CONCAT(IF(A44="completion", "Completion", IF(A44="cassette", "Cassette", IF(A44="gemheart", "Crystal Heart", IF(A44="strawberry", _xlfn.CONCAT("Strawberry ", D44+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B44)*(regions!$B$2:$B$28=C44), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E44">_xlfn.CONCAT(IF(A44="completion", "Completion", IF(A44="cassette", "Cassette", IF(A44="gemheart", "Crystal Heart", IF(A44="strawberry", _xlfn.CONCAT("Strawberry ", D44+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B44)*(regions!$B$2:$B$27=C44), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
       </c>
       <c r="F44" t="str">
@@ -1572,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="str" cm="1">
-        <f t="array" ref="E45">_xlfn.CONCAT(IF(A45="completion", "Completion", IF(A45="cassette", "Cassette", IF(A45="gemheart", "Crystal Heart", IF(A45="strawberry", _xlfn.CONCAT("Strawberry ", D45+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B45)*(regions!$B$2:$B$28=C45), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E45">_xlfn.CONCAT(IF(A45="completion", "Completion", IF(A45="cassette", "Cassette", IF(A45="gemheart", "Crystal Heart", IF(A45="strawberry", _xlfn.CONCAT("Strawberry ", D45+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B45)*(regions!$B$2:$B$27=C45), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
       </c>
       <c r="F45" t="str">
@@ -1595,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="str" cm="1">
-        <f t="array" ref="E46">_xlfn.CONCAT(IF(A46="completion", "Completion", IF(A46="cassette", "Cassette", IF(A46="gemheart", "Crystal Heart", IF(A46="strawberry", _xlfn.CONCAT("Strawberry ", D46+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B46)*(regions!$B$2:$B$28=C46), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E46">_xlfn.CONCAT(IF(A46="completion", "Completion", IF(A46="cassette", "Cassette", IF(A46="gemheart", "Crystal Heart", IF(A46="strawberry", _xlfn.CONCAT("Strawberry ", D46+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B46)*(regions!$B$2:$B$27=C46), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
       </c>
       <c r="F46" t="str">
@@ -1618,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="str" cm="1">
-        <f t="array" ref="E47">_xlfn.CONCAT(IF(A47="completion", "Completion", IF(A47="cassette", "Cassette", IF(A47="gemheart", "Crystal Heart", IF(A47="strawberry", _xlfn.CONCAT("Strawberry ", D47+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B47)*(regions!$B$2:$B$28=C47), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E47">_xlfn.CONCAT(IF(A47="completion", "Completion", IF(A47="cassette", "Cassette", IF(A47="gemheart", "Crystal Heart", IF(A47="strawberry", _xlfn.CONCAT("Strawberry ", D47+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B47)*(regions!$B$2:$B$27=C47), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
       </c>
       <c r="F47" t="str">
@@ -1641,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="str" cm="1">
-        <f t="array" ref="E48">_xlfn.CONCAT(IF(A48="completion", "Completion", IF(A48="cassette", "Cassette", IF(A48="gemheart", "Crystal Heart", IF(A48="strawberry", _xlfn.CONCAT("Strawberry ", D48+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B48)*(regions!$B$2:$B$28=C48), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E48">_xlfn.CONCAT(IF(A48="completion", "Completion", IF(A48="cassette", "Cassette", IF(A48="gemheart", "Crystal Heart", IF(A48="strawberry", _xlfn.CONCAT("Strawberry ", D48+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B48)*(regions!$B$2:$B$27=C48), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
       </c>
       <c r="F48" t="str">
@@ -1664,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="str" cm="1">
-        <f t="array" ref="E49">_xlfn.CONCAT(IF(A49="completion", "Completion", IF(A49="cassette", "Cassette", IF(A49="gemheart", "Crystal Heart", IF(A49="strawberry", _xlfn.CONCAT("Strawberry ", D49+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B49)*(regions!$B$2:$B$28=C49), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E49">_xlfn.CONCAT(IF(A49="completion", "Completion", IF(A49="cassette", "Cassette", IF(A49="gemheart", "Crystal Heart", IF(A49="strawberry", _xlfn.CONCAT("Strawberry ", D49+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B49)*(regions!$B$2:$B$27=C49), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
       </c>
       <c r="F49" t="str">
@@ -1687,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="str" cm="1">
-        <f t="array" ref="E50">_xlfn.CONCAT(IF(A50="completion", "Completion", IF(A50="cassette", "Cassette", IF(A50="gemheart", "Crystal Heart", IF(A50="strawberry", _xlfn.CONCAT("Strawberry ", D50+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B50)*(regions!$B$2:$B$28=C50), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E50">_xlfn.CONCAT(IF(A50="completion", "Completion", IF(A50="cassette", "Cassette", IF(A50="gemheart", "Crystal Heart", IF(A50="strawberry", _xlfn.CONCAT("Strawberry ", D50+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B50)*(regions!$B$2:$B$27=C50), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
       </c>
       <c r="F50" t="str">
@@ -1710,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="str" cm="1">
-        <f t="array" ref="E51">_xlfn.CONCAT(IF(A51="completion", "Completion", IF(A51="cassette", "Cassette", IF(A51="gemheart", "Crystal Heart", IF(A51="strawberry", _xlfn.CONCAT("Strawberry ", D51+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B51)*(regions!$B$2:$B$28=C51), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E51">_xlfn.CONCAT(IF(A51="completion", "Completion", IF(A51="cassette", "Cassette", IF(A51="gemheart", "Crystal Heart", IF(A51="strawberry", _xlfn.CONCAT("Strawberry ", D51+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B51)*(regions!$B$2:$B$27=C51), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 8: Core B-Side)</v>
       </c>
       <c r="F51" t="str">
@@ -1733,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="str" cm="1">
-        <f t="array" ref="E52">_xlfn.CONCAT(IF(A52="completion", "Completion", IF(A52="cassette", "Cassette", IF(A52="gemheart", "Crystal Heart", IF(A52="strawberry", _xlfn.CONCAT("Strawberry ", D52+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B52)*(regions!$B$2:$B$28=C52), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E52">_xlfn.CONCAT(IF(A52="completion", "Completion", IF(A52="cassette", "Cassette", IF(A52="gemheart", "Crystal Heart", IF(A52="strawberry", _xlfn.CONCAT("Strawberry ", D52+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B52)*(regions!$B$2:$B$27=C52), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
       </c>
       <c r="F52" t="str">
@@ -1756,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="str" cm="1">
-        <f t="array" ref="E53">_xlfn.CONCAT(IF(A53="completion", "Completion", IF(A53="cassette", "Cassette", IF(A53="gemheart", "Crystal Heart", IF(A53="strawberry", _xlfn.CONCAT("Strawberry ", D53+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B53)*(regions!$B$2:$B$28=C53), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E53">_xlfn.CONCAT(IF(A53="completion", "Completion", IF(A53="cassette", "Cassette", IF(A53="gemheart", "Crystal Heart", IF(A53="strawberry", _xlfn.CONCAT("Strawberry ", D53+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B53)*(regions!$B$2:$B$27=C53), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
       </c>
       <c r="F53" t="str">
@@ -1779,7 +1776,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="str" cm="1">
-        <f t="array" ref="E54">_xlfn.CONCAT(IF(A54="completion", "Completion", IF(A54="cassette", "Cassette", IF(A54="gemheart", "Crystal Heart", IF(A54="strawberry", _xlfn.CONCAT("Strawberry ", D54+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B54)*(regions!$B$2:$B$28=C54), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E54">_xlfn.CONCAT(IF(A54="completion", "Completion", IF(A54="cassette", "Cassette", IF(A54="gemheart", "Crystal Heart", IF(A54="strawberry", _xlfn.CONCAT("Strawberry ", D54+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B54)*(regions!$B$2:$B$27=C54), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
       </c>
       <c r="F54" t="str">
@@ -1802,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="str" cm="1">
-        <f t="array" ref="E55">_xlfn.CONCAT(IF(A55="completion", "Completion", IF(A55="cassette", "Cassette", IF(A55="gemheart", "Crystal Heart", IF(A55="strawberry", _xlfn.CONCAT("Strawberry ", D55+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B55)*(regions!$B$2:$B$28=C55), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E55">_xlfn.CONCAT(IF(A55="completion", "Completion", IF(A55="cassette", "Cassette", IF(A55="gemheart", "Crystal Heart", IF(A55="strawberry", _xlfn.CONCAT("Strawberry ", D55+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B55)*(regions!$B$2:$B$27=C55), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
       </c>
       <c r="F55" t="str">
@@ -1825,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="str" cm="1">
-        <f t="array" ref="E56">_xlfn.CONCAT(IF(A56="completion", "Completion", IF(A56="cassette", "Cassette", IF(A56="gemheart", "Crystal Heart", IF(A56="strawberry", _xlfn.CONCAT("Strawberry ", D56+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B56)*(regions!$B$2:$B$28=C56), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E56">_xlfn.CONCAT(IF(A56="completion", "Completion", IF(A56="cassette", "Cassette", IF(A56="gemheart", "Crystal Heart", IF(A56="strawberry", _xlfn.CONCAT("Strawberry ", D56+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B56)*(regions!$B$2:$B$27=C56), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
       </c>
       <c r="F56" t="str">
@@ -1848,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="str" cm="1">
-        <f t="array" ref="E57">_xlfn.CONCAT(IF(A57="completion", "Completion", IF(A57="cassette", "Cassette", IF(A57="gemheart", "Crystal Heart", IF(A57="strawberry", _xlfn.CONCAT("Strawberry ", D57+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B57)*(regions!$B$2:$B$28=C57), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E57">_xlfn.CONCAT(IF(A57="completion", "Completion", IF(A57="cassette", "Cassette", IF(A57="gemheart", "Crystal Heart", IF(A57="strawberry", _xlfn.CONCAT("Strawberry ", D57+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B57)*(regions!$B$2:$B$27=C57), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
       </c>
       <c r="F57" t="str">
@@ -1871,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="str" cm="1">
-        <f t="array" ref="E58">_xlfn.CONCAT(IF(A58="completion", "Completion", IF(A58="cassette", "Cassette", IF(A58="gemheart", "Crystal Heart", IF(A58="strawberry", _xlfn.CONCAT("Strawberry ", D58+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B58)*(regions!$B$2:$B$28=C58), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E58">_xlfn.CONCAT(IF(A58="completion", "Completion", IF(A58="cassette", "Cassette", IF(A58="gemheart", "Crystal Heart", IF(A58="strawberry", _xlfn.CONCAT("Strawberry ", D58+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B58)*(regions!$B$2:$B$27=C58), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
       </c>
       <c r="F58" t="str">
@@ -1894,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="str" cm="1">
-        <f t="array" ref="E59">_xlfn.CONCAT(IF(A59="completion", "Completion", IF(A59="cassette", "Cassette", IF(A59="gemheart", "Crystal Heart", IF(A59="strawberry", _xlfn.CONCAT("Strawberry ", D59+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B59)*(regions!$B$2:$B$28=C59), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E59">_xlfn.CONCAT(IF(A59="completion", "Completion", IF(A59="cassette", "Cassette", IF(A59="gemheart", "Crystal Heart", IF(A59="strawberry", _xlfn.CONCAT("Strawberry ", D59+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B59)*(regions!$B$2:$B$27=C59), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Crystal Heart (Chapter 8: Core C-Side)</v>
       </c>
       <c r="F59" t="str">
@@ -1917,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="str" cm="1">
-        <f t="array" ref="E60">_xlfn.CONCAT(IF(A60="completion", "Completion", IF(A60="cassette", "Cassette", IF(A60="gemheart", "Crystal Heart", IF(A60="strawberry", _xlfn.CONCAT("Strawberry ", D60+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B60)*(regions!$B$2:$B$28=C60), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E60">_xlfn.CONCAT(IF(A60="completion", "Completion", IF(A60="cassette", "Cassette", IF(A60="gemheart", "Crystal Heart", IF(A60="strawberry", _xlfn.CONCAT("Strawberry ", D60+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B60)*(regions!$B$2:$B$27=C60), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F60" t="str">
@@ -1940,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="str" cm="1">
-        <f t="array" ref="E61">_xlfn.CONCAT(IF(A61="completion", "Completion", IF(A61="cassette", "Cassette", IF(A61="gemheart", "Crystal Heart", IF(A61="strawberry", _xlfn.CONCAT("Strawberry ", D61+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B61)*(regions!$B$2:$B$28=C61), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E61">_xlfn.CONCAT(IF(A61="completion", "Completion", IF(A61="cassette", "Cassette", IF(A61="gemheart", "Crystal Heart", IF(A61="strawberry", _xlfn.CONCAT("Strawberry ", D61+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B61)*(regions!$B$2:$B$27=C61), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F61" t="str">
@@ -1963,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="E62" t="str" cm="1">
-        <f t="array" ref="E62">_xlfn.CONCAT(IF(A62="completion", "Completion", IF(A62="cassette", "Cassette", IF(A62="gemheart", "Crystal Heart", IF(A62="strawberry", _xlfn.CONCAT("Strawberry ", D62+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B62)*(regions!$B$2:$B$28=C62), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E62">_xlfn.CONCAT(IF(A62="completion", "Completion", IF(A62="cassette", "Cassette", IF(A62="gemheart", "Crystal Heart", IF(A62="strawberry", _xlfn.CONCAT("Strawberry ", D62+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B62)*(regions!$B$2:$B$27=C62), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F62" t="str">
@@ -1986,7 +1983,7 @@
         <v>3</v>
       </c>
       <c r="E63" t="str" cm="1">
-        <f t="array" ref="E63">_xlfn.CONCAT(IF(A63="completion", "Completion", IF(A63="cassette", "Cassette", IF(A63="gemheart", "Crystal Heart", IF(A63="strawberry", _xlfn.CONCAT("Strawberry ", D63+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B63)*(regions!$B$2:$B$28=C63), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E63">_xlfn.CONCAT(IF(A63="completion", "Completion", IF(A63="cassette", "Cassette", IF(A63="gemheart", "Crystal Heart", IF(A63="strawberry", _xlfn.CONCAT("Strawberry ", D63+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B63)*(regions!$B$2:$B$27=C63), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F63" t="str">
@@ -2009,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="E64" t="str" cm="1">
-        <f t="array" ref="E64">_xlfn.CONCAT(IF(A64="completion", "Completion", IF(A64="cassette", "Cassette", IF(A64="gemheart", "Crystal Heart", IF(A64="strawberry", _xlfn.CONCAT("Strawberry ", D64+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B64)*(regions!$B$2:$B$28=C64), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E64">_xlfn.CONCAT(IF(A64="completion", "Completion", IF(A64="cassette", "Cassette", IF(A64="gemheart", "Crystal Heart", IF(A64="strawberry", _xlfn.CONCAT("Strawberry ", D64+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B64)*(regions!$B$2:$B$27=C64), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F64" t="str">
@@ -2032,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="E65" t="str" cm="1">
-        <f t="array" ref="E65">_xlfn.CONCAT(IF(A65="completion", "Completion", IF(A65="cassette", "Cassette", IF(A65="gemheart", "Crystal Heart", IF(A65="strawberry", _xlfn.CONCAT("Strawberry ", D65+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B65)*(regions!$B$2:$B$28=C65), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E65">_xlfn.CONCAT(IF(A65="completion", "Completion", IF(A65="cassette", "Cassette", IF(A65="gemheart", "Crystal Heart", IF(A65="strawberry", _xlfn.CONCAT("Strawberry ", D65+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B65)*(regions!$B$2:$B$27=C65), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 6 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F65" t="str">
@@ -2055,7 +2052,7 @@
         <v>6</v>
       </c>
       <c r="E66" t="str" cm="1">
-        <f t="array" ref="E66">_xlfn.CONCAT(IF(A66="completion", "Completion", IF(A66="cassette", "Cassette", IF(A66="gemheart", "Crystal Heart", IF(A66="strawberry", _xlfn.CONCAT("Strawberry ", D66+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B66)*(regions!$B$2:$B$28=C66), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E66">_xlfn.CONCAT(IF(A66="completion", "Completion", IF(A66="cassette", "Cassette", IF(A66="gemheart", "Crystal Heart", IF(A66="strawberry", _xlfn.CONCAT("Strawberry ", D66+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B66)*(regions!$B$2:$B$27=C66), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 7 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F66" t="str">
@@ -2078,7 +2075,7 @@
         <v>7</v>
       </c>
       <c r="E67" t="str" cm="1">
-        <f t="array" ref="E67">_xlfn.CONCAT(IF(A67="completion", "Completion", IF(A67="cassette", "Cassette", IF(A67="gemheart", "Crystal Heart", IF(A67="strawberry", _xlfn.CONCAT("Strawberry ", D67+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B67)*(regions!$B$2:$B$28=C67), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E67">_xlfn.CONCAT(IF(A67="completion", "Completion", IF(A67="cassette", "Cassette", IF(A67="gemheart", "Crystal Heart", IF(A67="strawberry", _xlfn.CONCAT("Strawberry ", D67+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B67)*(regions!$B$2:$B$27=C67), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 8 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F67" t="str">
@@ -2101,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="E68" t="str" cm="1">
-        <f t="array" ref="E68">_xlfn.CONCAT(IF(A68="completion", "Completion", IF(A68="cassette", "Cassette", IF(A68="gemheart", "Crystal Heart", IF(A68="strawberry", _xlfn.CONCAT("Strawberry ", D68+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B68)*(regions!$B$2:$B$28=C68), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E68">_xlfn.CONCAT(IF(A68="completion", "Completion", IF(A68="cassette", "Cassette", IF(A68="gemheart", "Crystal Heart", IF(A68="strawberry", _xlfn.CONCAT("Strawberry ", D68+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B68)*(regions!$B$2:$B$27=C68), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 9 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F68" t="str">
@@ -2124,7 +2121,7 @@
         <v>9</v>
       </c>
       <c r="E69" t="str" cm="1">
-        <f t="array" ref="E69">_xlfn.CONCAT(IF(A69="completion", "Completion", IF(A69="cassette", "Cassette", IF(A69="gemheart", "Crystal Heart", IF(A69="strawberry", _xlfn.CONCAT("Strawberry ", D69+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B69)*(regions!$B$2:$B$28=C69), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E69">_xlfn.CONCAT(IF(A69="completion", "Completion", IF(A69="cassette", "Cassette", IF(A69="gemheart", "Crystal Heart", IF(A69="strawberry", _xlfn.CONCAT("Strawberry ", D69+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B69)*(regions!$B$2:$B$27=C69), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 10 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F69" t="str">
@@ -2147,7 +2144,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="str" cm="1">
-        <f t="array" ref="E70">_xlfn.CONCAT(IF(A70="completion", "Completion", IF(A70="cassette", "Cassette", IF(A70="gemheart", "Crystal Heart", IF(A70="strawberry", _xlfn.CONCAT("Strawberry ", D70+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B70)*(regions!$B$2:$B$28=C70), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E70">_xlfn.CONCAT(IF(A70="completion", "Completion", IF(A70="cassette", "Cassette", IF(A70="gemheart", "Crystal Heart", IF(A70="strawberry", _xlfn.CONCAT("Strawberry ", D70+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B70)*(regions!$B$2:$B$27=C70), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 11 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F70" t="str">
@@ -2170,7 +2167,7 @@
         <v>11</v>
       </c>
       <c r="E71" t="str" cm="1">
-        <f t="array" ref="E71">_xlfn.CONCAT(IF(A71="completion", "Completion", IF(A71="cassette", "Cassette", IF(A71="gemheart", "Crystal Heart", IF(A71="strawberry", _xlfn.CONCAT("Strawberry ", D71+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B71)*(regions!$B$2:$B$28=C71), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E71">_xlfn.CONCAT(IF(A71="completion", "Completion", IF(A71="cassette", "Cassette", IF(A71="gemheart", "Crystal Heart", IF(A71="strawberry", _xlfn.CONCAT("Strawberry ", D71+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B71)*(regions!$B$2:$B$27=C71), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 12 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F71" t="str">
@@ -2193,7 +2190,7 @@
         <v>12</v>
       </c>
       <c r="E72" t="str" cm="1">
-        <f t="array" ref="E72">_xlfn.CONCAT(IF(A72="completion", "Completion", IF(A72="cassette", "Cassette", IF(A72="gemheart", "Crystal Heart", IF(A72="strawberry", _xlfn.CONCAT("Strawberry ", D72+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B72)*(regions!$B$2:$B$28=C72), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E72">_xlfn.CONCAT(IF(A72="completion", "Completion", IF(A72="cassette", "Cassette", IF(A72="gemheart", "Crystal Heart", IF(A72="strawberry", _xlfn.CONCAT("Strawberry ", D72+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B72)*(regions!$B$2:$B$27=C72), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 13 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F72" t="str">
@@ -2216,7 +2213,7 @@
         <v>13</v>
       </c>
       <c r="E73" t="str" cm="1">
-        <f t="array" ref="E73">_xlfn.CONCAT(IF(A73="completion", "Completion", IF(A73="cassette", "Cassette", IF(A73="gemheart", "Crystal Heart", IF(A73="strawberry", _xlfn.CONCAT("Strawberry ", D73+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B73)*(regions!$B$2:$B$28=C73), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E73">_xlfn.CONCAT(IF(A73="completion", "Completion", IF(A73="cassette", "Cassette", IF(A73="gemheart", "Crystal Heart", IF(A73="strawberry", _xlfn.CONCAT("Strawberry ", D73+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B73)*(regions!$B$2:$B$27=C73), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 14 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F73" t="str">
@@ -2239,7 +2236,7 @@
         <v>14</v>
       </c>
       <c r="E74" t="str" cm="1">
-        <f t="array" ref="E74">_xlfn.CONCAT(IF(A74="completion", "Completion", IF(A74="cassette", "Cassette", IF(A74="gemheart", "Crystal Heart", IF(A74="strawberry", _xlfn.CONCAT("Strawberry ", D74+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B74)*(regions!$B$2:$B$28=C74), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E74">_xlfn.CONCAT(IF(A74="completion", "Completion", IF(A74="cassette", "Cassette", IF(A74="gemheart", "Crystal Heart", IF(A74="strawberry", _xlfn.CONCAT("Strawberry ", D74+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B74)*(regions!$B$2:$B$27=C74), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 15 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F74" t="str">
@@ -2262,7 +2259,7 @@
         <v>15</v>
       </c>
       <c r="E75" t="str" cm="1">
-        <f t="array" ref="E75">_xlfn.CONCAT(IF(A75="completion", "Completion", IF(A75="cassette", "Cassette", IF(A75="gemheart", "Crystal Heart", IF(A75="strawberry", _xlfn.CONCAT("Strawberry ", D75+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B75)*(regions!$B$2:$B$28=C75), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E75">_xlfn.CONCAT(IF(A75="completion", "Completion", IF(A75="cassette", "Cassette", IF(A75="gemheart", "Crystal Heart", IF(A75="strawberry", _xlfn.CONCAT("Strawberry ", D75+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B75)*(regions!$B$2:$B$27=C75), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 16 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F75" t="str">
@@ -2285,7 +2282,7 @@
         <v>16</v>
       </c>
       <c r="E76" t="str" cm="1">
-        <f t="array" ref="E76">_xlfn.CONCAT(IF(A76="completion", "Completion", IF(A76="cassette", "Cassette", IF(A76="gemheart", "Crystal Heart", IF(A76="strawberry", _xlfn.CONCAT("Strawberry ", D76+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B76)*(regions!$B$2:$B$28=C76), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E76">_xlfn.CONCAT(IF(A76="completion", "Completion", IF(A76="cassette", "Cassette", IF(A76="gemheart", "Crystal Heart", IF(A76="strawberry", _xlfn.CONCAT("Strawberry ", D76+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B76)*(regions!$B$2:$B$27=C76), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 17 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F76" t="str">
@@ -2308,7 +2305,7 @@
         <v>17</v>
       </c>
       <c r="E77" t="str" cm="1">
-        <f t="array" ref="E77">_xlfn.CONCAT(IF(A77="completion", "Completion", IF(A77="cassette", "Cassette", IF(A77="gemheart", "Crystal Heart", IF(A77="strawberry", _xlfn.CONCAT("Strawberry ", D77+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B77)*(regions!$B$2:$B$28=C77), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E77">_xlfn.CONCAT(IF(A77="completion", "Completion", IF(A77="cassette", "Cassette", IF(A77="gemheart", "Crystal Heart", IF(A77="strawberry", _xlfn.CONCAT("Strawberry ", D77+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B77)*(regions!$B$2:$B$27=C77), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 18 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F77" t="str">
@@ -2331,7 +2328,7 @@
         <v>18</v>
       </c>
       <c r="E78" t="str" cm="1">
-        <f t="array" ref="E78">_xlfn.CONCAT(IF(A78="completion", "Completion", IF(A78="cassette", "Cassette", IF(A78="gemheart", "Crystal Heart", IF(A78="strawberry", _xlfn.CONCAT("Strawberry ", D78+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B78)*(regions!$B$2:$B$28=C78), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E78">_xlfn.CONCAT(IF(A78="completion", "Completion", IF(A78="cassette", "Cassette", IF(A78="gemheart", "Crystal Heart", IF(A78="strawberry", _xlfn.CONCAT("Strawberry ", D78+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B78)*(regions!$B$2:$B$27=C78), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 19 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F78" t="str">
@@ -2354,7 +2351,7 @@
         <v>19</v>
       </c>
       <c r="E79" t="str" cm="1">
-        <f t="array" ref="E79">_xlfn.CONCAT(IF(A79="completion", "Completion", IF(A79="cassette", "Cassette", IF(A79="gemheart", "Crystal Heart", IF(A79="strawberry", _xlfn.CONCAT("Strawberry ", D79+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B79)*(regions!$B$2:$B$28=C79), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E79">_xlfn.CONCAT(IF(A79="completion", "Completion", IF(A79="cassette", "Cassette", IF(A79="gemheart", "Crystal Heart", IF(A79="strawberry", _xlfn.CONCAT("Strawberry ", D79+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B79)*(regions!$B$2:$B$27=C79), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 20 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F79" t="str">
@@ -2377,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="str" cm="1">
-        <f t="array" ref="E80">_xlfn.CONCAT(IF(A80="completion", "Completion", IF(A80="cassette", "Cassette", IF(A80="gemheart", "Crystal Heart", IF(A80="strawberry", _xlfn.CONCAT("Strawberry ", D80+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B80)*(regions!$B$2:$B$28=C80), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E80">_xlfn.CONCAT(IF(A80="completion", "Completion", IF(A80="cassette", "Cassette", IF(A80="gemheart", "Crystal Heart", IF(A80="strawberry", _xlfn.CONCAT("Strawberry ", D80+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B80)*(regions!$B$2:$B$27=C80), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F80" t="str">
@@ -2400,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="E81" t="str" cm="1">
-        <f t="array" ref="E81">_xlfn.CONCAT(IF(A81="completion", "Completion", IF(A81="cassette", "Cassette", IF(A81="gemheart", "Crystal Heart", IF(A81="strawberry", _xlfn.CONCAT("Strawberry ", D81+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B81)*(regions!$B$2:$B$28=C81), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E81">_xlfn.CONCAT(IF(A81="completion", "Completion", IF(A81="cassette", "Cassette", IF(A81="gemheart", "Crystal Heart", IF(A81="strawberry", _xlfn.CONCAT("Strawberry ", D81+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B81)*(regions!$B$2:$B$27=C81), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F81" t="str">
@@ -2423,7 +2420,7 @@
         <v>2</v>
       </c>
       <c r="E82" t="str" cm="1">
-        <f t="array" ref="E82">_xlfn.CONCAT(IF(A82="completion", "Completion", IF(A82="cassette", "Cassette", IF(A82="gemheart", "Crystal Heart", IF(A82="strawberry", _xlfn.CONCAT("Strawberry ", D82+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B82)*(regions!$B$2:$B$28=C82), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E82">_xlfn.CONCAT(IF(A82="completion", "Completion", IF(A82="cassette", "Cassette", IF(A82="gemheart", "Crystal Heart", IF(A82="strawberry", _xlfn.CONCAT("Strawberry ", D82+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B82)*(regions!$B$2:$B$27=C82), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F82" t="str">
@@ -2446,7 +2443,7 @@
         <v>3</v>
       </c>
       <c r="E83" t="str" cm="1">
-        <f t="array" ref="E83">_xlfn.CONCAT(IF(A83="completion", "Completion", IF(A83="cassette", "Cassette", IF(A83="gemheart", "Crystal Heart", IF(A83="strawberry", _xlfn.CONCAT("Strawberry ", D83+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B83)*(regions!$B$2:$B$28=C83), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E83">_xlfn.CONCAT(IF(A83="completion", "Completion", IF(A83="cassette", "Cassette", IF(A83="gemheart", "Crystal Heart", IF(A83="strawberry", _xlfn.CONCAT("Strawberry ", D83+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B83)*(regions!$B$2:$B$27=C83), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F83" t="str">
@@ -2469,7 +2466,7 @@
         <v>4</v>
       </c>
       <c r="E84" t="str" cm="1">
-        <f t="array" ref="E84">_xlfn.CONCAT(IF(A84="completion", "Completion", IF(A84="cassette", "Cassette", IF(A84="gemheart", "Crystal Heart", IF(A84="strawberry", _xlfn.CONCAT("Strawberry ", D84+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B84)*(regions!$B$2:$B$28=C84), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E84">_xlfn.CONCAT(IF(A84="completion", "Completion", IF(A84="cassette", "Cassette", IF(A84="gemheart", "Crystal Heart", IF(A84="strawberry", _xlfn.CONCAT("Strawberry ", D84+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B84)*(regions!$B$2:$B$27=C84), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F84" t="str">
@@ -2492,7 +2489,7 @@
         <v>5</v>
       </c>
       <c r="E85" t="str" cm="1">
-        <f t="array" ref="E85">_xlfn.CONCAT(IF(A85="completion", "Completion", IF(A85="cassette", "Cassette", IF(A85="gemheart", "Crystal Heart", IF(A85="strawberry", _xlfn.CONCAT("Strawberry ", D85+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B85)*(regions!$B$2:$B$28=C85), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E85">_xlfn.CONCAT(IF(A85="completion", "Completion", IF(A85="cassette", "Cassette", IF(A85="gemheart", "Crystal Heart", IF(A85="strawberry", _xlfn.CONCAT("Strawberry ", D85+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B85)*(regions!$B$2:$B$27=C85), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 6 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F85" t="str">
@@ -2515,7 +2512,7 @@
         <v>6</v>
       </c>
       <c r="E86" t="str" cm="1">
-        <f t="array" ref="E86">_xlfn.CONCAT(IF(A86="completion", "Completion", IF(A86="cassette", "Cassette", IF(A86="gemheart", "Crystal Heart", IF(A86="strawberry", _xlfn.CONCAT("Strawberry ", D86+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B86)*(regions!$B$2:$B$28=C86), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E86">_xlfn.CONCAT(IF(A86="completion", "Completion", IF(A86="cassette", "Cassette", IF(A86="gemheart", "Crystal Heart", IF(A86="strawberry", _xlfn.CONCAT("Strawberry ", D86+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B86)*(regions!$B$2:$B$27=C86), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 7 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F86" t="str">
@@ -2538,7 +2535,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="str" cm="1">
-        <f t="array" ref="E87">_xlfn.CONCAT(IF(A87="completion", "Completion", IF(A87="cassette", "Cassette", IF(A87="gemheart", "Crystal Heart", IF(A87="strawberry", _xlfn.CONCAT("Strawberry ", D87+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B87)*(regions!$B$2:$B$28=C87), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E87">_xlfn.CONCAT(IF(A87="completion", "Completion", IF(A87="cassette", "Cassette", IF(A87="gemheart", "Crystal Heart", IF(A87="strawberry", _xlfn.CONCAT("Strawberry ", D87+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B87)*(regions!$B$2:$B$27=C87), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 8 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F87" t="str">
@@ -2561,7 +2558,7 @@
         <v>8</v>
       </c>
       <c r="E88" t="str" cm="1">
-        <f t="array" ref="E88">_xlfn.CONCAT(IF(A88="completion", "Completion", IF(A88="cassette", "Cassette", IF(A88="gemheart", "Crystal Heart", IF(A88="strawberry", _xlfn.CONCAT("Strawberry ", D88+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B88)*(regions!$B$2:$B$28=C88), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E88">_xlfn.CONCAT(IF(A88="completion", "Completion", IF(A88="cassette", "Cassette", IF(A88="gemheart", "Crystal Heart", IF(A88="strawberry", _xlfn.CONCAT("Strawberry ", D88+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B88)*(regions!$B$2:$B$27=C88), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 9 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F88" t="str">
@@ -2584,7 +2581,7 @@
         <v>9</v>
       </c>
       <c r="E89" t="str" cm="1">
-        <f t="array" ref="E89">_xlfn.CONCAT(IF(A89="completion", "Completion", IF(A89="cassette", "Cassette", IF(A89="gemheart", "Crystal Heart", IF(A89="strawberry", _xlfn.CONCAT("Strawberry ", D89+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B89)*(regions!$B$2:$B$28=C89), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E89">_xlfn.CONCAT(IF(A89="completion", "Completion", IF(A89="cassette", "Cassette", IF(A89="gemheart", "Crystal Heart", IF(A89="strawberry", _xlfn.CONCAT("Strawberry ", D89+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B89)*(regions!$B$2:$B$27=C89), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 10 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F89" t="str">
@@ -2607,7 +2604,7 @@
         <v>10</v>
       </c>
       <c r="E90" t="str" cm="1">
-        <f t="array" ref="E90">_xlfn.CONCAT(IF(A90="completion", "Completion", IF(A90="cassette", "Cassette", IF(A90="gemheart", "Crystal Heart", IF(A90="strawberry", _xlfn.CONCAT("Strawberry ", D90+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B90)*(regions!$B$2:$B$28=C90), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E90">_xlfn.CONCAT(IF(A90="completion", "Completion", IF(A90="cassette", "Cassette", IF(A90="gemheart", "Crystal Heart", IF(A90="strawberry", _xlfn.CONCAT("Strawberry ", D90+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B90)*(regions!$B$2:$B$27=C90), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 11 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F90" t="str">
@@ -2630,7 +2627,7 @@
         <v>11</v>
       </c>
       <c r="E91" t="str" cm="1">
-        <f t="array" ref="E91">_xlfn.CONCAT(IF(A91="completion", "Completion", IF(A91="cassette", "Cassette", IF(A91="gemheart", "Crystal Heart", IF(A91="strawberry", _xlfn.CONCAT("Strawberry ", D91+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B91)*(regions!$B$2:$B$28=C91), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E91">_xlfn.CONCAT(IF(A91="completion", "Completion", IF(A91="cassette", "Cassette", IF(A91="gemheart", "Crystal Heart", IF(A91="strawberry", _xlfn.CONCAT("Strawberry ", D91+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B91)*(regions!$B$2:$B$27=C91), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 12 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F91" t="str">
@@ -2653,7 +2650,7 @@
         <v>12</v>
       </c>
       <c r="E92" t="str" cm="1">
-        <f t="array" ref="E92">_xlfn.CONCAT(IF(A92="completion", "Completion", IF(A92="cassette", "Cassette", IF(A92="gemheart", "Crystal Heart", IF(A92="strawberry", _xlfn.CONCAT("Strawberry ", D92+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B92)*(regions!$B$2:$B$28=C92), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E92">_xlfn.CONCAT(IF(A92="completion", "Completion", IF(A92="cassette", "Cassette", IF(A92="gemheart", "Crystal Heart", IF(A92="strawberry", _xlfn.CONCAT("Strawberry ", D92+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B92)*(regions!$B$2:$B$27=C92), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 13 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F92" t="str">
@@ -2676,7 +2673,7 @@
         <v>13</v>
       </c>
       <c r="E93" t="str" cm="1">
-        <f t="array" ref="E93">_xlfn.CONCAT(IF(A93="completion", "Completion", IF(A93="cassette", "Cassette", IF(A93="gemheart", "Crystal Heart", IF(A93="strawberry", _xlfn.CONCAT("Strawberry ", D93+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B93)*(regions!$B$2:$B$28=C93), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E93">_xlfn.CONCAT(IF(A93="completion", "Completion", IF(A93="cassette", "Cassette", IF(A93="gemheart", "Crystal Heart", IF(A93="strawberry", _xlfn.CONCAT("Strawberry ", D93+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B93)*(regions!$B$2:$B$27=C93), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 14 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F93" t="str">
@@ -2699,7 +2696,7 @@
         <v>14</v>
       </c>
       <c r="E94" t="str" cm="1">
-        <f t="array" ref="E94">_xlfn.CONCAT(IF(A94="completion", "Completion", IF(A94="cassette", "Cassette", IF(A94="gemheart", "Crystal Heart", IF(A94="strawberry", _xlfn.CONCAT("Strawberry ", D94+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B94)*(regions!$B$2:$B$28=C94), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E94">_xlfn.CONCAT(IF(A94="completion", "Completion", IF(A94="cassette", "Cassette", IF(A94="gemheart", "Crystal Heart", IF(A94="strawberry", _xlfn.CONCAT("Strawberry ", D94+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B94)*(regions!$B$2:$B$27=C94), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 15 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F94" t="str">
@@ -2722,7 +2719,7 @@
         <v>15</v>
       </c>
       <c r="E95" t="str" cm="1">
-        <f t="array" ref="E95">_xlfn.CONCAT(IF(A95="completion", "Completion", IF(A95="cassette", "Cassette", IF(A95="gemheart", "Crystal Heart", IF(A95="strawberry", _xlfn.CONCAT("Strawberry ", D95+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B95)*(regions!$B$2:$B$28=C95), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E95">_xlfn.CONCAT(IF(A95="completion", "Completion", IF(A95="cassette", "Cassette", IF(A95="gemheart", "Crystal Heart", IF(A95="strawberry", _xlfn.CONCAT("Strawberry ", D95+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B95)*(regions!$B$2:$B$27=C95), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 16 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F95" t="str">
@@ -2745,7 +2742,7 @@
         <v>16</v>
       </c>
       <c r="E96" t="str" cm="1">
-        <f t="array" ref="E96">_xlfn.CONCAT(IF(A96="completion", "Completion", IF(A96="cassette", "Cassette", IF(A96="gemheart", "Crystal Heart", IF(A96="strawberry", _xlfn.CONCAT("Strawberry ", D96+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B96)*(regions!$B$2:$B$28=C96), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E96">_xlfn.CONCAT(IF(A96="completion", "Completion", IF(A96="cassette", "Cassette", IF(A96="gemheart", "Crystal Heart", IF(A96="strawberry", _xlfn.CONCAT("Strawberry ", D96+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B96)*(regions!$B$2:$B$27=C96), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 17 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F96" t="str">
@@ -2768,7 +2765,7 @@
         <v>17</v>
       </c>
       <c r="E97" t="str" cm="1">
-        <f t="array" ref="E97">_xlfn.CONCAT(IF(A97="completion", "Completion", IF(A97="cassette", "Cassette", IF(A97="gemheart", "Crystal Heart", IF(A97="strawberry", _xlfn.CONCAT("Strawberry ", D97+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B97)*(regions!$B$2:$B$28=C97), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E97">_xlfn.CONCAT(IF(A97="completion", "Completion", IF(A97="cassette", "Cassette", IF(A97="gemheart", "Crystal Heart", IF(A97="strawberry", _xlfn.CONCAT("Strawberry ", D97+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B97)*(regions!$B$2:$B$27=C97), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 18 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F97" t="str">
@@ -2791,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="str" cm="1">
-        <f t="array" ref="E98">_xlfn.CONCAT(IF(A98="completion", "Completion", IF(A98="cassette", "Cassette", IF(A98="gemheart", "Crystal Heart", IF(A98="strawberry", _xlfn.CONCAT("Strawberry ", D98+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B98)*(regions!$B$2:$B$28=C98), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E98">_xlfn.CONCAT(IF(A98="completion", "Completion", IF(A98="cassette", "Cassette", IF(A98="gemheart", "Crystal Heart", IF(A98="strawberry", _xlfn.CONCAT("Strawberry ", D98+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B98)*(regions!$B$2:$B$27=C98), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F98" t="str">
@@ -2814,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="E99" t="str" cm="1">
-        <f t="array" ref="E99">_xlfn.CONCAT(IF(A99="completion", "Completion", IF(A99="cassette", "Cassette", IF(A99="gemheart", "Crystal Heart", IF(A99="strawberry", _xlfn.CONCAT("Strawberry ", D99+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B99)*(regions!$B$2:$B$28=C99), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E99">_xlfn.CONCAT(IF(A99="completion", "Completion", IF(A99="cassette", "Cassette", IF(A99="gemheart", "Crystal Heart", IF(A99="strawberry", _xlfn.CONCAT("Strawberry ", D99+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B99)*(regions!$B$2:$B$27=C99), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F99" t="str">
@@ -2837,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="E100" t="str" cm="1">
-        <f t="array" ref="E100">_xlfn.CONCAT(IF(A100="completion", "Completion", IF(A100="cassette", "Cassette", IF(A100="gemheart", "Crystal Heart", IF(A100="strawberry", _xlfn.CONCAT("Strawberry ", D100+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B100)*(regions!$B$2:$B$28=C100), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E100">_xlfn.CONCAT(IF(A100="completion", "Completion", IF(A100="cassette", "Cassette", IF(A100="gemheart", "Crystal Heart", IF(A100="strawberry", _xlfn.CONCAT("Strawberry ", D100+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B100)*(regions!$B$2:$B$27=C100), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F100" t="str">
@@ -2860,7 +2857,7 @@
         <v>3</v>
       </c>
       <c r="E101" t="str" cm="1">
-        <f t="array" ref="E101">_xlfn.CONCAT(IF(A101="completion", "Completion", IF(A101="cassette", "Cassette", IF(A101="gemheart", "Crystal Heart", IF(A101="strawberry", _xlfn.CONCAT("Strawberry ", D101+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B101)*(regions!$B$2:$B$28=C101), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E101">_xlfn.CONCAT(IF(A101="completion", "Completion", IF(A101="cassette", "Cassette", IF(A101="gemheart", "Crystal Heart", IF(A101="strawberry", _xlfn.CONCAT("Strawberry ", D101+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B101)*(regions!$B$2:$B$27=C101), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F101" t="str">
@@ -2883,7 +2880,7 @@
         <v>4</v>
       </c>
       <c r="E102" t="str" cm="1">
-        <f t="array" ref="E102">_xlfn.CONCAT(IF(A102="completion", "Completion", IF(A102="cassette", "Cassette", IF(A102="gemheart", "Crystal Heart", IF(A102="strawberry", _xlfn.CONCAT("Strawberry ", D102+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B102)*(regions!$B$2:$B$28=C102), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E102">_xlfn.CONCAT(IF(A102="completion", "Completion", IF(A102="cassette", "Cassette", IF(A102="gemheart", "Crystal Heart", IF(A102="strawberry", _xlfn.CONCAT("Strawberry ", D102+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B102)*(regions!$B$2:$B$27=C102), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F102" t="str">
@@ -2906,7 +2903,7 @@
         <v>5</v>
       </c>
       <c r="E103" t="str" cm="1">
-        <f t="array" ref="E103">_xlfn.CONCAT(IF(A103="completion", "Completion", IF(A103="cassette", "Cassette", IF(A103="gemheart", "Crystal Heart", IF(A103="strawberry", _xlfn.CONCAT("Strawberry ", D103+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B103)*(regions!$B$2:$B$28=C103), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E103">_xlfn.CONCAT(IF(A103="completion", "Completion", IF(A103="cassette", "Cassette", IF(A103="gemheart", "Crystal Heart", IF(A103="strawberry", _xlfn.CONCAT("Strawberry ", D103+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B103)*(regions!$B$2:$B$27=C103), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 6 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F103" t="str">
@@ -2929,7 +2926,7 @@
         <v>6</v>
       </c>
       <c r="E104" t="str" cm="1">
-        <f t="array" ref="E104">_xlfn.CONCAT(IF(A104="completion", "Completion", IF(A104="cassette", "Cassette", IF(A104="gemheart", "Crystal Heart", IF(A104="strawberry", _xlfn.CONCAT("Strawberry ", D104+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B104)*(regions!$B$2:$B$28=C104), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E104">_xlfn.CONCAT(IF(A104="completion", "Completion", IF(A104="cassette", "Cassette", IF(A104="gemheart", "Crystal Heart", IF(A104="strawberry", _xlfn.CONCAT("Strawberry ", D104+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B104)*(regions!$B$2:$B$27=C104), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 7 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F104" t="str">
@@ -2952,7 +2949,7 @@
         <v>7</v>
       </c>
       <c r="E105" t="str" cm="1">
-        <f t="array" ref="E105">_xlfn.CONCAT(IF(A105="completion", "Completion", IF(A105="cassette", "Cassette", IF(A105="gemheart", "Crystal Heart", IF(A105="strawberry", _xlfn.CONCAT("Strawberry ", D105+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B105)*(regions!$B$2:$B$28=C105), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E105">_xlfn.CONCAT(IF(A105="completion", "Completion", IF(A105="cassette", "Cassette", IF(A105="gemheart", "Crystal Heart", IF(A105="strawberry", _xlfn.CONCAT("Strawberry ", D105+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B105)*(regions!$B$2:$B$27=C105), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 8 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F105" t="str">
@@ -2975,7 +2972,7 @@
         <v>8</v>
       </c>
       <c r="E106" t="str" cm="1">
-        <f t="array" ref="E106">_xlfn.CONCAT(IF(A106="completion", "Completion", IF(A106="cassette", "Cassette", IF(A106="gemheart", "Crystal Heart", IF(A106="strawberry", _xlfn.CONCAT("Strawberry ", D106+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B106)*(regions!$B$2:$B$28=C106), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E106">_xlfn.CONCAT(IF(A106="completion", "Completion", IF(A106="cassette", "Cassette", IF(A106="gemheart", "Crystal Heart", IF(A106="strawberry", _xlfn.CONCAT("Strawberry ", D106+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B106)*(regions!$B$2:$B$27=C106), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 9 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F106" t="str">
@@ -2998,7 +2995,7 @@
         <v>9</v>
       </c>
       <c r="E107" t="str" cm="1">
-        <f t="array" ref="E107">_xlfn.CONCAT(IF(A107="completion", "Completion", IF(A107="cassette", "Cassette", IF(A107="gemheart", "Crystal Heart", IF(A107="strawberry", _xlfn.CONCAT("Strawberry ", D107+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B107)*(regions!$B$2:$B$28=C107), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E107">_xlfn.CONCAT(IF(A107="completion", "Completion", IF(A107="cassette", "Cassette", IF(A107="gemheart", "Crystal Heart", IF(A107="strawberry", _xlfn.CONCAT("Strawberry ", D107+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B107)*(regions!$B$2:$B$27=C107), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 10 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F107" t="str">
@@ -3021,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="E108" t="str" cm="1">
-        <f t="array" ref="E108">_xlfn.CONCAT(IF(A108="completion", "Completion", IF(A108="cassette", "Cassette", IF(A108="gemheart", "Crystal Heart", IF(A108="strawberry", _xlfn.CONCAT("Strawberry ", D108+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B108)*(regions!$B$2:$B$28=C108), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E108">_xlfn.CONCAT(IF(A108="completion", "Completion", IF(A108="cassette", "Cassette", IF(A108="gemheart", "Crystal Heart", IF(A108="strawberry", _xlfn.CONCAT("Strawberry ", D108+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B108)*(regions!$B$2:$B$27=C108), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 11 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F108" t="str">
@@ -3044,7 +3041,7 @@
         <v>11</v>
       </c>
       <c r="E109" t="str" cm="1">
-        <f t="array" ref="E109">_xlfn.CONCAT(IF(A109="completion", "Completion", IF(A109="cassette", "Cassette", IF(A109="gemheart", "Crystal Heart", IF(A109="strawberry", _xlfn.CONCAT("Strawberry ", D109+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B109)*(regions!$B$2:$B$28=C109), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E109">_xlfn.CONCAT(IF(A109="completion", "Completion", IF(A109="cassette", "Cassette", IF(A109="gemheart", "Crystal Heart", IF(A109="strawberry", _xlfn.CONCAT("Strawberry ", D109+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B109)*(regions!$B$2:$B$27=C109), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 12 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F109" t="str">
@@ -3067,7 +3064,7 @@
         <v>12</v>
       </c>
       <c r="E110" t="str" cm="1">
-        <f t="array" ref="E110">_xlfn.CONCAT(IF(A110="completion", "Completion", IF(A110="cassette", "Cassette", IF(A110="gemheart", "Crystal Heart", IF(A110="strawberry", _xlfn.CONCAT("Strawberry ", D110+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B110)*(regions!$B$2:$B$28=C110), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E110">_xlfn.CONCAT(IF(A110="completion", "Completion", IF(A110="cassette", "Cassette", IF(A110="gemheart", "Crystal Heart", IF(A110="strawberry", _xlfn.CONCAT("Strawberry ", D110+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B110)*(regions!$B$2:$B$27=C110), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 13 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F110" t="str">
@@ -3090,7 +3087,7 @@
         <v>13</v>
       </c>
       <c r="E111" t="str" cm="1">
-        <f t="array" ref="E111">_xlfn.CONCAT(IF(A111="completion", "Completion", IF(A111="cassette", "Cassette", IF(A111="gemheart", "Crystal Heart", IF(A111="strawberry", _xlfn.CONCAT("Strawberry ", D111+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B111)*(regions!$B$2:$B$28=C111), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E111">_xlfn.CONCAT(IF(A111="completion", "Completion", IF(A111="cassette", "Cassette", IF(A111="gemheart", "Crystal Heart", IF(A111="strawberry", _xlfn.CONCAT("Strawberry ", D111+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B111)*(regions!$B$2:$B$27=C111), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 14 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F111" t="str">
@@ -3113,7 +3110,7 @@
         <v>14</v>
       </c>
       <c r="E112" t="str" cm="1">
-        <f t="array" ref="E112">_xlfn.CONCAT(IF(A112="completion", "Completion", IF(A112="cassette", "Cassette", IF(A112="gemheart", "Crystal Heart", IF(A112="strawberry", _xlfn.CONCAT("Strawberry ", D112+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B112)*(regions!$B$2:$B$28=C112), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E112">_xlfn.CONCAT(IF(A112="completion", "Completion", IF(A112="cassette", "Cassette", IF(A112="gemheart", "Crystal Heart", IF(A112="strawberry", _xlfn.CONCAT("Strawberry ", D112+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B112)*(regions!$B$2:$B$27=C112), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 15 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F112" t="str">
@@ -3136,7 +3133,7 @@
         <v>15</v>
       </c>
       <c r="E113" t="str" cm="1">
-        <f t="array" ref="E113">_xlfn.CONCAT(IF(A113="completion", "Completion", IF(A113="cassette", "Cassette", IF(A113="gemheart", "Crystal Heart", IF(A113="strawberry", _xlfn.CONCAT("Strawberry ", D113+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B113)*(regions!$B$2:$B$28=C113), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E113">_xlfn.CONCAT(IF(A113="completion", "Completion", IF(A113="cassette", "Cassette", IF(A113="gemheart", "Crystal Heart", IF(A113="strawberry", _xlfn.CONCAT("Strawberry ", D113+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B113)*(regions!$B$2:$B$27=C113), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 16 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F113" t="str">
@@ -3159,7 +3156,7 @@
         <v>16</v>
       </c>
       <c r="E114" t="str" cm="1">
-        <f t="array" ref="E114">_xlfn.CONCAT(IF(A114="completion", "Completion", IF(A114="cassette", "Cassette", IF(A114="gemheart", "Crystal Heart", IF(A114="strawberry", _xlfn.CONCAT("Strawberry ", D114+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B114)*(regions!$B$2:$B$28=C114), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E114">_xlfn.CONCAT(IF(A114="completion", "Completion", IF(A114="cassette", "Cassette", IF(A114="gemheart", "Crystal Heart", IF(A114="strawberry", _xlfn.CONCAT("Strawberry ", D114+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B114)*(regions!$B$2:$B$27=C114), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 17 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F114" t="str">
@@ -3182,7 +3179,7 @@
         <v>17</v>
       </c>
       <c r="E115" t="str" cm="1">
-        <f t="array" ref="E115">_xlfn.CONCAT(IF(A115="completion", "Completion", IF(A115="cassette", "Cassette", IF(A115="gemheart", "Crystal Heart", IF(A115="strawberry", _xlfn.CONCAT("Strawberry ", D115+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B115)*(regions!$B$2:$B$28=C115), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E115">_xlfn.CONCAT(IF(A115="completion", "Completion", IF(A115="cassette", "Cassette", IF(A115="gemheart", "Crystal Heart", IF(A115="strawberry", _xlfn.CONCAT("Strawberry ", D115+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B115)*(regions!$B$2:$B$27=C115), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 18 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F115" t="str">
@@ -3205,7 +3202,7 @@
         <v>18</v>
       </c>
       <c r="E116" t="str" cm="1">
-        <f t="array" ref="E116">_xlfn.CONCAT(IF(A116="completion", "Completion", IF(A116="cassette", "Cassette", IF(A116="gemheart", "Crystal Heart", IF(A116="strawberry", _xlfn.CONCAT("Strawberry ", D116+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B116)*(regions!$B$2:$B$28=C116), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E116">_xlfn.CONCAT(IF(A116="completion", "Completion", IF(A116="cassette", "Cassette", IF(A116="gemheart", "Crystal Heart", IF(A116="strawberry", _xlfn.CONCAT("Strawberry ", D116+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B116)*(regions!$B$2:$B$27=C116), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 19 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F116" t="str">
@@ -3228,7 +3225,7 @@
         <v>19</v>
       </c>
       <c r="E117" t="str" cm="1">
-        <f t="array" ref="E117">_xlfn.CONCAT(IF(A117="completion", "Completion", IF(A117="cassette", "Cassette", IF(A117="gemheart", "Crystal Heart", IF(A117="strawberry", _xlfn.CONCAT("Strawberry ", D117+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B117)*(regions!$B$2:$B$28=C117), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E117">_xlfn.CONCAT(IF(A117="completion", "Completion", IF(A117="cassette", "Cassette", IF(A117="gemheart", "Crystal Heart", IF(A117="strawberry", _xlfn.CONCAT("Strawberry ", D117+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B117)*(regions!$B$2:$B$27=C117), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 20 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F117" t="str">
@@ -3251,7 +3248,7 @@
         <v>20</v>
       </c>
       <c r="E118" t="str" cm="1">
-        <f t="array" ref="E118">_xlfn.CONCAT(IF(A118="completion", "Completion", IF(A118="cassette", "Cassette", IF(A118="gemheart", "Crystal Heart", IF(A118="strawberry", _xlfn.CONCAT("Strawberry ", D118+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B118)*(regions!$B$2:$B$28=C118), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E118">_xlfn.CONCAT(IF(A118="completion", "Completion", IF(A118="cassette", "Cassette", IF(A118="gemheart", "Crystal Heart", IF(A118="strawberry", _xlfn.CONCAT("Strawberry ", D118+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B118)*(regions!$B$2:$B$27=C118), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 21 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F118" t="str">
@@ -3274,7 +3271,7 @@
         <v>21</v>
       </c>
       <c r="E119" t="str" cm="1">
-        <f t="array" ref="E119">_xlfn.CONCAT(IF(A119="completion", "Completion", IF(A119="cassette", "Cassette", IF(A119="gemheart", "Crystal Heart", IF(A119="strawberry", _xlfn.CONCAT("Strawberry ", D119+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B119)*(regions!$B$2:$B$28=C119), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E119">_xlfn.CONCAT(IF(A119="completion", "Completion", IF(A119="cassette", "Cassette", IF(A119="gemheart", "Crystal Heart", IF(A119="strawberry", _xlfn.CONCAT("Strawberry ", D119+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B119)*(regions!$B$2:$B$27=C119), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 22 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F119" t="str">
@@ -3297,7 +3294,7 @@
         <v>22</v>
       </c>
       <c r="E120" t="str" cm="1">
-        <f t="array" ref="E120">_xlfn.CONCAT(IF(A120="completion", "Completion", IF(A120="cassette", "Cassette", IF(A120="gemheart", "Crystal Heart", IF(A120="strawberry", _xlfn.CONCAT("Strawberry ", D120+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B120)*(regions!$B$2:$B$28=C120), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E120">_xlfn.CONCAT(IF(A120="completion", "Completion", IF(A120="cassette", "Cassette", IF(A120="gemheart", "Crystal Heart", IF(A120="strawberry", _xlfn.CONCAT("Strawberry ", D120+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B120)*(regions!$B$2:$B$27=C120), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 23 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F120" t="str">
@@ -3320,7 +3317,7 @@
         <v>23</v>
       </c>
       <c r="E121" t="str" cm="1">
-        <f t="array" ref="E121">_xlfn.CONCAT(IF(A121="completion", "Completion", IF(A121="cassette", "Cassette", IF(A121="gemheart", "Crystal Heart", IF(A121="strawberry", _xlfn.CONCAT("Strawberry ", D121+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B121)*(regions!$B$2:$B$28=C121), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E121">_xlfn.CONCAT(IF(A121="completion", "Completion", IF(A121="cassette", "Cassette", IF(A121="gemheart", "Crystal Heart", IF(A121="strawberry", _xlfn.CONCAT("Strawberry ", D121+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B121)*(regions!$B$2:$B$27=C121), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 24 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F121" t="str">
@@ -3343,7 +3340,7 @@
         <v>24</v>
       </c>
       <c r="E122" t="str" cm="1">
-        <f t="array" ref="E122">_xlfn.CONCAT(IF(A122="completion", "Completion", IF(A122="cassette", "Cassette", IF(A122="gemheart", "Crystal Heart", IF(A122="strawberry", _xlfn.CONCAT("Strawberry ", D122+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B122)*(regions!$B$2:$B$28=C122), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E122">_xlfn.CONCAT(IF(A122="completion", "Completion", IF(A122="cassette", "Cassette", IF(A122="gemheart", "Crystal Heart", IF(A122="strawberry", _xlfn.CONCAT("Strawberry ", D122+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B122)*(regions!$B$2:$B$27=C122), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 25 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F122" t="str">
@@ -3366,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="E123" t="str" cm="1">
-        <f t="array" ref="E123">_xlfn.CONCAT(IF(A123="completion", "Completion", IF(A123="cassette", "Cassette", IF(A123="gemheart", "Crystal Heart", IF(A123="strawberry", _xlfn.CONCAT("Strawberry ", D123+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B123)*(regions!$B$2:$B$28=C123), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E123">_xlfn.CONCAT(IF(A123="completion", "Completion", IF(A123="cassette", "Cassette", IF(A123="gemheart", "Crystal Heart", IF(A123="strawberry", _xlfn.CONCAT("Strawberry ", D123+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B123)*(regions!$B$2:$B$27=C123), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F123" t="str">
@@ -3389,7 +3386,7 @@
         <v>1</v>
       </c>
       <c r="E124" t="str" cm="1">
-        <f t="array" ref="E124">_xlfn.CONCAT(IF(A124="completion", "Completion", IF(A124="cassette", "Cassette", IF(A124="gemheart", "Crystal Heart", IF(A124="strawberry", _xlfn.CONCAT("Strawberry ", D124+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B124)*(regions!$B$2:$B$28=C124), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E124">_xlfn.CONCAT(IF(A124="completion", "Completion", IF(A124="cassette", "Cassette", IF(A124="gemheart", "Crystal Heart", IF(A124="strawberry", _xlfn.CONCAT("Strawberry ", D124+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B124)*(regions!$B$2:$B$27=C124), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F124" t="str">
@@ -3412,7 +3409,7 @@
         <v>2</v>
       </c>
       <c r="E125" t="str" cm="1">
-        <f t="array" ref="E125">_xlfn.CONCAT(IF(A125="completion", "Completion", IF(A125="cassette", "Cassette", IF(A125="gemheart", "Crystal Heart", IF(A125="strawberry", _xlfn.CONCAT("Strawberry ", D125+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B125)*(regions!$B$2:$B$28=C125), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E125">_xlfn.CONCAT(IF(A125="completion", "Completion", IF(A125="cassette", "Cassette", IF(A125="gemheart", "Crystal Heart", IF(A125="strawberry", _xlfn.CONCAT("Strawberry ", D125+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B125)*(regions!$B$2:$B$27=C125), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F125" t="str">
@@ -3435,7 +3432,7 @@
         <v>3</v>
       </c>
       <c r="E126" t="str" cm="1">
-        <f t="array" ref="E126">_xlfn.CONCAT(IF(A126="completion", "Completion", IF(A126="cassette", "Cassette", IF(A126="gemheart", "Crystal Heart", IF(A126="strawberry", _xlfn.CONCAT("Strawberry ", D126+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B126)*(regions!$B$2:$B$28=C126), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E126">_xlfn.CONCAT(IF(A126="completion", "Completion", IF(A126="cassette", "Cassette", IF(A126="gemheart", "Crystal Heart", IF(A126="strawberry", _xlfn.CONCAT("Strawberry ", D126+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B126)*(regions!$B$2:$B$27=C126), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F126" t="str">
@@ -3458,7 +3455,7 @@
         <v>4</v>
       </c>
       <c r="E127" t="str" cm="1">
-        <f t="array" ref="E127">_xlfn.CONCAT(IF(A127="completion", "Completion", IF(A127="cassette", "Cassette", IF(A127="gemheart", "Crystal Heart", IF(A127="strawberry", _xlfn.CONCAT("Strawberry ", D127+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B127)*(regions!$B$2:$B$28=C127), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E127">_xlfn.CONCAT(IF(A127="completion", "Completion", IF(A127="cassette", "Cassette", IF(A127="gemheart", "Crystal Heart", IF(A127="strawberry", _xlfn.CONCAT("Strawberry ", D127+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B127)*(regions!$B$2:$B$27=C127), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F127" t="str">
@@ -3481,7 +3478,7 @@
         <v>5</v>
       </c>
       <c r="E128" t="str" cm="1">
-        <f t="array" ref="E128">_xlfn.CONCAT(IF(A128="completion", "Completion", IF(A128="cassette", "Cassette", IF(A128="gemheart", "Crystal Heart", IF(A128="strawberry", _xlfn.CONCAT("Strawberry ", D128+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B128)*(regions!$B$2:$B$28=C128), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E128">_xlfn.CONCAT(IF(A128="completion", "Completion", IF(A128="cassette", "Cassette", IF(A128="gemheart", "Crystal Heart", IF(A128="strawberry", _xlfn.CONCAT("Strawberry ", D128+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B128)*(regions!$B$2:$B$27=C128), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 6 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F128" t="str">
@@ -3504,7 +3501,7 @@
         <v>6</v>
       </c>
       <c r="E129" t="str" cm="1">
-        <f t="array" ref="E129">_xlfn.CONCAT(IF(A129="completion", "Completion", IF(A129="cassette", "Cassette", IF(A129="gemheart", "Crystal Heart", IF(A129="strawberry", _xlfn.CONCAT("Strawberry ", D129+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B129)*(regions!$B$2:$B$28=C129), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E129">_xlfn.CONCAT(IF(A129="completion", "Completion", IF(A129="cassette", "Cassette", IF(A129="gemheart", "Crystal Heart", IF(A129="strawberry", _xlfn.CONCAT("Strawberry ", D129+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B129)*(regions!$B$2:$B$27=C129), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 7 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F129" t="str">
@@ -3527,7 +3524,7 @@
         <v>7</v>
       </c>
       <c r="E130" t="str" cm="1">
-        <f t="array" ref="E130">_xlfn.CONCAT(IF(A130="completion", "Completion", IF(A130="cassette", "Cassette", IF(A130="gemheart", "Crystal Heart", IF(A130="strawberry", _xlfn.CONCAT("Strawberry ", D130+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B130)*(regions!$B$2:$B$28=C130), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E130">_xlfn.CONCAT(IF(A130="completion", "Completion", IF(A130="cassette", "Cassette", IF(A130="gemheart", "Crystal Heart", IF(A130="strawberry", _xlfn.CONCAT("Strawberry ", D130+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B130)*(regions!$B$2:$B$27=C130), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 8 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F130" t="str">
@@ -3550,7 +3547,7 @@
         <v>8</v>
       </c>
       <c r="E131" t="str" cm="1">
-        <f t="array" ref="E131">_xlfn.CONCAT(IF(A131="completion", "Completion", IF(A131="cassette", "Cassette", IF(A131="gemheart", "Crystal Heart", IF(A131="strawberry", _xlfn.CONCAT("Strawberry ", D131+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B131)*(regions!$B$2:$B$28=C131), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E131">_xlfn.CONCAT(IF(A131="completion", "Completion", IF(A131="cassette", "Cassette", IF(A131="gemheart", "Crystal Heart", IF(A131="strawberry", _xlfn.CONCAT("Strawberry ", D131+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B131)*(regions!$B$2:$B$27=C131), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 9 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F131" t="str">
@@ -3573,7 +3570,7 @@
         <v>9</v>
       </c>
       <c r="E132" t="str" cm="1">
-        <f t="array" ref="E132">_xlfn.CONCAT(IF(A132="completion", "Completion", IF(A132="cassette", "Cassette", IF(A132="gemheart", "Crystal Heart", IF(A132="strawberry", _xlfn.CONCAT("Strawberry ", D132+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B132)*(regions!$B$2:$B$28=C132), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E132">_xlfn.CONCAT(IF(A132="completion", "Completion", IF(A132="cassette", "Cassette", IF(A132="gemheart", "Crystal Heart", IF(A132="strawberry", _xlfn.CONCAT("Strawberry ", D132+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B132)*(regions!$B$2:$B$27=C132), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 10 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F132" t="str">
@@ -3596,7 +3593,7 @@
         <v>10</v>
       </c>
       <c r="E133" t="str" cm="1">
-        <f t="array" ref="E133">_xlfn.CONCAT(IF(A133="completion", "Completion", IF(A133="cassette", "Cassette", IF(A133="gemheart", "Crystal Heart", IF(A133="strawberry", _xlfn.CONCAT("Strawberry ", D133+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B133)*(regions!$B$2:$B$28=C133), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E133">_xlfn.CONCAT(IF(A133="completion", "Completion", IF(A133="cassette", "Cassette", IF(A133="gemheart", "Crystal Heart", IF(A133="strawberry", _xlfn.CONCAT("Strawberry ", D133+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B133)*(regions!$B$2:$B$27=C133), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 11 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F133" t="str">
@@ -3619,7 +3616,7 @@
         <v>11</v>
       </c>
       <c r="E134" t="str" cm="1">
-        <f t="array" ref="E134">_xlfn.CONCAT(IF(A134="completion", "Completion", IF(A134="cassette", "Cassette", IF(A134="gemheart", "Crystal Heart", IF(A134="strawberry", _xlfn.CONCAT("Strawberry ", D134+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B134)*(regions!$B$2:$B$28=C134), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E134">_xlfn.CONCAT(IF(A134="completion", "Completion", IF(A134="cassette", "Cassette", IF(A134="gemheart", "Crystal Heart", IF(A134="strawberry", _xlfn.CONCAT("Strawberry ", D134+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B134)*(regions!$B$2:$B$27=C134), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 12 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F134" t="str">
@@ -3642,7 +3639,7 @@
         <v>12</v>
       </c>
       <c r="E135" t="str" cm="1">
-        <f t="array" ref="E135">_xlfn.CONCAT(IF(A135="completion", "Completion", IF(A135="cassette", "Cassette", IF(A135="gemheart", "Crystal Heart", IF(A135="strawberry", _xlfn.CONCAT("Strawberry ", D135+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B135)*(regions!$B$2:$B$28=C135), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E135">_xlfn.CONCAT(IF(A135="completion", "Completion", IF(A135="cassette", "Cassette", IF(A135="gemheart", "Crystal Heart", IF(A135="strawberry", _xlfn.CONCAT("Strawberry ", D135+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B135)*(regions!$B$2:$B$27=C135), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 13 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F135" t="str">
@@ -3665,7 +3662,7 @@
         <v>13</v>
       </c>
       <c r="E136" t="str" cm="1">
-        <f t="array" ref="E136">_xlfn.CONCAT(IF(A136="completion", "Completion", IF(A136="cassette", "Cassette", IF(A136="gemheart", "Crystal Heart", IF(A136="strawberry", _xlfn.CONCAT("Strawberry ", D136+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B136)*(regions!$B$2:$B$28=C136), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E136">_xlfn.CONCAT(IF(A136="completion", "Completion", IF(A136="cassette", "Cassette", IF(A136="gemheart", "Crystal Heart", IF(A136="strawberry", _xlfn.CONCAT("Strawberry ", D136+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B136)*(regions!$B$2:$B$27=C136), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 14 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F136" t="str">
@@ -3688,7 +3685,7 @@
         <v>14</v>
       </c>
       <c r="E137" t="str" cm="1">
-        <f t="array" ref="E137">_xlfn.CONCAT(IF(A137="completion", "Completion", IF(A137="cassette", "Cassette", IF(A137="gemheart", "Crystal Heart", IF(A137="strawberry", _xlfn.CONCAT("Strawberry ", D137+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B137)*(regions!$B$2:$B$28=C137), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E137">_xlfn.CONCAT(IF(A137="completion", "Completion", IF(A137="cassette", "Cassette", IF(A137="gemheart", "Crystal Heart", IF(A137="strawberry", _xlfn.CONCAT("Strawberry ", D137+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B137)*(regions!$B$2:$B$27=C137), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 15 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F137" t="str">
@@ -3711,7 +3708,7 @@
         <v>15</v>
       </c>
       <c r="E138" t="str" cm="1">
-        <f t="array" ref="E138">_xlfn.CONCAT(IF(A138="completion", "Completion", IF(A138="cassette", "Cassette", IF(A138="gemheart", "Crystal Heart", IF(A138="strawberry", _xlfn.CONCAT("Strawberry ", D138+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B138)*(regions!$B$2:$B$28=C138), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E138">_xlfn.CONCAT(IF(A138="completion", "Completion", IF(A138="cassette", "Cassette", IF(A138="gemheart", "Crystal Heart", IF(A138="strawberry", _xlfn.CONCAT("Strawberry ", D138+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B138)*(regions!$B$2:$B$27=C138), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 16 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F138" t="str">
@@ -3734,7 +3731,7 @@
         <v>16</v>
       </c>
       <c r="E139" t="str" cm="1">
-        <f t="array" ref="E139">_xlfn.CONCAT(IF(A139="completion", "Completion", IF(A139="cassette", "Cassette", IF(A139="gemheart", "Crystal Heart", IF(A139="strawberry", _xlfn.CONCAT("Strawberry ", D139+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B139)*(regions!$B$2:$B$28=C139), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E139">_xlfn.CONCAT(IF(A139="completion", "Completion", IF(A139="cassette", "Cassette", IF(A139="gemheart", "Crystal Heart", IF(A139="strawberry", _xlfn.CONCAT("Strawberry ", D139+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B139)*(regions!$B$2:$B$27=C139), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 17 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F139" t="str">
@@ -3757,7 +3754,7 @@
         <v>17</v>
       </c>
       <c r="E140" t="str" cm="1">
-        <f t="array" ref="E140">_xlfn.CONCAT(IF(A140="completion", "Completion", IF(A140="cassette", "Cassette", IF(A140="gemheart", "Crystal Heart", IF(A140="strawberry", _xlfn.CONCAT("Strawberry ", D140+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B140)*(regions!$B$2:$B$28=C140), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E140">_xlfn.CONCAT(IF(A140="completion", "Completion", IF(A140="cassette", "Cassette", IF(A140="gemheart", "Crystal Heart", IF(A140="strawberry", _xlfn.CONCAT("Strawberry ", D140+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B140)*(regions!$B$2:$B$27=C140), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 18 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F140" t="str">
@@ -3780,7 +3777,7 @@
         <v>18</v>
       </c>
       <c r="E141" t="str" cm="1">
-        <f t="array" ref="E141">_xlfn.CONCAT(IF(A141="completion", "Completion", IF(A141="cassette", "Cassette", IF(A141="gemheart", "Crystal Heart", IF(A141="strawberry", _xlfn.CONCAT("Strawberry ", D141+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B141)*(regions!$B$2:$B$28=C141), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E141">_xlfn.CONCAT(IF(A141="completion", "Completion", IF(A141="cassette", "Cassette", IF(A141="gemheart", "Crystal Heart", IF(A141="strawberry", _xlfn.CONCAT("Strawberry ", D141+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B141)*(regions!$B$2:$B$27=C141), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 19 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F141" t="str">
@@ -3803,7 +3800,7 @@
         <v>19</v>
       </c>
       <c r="E142" t="str" cm="1">
-        <f t="array" ref="E142">_xlfn.CONCAT(IF(A142="completion", "Completion", IF(A142="cassette", "Cassette", IF(A142="gemheart", "Crystal Heart", IF(A142="strawberry", _xlfn.CONCAT("Strawberry ", D142+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B142)*(regions!$B$2:$B$28=C142), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E142">_xlfn.CONCAT(IF(A142="completion", "Completion", IF(A142="cassette", "Cassette", IF(A142="gemheart", "Crystal Heart", IF(A142="strawberry", _xlfn.CONCAT("Strawberry ", D142+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B142)*(regions!$B$2:$B$27=C142), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 20 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F142" t="str">
@@ -3826,7 +3823,7 @@
         <v>20</v>
       </c>
       <c r="E143" t="str" cm="1">
-        <f t="array" ref="E143">_xlfn.CONCAT(IF(A143="completion", "Completion", IF(A143="cassette", "Cassette", IF(A143="gemheart", "Crystal Heart", IF(A143="strawberry", _xlfn.CONCAT("Strawberry ", D143+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B143)*(regions!$B$2:$B$28=C143), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E143">_xlfn.CONCAT(IF(A143="completion", "Completion", IF(A143="cassette", "Cassette", IF(A143="gemheart", "Crystal Heart", IF(A143="strawberry", _xlfn.CONCAT("Strawberry ", D143+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B143)*(regions!$B$2:$B$27=C143), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 21 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F143" t="str">
@@ -3849,7 +3846,7 @@
         <v>21</v>
       </c>
       <c r="E144" t="str" cm="1">
-        <f t="array" ref="E144">_xlfn.CONCAT(IF(A144="completion", "Completion", IF(A144="cassette", "Cassette", IF(A144="gemheart", "Crystal Heart", IF(A144="strawberry", _xlfn.CONCAT("Strawberry ", D144+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B144)*(regions!$B$2:$B$28=C144), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E144">_xlfn.CONCAT(IF(A144="completion", "Completion", IF(A144="cassette", "Cassette", IF(A144="gemheart", "Crystal Heart", IF(A144="strawberry", _xlfn.CONCAT("Strawberry ", D144+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B144)*(regions!$B$2:$B$27=C144), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 22 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F144" t="str">
@@ -3872,7 +3869,7 @@
         <v>22</v>
       </c>
       <c r="E145" t="str" cm="1">
-        <f t="array" ref="E145">_xlfn.CONCAT(IF(A145="completion", "Completion", IF(A145="cassette", "Cassette", IF(A145="gemheart", "Crystal Heart", IF(A145="strawberry", _xlfn.CONCAT("Strawberry ", D145+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B145)*(regions!$B$2:$B$28=C145), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E145">_xlfn.CONCAT(IF(A145="completion", "Completion", IF(A145="cassette", "Cassette", IF(A145="gemheart", "Crystal Heart", IF(A145="strawberry", _xlfn.CONCAT("Strawberry ", D145+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B145)*(regions!$B$2:$B$27=C145), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 23 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F145" t="str">
@@ -3895,7 +3892,7 @@
         <v>23</v>
       </c>
       <c r="E146" t="str" cm="1">
-        <f t="array" ref="E146">_xlfn.CONCAT(IF(A146="completion", "Completion", IF(A146="cassette", "Cassette", IF(A146="gemheart", "Crystal Heart", IF(A146="strawberry", _xlfn.CONCAT("Strawberry ", D146+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B146)*(regions!$B$2:$B$28=C146), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E146">_xlfn.CONCAT(IF(A146="completion", "Completion", IF(A146="cassette", "Cassette", IF(A146="gemheart", "Crystal Heart", IF(A146="strawberry", _xlfn.CONCAT("Strawberry ", D146+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B146)*(regions!$B$2:$B$27=C146), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 24 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F146" t="str">
@@ -3918,7 +3915,7 @@
         <v>24</v>
       </c>
       <c r="E147" t="str" cm="1">
-        <f t="array" ref="E147">_xlfn.CONCAT(IF(A147="completion", "Completion", IF(A147="cassette", "Cassette", IF(A147="gemheart", "Crystal Heart", IF(A147="strawberry", _xlfn.CONCAT("Strawberry ", D147+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B147)*(regions!$B$2:$B$28=C147), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E147">_xlfn.CONCAT(IF(A147="completion", "Completion", IF(A147="cassette", "Cassette", IF(A147="gemheart", "Crystal Heart", IF(A147="strawberry", _xlfn.CONCAT("Strawberry ", D147+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B147)*(regions!$B$2:$B$27=C147), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 25 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F147" t="str">
@@ -3941,7 +3938,7 @@
         <v>25</v>
       </c>
       <c r="E148" t="str" cm="1">
-        <f t="array" ref="E148">_xlfn.CONCAT(IF(A148="completion", "Completion", IF(A148="cassette", "Cassette", IF(A148="gemheart", "Crystal Heart", IF(A148="strawberry", _xlfn.CONCAT("Strawberry ", D148+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B148)*(regions!$B$2:$B$28=C148), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E148">_xlfn.CONCAT(IF(A148="completion", "Completion", IF(A148="cassette", "Cassette", IF(A148="gemheart", "Crystal Heart", IF(A148="strawberry", _xlfn.CONCAT("Strawberry ", D148+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B148)*(regions!$B$2:$B$27=C148), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 26 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F148" t="str">
@@ -3964,7 +3961,7 @@
         <v>26</v>
       </c>
       <c r="E149" t="str" cm="1">
-        <f t="array" ref="E149">_xlfn.CONCAT(IF(A149="completion", "Completion", IF(A149="cassette", "Cassette", IF(A149="gemheart", "Crystal Heart", IF(A149="strawberry", _xlfn.CONCAT("Strawberry ", D149+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B149)*(regions!$B$2:$B$28=C149), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E149">_xlfn.CONCAT(IF(A149="completion", "Completion", IF(A149="cassette", "Cassette", IF(A149="gemheart", "Crystal Heart", IF(A149="strawberry", _xlfn.CONCAT("Strawberry ", D149+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B149)*(regions!$B$2:$B$27=C149), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 27 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F149" t="str">
@@ -3987,7 +3984,7 @@
         <v>27</v>
       </c>
       <c r="E150" t="str" cm="1">
-        <f t="array" ref="E150">_xlfn.CONCAT(IF(A150="completion", "Completion", IF(A150="cassette", "Cassette", IF(A150="gemheart", "Crystal Heart", IF(A150="strawberry", _xlfn.CONCAT("Strawberry ", D150+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B150)*(regions!$B$2:$B$28=C150), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E150">_xlfn.CONCAT(IF(A150="completion", "Completion", IF(A150="cassette", "Cassette", IF(A150="gemheart", "Crystal Heart", IF(A150="strawberry", _xlfn.CONCAT("Strawberry ", D150+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B150)*(regions!$B$2:$B$27=C150), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 28 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F150" t="str">
@@ -4010,7 +4007,7 @@
         <v>28</v>
       </c>
       <c r="E151" t="str" cm="1">
-        <f t="array" ref="E151">_xlfn.CONCAT(IF(A151="completion", "Completion", IF(A151="cassette", "Cassette", IF(A151="gemheart", "Crystal Heart", IF(A151="strawberry", _xlfn.CONCAT("Strawberry ", D151+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B151)*(regions!$B$2:$B$28=C151), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E151">_xlfn.CONCAT(IF(A151="completion", "Completion", IF(A151="cassette", "Cassette", IF(A151="gemheart", "Crystal Heart", IF(A151="strawberry", _xlfn.CONCAT("Strawberry ", D151+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B151)*(regions!$B$2:$B$27=C151), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 29 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F151" t="str">
@@ -4033,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="E152" t="str" cm="1">
-        <f t="array" ref="E152">_xlfn.CONCAT(IF(A152="completion", "Completion", IF(A152="cassette", "Cassette", IF(A152="gemheart", "Crystal Heart", IF(A152="strawberry", _xlfn.CONCAT("Strawberry ", D152+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B152)*(regions!$B$2:$B$28=C152), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E152">_xlfn.CONCAT(IF(A152="completion", "Completion", IF(A152="cassette", "Cassette", IF(A152="gemheart", "Crystal Heart", IF(A152="strawberry", _xlfn.CONCAT("Strawberry ", D152+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B152)*(regions!$B$2:$B$27=C152), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F152" t="str">
@@ -4056,7 +4053,7 @@
         <v>1</v>
       </c>
       <c r="E153" t="str" cm="1">
-        <f t="array" ref="E153">_xlfn.CONCAT(IF(A153="completion", "Completion", IF(A153="cassette", "Cassette", IF(A153="gemheart", "Crystal Heart", IF(A153="strawberry", _xlfn.CONCAT("Strawberry ", D153+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B153)*(regions!$B$2:$B$28=C153), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E153">_xlfn.CONCAT(IF(A153="completion", "Completion", IF(A153="cassette", "Cassette", IF(A153="gemheart", "Crystal Heart", IF(A153="strawberry", _xlfn.CONCAT("Strawberry ", D153+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B153)*(regions!$B$2:$B$27=C153), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F153" t="str">
@@ -4079,7 +4076,7 @@
         <v>2</v>
       </c>
       <c r="E154" t="str" cm="1">
-        <f t="array" ref="E154">_xlfn.CONCAT(IF(A154="completion", "Completion", IF(A154="cassette", "Cassette", IF(A154="gemheart", "Crystal Heart", IF(A154="strawberry", _xlfn.CONCAT("Strawberry ", D154+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B154)*(regions!$B$2:$B$28=C154), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E154">_xlfn.CONCAT(IF(A154="completion", "Completion", IF(A154="cassette", "Cassette", IF(A154="gemheart", "Crystal Heart", IF(A154="strawberry", _xlfn.CONCAT("Strawberry ", D154+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B154)*(regions!$B$2:$B$27=C154), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F154" t="str">
@@ -4102,7 +4099,7 @@
         <v>3</v>
       </c>
       <c r="E155" t="str" cm="1">
-        <f t="array" ref="E155">_xlfn.CONCAT(IF(A155="completion", "Completion", IF(A155="cassette", "Cassette", IF(A155="gemheart", "Crystal Heart", IF(A155="strawberry", _xlfn.CONCAT("Strawberry ", D155+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B155)*(regions!$B$2:$B$28=C155), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E155">_xlfn.CONCAT(IF(A155="completion", "Completion", IF(A155="cassette", "Cassette", IF(A155="gemheart", "Crystal Heart", IF(A155="strawberry", _xlfn.CONCAT("Strawberry ", D155+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B155)*(regions!$B$2:$B$27=C155), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F155" t="str">
@@ -4125,7 +4122,7 @@
         <v>4</v>
       </c>
       <c r="E156" t="str" cm="1">
-        <f t="array" ref="E156">_xlfn.CONCAT(IF(A156="completion", "Completion", IF(A156="cassette", "Cassette", IF(A156="gemheart", "Crystal Heart", IF(A156="strawberry", _xlfn.CONCAT("Strawberry ", D156+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B156)*(regions!$B$2:$B$28=C156), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E156">_xlfn.CONCAT(IF(A156="completion", "Completion", IF(A156="cassette", "Cassette", IF(A156="gemheart", "Crystal Heart", IF(A156="strawberry", _xlfn.CONCAT("Strawberry ", D156+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B156)*(regions!$B$2:$B$27=C156), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F156" t="str">
@@ -4148,7 +4145,7 @@
         <v>5</v>
       </c>
       <c r="E157" t="str" cm="1">
-        <f t="array" ref="E157">_xlfn.CONCAT(IF(A157="completion", "Completion", IF(A157="cassette", "Cassette", IF(A157="gemheart", "Crystal Heart", IF(A157="strawberry", _xlfn.CONCAT("Strawberry ", D157+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B157)*(regions!$B$2:$B$28=C157), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E157">_xlfn.CONCAT(IF(A157="completion", "Completion", IF(A157="cassette", "Cassette", IF(A157="gemheart", "Crystal Heart", IF(A157="strawberry", _xlfn.CONCAT("Strawberry ", D157+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B157)*(regions!$B$2:$B$27=C157), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 6 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F157" t="str">
@@ -4171,7 +4168,7 @@
         <v>6</v>
       </c>
       <c r="E158" t="str" cm="1">
-        <f t="array" ref="E158">_xlfn.CONCAT(IF(A158="completion", "Completion", IF(A158="cassette", "Cassette", IF(A158="gemheart", "Crystal Heart", IF(A158="strawberry", _xlfn.CONCAT("Strawberry ", D158+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B158)*(regions!$B$2:$B$28=C158), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E158">_xlfn.CONCAT(IF(A158="completion", "Completion", IF(A158="cassette", "Cassette", IF(A158="gemheart", "Crystal Heart", IF(A158="strawberry", _xlfn.CONCAT("Strawberry ", D158+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B158)*(regions!$B$2:$B$27=C158), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 7 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F158" t="str">
@@ -4194,7 +4191,7 @@
         <v>7</v>
       </c>
       <c r="E159" t="str" cm="1">
-        <f t="array" ref="E159">_xlfn.CONCAT(IF(A159="completion", "Completion", IF(A159="cassette", "Cassette", IF(A159="gemheart", "Crystal Heart", IF(A159="strawberry", _xlfn.CONCAT("Strawberry ", D159+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B159)*(regions!$B$2:$B$28=C159), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E159">_xlfn.CONCAT(IF(A159="completion", "Completion", IF(A159="cassette", "Cassette", IF(A159="gemheart", "Crystal Heart", IF(A159="strawberry", _xlfn.CONCAT("Strawberry ", D159+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B159)*(regions!$B$2:$B$27=C159), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 8 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F159" t="str">
@@ -4217,7 +4214,7 @@
         <v>8</v>
       </c>
       <c r="E160" t="str" cm="1">
-        <f t="array" ref="E160">_xlfn.CONCAT(IF(A160="completion", "Completion", IF(A160="cassette", "Cassette", IF(A160="gemheart", "Crystal Heart", IF(A160="strawberry", _xlfn.CONCAT("Strawberry ", D160+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B160)*(regions!$B$2:$B$28=C160), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E160">_xlfn.CONCAT(IF(A160="completion", "Completion", IF(A160="cassette", "Cassette", IF(A160="gemheart", "Crystal Heart", IF(A160="strawberry", _xlfn.CONCAT("Strawberry ", D160+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B160)*(regions!$B$2:$B$27=C160), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 9 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F160" t="str">
@@ -4240,7 +4237,7 @@
         <v>9</v>
       </c>
       <c r="E161" t="str" cm="1">
-        <f t="array" ref="E161">_xlfn.CONCAT(IF(A161="completion", "Completion", IF(A161="cassette", "Cassette", IF(A161="gemheart", "Crystal Heart", IF(A161="strawberry", _xlfn.CONCAT("Strawberry ", D161+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B161)*(regions!$B$2:$B$28=C161), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E161">_xlfn.CONCAT(IF(A161="completion", "Completion", IF(A161="cassette", "Cassette", IF(A161="gemheart", "Crystal Heart", IF(A161="strawberry", _xlfn.CONCAT("Strawberry ", D161+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B161)*(regions!$B$2:$B$27=C161), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 10 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F161" t="str">
@@ -4263,7 +4260,7 @@
         <v>10</v>
       </c>
       <c r="E162" t="str" cm="1">
-        <f t="array" ref="E162">_xlfn.CONCAT(IF(A162="completion", "Completion", IF(A162="cassette", "Cassette", IF(A162="gemheart", "Crystal Heart", IF(A162="strawberry", _xlfn.CONCAT("Strawberry ", D162+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B162)*(regions!$B$2:$B$28=C162), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E162">_xlfn.CONCAT(IF(A162="completion", "Completion", IF(A162="cassette", "Cassette", IF(A162="gemheart", "Crystal Heart", IF(A162="strawberry", _xlfn.CONCAT("Strawberry ", D162+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B162)*(regions!$B$2:$B$27=C162), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 11 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F162" t="str">
@@ -4286,7 +4283,7 @@
         <v>11</v>
       </c>
       <c r="E163" t="str" cm="1">
-        <f t="array" ref="E163">_xlfn.CONCAT(IF(A163="completion", "Completion", IF(A163="cassette", "Cassette", IF(A163="gemheart", "Crystal Heart", IF(A163="strawberry", _xlfn.CONCAT("Strawberry ", D163+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B163)*(regions!$B$2:$B$28=C163), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E163">_xlfn.CONCAT(IF(A163="completion", "Completion", IF(A163="cassette", "Cassette", IF(A163="gemheart", "Crystal Heart", IF(A163="strawberry", _xlfn.CONCAT("Strawberry ", D163+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B163)*(regions!$B$2:$B$27=C163), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 12 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F163" t="str">
@@ -4309,7 +4306,7 @@
         <v>12</v>
       </c>
       <c r="E164" t="str" cm="1">
-        <f t="array" ref="E164">_xlfn.CONCAT(IF(A164="completion", "Completion", IF(A164="cassette", "Cassette", IF(A164="gemheart", "Crystal Heart", IF(A164="strawberry", _xlfn.CONCAT("Strawberry ", D164+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B164)*(regions!$B$2:$B$28=C164), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E164">_xlfn.CONCAT(IF(A164="completion", "Completion", IF(A164="cassette", "Cassette", IF(A164="gemheart", "Crystal Heart", IF(A164="strawberry", _xlfn.CONCAT("Strawberry ", D164+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B164)*(regions!$B$2:$B$27=C164), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 13 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F164" t="str">
@@ -4332,7 +4329,7 @@
         <v>13</v>
       </c>
       <c r="E165" t="str" cm="1">
-        <f t="array" ref="E165">_xlfn.CONCAT(IF(A165="completion", "Completion", IF(A165="cassette", "Cassette", IF(A165="gemheart", "Crystal Heart", IF(A165="strawberry", _xlfn.CONCAT("Strawberry ", D165+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B165)*(regions!$B$2:$B$28=C165), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E165">_xlfn.CONCAT(IF(A165="completion", "Completion", IF(A165="cassette", "Cassette", IF(A165="gemheart", "Crystal Heart", IF(A165="strawberry", _xlfn.CONCAT("Strawberry ", D165+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B165)*(regions!$B$2:$B$27=C165), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 14 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F165" t="str">
@@ -4355,7 +4352,7 @@
         <v>14</v>
       </c>
       <c r="E166" t="str" cm="1">
-        <f t="array" ref="E166">_xlfn.CONCAT(IF(A166="completion", "Completion", IF(A166="cassette", "Cassette", IF(A166="gemheart", "Crystal Heart", IF(A166="strawberry", _xlfn.CONCAT("Strawberry ", D166+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B166)*(regions!$B$2:$B$28=C166), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E166">_xlfn.CONCAT(IF(A166="completion", "Completion", IF(A166="cassette", "Cassette", IF(A166="gemheart", "Crystal Heart", IF(A166="strawberry", _xlfn.CONCAT("Strawberry ", D166+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B166)*(regions!$B$2:$B$27=C166), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 15 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F166" t="str">
@@ -4378,7 +4375,7 @@
         <v>15</v>
       </c>
       <c r="E167" t="str" cm="1">
-        <f t="array" ref="E167">_xlfn.CONCAT(IF(A167="completion", "Completion", IF(A167="cassette", "Cassette", IF(A167="gemheart", "Crystal Heart", IF(A167="strawberry", _xlfn.CONCAT("Strawberry ", D167+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B167)*(regions!$B$2:$B$28=C167), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E167">_xlfn.CONCAT(IF(A167="completion", "Completion", IF(A167="cassette", "Cassette", IF(A167="gemheart", "Crystal Heart", IF(A167="strawberry", _xlfn.CONCAT("Strawberry ", D167+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B167)*(regions!$B$2:$B$27=C167), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 16 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F167" t="str">
@@ -4401,7 +4398,7 @@
         <v>16</v>
       </c>
       <c r="E168" t="str" cm="1">
-        <f t="array" ref="E168">_xlfn.CONCAT(IF(A168="completion", "Completion", IF(A168="cassette", "Cassette", IF(A168="gemheart", "Crystal Heart", IF(A168="strawberry", _xlfn.CONCAT("Strawberry ", D168+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B168)*(regions!$B$2:$B$28=C168), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E168">_xlfn.CONCAT(IF(A168="completion", "Completion", IF(A168="cassette", "Cassette", IF(A168="gemheart", "Crystal Heart", IF(A168="strawberry", _xlfn.CONCAT("Strawberry ", D168+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B168)*(regions!$B$2:$B$27=C168), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 17 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F168" t="str">
@@ -4424,7 +4421,7 @@
         <v>17</v>
       </c>
       <c r="E169" t="str" cm="1">
-        <f t="array" ref="E169">_xlfn.CONCAT(IF(A169="completion", "Completion", IF(A169="cassette", "Cassette", IF(A169="gemheart", "Crystal Heart", IF(A169="strawberry", _xlfn.CONCAT("Strawberry ", D169+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B169)*(regions!$B$2:$B$28=C169), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E169">_xlfn.CONCAT(IF(A169="completion", "Completion", IF(A169="cassette", "Cassette", IF(A169="gemheart", "Crystal Heart", IF(A169="strawberry", _xlfn.CONCAT("Strawberry ", D169+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B169)*(regions!$B$2:$B$27=C169), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 18 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F169" t="str">
@@ -4447,7 +4444,7 @@
         <v>18</v>
       </c>
       <c r="E170" t="str" cm="1">
-        <f t="array" ref="E170">_xlfn.CONCAT(IF(A170="completion", "Completion", IF(A170="cassette", "Cassette", IF(A170="gemheart", "Crystal Heart", IF(A170="strawberry", _xlfn.CONCAT("Strawberry ", D170+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B170)*(regions!$B$2:$B$28=C170), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E170">_xlfn.CONCAT(IF(A170="completion", "Completion", IF(A170="cassette", "Cassette", IF(A170="gemheart", "Crystal Heart", IF(A170="strawberry", _xlfn.CONCAT("Strawberry ", D170+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B170)*(regions!$B$2:$B$27=C170), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 19 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F170" t="str">
@@ -4470,7 +4467,7 @@
         <v>19</v>
       </c>
       <c r="E171" t="str" cm="1">
-        <f t="array" ref="E171">_xlfn.CONCAT(IF(A171="completion", "Completion", IF(A171="cassette", "Cassette", IF(A171="gemheart", "Crystal Heart", IF(A171="strawberry", _xlfn.CONCAT("Strawberry ", D171+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B171)*(regions!$B$2:$B$28=C171), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E171">_xlfn.CONCAT(IF(A171="completion", "Completion", IF(A171="cassette", "Cassette", IF(A171="gemheart", "Crystal Heart", IF(A171="strawberry", _xlfn.CONCAT("Strawberry ", D171+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B171)*(regions!$B$2:$B$27=C171), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 20 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F171" t="str">
@@ -4493,7 +4490,7 @@
         <v>20</v>
       </c>
       <c r="E172" t="str" cm="1">
-        <f t="array" ref="E172">_xlfn.CONCAT(IF(A172="completion", "Completion", IF(A172="cassette", "Cassette", IF(A172="gemheart", "Crystal Heart", IF(A172="strawberry", _xlfn.CONCAT("Strawberry ", D172+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B172)*(regions!$B$2:$B$28=C172), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E172">_xlfn.CONCAT(IF(A172="completion", "Completion", IF(A172="cassette", "Cassette", IF(A172="gemheart", "Crystal Heart", IF(A172="strawberry", _xlfn.CONCAT("Strawberry ", D172+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B172)*(regions!$B$2:$B$27=C172), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 21 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F172" t="str">
@@ -4516,7 +4513,7 @@
         <v>21</v>
       </c>
       <c r="E173" t="str" cm="1">
-        <f t="array" ref="E173">_xlfn.CONCAT(IF(A173="completion", "Completion", IF(A173="cassette", "Cassette", IF(A173="gemheart", "Crystal Heart", IF(A173="strawberry", _xlfn.CONCAT("Strawberry ", D173+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B173)*(regions!$B$2:$B$28=C173), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E173">_xlfn.CONCAT(IF(A173="completion", "Completion", IF(A173="cassette", "Cassette", IF(A173="gemheart", "Crystal Heart", IF(A173="strawberry", _xlfn.CONCAT("Strawberry ", D173+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B173)*(regions!$B$2:$B$27=C173), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 22 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F173" t="str">
@@ -4539,7 +4536,7 @@
         <v>22</v>
       </c>
       <c r="E174" t="str" cm="1">
-        <f t="array" ref="E174">_xlfn.CONCAT(IF(A174="completion", "Completion", IF(A174="cassette", "Cassette", IF(A174="gemheart", "Crystal Heart", IF(A174="strawberry", _xlfn.CONCAT("Strawberry ", D174+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B174)*(regions!$B$2:$B$28=C174), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E174">_xlfn.CONCAT(IF(A174="completion", "Completion", IF(A174="cassette", "Cassette", IF(A174="gemheart", "Crystal Heart", IF(A174="strawberry", _xlfn.CONCAT("Strawberry ", D174+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B174)*(regions!$B$2:$B$27=C174), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 23 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F174" t="str">
@@ -4562,7 +4559,7 @@
         <v>23</v>
       </c>
       <c r="E175" t="str" cm="1">
-        <f t="array" ref="E175">_xlfn.CONCAT(IF(A175="completion", "Completion", IF(A175="cassette", "Cassette", IF(A175="gemheart", "Crystal Heart", IF(A175="strawberry", _xlfn.CONCAT("Strawberry ", D175+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B175)*(regions!$B$2:$B$28=C175), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E175">_xlfn.CONCAT(IF(A175="completion", "Completion", IF(A175="cassette", "Cassette", IF(A175="gemheart", "Crystal Heart", IF(A175="strawberry", _xlfn.CONCAT("Strawberry ", D175+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B175)*(regions!$B$2:$B$27=C175), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 24 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F175" t="str">
@@ -4585,7 +4582,7 @@
         <v>24</v>
       </c>
       <c r="E176" t="str" cm="1">
-        <f t="array" ref="E176">_xlfn.CONCAT(IF(A176="completion", "Completion", IF(A176="cassette", "Cassette", IF(A176="gemheart", "Crystal Heart", IF(A176="strawberry", _xlfn.CONCAT("Strawberry ", D176+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B176)*(regions!$B$2:$B$28=C176), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E176">_xlfn.CONCAT(IF(A176="completion", "Completion", IF(A176="cassette", "Cassette", IF(A176="gemheart", "Crystal Heart", IF(A176="strawberry", _xlfn.CONCAT("Strawberry ", D176+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B176)*(regions!$B$2:$B$27=C176), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 25 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F176" t="str">
@@ -4608,7 +4605,7 @@
         <v>25</v>
       </c>
       <c r="E177" t="str" cm="1">
-        <f t="array" ref="E177">_xlfn.CONCAT(IF(A177="completion", "Completion", IF(A177="cassette", "Cassette", IF(A177="gemheart", "Crystal Heart", IF(A177="strawberry", _xlfn.CONCAT("Strawberry ", D177+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B177)*(regions!$B$2:$B$28=C177), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E177">_xlfn.CONCAT(IF(A177="completion", "Completion", IF(A177="cassette", "Cassette", IF(A177="gemheart", "Crystal Heart", IF(A177="strawberry", _xlfn.CONCAT("Strawberry ", D177+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B177)*(regions!$B$2:$B$27=C177), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 26 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F177" t="str">
@@ -4631,7 +4628,7 @@
         <v>26</v>
       </c>
       <c r="E178" t="str" cm="1">
-        <f t="array" ref="E178">_xlfn.CONCAT(IF(A178="completion", "Completion", IF(A178="cassette", "Cassette", IF(A178="gemheart", "Crystal Heart", IF(A178="strawberry", _xlfn.CONCAT("Strawberry ", D178+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B178)*(regions!$B$2:$B$28=C178), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E178">_xlfn.CONCAT(IF(A178="completion", "Completion", IF(A178="cassette", "Cassette", IF(A178="gemheart", "Crystal Heart", IF(A178="strawberry", _xlfn.CONCAT("Strawberry ", D178+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B178)*(regions!$B$2:$B$27=C178), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 27 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F178" t="str">
@@ -4654,7 +4651,7 @@
         <v>27</v>
       </c>
       <c r="E179" t="str" cm="1">
-        <f t="array" ref="E179">_xlfn.CONCAT(IF(A179="completion", "Completion", IF(A179="cassette", "Cassette", IF(A179="gemheart", "Crystal Heart", IF(A179="strawberry", _xlfn.CONCAT("Strawberry ", D179+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B179)*(regions!$B$2:$B$28=C179), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E179">_xlfn.CONCAT(IF(A179="completion", "Completion", IF(A179="cassette", "Cassette", IF(A179="gemheart", "Crystal Heart", IF(A179="strawberry", _xlfn.CONCAT("Strawberry ", D179+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B179)*(regions!$B$2:$B$27=C179), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 28 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F179" t="str">
@@ -4677,7 +4674,7 @@
         <v>28</v>
       </c>
       <c r="E180" t="str" cm="1">
-        <f t="array" ref="E180">_xlfn.CONCAT(IF(A180="completion", "Completion", IF(A180="cassette", "Cassette", IF(A180="gemheart", "Crystal Heart", IF(A180="strawberry", _xlfn.CONCAT("Strawberry ", D180+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B180)*(regions!$B$2:$B$28=C180), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E180">_xlfn.CONCAT(IF(A180="completion", "Completion", IF(A180="cassette", "Cassette", IF(A180="gemheart", "Crystal Heart", IF(A180="strawberry", _xlfn.CONCAT("Strawberry ", D180+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B180)*(regions!$B$2:$B$27=C180), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 29 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F180" t="str">
@@ -4700,7 +4697,7 @@
         <v>29</v>
       </c>
       <c r="E181" t="str" cm="1">
-        <f t="array" ref="E181">_xlfn.CONCAT(IF(A181="completion", "Completion", IF(A181="cassette", "Cassette", IF(A181="gemheart", "Crystal Heart", IF(A181="strawberry", _xlfn.CONCAT("Strawberry ", D181+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B181)*(regions!$B$2:$B$28=C181), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E181">_xlfn.CONCAT(IF(A181="completion", "Completion", IF(A181="cassette", "Cassette", IF(A181="gemheart", "Crystal Heart", IF(A181="strawberry", _xlfn.CONCAT("Strawberry ", D181+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B181)*(regions!$B$2:$B$27=C181), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 30 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F181" t="str">
@@ -4723,7 +4720,7 @@
         <v>30</v>
       </c>
       <c r="E182" t="str" cm="1">
-        <f t="array" ref="E182">_xlfn.CONCAT(IF(A182="completion", "Completion", IF(A182="cassette", "Cassette", IF(A182="gemheart", "Crystal Heart", IF(A182="strawberry", _xlfn.CONCAT("Strawberry ", D182+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B182)*(regions!$B$2:$B$28=C182), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E182">_xlfn.CONCAT(IF(A182="completion", "Completion", IF(A182="cassette", "Cassette", IF(A182="gemheart", "Crystal Heart", IF(A182="strawberry", _xlfn.CONCAT("Strawberry ", D182+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B182)*(regions!$B$2:$B$27=C182), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 31 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F182" t="str">
@@ -4746,7 +4743,7 @@
         <v>0</v>
       </c>
       <c r="E183" t="str" cm="1">
-        <f t="array" ref="E183">_xlfn.CONCAT(IF(A183="completion", "Completion", IF(A183="cassette", "Cassette", IF(A183="gemheart", "Crystal Heart", IF(A183="strawberry", _xlfn.CONCAT("Strawberry ", D183+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B183)*(regions!$B$2:$B$28=C183), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E183">_xlfn.CONCAT(IF(A183="completion", "Completion", IF(A183="cassette", "Cassette", IF(A183="gemheart", "Crystal Heart", IF(A183="strawberry", _xlfn.CONCAT("Strawberry ", D183+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B183)*(regions!$B$2:$B$27=C183), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F183" t="str">
@@ -4769,7 +4766,7 @@
         <v>1</v>
       </c>
       <c r="E184" t="str" cm="1">
-        <f t="array" ref="E184">_xlfn.CONCAT(IF(A184="completion", "Completion", IF(A184="cassette", "Cassette", IF(A184="gemheart", "Crystal Heart", IF(A184="strawberry", _xlfn.CONCAT("Strawberry ", D184+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B184)*(regions!$B$2:$B$28=C184), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E184">_xlfn.CONCAT(IF(A184="completion", "Completion", IF(A184="cassette", "Cassette", IF(A184="gemheart", "Crystal Heart", IF(A184="strawberry", _xlfn.CONCAT("Strawberry ", D184+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B184)*(regions!$B$2:$B$27=C184), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F184" t="str">
@@ -4792,7 +4789,7 @@
         <v>2</v>
       </c>
       <c r="E185" t="str" cm="1">
-        <f t="array" ref="E185">_xlfn.CONCAT(IF(A185="completion", "Completion", IF(A185="cassette", "Cassette", IF(A185="gemheart", "Crystal Heart", IF(A185="strawberry", _xlfn.CONCAT("Strawberry ", D185+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B185)*(regions!$B$2:$B$28=C185), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E185">_xlfn.CONCAT(IF(A185="completion", "Completion", IF(A185="cassette", "Cassette", IF(A185="gemheart", "Crystal Heart", IF(A185="strawberry", _xlfn.CONCAT("Strawberry ", D185+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B185)*(regions!$B$2:$B$27=C185), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F185" t="str">
@@ -4815,7 +4812,7 @@
         <v>3</v>
       </c>
       <c r="E186" t="str" cm="1">
-        <f t="array" ref="E186">_xlfn.CONCAT(IF(A186="completion", "Completion", IF(A186="cassette", "Cassette", IF(A186="gemheart", "Crystal Heart", IF(A186="strawberry", _xlfn.CONCAT("Strawberry ", D186+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B186)*(regions!$B$2:$B$28=C186), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E186">_xlfn.CONCAT(IF(A186="completion", "Completion", IF(A186="cassette", "Cassette", IF(A186="gemheart", "Crystal Heart", IF(A186="strawberry", _xlfn.CONCAT("Strawberry ", D186+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B186)*(regions!$B$2:$B$27=C186), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F186" t="str">
@@ -4838,7 +4835,7 @@
         <v>4</v>
       </c>
       <c r="E187" t="str" cm="1">
-        <f t="array" ref="E187">_xlfn.CONCAT(IF(A187="completion", "Completion", IF(A187="cassette", "Cassette", IF(A187="gemheart", "Crystal Heart", IF(A187="strawberry", _xlfn.CONCAT("Strawberry ", D187+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B187)*(regions!$B$2:$B$28=C187), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E187">_xlfn.CONCAT(IF(A187="completion", "Completion", IF(A187="cassette", "Cassette", IF(A187="gemheart", "Crystal Heart", IF(A187="strawberry", _xlfn.CONCAT("Strawberry ", D187+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B187)*(regions!$B$2:$B$27=C187), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F187" t="str">
@@ -4861,7 +4858,7 @@
         <v>5</v>
       </c>
       <c r="E188" t="str" cm="1">
-        <f t="array" ref="E188">_xlfn.CONCAT(IF(A188="completion", "Completion", IF(A188="cassette", "Cassette", IF(A188="gemheart", "Crystal Heart", IF(A188="strawberry", _xlfn.CONCAT("Strawberry ", D188+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B188)*(regions!$B$2:$B$28=C188), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E188">_xlfn.CONCAT(IF(A188="completion", "Completion", IF(A188="cassette", "Cassette", IF(A188="gemheart", "Crystal Heart", IF(A188="strawberry", _xlfn.CONCAT("Strawberry ", D188+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B188)*(regions!$B$2:$B$27=C188), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 6 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F188" t="str">
@@ -4884,7 +4881,7 @@
         <v>6</v>
       </c>
       <c r="E189" t="str" cm="1">
-        <f t="array" ref="E189">_xlfn.CONCAT(IF(A189="completion", "Completion", IF(A189="cassette", "Cassette", IF(A189="gemheart", "Crystal Heart", IF(A189="strawberry", _xlfn.CONCAT("Strawberry ", D189+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B189)*(regions!$B$2:$B$28=C189), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E189">_xlfn.CONCAT(IF(A189="completion", "Completion", IF(A189="cassette", "Cassette", IF(A189="gemheart", "Crystal Heart", IF(A189="strawberry", _xlfn.CONCAT("Strawberry ", D189+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B189)*(regions!$B$2:$B$27=C189), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 7 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F189" t="str">
@@ -4907,7 +4904,7 @@
         <v>7</v>
       </c>
       <c r="E190" t="str" cm="1">
-        <f t="array" ref="E190">_xlfn.CONCAT(IF(A190="completion", "Completion", IF(A190="cassette", "Cassette", IF(A190="gemheart", "Crystal Heart", IF(A190="strawberry", _xlfn.CONCAT("Strawberry ", D190+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B190)*(regions!$B$2:$B$28=C190), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E190">_xlfn.CONCAT(IF(A190="completion", "Completion", IF(A190="cassette", "Cassette", IF(A190="gemheart", "Crystal Heart", IF(A190="strawberry", _xlfn.CONCAT("Strawberry ", D190+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B190)*(regions!$B$2:$B$27=C190), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 8 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F190" t="str">
@@ -4930,7 +4927,7 @@
         <v>8</v>
       </c>
       <c r="E191" t="str" cm="1">
-        <f t="array" ref="E191">_xlfn.CONCAT(IF(A191="completion", "Completion", IF(A191="cassette", "Cassette", IF(A191="gemheart", "Crystal Heart", IF(A191="strawberry", _xlfn.CONCAT("Strawberry ", D191+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B191)*(regions!$B$2:$B$28=C191), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E191">_xlfn.CONCAT(IF(A191="completion", "Completion", IF(A191="cassette", "Cassette", IF(A191="gemheart", "Crystal Heart", IF(A191="strawberry", _xlfn.CONCAT("Strawberry ", D191+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B191)*(regions!$B$2:$B$27=C191), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 9 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F191" t="str">
@@ -4953,7 +4950,7 @@
         <v>9</v>
       </c>
       <c r="E192" t="str" cm="1">
-        <f t="array" ref="E192">_xlfn.CONCAT(IF(A192="completion", "Completion", IF(A192="cassette", "Cassette", IF(A192="gemheart", "Crystal Heart", IF(A192="strawberry", _xlfn.CONCAT("Strawberry ", D192+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B192)*(regions!$B$2:$B$28=C192), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E192">_xlfn.CONCAT(IF(A192="completion", "Completion", IF(A192="cassette", "Cassette", IF(A192="gemheart", "Crystal Heart", IF(A192="strawberry", _xlfn.CONCAT("Strawberry ", D192+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B192)*(regions!$B$2:$B$27=C192), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 10 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F192" t="str">
@@ -4976,7 +4973,7 @@
         <v>10</v>
       </c>
       <c r="E193" t="str" cm="1">
-        <f t="array" ref="E193">_xlfn.CONCAT(IF(A193="completion", "Completion", IF(A193="cassette", "Cassette", IF(A193="gemheart", "Crystal Heart", IF(A193="strawberry", _xlfn.CONCAT("Strawberry ", D193+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B193)*(regions!$B$2:$B$28=C193), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E193">_xlfn.CONCAT(IF(A193="completion", "Completion", IF(A193="cassette", "Cassette", IF(A193="gemheart", "Crystal Heart", IF(A193="strawberry", _xlfn.CONCAT("Strawberry ", D193+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B193)*(regions!$B$2:$B$27=C193), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 11 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F193" t="str">
@@ -4999,11 +4996,11 @@
         <v>11</v>
       </c>
       <c r="E194" t="str" cm="1">
-        <f t="array" ref="E194">_xlfn.CONCAT(IF(A194="completion", "Completion", IF(A194="cassette", "Cassette", IF(A194="gemheart", "Crystal Heart", IF(A194="strawberry", _xlfn.CONCAT("Strawberry ", D194+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B194)*(regions!$B$2:$B$28=C194), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E194">_xlfn.CONCAT(IF(A194="completion", "Completion", IF(A194="cassette", "Cassette", IF(A194="gemheart", "Crystal Heart", IF(A194="strawberry", _xlfn.CONCAT("Strawberry ", D194+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B194)*(regions!$B$2:$B$27=C194), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 12 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F194" t="str">
-        <f t="shared" ref="F194:F257" si="3">IF(A194="strawberry", "Strawberry", E194)</f>
+        <f t="shared" ref="F194:F234" si="3">IF(A194="strawberry", "Strawberry", E194)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -5022,7 +5019,7 @@
         <v>12</v>
       </c>
       <c r="E195" t="str" cm="1">
-        <f t="array" ref="E195">_xlfn.CONCAT(IF(A195="completion", "Completion", IF(A195="cassette", "Cassette", IF(A195="gemheart", "Crystal Heart", IF(A195="strawberry", _xlfn.CONCAT("Strawberry ", D195+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B195)*(regions!$B$2:$B$28=C195), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E195">_xlfn.CONCAT(IF(A195="completion", "Completion", IF(A195="cassette", "Cassette", IF(A195="gemheart", "Crystal Heart", IF(A195="strawberry", _xlfn.CONCAT("Strawberry ", D195+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B195)*(regions!$B$2:$B$27=C195), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 13 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F195" t="str">
@@ -5045,7 +5042,7 @@
         <v>13</v>
       </c>
       <c r="E196" t="str" cm="1">
-        <f t="array" ref="E196">_xlfn.CONCAT(IF(A196="completion", "Completion", IF(A196="cassette", "Cassette", IF(A196="gemheart", "Crystal Heart", IF(A196="strawberry", _xlfn.CONCAT("Strawberry ", D196+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B196)*(regions!$B$2:$B$28=C196), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E196">_xlfn.CONCAT(IF(A196="completion", "Completion", IF(A196="cassette", "Cassette", IF(A196="gemheart", "Crystal Heart", IF(A196="strawberry", _xlfn.CONCAT("Strawberry ", D196+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B196)*(regions!$B$2:$B$27=C196), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 14 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F196" t="str">
@@ -5068,7 +5065,7 @@
         <v>14</v>
       </c>
       <c r="E197" t="str" cm="1">
-        <f t="array" ref="E197">_xlfn.CONCAT(IF(A197="completion", "Completion", IF(A197="cassette", "Cassette", IF(A197="gemheart", "Crystal Heart", IF(A197="strawberry", _xlfn.CONCAT("Strawberry ", D197+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B197)*(regions!$B$2:$B$28=C197), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E197">_xlfn.CONCAT(IF(A197="completion", "Completion", IF(A197="cassette", "Cassette", IF(A197="gemheart", "Crystal Heart", IF(A197="strawberry", _xlfn.CONCAT("Strawberry ", D197+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B197)*(regions!$B$2:$B$27=C197), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 15 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F197" t="str">
@@ -5091,7 +5088,7 @@
         <v>15</v>
       </c>
       <c r="E198" t="str" cm="1">
-        <f t="array" ref="E198">_xlfn.CONCAT(IF(A198="completion", "Completion", IF(A198="cassette", "Cassette", IF(A198="gemheart", "Crystal Heart", IF(A198="strawberry", _xlfn.CONCAT("Strawberry ", D198+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B198)*(regions!$B$2:$B$28=C198), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E198">_xlfn.CONCAT(IF(A198="completion", "Completion", IF(A198="cassette", "Cassette", IF(A198="gemheart", "Crystal Heart", IF(A198="strawberry", _xlfn.CONCAT("Strawberry ", D198+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B198)*(regions!$B$2:$B$27=C198), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 16 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F198" t="str">
@@ -5114,7 +5111,7 @@
         <v>16</v>
       </c>
       <c r="E199" t="str" cm="1">
-        <f t="array" ref="E199">_xlfn.CONCAT(IF(A199="completion", "Completion", IF(A199="cassette", "Cassette", IF(A199="gemheart", "Crystal Heart", IF(A199="strawberry", _xlfn.CONCAT("Strawberry ", D199+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B199)*(regions!$B$2:$B$28=C199), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E199">_xlfn.CONCAT(IF(A199="completion", "Completion", IF(A199="cassette", "Cassette", IF(A199="gemheart", "Crystal Heart", IF(A199="strawberry", _xlfn.CONCAT("Strawberry ", D199+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B199)*(regions!$B$2:$B$27=C199), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 17 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F199" t="str">
@@ -5137,7 +5134,7 @@
         <v>17</v>
       </c>
       <c r="E200" t="str" cm="1">
-        <f t="array" ref="E200">_xlfn.CONCAT(IF(A200="completion", "Completion", IF(A200="cassette", "Cassette", IF(A200="gemheart", "Crystal Heart", IF(A200="strawberry", _xlfn.CONCAT("Strawberry ", D200+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B200)*(regions!$B$2:$B$28=C200), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E200">_xlfn.CONCAT(IF(A200="completion", "Completion", IF(A200="cassette", "Cassette", IF(A200="gemheart", "Crystal Heart", IF(A200="strawberry", _xlfn.CONCAT("Strawberry ", D200+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B200)*(regions!$B$2:$B$27=C200), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 18 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F200" t="str">
@@ -5160,7 +5157,7 @@
         <v>18</v>
       </c>
       <c r="E201" t="str" cm="1">
-        <f t="array" ref="E201">_xlfn.CONCAT(IF(A201="completion", "Completion", IF(A201="cassette", "Cassette", IF(A201="gemheart", "Crystal Heart", IF(A201="strawberry", _xlfn.CONCAT("Strawberry ", D201+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B201)*(regions!$B$2:$B$28=C201), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E201">_xlfn.CONCAT(IF(A201="completion", "Completion", IF(A201="cassette", "Cassette", IF(A201="gemheart", "Crystal Heart", IF(A201="strawberry", _xlfn.CONCAT("Strawberry ", D201+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B201)*(regions!$B$2:$B$27=C201), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 19 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F201" t="str">
@@ -5183,7 +5180,7 @@
         <v>19</v>
       </c>
       <c r="E202" t="str" cm="1">
-        <f t="array" ref="E202">_xlfn.CONCAT(IF(A202="completion", "Completion", IF(A202="cassette", "Cassette", IF(A202="gemheart", "Crystal Heart", IF(A202="strawberry", _xlfn.CONCAT("Strawberry ", D202+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B202)*(regions!$B$2:$B$28=C202), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E202">_xlfn.CONCAT(IF(A202="completion", "Completion", IF(A202="cassette", "Cassette", IF(A202="gemheart", "Crystal Heart", IF(A202="strawberry", _xlfn.CONCAT("Strawberry ", D202+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B202)*(regions!$B$2:$B$27=C202), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 20 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F202" t="str">
@@ -5206,7 +5203,7 @@
         <v>20</v>
       </c>
       <c r="E203" t="str" cm="1">
-        <f t="array" ref="E203">_xlfn.CONCAT(IF(A203="completion", "Completion", IF(A203="cassette", "Cassette", IF(A203="gemheart", "Crystal Heart", IF(A203="strawberry", _xlfn.CONCAT("Strawberry ", D203+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B203)*(regions!$B$2:$B$28=C203), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E203">_xlfn.CONCAT(IF(A203="completion", "Completion", IF(A203="cassette", "Cassette", IF(A203="gemheart", "Crystal Heart", IF(A203="strawberry", _xlfn.CONCAT("Strawberry ", D203+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B203)*(regions!$B$2:$B$27=C203), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 21 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F203" t="str">
@@ -5229,7 +5226,7 @@
         <v>21</v>
       </c>
       <c r="E204" t="str" cm="1">
-        <f t="array" ref="E204">_xlfn.CONCAT(IF(A204="completion", "Completion", IF(A204="cassette", "Cassette", IF(A204="gemheart", "Crystal Heart", IF(A204="strawberry", _xlfn.CONCAT("Strawberry ", D204+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B204)*(regions!$B$2:$B$28=C204), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E204">_xlfn.CONCAT(IF(A204="completion", "Completion", IF(A204="cassette", "Cassette", IF(A204="gemheart", "Crystal Heart", IF(A204="strawberry", _xlfn.CONCAT("Strawberry ", D204+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B204)*(regions!$B$2:$B$27=C204), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 22 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F204" t="str">
@@ -5252,7 +5249,7 @@
         <v>22</v>
       </c>
       <c r="E205" t="str" cm="1">
-        <f t="array" ref="E205">_xlfn.CONCAT(IF(A205="completion", "Completion", IF(A205="cassette", "Cassette", IF(A205="gemheart", "Crystal Heart", IF(A205="strawberry", _xlfn.CONCAT("Strawberry ", D205+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B205)*(regions!$B$2:$B$28=C205), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E205">_xlfn.CONCAT(IF(A205="completion", "Completion", IF(A205="cassette", "Cassette", IF(A205="gemheart", "Crystal Heart", IF(A205="strawberry", _xlfn.CONCAT("Strawberry ", D205+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B205)*(regions!$B$2:$B$27=C205), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 23 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F205" t="str">
@@ -5275,7 +5272,7 @@
         <v>23</v>
       </c>
       <c r="E206" t="str" cm="1">
-        <f t="array" ref="E206">_xlfn.CONCAT(IF(A206="completion", "Completion", IF(A206="cassette", "Cassette", IF(A206="gemheart", "Crystal Heart", IF(A206="strawberry", _xlfn.CONCAT("Strawberry ", D206+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B206)*(regions!$B$2:$B$28=C206), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E206">_xlfn.CONCAT(IF(A206="completion", "Completion", IF(A206="cassette", "Cassette", IF(A206="gemheart", "Crystal Heart", IF(A206="strawberry", _xlfn.CONCAT("Strawberry ", D206+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B206)*(regions!$B$2:$B$27=C206), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 24 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F206" t="str">
@@ -5298,7 +5295,7 @@
         <v>24</v>
       </c>
       <c r="E207" t="str" cm="1">
-        <f t="array" ref="E207">_xlfn.CONCAT(IF(A207="completion", "Completion", IF(A207="cassette", "Cassette", IF(A207="gemheart", "Crystal Heart", IF(A207="strawberry", _xlfn.CONCAT("Strawberry ", D207+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B207)*(regions!$B$2:$B$28=C207), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E207">_xlfn.CONCAT(IF(A207="completion", "Completion", IF(A207="cassette", "Cassette", IF(A207="gemheart", "Crystal Heart", IF(A207="strawberry", _xlfn.CONCAT("Strawberry ", D207+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B207)*(regions!$B$2:$B$27=C207), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 25 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F207" t="str">
@@ -5321,7 +5318,7 @@
         <v>25</v>
       </c>
       <c r="E208" t="str" cm="1">
-        <f t="array" ref="E208">_xlfn.CONCAT(IF(A208="completion", "Completion", IF(A208="cassette", "Cassette", IF(A208="gemheart", "Crystal Heart", IF(A208="strawberry", _xlfn.CONCAT("Strawberry ", D208+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B208)*(regions!$B$2:$B$28=C208), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E208">_xlfn.CONCAT(IF(A208="completion", "Completion", IF(A208="cassette", "Cassette", IF(A208="gemheart", "Crystal Heart", IF(A208="strawberry", _xlfn.CONCAT("Strawberry ", D208+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B208)*(regions!$B$2:$B$27=C208), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 26 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F208" t="str">
@@ -5344,7 +5341,7 @@
         <v>26</v>
       </c>
       <c r="E209" t="str" cm="1">
-        <f t="array" ref="E209">_xlfn.CONCAT(IF(A209="completion", "Completion", IF(A209="cassette", "Cassette", IF(A209="gemheart", "Crystal Heart", IF(A209="strawberry", _xlfn.CONCAT("Strawberry ", D209+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B209)*(regions!$B$2:$B$28=C209), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E209">_xlfn.CONCAT(IF(A209="completion", "Completion", IF(A209="cassette", "Cassette", IF(A209="gemheart", "Crystal Heart", IF(A209="strawberry", _xlfn.CONCAT("Strawberry ", D209+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B209)*(regions!$B$2:$B$27=C209), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 27 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F209" t="str">
@@ -5367,7 +5364,7 @@
         <v>27</v>
       </c>
       <c r="E210" t="str" cm="1">
-        <f t="array" ref="E210">_xlfn.CONCAT(IF(A210="completion", "Completion", IF(A210="cassette", "Cassette", IF(A210="gemheart", "Crystal Heart", IF(A210="strawberry", _xlfn.CONCAT("Strawberry ", D210+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B210)*(regions!$B$2:$B$28=C210), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E210">_xlfn.CONCAT(IF(A210="completion", "Completion", IF(A210="cassette", "Cassette", IF(A210="gemheart", "Crystal Heart", IF(A210="strawberry", _xlfn.CONCAT("Strawberry ", D210+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B210)*(regions!$B$2:$B$27=C210), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 28 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F210" t="str">
@@ -5390,7 +5387,7 @@
         <v>28</v>
       </c>
       <c r="E211" t="str" cm="1">
-        <f t="array" ref="E211">_xlfn.CONCAT(IF(A211="completion", "Completion", IF(A211="cassette", "Cassette", IF(A211="gemheart", "Crystal Heart", IF(A211="strawberry", _xlfn.CONCAT("Strawberry ", D211+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B211)*(regions!$B$2:$B$28=C211), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E211">_xlfn.CONCAT(IF(A211="completion", "Completion", IF(A211="cassette", "Cassette", IF(A211="gemheart", "Crystal Heart", IF(A211="strawberry", _xlfn.CONCAT("Strawberry ", D211+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B211)*(regions!$B$2:$B$27=C211), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 29 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F211" t="str">
@@ -5413,7 +5410,7 @@
         <v>29</v>
       </c>
       <c r="E212" t="str" cm="1">
-        <f t="array" ref="E212">_xlfn.CONCAT(IF(A212="completion", "Completion", IF(A212="cassette", "Cassette", IF(A212="gemheart", "Crystal Heart", IF(A212="strawberry", _xlfn.CONCAT("Strawberry ", D212+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B212)*(regions!$B$2:$B$28=C212), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E212">_xlfn.CONCAT(IF(A212="completion", "Completion", IF(A212="cassette", "Cassette", IF(A212="gemheart", "Crystal Heart", IF(A212="strawberry", _xlfn.CONCAT("Strawberry ", D212+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B212)*(regions!$B$2:$B$27=C212), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 30 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F212" t="str">
@@ -5436,7 +5433,7 @@
         <v>30</v>
       </c>
       <c r="E213" t="str" cm="1">
-        <f t="array" ref="E213">_xlfn.CONCAT(IF(A213="completion", "Completion", IF(A213="cassette", "Cassette", IF(A213="gemheart", "Crystal Heart", IF(A213="strawberry", _xlfn.CONCAT("Strawberry ", D213+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B213)*(regions!$B$2:$B$28=C213), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E213">_xlfn.CONCAT(IF(A213="completion", "Completion", IF(A213="cassette", "Cassette", IF(A213="gemheart", "Crystal Heart", IF(A213="strawberry", _xlfn.CONCAT("Strawberry ", D213+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B213)*(regions!$B$2:$B$27=C213), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 31 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F213" t="str">
@@ -5459,7 +5456,7 @@
         <v>31</v>
       </c>
       <c r="E214" t="str" cm="1">
-        <f t="array" ref="E214">_xlfn.CONCAT(IF(A214="completion", "Completion", IF(A214="cassette", "Cassette", IF(A214="gemheart", "Crystal Heart", IF(A214="strawberry", _xlfn.CONCAT("Strawberry ", D214+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B214)*(regions!$B$2:$B$28=C214), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E214">_xlfn.CONCAT(IF(A214="completion", "Completion", IF(A214="cassette", "Cassette", IF(A214="gemheart", "Crystal Heart", IF(A214="strawberry", _xlfn.CONCAT("Strawberry ", D214+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B214)*(regions!$B$2:$B$27=C214), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 32 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F214" t="str">
@@ -5482,7 +5479,7 @@
         <v>32</v>
       </c>
       <c r="E215" t="str" cm="1">
-        <f t="array" ref="E215">_xlfn.CONCAT(IF(A215="completion", "Completion", IF(A215="cassette", "Cassette", IF(A215="gemheart", "Crystal Heart", IF(A215="strawberry", _xlfn.CONCAT("Strawberry ", D215+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B215)*(regions!$B$2:$B$28=C215), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E215">_xlfn.CONCAT(IF(A215="completion", "Completion", IF(A215="cassette", "Cassette", IF(A215="gemheart", "Crystal Heart", IF(A215="strawberry", _xlfn.CONCAT("Strawberry ", D215+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B215)*(regions!$B$2:$B$27=C215), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 33 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F215" t="str">
@@ -5505,7 +5502,7 @@
         <v>33</v>
       </c>
       <c r="E216" t="str" cm="1">
-        <f t="array" ref="E216">_xlfn.CONCAT(IF(A216="completion", "Completion", IF(A216="cassette", "Cassette", IF(A216="gemheart", "Crystal Heart", IF(A216="strawberry", _xlfn.CONCAT("Strawberry ", D216+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B216)*(regions!$B$2:$B$28=C216), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E216">_xlfn.CONCAT(IF(A216="completion", "Completion", IF(A216="cassette", "Cassette", IF(A216="gemheart", "Crystal Heart", IF(A216="strawberry", _xlfn.CONCAT("Strawberry ", D216+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B216)*(regions!$B$2:$B$27=C216), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 34 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F216" t="str">
@@ -5528,7 +5525,7 @@
         <v>34</v>
       </c>
       <c r="E217" t="str" cm="1">
-        <f t="array" ref="E217">_xlfn.CONCAT(IF(A217="completion", "Completion", IF(A217="cassette", "Cassette", IF(A217="gemheart", "Crystal Heart", IF(A217="strawberry", _xlfn.CONCAT("Strawberry ", D217+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B217)*(regions!$B$2:$B$28=C217), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E217">_xlfn.CONCAT(IF(A217="completion", "Completion", IF(A217="cassette", "Cassette", IF(A217="gemheart", "Crystal Heart", IF(A217="strawberry", _xlfn.CONCAT("Strawberry ", D217+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B217)*(regions!$B$2:$B$27=C217), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 35 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F217" t="str">
@@ -5551,7 +5548,7 @@
         <v>35</v>
       </c>
       <c r="E218" t="str" cm="1">
-        <f t="array" ref="E218">_xlfn.CONCAT(IF(A218="completion", "Completion", IF(A218="cassette", "Cassette", IF(A218="gemheart", "Crystal Heart", IF(A218="strawberry", _xlfn.CONCAT("Strawberry ", D218+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B218)*(regions!$B$2:$B$28=C218), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E218">_xlfn.CONCAT(IF(A218="completion", "Completion", IF(A218="cassette", "Cassette", IF(A218="gemheart", "Crystal Heart", IF(A218="strawberry", _xlfn.CONCAT("Strawberry ", D218+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B218)*(regions!$B$2:$B$27=C218), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 36 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F218" t="str">
@@ -5574,7 +5571,7 @@
         <v>36</v>
       </c>
       <c r="E219" t="str" cm="1">
-        <f t="array" ref="E219">_xlfn.CONCAT(IF(A219="completion", "Completion", IF(A219="cassette", "Cassette", IF(A219="gemheart", "Crystal Heart", IF(A219="strawberry", _xlfn.CONCAT("Strawberry ", D219+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B219)*(regions!$B$2:$B$28=C219), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E219">_xlfn.CONCAT(IF(A219="completion", "Completion", IF(A219="cassette", "Cassette", IF(A219="gemheart", "Crystal Heart", IF(A219="strawberry", _xlfn.CONCAT("Strawberry ", D219+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B219)*(regions!$B$2:$B$27=C219), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 37 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F219" t="str">
@@ -5597,7 +5594,7 @@
         <v>37</v>
       </c>
       <c r="E220" t="str" cm="1">
-        <f t="array" ref="E220">_xlfn.CONCAT(IF(A220="completion", "Completion", IF(A220="cassette", "Cassette", IF(A220="gemheart", "Crystal Heart", IF(A220="strawberry", _xlfn.CONCAT("Strawberry ", D220+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B220)*(regions!$B$2:$B$28=C220), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E220">_xlfn.CONCAT(IF(A220="completion", "Completion", IF(A220="cassette", "Cassette", IF(A220="gemheart", "Crystal Heart", IF(A220="strawberry", _xlfn.CONCAT("Strawberry ", D220+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B220)*(regions!$B$2:$B$27=C220), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 38 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F220" t="str">
@@ -5620,7 +5617,7 @@
         <v>38</v>
       </c>
       <c r="E221" t="str" cm="1">
-        <f t="array" ref="E221">_xlfn.CONCAT(IF(A221="completion", "Completion", IF(A221="cassette", "Cassette", IF(A221="gemheart", "Crystal Heart", IF(A221="strawberry", _xlfn.CONCAT("Strawberry ", D221+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B221)*(regions!$B$2:$B$28=C221), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E221">_xlfn.CONCAT(IF(A221="completion", "Completion", IF(A221="cassette", "Cassette", IF(A221="gemheart", "Crystal Heart", IF(A221="strawberry", _xlfn.CONCAT("Strawberry ", D221+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B221)*(regions!$B$2:$B$27=C221), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 39 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F221" t="str">
@@ -5643,7 +5640,7 @@
         <v>39</v>
       </c>
       <c r="E222" t="str" cm="1">
-        <f t="array" ref="E222">_xlfn.CONCAT(IF(A222="completion", "Completion", IF(A222="cassette", "Cassette", IF(A222="gemheart", "Crystal Heart", IF(A222="strawberry", _xlfn.CONCAT("Strawberry ", D222+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B222)*(regions!$B$2:$B$28=C222), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E222">_xlfn.CONCAT(IF(A222="completion", "Completion", IF(A222="cassette", "Cassette", IF(A222="gemheart", "Crystal Heart", IF(A222="strawberry", _xlfn.CONCAT("Strawberry ", D222+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B222)*(regions!$B$2:$B$27=C222), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 40 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F222" t="str">
@@ -5666,7 +5663,7 @@
         <v>40</v>
       </c>
       <c r="E223" t="str" cm="1">
-        <f t="array" ref="E223">_xlfn.CONCAT(IF(A223="completion", "Completion", IF(A223="cassette", "Cassette", IF(A223="gemheart", "Crystal Heart", IF(A223="strawberry", _xlfn.CONCAT("Strawberry ", D223+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B223)*(regions!$B$2:$B$28=C223), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E223">_xlfn.CONCAT(IF(A223="completion", "Completion", IF(A223="cassette", "Cassette", IF(A223="gemheart", "Crystal Heart", IF(A223="strawberry", _xlfn.CONCAT("Strawberry ", D223+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B223)*(regions!$B$2:$B$27=C223), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 41 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F223" t="str">
@@ -5689,7 +5686,7 @@
         <v>41</v>
       </c>
       <c r="E224" t="str" cm="1">
-        <f t="array" ref="E224">_xlfn.CONCAT(IF(A224="completion", "Completion", IF(A224="cassette", "Cassette", IF(A224="gemheart", "Crystal Heart", IF(A224="strawberry", _xlfn.CONCAT("Strawberry ", D224+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B224)*(regions!$B$2:$B$28=C224), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E224">_xlfn.CONCAT(IF(A224="completion", "Completion", IF(A224="cassette", "Cassette", IF(A224="gemheart", "Crystal Heart", IF(A224="strawberry", _xlfn.CONCAT("Strawberry ", D224+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B224)*(regions!$B$2:$B$27=C224), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 42 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F224" t="str">
@@ -5712,7 +5709,7 @@
         <v>42</v>
       </c>
       <c r="E225" t="str" cm="1">
-        <f t="array" ref="E225">_xlfn.CONCAT(IF(A225="completion", "Completion", IF(A225="cassette", "Cassette", IF(A225="gemheart", "Crystal Heart", IF(A225="strawberry", _xlfn.CONCAT("Strawberry ", D225+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B225)*(regions!$B$2:$B$28=C225), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E225">_xlfn.CONCAT(IF(A225="completion", "Completion", IF(A225="cassette", "Cassette", IF(A225="gemheart", "Crystal Heart", IF(A225="strawberry", _xlfn.CONCAT("Strawberry ", D225+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B225)*(regions!$B$2:$B$27=C225), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 43 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F225" t="str">
@@ -5735,7 +5732,7 @@
         <v>43</v>
       </c>
       <c r="E226" t="str" cm="1">
-        <f t="array" ref="E226">_xlfn.CONCAT(IF(A226="completion", "Completion", IF(A226="cassette", "Cassette", IF(A226="gemheart", "Crystal Heart", IF(A226="strawberry", _xlfn.CONCAT("Strawberry ", D226+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B226)*(regions!$B$2:$B$28=C226), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E226">_xlfn.CONCAT(IF(A226="completion", "Completion", IF(A226="cassette", "Cassette", IF(A226="gemheart", "Crystal Heart", IF(A226="strawberry", _xlfn.CONCAT("Strawberry ", D226+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B226)*(regions!$B$2:$B$27=C226), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 44 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F226" t="str">
@@ -5758,7 +5755,7 @@
         <v>44</v>
       </c>
       <c r="E227" t="str" cm="1">
-        <f t="array" ref="E227">_xlfn.CONCAT(IF(A227="completion", "Completion", IF(A227="cassette", "Cassette", IF(A227="gemheart", "Crystal Heart", IF(A227="strawberry", _xlfn.CONCAT("Strawberry ", D227+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B227)*(regions!$B$2:$B$28=C227), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E227">_xlfn.CONCAT(IF(A227="completion", "Completion", IF(A227="cassette", "Cassette", IF(A227="gemheart", "Crystal Heart", IF(A227="strawberry", _xlfn.CONCAT("Strawberry ", D227+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B227)*(regions!$B$2:$B$27=C227), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 45 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F227" t="str">
@@ -5781,7 +5778,7 @@
         <v>45</v>
       </c>
       <c r="E228" t="str" cm="1">
-        <f t="array" ref="E228">_xlfn.CONCAT(IF(A228="completion", "Completion", IF(A228="cassette", "Cassette", IF(A228="gemheart", "Crystal Heart", IF(A228="strawberry", _xlfn.CONCAT("Strawberry ", D228+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B228)*(regions!$B$2:$B$28=C228), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E228">_xlfn.CONCAT(IF(A228="completion", "Completion", IF(A228="cassette", "Cassette", IF(A228="gemheart", "Crystal Heart", IF(A228="strawberry", _xlfn.CONCAT("Strawberry ", D228+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B228)*(regions!$B$2:$B$27=C228), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 46 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F228" t="str">
@@ -5804,7 +5801,7 @@
         <v>46</v>
       </c>
       <c r="E229" t="str" cm="1">
-        <f t="array" ref="E229">_xlfn.CONCAT(IF(A229="completion", "Completion", IF(A229="cassette", "Cassette", IF(A229="gemheart", "Crystal Heart", IF(A229="strawberry", _xlfn.CONCAT("Strawberry ", D229+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B229)*(regions!$B$2:$B$28=C229), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E229">_xlfn.CONCAT(IF(A229="completion", "Completion", IF(A229="cassette", "Cassette", IF(A229="gemheart", "Crystal Heart", IF(A229="strawberry", _xlfn.CONCAT("Strawberry ", D229+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B229)*(regions!$B$2:$B$27=C229), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 47 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F229" t="str">
@@ -5827,7 +5824,7 @@
         <v>0</v>
       </c>
       <c r="E230" t="str" cm="1">
-        <f t="array" ref="E230">_xlfn.CONCAT(IF(A230="completion", "Completion", IF(A230="cassette", "Cassette", IF(A230="gemheart", "Crystal Heart", IF(A230="strawberry", _xlfn.CONCAT("Strawberry ", D230+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B230)*(regions!$B$2:$B$28=C230), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E230">_xlfn.CONCAT(IF(A230="completion", "Completion", IF(A230="cassette", "Cassette", IF(A230="gemheart", "Crystal Heart", IF(A230="strawberry", _xlfn.CONCAT("Strawberry ", D230+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B230)*(regions!$B$2:$B$27=C230), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 1 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F230" t="str">
@@ -5850,7 +5847,7 @@
         <v>1</v>
       </c>
       <c r="E231" t="str" cm="1">
-        <f t="array" ref="E231">_xlfn.CONCAT(IF(A231="completion", "Completion", IF(A231="cassette", "Cassette", IF(A231="gemheart", "Crystal Heart", IF(A231="strawberry", _xlfn.CONCAT("Strawberry ", D231+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B231)*(regions!$B$2:$B$28=C231), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E231">_xlfn.CONCAT(IF(A231="completion", "Completion", IF(A231="cassette", "Cassette", IF(A231="gemheart", "Crystal Heart", IF(A231="strawberry", _xlfn.CONCAT("Strawberry ", D231+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B231)*(regions!$B$2:$B$27=C231), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 2 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F231" t="str">
@@ -5873,7 +5870,7 @@
         <v>2</v>
       </c>
       <c r="E232" t="str" cm="1">
-        <f t="array" ref="E232">_xlfn.CONCAT(IF(A232="completion", "Completion", IF(A232="cassette", "Cassette", IF(A232="gemheart", "Crystal Heart", IF(A232="strawberry", _xlfn.CONCAT("Strawberry ", D232+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B232)*(regions!$B$2:$B$28=C232), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E232">_xlfn.CONCAT(IF(A232="completion", "Completion", IF(A232="cassette", "Cassette", IF(A232="gemheart", "Crystal Heart", IF(A232="strawberry", _xlfn.CONCAT("Strawberry ", D232+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B232)*(regions!$B$2:$B$27=C232), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 3 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F232" t="str">
@@ -5896,7 +5893,7 @@
         <v>3</v>
       </c>
       <c r="E233" t="str" cm="1">
-        <f t="array" ref="E233">_xlfn.CONCAT(IF(A233="completion", "Completion", IF(A233="cassette", "Cassette", IF(A233="gemheart", "Crystal Heart", IF(A233="strawberry", _xlfn.CONCAT("Strawberry ", D233+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B233)*(regions!$B$2:$B$28=C233), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E233">_xlfn.CONCAT(IF(A233="completion", "Completion", IF(A233="cassette", "Cassette", IF(A233="gemheart", "Crystal Heart", IF(A233="strawberry", _xlfn.CONCAT("Strawberry ", D233+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B233)*(regions!$B$2:$B$27=C233), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 4 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F233" t="str">
@@ -5919,7 +5916,7 @@
         <v>4</v>
       </c>
       <c r="E234" t="str" cm="1">
-        <f t="array" ref="E234">_xlfn.CONCAT(IF(A234="completion", "Completion", IF(A234="cassette", "Cassette", IF(A234="gemheart", "Crystal Heart", IF(A234="strawberry", _xlfn.CONCAT("Strawberry ", D234+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$28=B234)*(regions!$B$2:$B$28=C234), regions!$C$2:$C$28, "", 0, 1), ")")</f>
+        <f t="array" ref="E234">_xlfn.CONCAT(IF(A234="completion", "Completion", IF(A234="cassette", "Cassette", IF(A234="gemheart", "Crystal Heart", IF(A234="strawberry", _xlfn.CONCAT("Strawberry ", D234+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B234)*(regions!$B$2:$B$27=C234), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F234" t="str">
@@ -5935,10 +5932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1A1AF2-907D-41B3-B0A4-149E1E23A84D}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5954,23 +5951,23 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5981,7 +5978,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5992,7 +5989,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6003,7 +6000,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6014,7 +6011,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6025,7 +6022,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6036,29 +6033,29 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6069,10 +6066,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -6080,7 +6077,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -6091,7 +6088,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6102,7 +6099,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -6113,7 +6110,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -6124,7 +6121,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -6135,7 +6132,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -6146,7 +6143,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -6157,10 +6154,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -6168,7 +6165,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -6179,7 +6176,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -6190,7 +6187,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -6201,7 +6198,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -6212,7 +6209,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -6223,7 +6220,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -6234,24 +6231,13 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>9</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted Celeste world to use dependency injection for handling different progressions
</commit_message>
<xml_diff>
--- a/worlds/celeste/data/items.xlsx
+++ b/worlds/celeste/data/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Archipelago\worlds\celeste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D73B774-C4CE-42B9-80B0-DD5C3012104C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB511E2F-18EF-413B-9DBB-A860AE52C27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="0" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{C0CD6F56-D694-4BE6-8516-FA8CA6FB3D5E}"/>
+    <workbookView xWindow="-30828" yWindow="0" windowWidth="30936" windowHeight="16896" xr2:uid="{C0CD6F56-D694-4BE6-8516-FA8CA6FB3D5E}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="39">
   <si>
     <t>level</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>region_name</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>Victory (Celeste)</t>
   </si>
 </sst>
 </file>
@@ -530,11 +536,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A95FA-F51A-42F8-84DA-309114F88AAA}">
-  <dimension ref="A1:F234"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,25 +573,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>COUNTIFS($A$2:A2, A2, $B$2:B2, B2, $C$2:C2, C2) - 1</f>
-        <v>0</v>
-      </c>
-      <c r="E2" t="str" cm="1">
-        <f t="array" ref="E2">_xlfn.CONCAT(IF(A2="completion", "Completion", IF(A2="cassette", "Cassette", IF(A2="gemheart", "Crystal Heart", IF(A2="strawberry", _xlfn.CONCAT("Strawberry ", D2+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B2)*(regions!$B$2:$B$27=C2), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F65" si="0">IF(A2="strawberry", "Strawberry", E2)</f>
-        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -593,22 +596,22 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f>COUNTIFS($A$2:A3, A3, $B$2:B3, B3, $C$2:C3, C3) - 1</f>
+        <f>COUNTIFS($A$3:A3, A3, $B$3:B3, B3, $C$3:C3, C3) - 1</f>
         <v>0</v>
       </c>
       <c r="E3" t="str" cm="1">
         <f t="array" ref="E3">_xlfn.CONCAT(IF(A3="completion", "Completion", IF(A3="cassette", "Cassette", IF(A3="gemheart", "Crystal Heart", IF(A3="strawberry", _xlfn.CONCAT("Strawberry ", D3+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B3)*(regions!$B$2:$B$27=C3), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 2: Old Site A-Side)</v>
+        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>Cassette (Chapter 2: Old Site A-Side)</v>
+        <f t="shared" ref="F3:F66" si="0">IF(A3="strawberry", "Strawberry", E3)</f>
+        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -616,22 +619,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f>COUNTIFS($A$2:A4, A4, $B$2:B4, B4, $C$2:C4, C4) - 1</f>
+        <f>COUNTIFS($A$3:A4, A4, $B$3:B4, B4, $C$3:C4, C4) - 1</f>
         <v>0</v>
       </c>
       <c r="E4" t="str" cm="1">
         <f t="array" ref="E4">_xlfn.CONCAT(IF(A4="completion", "Completion", IF(A4="cassette", "Cassette", IF(A4="gemheart", "Crystal Heart", IF(A4="strawberry", _xlfn.CONCAT("Strawberry ", D4+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B4)*(regions!$B$2:$B$27=C4), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Cassette (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Cassette (Chapter 2: Old Site A-Side)</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -639,22 +642,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <f>COUNTIFS($A$2:A5, A5, $B$2:B5, B5, $C$2:C5, C5) - 1</f>
+        <f>COUNTIFS($A$3:A5, A5, $B$3:B5, B5, $C$3:C5, C5) - 1</f>
         <v>0</v>
       </c>
       <c r="E5" t="str" cm="1">
         <f t="array" ref="E5">_xlfn.CONCAT(IF(A5="completion", "Completion", IF(A5="cassette", "Cassette", IF(A5="gemheart", "Crystal Heart", IF(A5="strawberry", _xlfn.CONCAT("Strawberry ", D5+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B5)*(regions!$B$2:$B$27=C5), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -662,22 +665,22 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <f>COUNTIFS($A$2:A6, A6, $B$2:B6, B6, $C$2:C6, C6) - 1</f>
+        <f>COUNTIFS($A$3:A6, A6, $B$3:B6, B6, $C$3:C6, C6) - 1</f>
         <v>0</v>
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.CONCAT(IF(A6="completion", "Completion", IF(A6="cassette", "Cassette", IF(A6="gemheart", "Crystal Heart", IF(A6="strawberry", _xlfn.CONCAT("Strawberry ", D6+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B6)*(regions!$B$2:$B$27=C6), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -685,22 +688,22 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f>COUNTIFS($A$2:A7, A7, $B$2:B7, B7, $C$2:C7, C7) - 1</f>
+        <f>COUNTIFS($A$3:A7, A7, $B$3:B7, B7, $C$3:C7, C7) - 1</f>
         <v>0</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xlfn.CONCAT(IF(A7="completion", "Completion", IF(A7="cassette", "Cassette", IF(A7="gemheart", "Crystal Heart", IF(A7="strawberry", _xlfn.CONCAT("Strawberry ", D7+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B7)*(regions!$B$2:$B$27=C7), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 6: Reflection A-Side)</v>
+        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 6: Reflection A-Side)</v>
+        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -708,22 +711,22 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <f>COUNTIFS($A$2:A8, A8, $B$2:B8, B8, $C$2:C8, C8) - 1</f>
+        <f>COUNTIFS($A$3:A8, A8, $B$3:B8, B8, $C$3:C8, C8) - 1</f>
         <v>0</v>
       </c>
       <c r="E8" t="str" cm="1">
         <f t="array" ref="E8">_xlfn.CONCAT(IF(A8="completion", "Completion", IF(A8="cassette", "Cassette", IF(A8="gemheart", "Crystal Heart", IF(A8="strawberry", _xlfn.CONCAT("Strawberry ", D8+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B8)*(regions!$B$2:$B$27=C8), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 7: The Summit A-Side)</v>
+        <v>Cassette (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 7: The Summit A-Side)</v>
+        <v>Cassette (Chapter 6: Reflection A-Side)</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -731,45 +734,45 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <f>COUNTIFS($A$2:A9, A9, $B$2:B9, B9, $C$2:C9, C9) - 1</f>
+        <f>COUNTIFS($A$3:A9, A9, $B$3:B9, B9, $C$3:C9, C9) - 1</f>
         <v>0</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xlfn.CONCAT(IF(A9="completion", "Completion", IF(A9="cassette", "Cassette", IF(A9="gemheart", "Crystal Heart", IF(A9="strawberry", _xlfn.CONCAT("Strawberry ", D9+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B9)*(regions!$B$2:$B$27=C9), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 8: Core A-Side)</v>
+        <v>Cassette (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 8: Core A-Side)</v>
+        <v>Cassette (Chapter 7: The Summit A-Side)</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <f>COUNTIFS($A$2:A10, A10, $B$2:B10, B10, $C$2:C10, C10) - 1</f>
+        <f>COUNTIFS($A$3:A10, A10, $B$3:B10, B10, $C$3:C10, C10) - 1</f>
         <v>0</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10">_xlfn.CONCAT(IF(A10="completion", "Completion", IF(A10="cassette", "Cassette", IF(A10="gemheart", "Crystal Heart", IF(A10="strawberry", _xlfn.CONCAT("Strawberry ", D10+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B10)*(regions!$B$2:$B$27=C10), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
+        <v>Cassette (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
+        <v>Cassette (Chapter 8: Core A-Side)</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,22 +780,22 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <f>COUNTIFS($A$2:A11, A11, $B$2:B11, B11, $C$2:C11, C11) - 1</f>
+        <f>COUNTIFS($A$3:A11, A11, $B$3:B11, B11, $C$3:C11, C11) - 1</f>
         <v>0</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xlfn.CONCAT(IF(A11="completion", "Completion", IF(A11="cassette", "Cassette", IF(A11="gemheart", "Crystal Heart", IF(A11="strawberry", _xlfn.CONCAT("Strawberry ", D11+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B11)*(regions!$B$2:$B$27=C11), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 2: Old Site A-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 2: Old Site A-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -800,22 +803,22 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <f>COUNTIFS($A$2:A12, A12, $B$2:B12, B12, $C$2:C12, C12) - 1</f>
+        <f>COUNTIFS($A$3:A12, A12, $B$3:B12, B12, $C$3:C12, C12) - 1</f>
         <v>0</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" ref="E12">_xlfn.CONCAT(IF(A12="completion", "Completion", IF(A12="cassette", "Cassette", IF(A12="gemheart", "Crystal Heart", IF(A12="strawberry", _xlfn.CONCAT("Strawberry ", D12+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B12)*(regions!$B$2:$B$27=C12), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Completion (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Completion (Chapter 2: Old Site A-Side)</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,22 +826,22 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <f>COUNTIFS($A$2:A13, A13, $B$2:B13, B13, $C$2:C13, C13) - 1</f>
+        <f>COUNTIFS($A$3:A13, A13, $B$3:B13, B13, $C$3:C13, C13) - 1</f>
         <v>0</v>
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xlfn.CONCAT(IF(A13="completion", "Completion", IF(A13="cassette", "Cassette", IF(A13="gemheart", "Crystal Heart", IF(A13="strawberry", _xlfn.CONCAT("Strawberry ", D13+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B13)*(regions!$B$2:$B$27=C13), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -846,22 +849,22 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <f>COUNTIFS($A$2:A14, A14, $B$2:B14, B14, $C$2:C14, C14) - 1</f>
+        <f>COUNTIFS($A$3:A14, A14, $B$3:B14, B14, $C$3:C14, C14) - 1</f>
         <v>0</v>
       </c>
       <c r="E14" t="str" cm="1">
         <f t="array" ref="E14">_xlfn.CONCAT(IF(A14="completion", "Completion", IF(A14="cassette", "Cassette", IF(A14="gemheart", "Crystal Heart", IF(A14="strawberry", _xlfn.CONCAT("Strawberry ", D14+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B14)*(regions!$B$2:$B$27=C14), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -869,22 +872,22 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f>COUNTIFS($A$2:A15, A15, $B$2:B15, B15, $C$2:C15, C15) - 1</f>
+        <f>COUNTIFS($A$3:A15, A15, $B$3:B15, B15, $C$3:C15, C15) - 1</f>
         <v>0</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xlfn.CONCAT(IF(A15="completion", "Completion", IF(A15="cassette", "Cassette", IF(A15="gemheart", "Crystal Heart", IF(A15="strawberry", _xlfn.CONCAT("Strawberry ", D15+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B15)*(regions!$B$2:$B$27=C15), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 6: Reflection A-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 6: Reflection A-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -892,22 +895,22 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f>COUNTIFS($A$2:A16, A16, $B$2:B16, B16, $C$2:C16, C16) - 1</f>
+        <f>COUNTIFS($A$3:A16, A16, $B$3:B16, B16, $C$3:C16, C16) - 1</f>
         <v>0</v>
       </c>
       <c r="E16" t="str" cm="1">
         <f t="array" ref="E16">_xlfn.CONCAT(IF(A16="completion", "Completion", IF(A16="cassette", "Cassette", IF(A16="gemheart", "Crystal Heart", IF(A16="strawberry", _xlfn.CONCAT("Strawberry ", D16+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B16)*(regions!$B$2:$B$27=C16), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 7: The Summit A-Side)</v>
+        <v>Completion (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 7: The Summit A-Side)</v>
+        <v>Completion (Chapter 6: Reflection A-Side)</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,22 +918,22 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f>COUNTIFS($A$2:A17, A17, $B$2:B17, B17, $C$2:C17, C17) - 1</f>
+        <f>COUNTIFS($A$3:A17, A17, $B$3:B17, B17, $C$3:C17, C17) - 1</f>
         <v>0</v>
       </c>
       <c r="E17" t="str" cm="1">
         <f t="array" ref="E17">_xlfn.CONCAT(IF(A17="completion", "Completion", IF(A17="cassette", "Cassette", IF(A17="gemheart", "Crystal Heart", IF(A17="strawberry", _xlfn.CONCAT("Strawberry ", D17+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B17)*(regions!$B$2:$B$27=C17), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Epilogue)</v>
+        <v>Completion (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Epilogue)</v>
+        <v>Completion (Chapter 7: The Summit A-Side)</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -938,22 +941,22 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <f>COUNTIFS($A$2:A18, A18, $B$2:B18, B18, $C$2:C18, C18) - 1</f>
+        <f>COUNTIFS($A$3:A18, A18, $B$3:B18, B18, $C$3:C18, C18) - 1</f>
         <v>0</v>
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" ref="E18">_xlfn.CONCAT(IF(A18="completion", "Completion", IF(A18="cassette", "Cassette", IF(A18="gemheart", "Crystal Heart", IF(A18="strawberry", _xlfn.CONCAT("Strawberry ", D18+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B18)*(regions!$B$2:$B$27=C18), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 8: Core A-Side)</v>
+        <v>Completion (Epilogue)</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 8: Core A-Side)</v>
+        <v>Completion (Epilogue)</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,22 +964,22 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f>COUNTIFS($A$2:A19, A19, $B$2:B19, B19, $C$2:C19, C19) - 1</f>
+        <f>COUNTIFS($A$3:A19, A19, $B$3:B19, B19, $C$3:C19, C19) - 1</f>
         <v>0</v>
       </c>
       <c r="E19" t="str" cm="1">
         <f t="array" ref="E19">_xlfn.CONCAT(IF(A19="completion", "Completion", IF(A19="cassette", "Cassette", IF(A19="gemheart", "Crystal Heart", IF(A19="strawberry", _xlfn.CONCAT("Strawberry ", D19+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B19)*(regions!$B$2:$B$27=C19), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 9: Farewell A-Side)</v>
+        <v>Completion (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 9: Farewell A-Side)</v>
+        <v>Completion (Chapter 8: Core A-Side)</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -984,22 +987,22 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f>COUNTIFS($A$2:A20, A20, $B$2:B20, B20, $C$2:C20, C20) - 1</f>
+        <f>COUNTIFS($A$3:A20, A20, $B$3:B20, B20, $C$3:C20, C20) - 1</f>
         <v>0</v>
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.CONCAT(IF(A20="completion", "Completion", IF(A20="cassette", "Cassette", IF(A20="gemheart", "Crystal Heart", IF(A20="strawberry", _xlfn.CONCAT("Strawberry ", D20+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B20)*(regions!$B$2:$B$27=C20), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
+        <v>Completion (Chapter 9: Farewell A-Side)</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
+        <v>Completion (Chapter 9: Farewell A-Side)</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1007,22 +1010,22 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <f>COUNTIFS($A$2:A21, A21, $B$2:B21, B21, $C$2:C21, C21) - 1</f>
+        <f>COUNTIFS($A$3:A21, A21, $B$3:B21, B21, $C$3:C21, C21) - 1</f>
         <v>0</v>
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.CONCAT(IF(A21="completion", "Completion", IF(A21="cassette", "Cassette", IF(A21="gemheart", "Crystal Heart", IF(A21="strawberry", _xlfn.CONCAT("Strawberry ", D21+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B21)*(regions!$B$2:$B$27=C21), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 2: Old Site B-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 2: Old Site B-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,22 +1033,22 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <f>COUNTIFS($A$2:A22, A22, $B$2:B22, B22, $C$2:C22, C22) - 1</f>
+        <f>COUNTIFS($A$3:A22, A22, $B$3:B22, B22, $C$3:C22, C22) - 1</f>
         <v>0</v>
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.CONCAT(IF(A22="completion", "Completion", IF(A22="cassette", "Cassette", IF(A22="gemheart", "Crystal Heart", IF(A22="strawberry", _xlfn.CONCAT("Strawberry ", D22+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B22)*(regions!$B$2:$B$27=C22), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Completion (Chapter 2: Old Site B-Side)</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Completion (Chapter 2: Old Site B-Side)</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1053,22 +1056,22 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <f>COUNTIFS($A$2:A23, A23, $B$2:B23, B23, $C$2:C23, C23) - 1</f>
+        <f>COUNTIFS($A$3:A23, A23, $B$3:B23, B23, $C$3:C23, C23) - 1</f>
         <v>0</v>
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.CONCAT(IF(A23="completion", "Completion", IF(A23="cassette", "Cassette", IF(A23="gemheart", "Crystal Heart", IF(A23="strawberry", _xlfn.CONCAT("Strawberry ", D23+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B23)*(regions!$B$2:$B$27=C23), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1076,22 +1079,22 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <f>COUNTIFS($A$2:A24, A24, $B$2:B24, B24, $C$2:C24, C24) - 1</f>
+        <f>COUNTIFS($A$3:A24, A24, $B$3:B24, B24, $C$3:C24, C24) - 1</f>
         <v>0</v>
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.CONCAT(IF(A24="completion", "Completion", IF(A24="cassette", "Cassette", IF(A24="gemheart", "Crystal Heart", IF(A24="strawberry", _xlfn.CONCAT("Strawberry ", D24+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B24)*(regions!$B$2:$B$27=C24), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1099,22 +1102,22 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <f>COUNTIFS($A$2:A25, A25, $B$2:B25, B25, $C$2:C25, C25) - 1</f>
+        <f>COUNTIFS($A$3:A25, A25, $B$3:B25, B25, $C$3:C25, C25) - 1</f>
         <v>0</v>
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.CONCAT(IF(A25="completion", "Completion", IF(A25="cassette", "Cassette", IF(A25="gemheart", "Crystal Heart", IF(A25="strawberry", _xlfn.CONCAT("Strawberry ", D25+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B25)*(regions!$B$2:$B$27=C25), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 6: Reflection B-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 6: Reflection B-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1122,22 +1125,22 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <f>COUNTIFS($A$2:A26, A26, $B$2:B26, B26, $C$2:C26, C26) - 1</f>
+        <f>COUNTIFS($A$3:A26, A26, $B$3:B26, B26, $C$3:C26, C26) - 1</f>
         <v>0</v>
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.CONCAT(IF(A26="completion", "Completion", IF(A26="cassette", "Cassette", IF(A26="gemheart", "Crystal Heart", IF(A26="strawberry", _xlfn.CONCAT("Strawberry ", D26+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B26)*(regions!$B$2:$B$27=C26), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 7: The Summit B-Side)</v>
+        <v>Completion (Chapter 6: Reflection B-Side)</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 7: The Summit B-Side)</v>
+        <v>Completion (Chapter 6: Reflection B-Side)</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1145,22 +1148,22 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <f>COUNTIFS($A$2:A27, A27, $B$2:B27, B27, $C$2:C27, C27) - 1</f>
+        <f>COUNTIFS($A$3:A27, A27, $B$3:B27, B27, $C$3:C27, C27) - 1</f>
         <v>0</v>
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.CONCAT(IF(A27="completion", "Completion", IF(A27="cassette", "Cassette", IF(A27="gemheart", "Crystal Heart", IF(A27="strawberry", _xlfn.CONCAT("Strawberry ", D27+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B27)*(regions!$B$2:$B$27=C27), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 8: Core B-Side)</v>
+        <v>Completion (Chapter 7: The Summit B-Side)</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 8: Core B-Side)</v>
+        <v>Completion (Chapter 7: The Summit B-Side)</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1168,22 +1171,22 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <f>COUNTIFS($A$2:A28, A28, $B$2:B28, B28, $C$2:C28, C28) - 1</f>
+        <f>COUNTIFS($A$3:A28, A28, $B$3:B28, B28, $C$3:C28, C28) - 1</f>
         <v>0</v>
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.CONCAT(IF(A28="completion", "Completion", IF(A28="cassette", "Cassette", IF(A28="gemheart", "Crystal Heart", IF(A28="strawberry", _xlfn.CONCAT("Strawberry ", D28+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B28)*(regions!$B$2:$B$27=C28), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
+        <v>Completion (Chapter 8: Core B-Side)</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
+        <v>Completion (Chapter 8: Core B-Side)</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,22 +1194,22 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29">
-        <f>COUNTIFS($A$2:A29, A29, $B$2:B29, B29, $C$2:C29, C29) - 1</f>
+        <f>COUNTIFS($A$3:A29, A29, $B$3:B29, B29, $C$3:C29, C29) - 1</f>
         <v>0</v>
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.CONCAT(IF(A29="completion", "Completion", IF(A29="cassette", "Cassette", IF(A29="gemheart", "Crystal Heart", IF(A29="strawberry", _xlfn.CONCAT("Strawberry ", D29+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B29)*(regions!$B$2:$B$27=C29), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 2: Old Site C-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 2: Old Site C-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1214,22 +1217,22 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30">
-        <f>COUNTIFS($A$2:A30, A30, $B$2:B30, B30, $C$2:C30, C30) - 1</f>
+        <f>COUNTIFS($A$3:A30, A30, $B$3:B30, B30, $C$3:C30, C30) - 1</f>
         <v>0</v>
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.CONCAT(IF(A30="completion", "Completion", IF(A30="cassette", "Cassette", IF(A30="gemheart", "Crystal Heart", IF(A30="strawberry", _xlfn.CONCAT("Strawberry ", D30+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B30)*(regions!$B$2:$B$27=C30), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Completion (Chapter 2: Old Site C-Side)</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Completion (Chapter 2: Old Site C-Side)</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,22 +1240,22 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31">
-        <f>COUNTIFS($A$2:A31, A31, $B$2:B31, B31, $C$2:C31, C31) - 1</f>
+        <f>COUNTIFS($A$3:A31, A31, $B$3:B31, B31, $C$3:C31, C31) - 1</f>
         <v>0</v>
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.CONCAT(IF(A31="completion", "Completion", IF(A31="cassette", "Cassette", IF(A31="gemheart", "Crystal Heart", IF(A31="strawberry", _xlfn.CONCAT("Strawberry ", D31+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B31)*(regions!$B$2:$B$27=C31), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1260,22 +1263,22 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32">
-        <f>COUNTIFS($A$2:A32, A32, $B$2:B32, B32, $C$2:C32, C32) - 1</f>
+        <f>COUNTIFS($A$3:A32, A32, $B$3:B32, B32, $C$3:C32, C32) - 1</f>
         <v>0</v>
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.CONCAT(IF(A32="completion", "Completion", IF(A32="cassette", "Cassette", IF(A32="gemheart", "Crystal Heart", IF(A32="strawberry", _xlfn.CONCAT("Strawberry ", D32+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B32)*(regions!$B$2:$B$27=C32), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1283,22 +1286,22 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33">
-        <f>COUNTIFS($A$2:A33, A33, $B$2:B33, B33, $C$2:C33, C33) - 1</f>
+        <f>COUNTIFS($A$3:A33, A33, $B$3:B33, B33, $C$3:C33, C33) - 1</f>
         <v>0</v>
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.CONCAT(IF(A33="completion", "Completion", IF(A33="cassette", "Cassette", IF(A33="gemheart", "Crystal Heart", IF(A33="strawberry", _xlfn.CONCAT("Strawberry ", D33+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B33)*(regions!$B$2:$B$27=C33), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 6: Reflection C-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 6: Reflection C-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1306,22 +1309,22 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <f>COUNTIFS($A$2:A34, A34, $B$2:B34, B34, $C$2:C34, C34) - 1</f>
+        <f>COUNTIFS($A$3:A34, A34, $B$3:B34, B34, $C$3:C34, C34) - 1</f>
         <v>0</v>
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.CONCAT(IF(A34="completion", "Completion", IF(A34="cassette", "Cassette", IF(A34="gemheart", "Crystal Heart", IF(A34="strawberry", _xlfn.CONCAT("Strawberry ", D34+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B34)*(regions!$B$2:$B$27=C34), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 7: The Summit C-Side)</v>
+        <v>Completion (Chapter 6: Reflection C-Side)</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 7: The Summit C-Side)</v>
+        <v>Completion (Chapter 6: Reflection C-Side)</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1329,45 +1332,45 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35">
-        <f>COUNTIFS($A$2:A35, A35, $B$2:B35, B35, $C$2:C35, C35) - 1</f>
+        <f>COUNTIFS($A$3:A35, A35, $B$3:B35, B35, $C$3:C35, C35) - 1</f>
         <v>0</v>
       </c>
       <c r="E35" t="str" cm="1">
         <f t="array" ref="E35">_xlfn.CONCAT(IF(A35="completion", "Completion", IF(A35="cassette", "Cassette", IF(A35="gemheart", "Crystal Heart", IF(A35="strawberry", _xlfn.CONCAT("Strawberry ", D35+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B35)*(regions!$B$2:$B$27=C35), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 8: Core C-Side)</v>
+        <v>Completion (Chapter 7: The Summit C-Side)</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 8: Core C-Side)</v>
+        <v>Completion (Chapter 7: The Summit C-Side)</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <f>COUNTIFS($A$2:A36, A36, $B$2:B36, B36, $C$2:C36, C36) - 1</f>
+        <f>COUNTIFS($A$3:A36, A36, $B$3:B36, B36, $C$3:C36, C36) - 1</f>
         <v>0</v>
       </c>
       <c r="E36" t="str" cm="1">
         <f t="array" ref="E36">_xlfn.CONCAT(IF(A36="completion", "Completion", IF(A36="cassette", "Cassette", IF(A36="gemheart", "Crystal Heart", IF(A36="strawberry", _xlfn.CONCAT("Strawberry ", D36+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B36)*(regions!$B$2:$B$27=C36), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
+        <v>Completion (Chapter 8: Core C-Side)</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
+        <v>Completion (Chapter 8: Core C-Side)</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1375,22 +1378,22 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <f>COUNTIFS($A$2:A37, A37, $B$2:B37, B37, $C$2:C37, C37) - 1</f>
+        <f>COUNTIFS($A$3:A37, A37, $B$3:B37, B37, $C$3:C37, C37) - 1</f>
         <v>0</v>
       </c>
       <c r="E37" t="str" cm="1">
         <f t="array" ref="E37">_xlfn.CONCAT(IF(A37="completion", "Completion", IF(A37="cassette", "Cassette", IF(A37="gemheart", "Crystal Heart", IF(A37="strawberry", _xlfn.CONCAT("Strawberry ", D37+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B37)*(regions!$B$2:$B$27=C37), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1398,22 +1401,22 @@
         <v>5</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <f>COUNTIFS($A$2:A38, A38, $B$2:B38, B38, $C$2:C38, C38) - 1</f>
+        <f>COUNTIFS($A$3:A38, A38, $B$3:B38, B38, $C$3:C38, C38) - 1</f>
         <v>0</v>
       </c>
       <c r="E38" t="str" cm="1">
         <f t="array" ref="E38">_xlfn.CONCAT(IF(A38="completion", "Completion", IF(A38="cassette", "Cassette", IF(A38="gemheart", "Crystal Heart", IF(A38="strawberry", _xlfn.CONCAT("Strawberry ", D38+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B38)*(regions!$B$2:$B$27=C38), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1421,22 +1424,22 @@
         <v>5</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <f>COUNTIFS($A$2:A39, A39, $B$2:B39, B39, $C$2:C39, C39) - 1</f>
+        <f>COUNTIFS($A$3:A39, A39, $B$3:B39, B39, $C$3:C39, C39) - 1</f>
         <v>0</v>
       </c>
       <c r="E39" t="str" cm="1">
         <f t="array" ref="E39">_xlfn.CONCAT(IF(A39="completion", "Completion", IF(A39="cassette", "Cassette", IF(A39="gemheart", "Crystal Heart", IF(A39="strawberry", _xlfn.CONCAT("Strawberry ", D39+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B39)*(regions!$B$2:$B$27=C39), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1444,22 +1447,22 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <f>COUNTIFS($A$2:A40, A40, $B$2:B40, B40, $C$2:C40, C40) - 1</f>
+        <f>COUNTIFS($A$3:A40, A40, $B$3:B40, B40, $C$3:C40, C40) - 1</f>
         <v>0</v>
       </c>
       <c r="E40" t="str" cm="1">
         <f t="array" ref="E40">_xlfn.CONCAT(IF(A40="completion", "Completion", IF(A40="cassette", "Cassette", IF(A40="gemheart", "Crystal Heart", IF(A40="strawberry", _xlfn.CONCAT("Strawberry ", D40+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B40)*(regions!$B$2:$B$27=C40), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1467,22 +1470,22 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <f>COUNTIFS($A$2:A41, A41, $B$2:B41, B41, $C$2:C41, C41) - 1</f>
+        <f>COUNTIFS($A$3:A41, A41, $B$3:B41, B41, $C$3:C41, C41) - 1</f>
         <v>0</v>
       </c>
       <c r="E41" t="str" cm="1">
         <f t="array" ref="E41">_xlfn.CONCAT(IF(A41="completion", "Completion", IF(A41="cassette", "Cassette", IF(A41="gemheart", "Crystal Heart", IF(A41="strawberry", _xlfn.CONCAT("Strawberry ", D41+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B41)*(regions!$B$2:$B$27=C41), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1490,22 +1493,22 @@
         <v>5</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <f>COUNTIFS($A$2:A42, A42, $B$2:B42, B42, $C$2:C42, C42) - 1</f>
+        <f>COUNTIFS($A$3:A42, A42, $B$3:B42, B42, $C$3:C42, C42) - 1</f>
         <v>0</v>
       </c>
       <c r="E42" t="str" cm="1">
         <f t="array" ref="E42">_xlfn.CONCAT(IF(A42="completion", "Completion", IF(A42="cassette", "Cassette", IF(A42="gemheart", "Crystal Heart", IF(A42="strawberry", _xlfn.CONCAT("Strawberry ", D42+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B42)*(regions!$B$2:$B$27=C42), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,22 +1516,22 @@
         <v>5</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <f>COUNTIFS($A$2:A43, A43, $B$2:B43, B43, $C$2:C43, C43) - 1</f>
+        <f>COUNTIFS($A$3:A43, A43, $B$3:B43, B43, $C$3:C43, C43) - 1</f>
         <v>0</v>
       </c>
       <c r="E43" t="str" cm="1">
         <f t="array" ref="E43">_xlfn.CONCAT(IF(A43="completion", "Completion", IF(A43="cassette", "Cassette", IF(A43="gemheart", "Crystal Heart", IF(A43="strawberry", _xlfn.CONCAT("Strawberry ", D43+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B43)*(regions!$B$2:$B$27=C43), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1536,22 +1539,22 @@
         <v>5</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <f>COUNTIFS($A$2:A44, A44, $B$2:B44, B44, $C$2:C44, C44) - 1</f>
+        <f>COUNTIFS($A$3:A44, A44, $B$3:B44, B44, $C$3:C44, C44) - 1</f>
         <v>0</v>
       </c>
       <c r="E44" t="str" cm="1">
         <f t="array" ref="E44">_xlfn.CONCAT(IF(A44="completion", "Completion", IF(A44="cassette", "Cassette", IF(A44="gemheart", "Crystal Heart", IF(A44="strawberry", _xlfn.CONCAT("Strawberry ", D44+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B44)*(regions!$B$2:$B$27=C44), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1559,22 +1562,22 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <f>COUNTIFS($A$2:A45, A45, $B$2:B45, B45, $C$2:C45, C45) - 1</f>
+        <f>COUNTIFS($A$3:A45, A45, $B$3:B45, B45, $C$3:C45, C45) - 1</f>
         <v>0</v>
       </c>
       <c r="E45" t="str" cm="1">
         <f t="array" ref="E45">_xlfn.CONCAT(IF(A45="completion", "Completion", IF(A45="cassette", "Cassette", IF(A45="gemheart", "Crystal Heart", IF(A45="strawberry", _xlfn.CONCAT("Strawberry ", D45+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B45)*(regions!$B$2:$B$27=C45), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1582,22 +1585,22 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <f>COUNTIFS($A$2:A46, A46, $B$2:B46, B46, $C$2:C46, C46) - 1</f>
+        <f>COUNTIFS($A$3:A46, A46, $B$3:B46, B46, $C$3:C46, C46) - 1</f>
         <v>0</v>
       </c>
       <c r="E46" t="str" cm="1">
         <f t="array" ref="E46">_xlfn.CONCAT(IF(A46="completion", "Completion", IF(A46="cassette", "Cassette", IF(A46="gemheart", "Crystal Heart", IF(A46="strawberry", _xlfn.CONCAT("Strawberry ", D46+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B46)*(regions!$B$2:$B$27=C46), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1605,22 +1608,22 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <f>COUNTIFS($A$2:A47, A47, $B$2:B47, B47, $C$2:C47, C47) - 1</f>
+        <f>COUNTIFS($A$3:A47, A47, $B$3:B47, B47, $C$3:C47, C47) - 1</f>
         <v>0</v>
       </c>
       <c r="E47" t="str" cm="1">
         <f t="array" ref="E47">_xlfn.CONCAT(IF(A47="completion", "Completion", IF(A47="cassette", "Cassette", IF(A47="gemheart", "Crystal Heart", IF(A47="strawberry", _xlfn.CONCAT("Strawberry ", D47+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B47)*(regions!$B$2:$B$27=C47), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1628,22 +1631,22 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <f>COUNTIFS($A$2:A48, A48, $B$2:B48, B48, $C$2:C48, C48) - 1</f>
+        <f>COUNTIFS($A$3:A48, A48, $B$3:B48, B48, $C$3:C48, C48) - 1</f>
         <v>0</v>
       </c>
       <c r="E48" t="str" cm="1">
         <f t="array" ref="E48">_xlfn.CONCAT(IF(A48="completion", "Completion", IF(A48="cassette", "Cassette", IF(A48="gemheart", "Crystal Heart", IF(A48="strawberry", _xlfn.CONCAT("Strawberry ", D48+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B48)*(regions!$B$2:$B$27=C48), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,22 +1654,22 @@
         <v>5</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <f>COUNTIFS($A$2:A49, A49, $B$2:B49, B49, $C$2:C49, C49) - 1</f>
+        <f>COUNTIFS($A$3:A49, A49, $B$3:B49, B49, $C$3:C49, C49) - 1</f>
         <v>0</v>
       </c>
       <c r="E49" t="str" cm="1">
         <f t="array" ref="E49">_xlfn.CONCAT(IF(A49="completion", "Completion", IF(A49="cassette", "Cassette", IF(A49="gemheart", "Crystal Heart", IF(A49="strawberry", _xlfn.CONCAT("Strawberry ", D49+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B49)*(regions!$B$2:$B$27=C49), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1674,22 +1677,22 @@
         <v>5</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <f>COUNTIFS($A$2:A50, A50, $B$2:B50, B50, $C$2:C50, C50) - 1</f>
+        <f>COUNTIFS($A$3:A50, A50, $B$3:B50, B50, $C$3:C50, C50) - 1</f>
         <v>0</v>
       </c>
       <c r="E50" t="str" cm="1">
         <f t="array" ref="E50">_xlfn.CONCAT(IF(A50="completion", "Completion", IF(A50="cassette", "Cassette", IF(A50="gemheart", "Crystal Heart", IF(A50="strawberry", _xlfn.CONCAT("Strawberry ", D50+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B50)*(regions!$B$2:$B$27=C50), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1697,22 +1700,22 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <f>COUNTIFS($A$2:A51, A51, $B$2:B51, B51, $C$2:C51, C51) - 1</f>
+        <f>COUNTIFS($A$3:A51, A51, $B$3:B51, B51, $C$3:C51, C51) - 1</f>
         <v>0</v>
       </c>
       <c r="E51" t="str" cm="1">
         <f t="array" ref="E51">_xlfn.CONCAT(IF(A51="completion", "Completion", IF(A51="cassette", "Cassette", IF(A51="gemheart", "Crystal Heart", IF(A51="strawberry", _xlfn.CONCAT("Strawberry ", D51+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B51)*(regions!$B$2:$B$27=C51), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1720,22 +1723,22 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <f>COUNTIFS($A$2:A52, A52, $B$2:B52, B52, $C$2:C52, C52) - 1</f>
+        <f>COUNTIFS($A$3:A52, A52, $B$3:B52, B52, $C$3:C52, C52) - 1</f>
         <v>0</v>
       </c>
       <c r="E52" t="str" cm="1">
         <f t="array" ref="E52">_xlfn.CONCAT(IF(A52="completion", "Completion", IF(A52="cassette", "Cassette", IF(A52="gemheart", "Crystal Heart", IF(A52="strawberry", _xlfn.CONCAT("Strawberry ", D52+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B52)*(regions!$B$2:$B$27=C52), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1743,22 +1746,22 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <f>COUNTIFS($A$2:A53, A53, $B$2:B53, B53, $C$2:C53, C53) - 1</f>
+        <f>COUNTIFS($A$3:A53, A53, $B$3:B53, B53, $C$3:C53, C53) - 1</f>
         <v>0</v>
       </c>
       <c r="E53" t="str" cm="1">
         <f t="array" ref="E53">_xlfn.CONCAT(IF(A53="completion", "Completion", IF(A53="cassette", "Cassette", IF(A53="gemheart", "Crystal Heart", IF(A53="strawberry", _xlfn.CONCAT("Strawberry ", D53+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B53)*(regions!$B$2:$B$27=C53), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,22 +1769,22 @@
         <v>5</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54">
-        <f>COUNTIFS($A$2:A54, A54, $B$2:B54, B54, $C$2:C54, C54) - 1</f>
+        <f>COUNTIFS($A$3:A54, A54, $B$3:B54, B54, $C$3:C54, C54) - 1</f>
         <v>0</v>
       </c>
       <c r="E54" t="str" cm="1">
         <f t="array" ref="E54">_xlfn.CONCAT(IF(A54="completion", "Completion", IF(A54="cassette", "Cassette", IF(A54="gemheart", "Crystal Heart", IF(A54="strawberry", _xlfn.CONCAT("Strawberry ", D54+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B54)*(regions!$B$2:$B$27=C54), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1789,22 +1792,22 @@
         <v>5</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C55">
         <v>2</v>
       </c>
       <c r="D55">
-        <f>COUNTIFS($A$2:A55, A55, $B$2:B55, B55, $C$2:C55, C55) - 1</f>
+        <f>COUNTIFS($A$3:A55, A55, $B$3:B55, B55, $C$3:C55, C55) - 1</f>
         <v>0</v>
       </c>
       <c r="E55" t="str" cm="1">
         <f t="array" ref="E55">_xlfn.CONCAT(IF(A55="completion", "Completion", IF(A55="cassette", "Cassette", IF(A55="gemheart", "Crystal Heart", IF(A55="strawberry", _xlfn.CONCAT("Strawberry ", D55+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B55)*(regions!$B$2:$B$27=C55), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1812,22 +1815,22 @@
         <v>5</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
       <c r="D56">
-        <f>COUNTIFS($A$2:A56, A56, $B$2:B56, B56, $C$2:C56, C56) - 1</f>
+        <f>COUNTIFS($A$3:A56, A56, $B$3:B56, B56, $C$3:C56, C56) - 1</f>
         <v>0</v>
       </c>
       <c r="E56" t="str" cm="1">
         <f t="array" ref="E56">_xlfn.CONCAT(IF(A56="completion", "Completion", IF(A56="cassette", "Cassette", IF(A56="gemheart", "Crystal Heart", IF(A56="strawberry", _xlfn.CONCAT("Strawberry ", D56+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B56)*(regions!$B$2:$B$27=C56), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1835,22 +1838,22 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="D57">
-        <f>COUNTIFS($A$2:A57, A57, $B$2:B57, B57, $C$2:C57, C57) - 1</f>
+        <f>COUNTIFS($A$3:A57, A57, $B$3:B57, B57, $C$3:C57, C57) - 1</f>
         <v>0</v>
       </c>
       <c r="E57" t="str" cm="1">
         <f t="array" ref="E57">_xlfn.CONCAT(IF(A57="completion", "Completion", IF(A57="cassette", "Cassette", IF(A57="gemheart", "Crystal Heart", IF(A57="strawberry", _xlfn.CONCAT("Strawberry ", D57+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B57)*(regions!$B$2:$B$27=C57), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1858,22 +1861,22 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58">
         <v>2</v>
       </c>
       <c r="D58">
-        <f>COUNTIFS($A$2:A58, A58, $B$2:B58, B58, $C$2:C58, C58) - 1</f>
+        <f>COUNTIFS($A$3:A58, A58, $B$3:B58, B58, $C$3:C58, C58) - 1</f>
         <v>0</v>
       </c>
       <c r="E58" t="str" cm="1">
         <f t="array" ref="E58">_xlfn.CONCAT(IF(A58="completion", "Completion", IF(A58="cassette", "Cassette", IF(A58="gemheart", "Crystal Heart", IF(A58="strawberry", _xlfn.CONCAT("Strawberry ", D58+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B58)*(regions!$B$2:$B$27=C58), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1881,45 +1884,45 @@
         <v>5</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59">
-        <f>COUNTIFS($A$2:A59, A59, $B$2:B59, B59, $C$2:C59, C59) - 1</f>
+        <f>COUNTIFS($A$3:A59, A59, $B$3:B59, B59, $C$3:C59, C59) - 1</f>
         <v>0</v>
       </c>
       <c r="E59" t="str" cm="1">
         <f t="array" ref="E59">_xlfn.CONCAT(IF(A59="completion", "Completion", IF(A59="cassette", "Cassette", IF(A59="gemheart", "Crystal Heart", IF(A59="strawberry", _xlfn.CONCAT("Strawberry ", D59+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B59)*(regions!$B$2:$B$27=C59), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60">
-        <f>COUNTIFS($A$2:A60, A60, $B$2:B60, B60, $C$2:C60, C60) - 1</f>
+        <f>COUNTIFS($A$3:A60, A60, $B$3:B60, B60, $C$3:C60, C60) - 1</f>
         <v>0</v>
       </c>
       <c r="E60" t="str" cm="1">
         <f t="array" ref="E60">_xlfn.CONCAT(IF(A60="completion", "Completion", IF(A60="cassette", "Cassette", IF(A60="gemheart", "Crystal Heart", IF(A60="strawberry", _xlfn.CONCAT("Strawberry ", D60+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B60)*(regions!$B$2:$B$27=C60), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>Strawberry</v>
+        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1933,12 +1936,12 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <f>COUNTIFS($A$2:A61, A61, $B$2:B61, B61, $C$2:C61, C61) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A61, A61, $B$3:B61, B61, $C$3:C61, C61) - 1</f>
+        <v>0</v>
       </c>
       <c r="E61" t="str" cm="1">
         <f t="array" ref="E61">_xlfn.CONCAT(IF(A61="completion", "Completion", IF(A61="cassette", "Cassette", IF(A61="gemheart", "Crystal Heart", IF(A61="strawberry", _xlfn.CONCAT("Strawberry ", D61+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B61)*(regions!$B$2:$B$27=C61), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 1 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
@@ -1956,12 +1959,12 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <f>COUNTIFS($A$2:A62, A62, $B$2:B62, B62, $C$2:C62, C62) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A62, A62, $B$3:B62, B62, $C$3:C62, C62) - 1</f>
+        <v>1</v>
       </c>
       <c r="E62" t="str" cm="1">
         <f t="array" ref="E62">_xlfn.CONCAT(IF(A62="completion", "Completion", IF(A62="cassette", "Cassette", IF(A62="gemheart", "Crystal Heart", IF(A62="strawberry", _xlfn.CONCAT("Strawberry ", D62+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B62)*(regions!$B$2:$B$27=C62), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 2 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
@@ -1979,12 +1982,12 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <f>COUNTIFS($A$2:A63, A63, $B$2:B63, B63, $C$2:C63, C63) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A63, A63, $B$3:B63, B63, $C$3:C63, C63) - 1</f>
+        <v>2</v>
       </c>
       <c r="E63" t="str" cm="1">
         <f t="array" ref="E63">_xlfn.CONCAT(IF(A63="completion", "Completion", IF(A63="cassette", "Cassette", IF(A63="gemheart", "Crystal Heart", IF(A63="strawberry", _xlfn.CONCAT("Strawberry ", D63+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B63)*(regions!$B$2:$B$27=C63), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 3 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
@@ -2002,12 +2005,12 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <f>COUNTIFS($A$2:A64, A64, $B$2:B64, B64, $C$2:C64, C64) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A64, A64, $B$3:B64, B64, $C$3:C64, C64) - 1</f>
+        <v>3</v>
       </c>
       <c r="E64" t="str" cm="1">
         <f t="array" ref="E64">_xlfn.CONCAT(IF(A64="completion", "Completion", IF(A64="cassette", "Cassette", IF(A64="gemheart", "Crystal Heart", IF(A64="strawberry", _xlfn.CONCAT("Strawberry ", D64+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B64)*(regions!$B$2:$B$27=C64), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 4 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
@@ -2025,12 +2028,12 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <f>COUNTIFS($A$2:A65, A65, $B$2:B65, B65, $C$2:C65, C65) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A65, A65, $B$3:B65, B65, $C$3:C65, C65) - 1</f>
+        <v>4</v>
       </c>
       <c r="E65" t="str" cm="1">
         <f t="array" ref="E65">_xlfn.CONCAT(IF(A65="completion", "Completion", IF(A65="cassette", "Cassette", IF(A65="gemheart", "Crystal Heart", IF(A65="strawberry", _xlfn.CONCAT("Strawberry ", D65+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B65)*(regions!$B$2:$B$27=C65), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 5 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
@@ -2048,15 +2051,15 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <f>COUNTIFS($A$2:A66, A66, $B$2:B66, B66, $C$2:C66, C66) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A66, A66, $B$3:B66, B66, $C$3:C66, C66) - 1</f>
+        <v>5</v>
       </c>
       <c r="E66" t="str" cm="1">
         <f t="array" ref="E66">_xlfn.CONCAT(IF(A66="completion", "Completion", IF(A66="cassette", "Cassette", IF(A66="gemheart", "Crystal Heart", IF(A66="strawberry", _xlfn.CONCAT("Strawberry ", D66+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B66)*(regions!$B$2:$B$27=C66), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 6 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F129" si="1">IF(A66="strawberry", "Strawberry", E66)</f>
+        <f t="shared" si="0"/>
         <v>Strawberry</v>
       </c>
     </row>
@@ -2071,15 +2074,15 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <f>COUNTIFS($A$2:A67, A67, $B$2:B67, B67, $C$2:C67, C67) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A67, A67, $B$3:B67, B67, $C$3:C67, C67) - 1</f>
+        <v>6</v>
       </c>
       <c r="E67" t="str" cm="1">
         <f t="array" ref="E67">_xlfn.CONCAT(IF(A67="completion", "Completion", IF(A67="cassette", "Cassette", IF(A67="gemheart", "Crystal Heart", IF(A67="strawberry", _xlfn.CONCAT("Strawberry ", D67+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B67)*(regions!$B$2:$B$27=C67), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 7 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F67:F130" si="1">IF(A67="strawberry", "Strawberry", E67)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -2094,12 +2097,12 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <f>COUNTIFS($A$2:A68, A68, $B$2:B68, B68, $C$2:C68, C68) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A68, A68, $B$3:B68, B68, $C$3:C68, C68) - 1</f>
+        <v>7</v>
       </c>
       <c r="E68" t="str" cm="1">
         <f t="array" ref="E68">_xlfn.CONCAT(IF(A68="completion", "Completion", IF(A68="cassette", "Cassette", IF(A68="gemheart", "Crystal Heart", IF(A68="strawberry", _xlfn.CONCAT("Strawberry ", D68+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B68)*(regions!$B$2:$B$27=C68), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 8 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
@@ -2117,12 +2120,12 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f>COUNTIFS($A$2:A69, A69, $B$2:B69, B69, $C$2:C69, C69) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A69, A69, $B$3:B69, B69, $C$3:C69, C69) - 1</f>
+        <v>8</v>
       </c>
       <c r="E69" t="str" cm="1">
         <f t="array" ref="E69">_xlfn.CONCAT(IF(A69="completion", "Completion", IF(A69="cassette", "Cassette", IF(A69="gemheart", "Crystal Heart", IF(A69="strawberry", _xlfn.CONCAT("Strawberry ", D69+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B69)*(regions!$B$2:$B$27=C69), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 9 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
@@ -2140,12 +2143,12 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f>COUNTIFS($A$2:A70, A70, $B$2:B70, B70, $C$2:C70, C70) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A70, A70, $B$3:B70, B70, $C$3:C70, C70) - 1</f>
+        <v>9</v>
       </c>
       <c r="E70" t="str" cm="1">
         <f t="array" ref="E70">_xlfn.CONCAT(IF(A70="completion", "Completion", IF(A70="cassette", "Cassette", IF(A70="gemheart", "Crystal Heart", IF(A70="strawberry", _xlfn.CONCAT("Strawberry ", D70+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B70)*(regions!$B$2:$B$27=C70), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 10 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
@@ -2163,12 +2166,12 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <f>COUNTIFS($A$2:A71, A71, $B$2:B71, B71, $C$2:C71, C71) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A71, A71, $B$3:B71, B71, $C$3:C71, C71) - 1</f>
+        <v>10</v>
       </c>
       <c r="E71" t="str" cm="1">
         <f t="array" ref="E71">_xlfn.CONCAT(IF(A71="completion", "Completion", IF(A71="cassette", "Cassette", IF(A71="gemheart", "Crystal Heart", IF(A71="strawberry", _xlfn.CONCAT("Strawberry ", D71+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B71)*(regions!$B$2:$B$27=C71), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 11 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
@@ -2186,12 +2189,12 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f>COUNTIFS($A$2:A72, A72, $B$2:B72, B72, $C$2:C72, C72) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A72, A72, $B$3:B72, B72, $C$3:C72, C72) - 1</f>
+        <v>11</v>
       </c>
       <c r="E72" t="str" cm="1">
         <f t="array" ref="E72">_xlfn.CONCAT(IF(A72="completion", "Completion", IF(A72="cassette", "Cassette", IF(A72="gemheart", "Crystal Heart", IF(A72="strawberry", _xlfn.CONCAT("Strawberry ", D72+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B72)*(regions!$B$2:$B$27=C72), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 12 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
@@ -2209,12 +2212,12 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <f>COUNTIFS($A$2:A73, A73, $B$2:B73, B73, $C$2:C73, C73) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A73, A73, $B$3:B73, B73, $C$3:C73, C73) - 1</f>
+        <v>12</v>
       </c>
       <c r="E73" t="str" cm="1">
         <f t="array" ref="E73">_xlfn.CONCAT(IF(A73="completion", "Completion", IF(A73="cassette", "Cassette", IF(A73="gemheart", "Crystal Heart", IF(A73="strawberry", _xlfn.CONCAT("Strawberry ", D73+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B73)*(regions!$B$2:$B$27=C73), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 13 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
@@ -2232,12 +2235,12 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <f>COUNTIFS($A$2:A74, A74, $B$2:B74, B74, $C$2:C74, C74) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A74, A74, $B$3:B74, B74, $C$3:C74, C74) - 1</f>
+        <v>13</v>
       </c>
       <c r="E74" t="str" cm="1">
         <f t="array" ref="E74">_xlfn.CONCAT(IF(A74="completion", "Completion", IF(A74="cassette", "Cassette", IF(A74="gemheart", "Crystal Heart", IF(A74="strawberry", _xlfn.CONCAT("Strawberry ", D74+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B74)*(regions!$B$2:$B$27=C74), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 14 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
@@ -2255,12 +2258,12 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <f>COUNTIFS($A$2:A75, A75, $B$2:B75, B75, $C$2:C75, C75) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A75, A75, $B$3:B75, B75, $C$3:C75, C75) - 1</f>
+        <v>14</v>
       </c>
       <c r="E75" t="str" cm="1">
         <f t="array" ref="E75">_xlfn.CONCAT(IF(A75="completion", "Completion", IF(A75="cassette", "Cassette", IF(A75="gemheart", "Crystal Heart", IF(A75="strawberry", _xlfn.CONCAT("Strawberry ", D75+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B75)*(regions!$B$2:$B$27=C75), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 15 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
@@ -2278,12 +2281,12 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <f>COUNTIFS($A$2:A76, A76, $B$2:B76, B76, $C$2:C76, C76) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A76, A76, $B$3:B76, B76, $C$3:C76, C76) - 1</f>
+        <v>15</v>
       </c>
       <c r="E76" t="str" cm="1">
         <f t="array" ref="E76">_xlfn.CONCAT(IF(A76="completion", "Completion", IF(A76="cassette", "Cassette", IF(A76="gemheart", "Crystal Heart", IF(A76="strawberry", _xlfn.CONCAT("Strawberry ", D76+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B76)*(regions!$B$2:$B$27=C76), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 16 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
@@ -2301,12 +2304,12 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <f>COUNTIFS($A$2:A77, A77, $B$2:B77, B77, $C$2:C77, C77) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A77, A77, $B$3:B77, B77, $C$3:C77, C77) - 1</f>
+        <v>16</v>
       </c>
       <c r="E77" t="str" cm="1">
         <f t="array" ref="E77">_xlfn.CONCAT(IF(A77="completion", "Completion", IF(A77="cassette", "Cassette", IF(A77="gemheart", "Crystal Heart", IF(A77="strawberry", _xlfn.CONCAT("Strawberry ", D77+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B77)*(regions!$B$2:$B$27=C77), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 17 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
@@ -2324,12 +2327,12 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <f>COUNTIFS($A$2:A78, A78, $B$2:B78, B78, $C$2:C78, C78) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A78, A78, $B$3:B78, B78, $C$3:C78, C78) - 1</f>
+        <v>17</v>
       </c>
       <c r="E78" t="str" cm="1">
         <f t="array" ref="E78">_xlfn.CONCAT(IF(A78="completion", "Completion", IF(A78="cassette", "Cassette", IF(A78="gemheart", "Crystal Heart", IF(A78="strawberry", _xlfn.CONCAT("Strawberry ", D78+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B78)*(regions!$B$2:$B$27=C78), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 18 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
@@ -2347,12 +2350,12 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <f>COUNTIFS($A$2:A79, A79, $B$2:B79, B79, $C$2:C79, C79) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A79, A79, $B$3:B79, B79, $C$3:C79, C79) - 1</f>
+        <v>18</v>
       </c>
       <c r="E79" t="str" cm="1">
         <f t="array" ref="E79">_xlfn.CONCAT(IF(A79="completion", "Completion", IF(A79="cassette", "Cassette", IF(A79="gemheart", "Crystal Heart", IF(A79="strawberry", _xlfn.CONCAT("Strawberry ", D79+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B79)*(regions!$B$2:$B$27=C79), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 19 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
@@ -2364,18 +2367,18 @@
         <v>6</v>
       </c>
       <c r="B80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <f>COUNTIFS($A$2:A80, A80, $B$2:B80, B80, $C$2:C80, C80) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A80, A80, $B$3:B80, B80, $C$3:C80, C80) - 1</f>
+        <v>19</v>
       </c>
       <c r="E80" t="str" cm="1">
         <f t="array" ref="E80">_xlfn.CONCAT(IF(A80="completion", "Completion", IF(A80="cassette", "Cassette", IF(A80="gemheart", "Crystal Heart", IF(A80="strawberry", _xlfn.CONCAT("Strawberry ", D80+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B80)*(regions!$B$2:$B$27=C80), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 20 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
@@ -2393,12 +2396,12 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <f>COUNTIFS($A$2:A81, A81, $B$2:B81, B81, $C$2:C81, C81) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A81, A81, $B$3:B81, B81, $C$3:C81, C81) - 1</f>
+        <v>0</v>
       </c>
       <c r="E81" t="str" cm="1">
         <f t="array" ref="E81">_xlfn.CONCAT(IF(A81="completion", "Completion", IF(A81="cassette", "Cassette", IF(A81="gemheart", "Crystal Heart", IF(A81="strawberry", _xlfn.CONCAT("Strawberry ", D81+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B81)*(regions!$B$2:$B$27=C81), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 1 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
@@ -2416,12 +2419,12 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <f>COUNTIFS($A$2:A82, A82, $B$2:B82, B82, $C$2:C82, C82) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A82, A82, $B$3:B82, B82, $C$3:C82, C82) - 1</f>
+        <v>1</v>
       </c>
       <c r="E82" t="str" cm="1">
         <f t="array" ref="E82">_xlfn.CONCAT(IF(A82="completion", "Completion", IF(A82="cassette", "Cassette", IF(A82="gemheart", "Crystal Heart", IF(A82="strawberry", _xlfn.CONCAT("Strawberry ", D82+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B82)*(regions!$B$2:$B$27=C82), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 2 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
@@ -2439,12 +2442,12 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <f>COUNTIFS($A$2:A83, A83, $B$2:B83, B83, $C$2:C83, C83) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A83, A83, $B$3:B83, B83, $C$3:C83, C83) - 1</f>
+        <v>2</v>
       </c>
       <c r="E83" t="str" cm="1">
         <f t="array" ref="E83">_xlfn.CONCAT(IF(A83="completion", "Completion", IF(A83="cassette", "Cassette", IF(A83="gemheart", "Crystal Heart", IF(A83="strawberry", _xlfn.CONCAT("Strawberry ", D83+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B83)*(regions!$B$2:$B$27=C83), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 3 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
@@ -2462,12 +2465,12 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <f>COUNTIFS($A$2:A84, A84, $B$2:B84, B84, $C$2:C84, C84) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A84, A84, $B$3:B84, B84, $C$3:C84, C84) - 1</f>
+        <v>3</v>
       </c>
       <c r="E84" t="str" cm="1">
         <f t="array" ref="E84">_xlfn.CONCAT(IF(A84="completion", "Completion", IF(A84="cassette", "Cassette", IF(A84="gemheart", "Crystal Heart", IF(A84="strawberry", _xlfn.CONCAT("Strawberry ", D84+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B84)*(regions!$B$2:$B$27=C84), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 4 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
@@ -2485,12 +2488,12 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <f>COUNTIFS($A$2:A85, A85, $B$2:B85, B85, $C$2:C85, C85) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A85, A85, $B$3:B85, B85, $C$3:C85, C85) - 1</f>
+        <v>4</v>
       </c>
       <c r="E85" t="str" cm="1">
         <f t="array" ref="E85">_xlfn.CONCAT(IF(A85="completion", "Completion", IF(A85="cassette", "Cassette", IF(A85="gemheart", "Crystal Heart", IF(A85="strawberry", _xlfn.CONCAT("Strawberry ", D85+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B85)*(regions!$B$2:$B$27=C85), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 5 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
@@ -2508,12 +2511,12 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <f>COUNTIFS($A$2:A86, A86, $B$2:B86, B86, $C$2:C86, C86) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A86, A86, $B$3:B86, B86, $C$3:C86, C86) - 1</f>
+        <v>5</v>
       </c>
       <c r="E86" t="str" cm="1">
         <f t="array" ref="E86">_xlfn.CONCAT(IF(A86="completion", "Completion", IF(A86="cassette", "Cassette", IF(A86="gemheart", "Crystal Heart", IF(A86="strawberry", _xlfn.CONCAT("Strawberry ", D86+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B86)*(regions!$B$2:$B$27=C86), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 6 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
@@ -2531,12 +2534,12 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <f>COUNTIFS($A$2:A87, A87, $B$2:B87, B87, $C$2:C87, C87) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A87, A87, $B$3:B87, B87, $C$3:C87, C87) - 1</f>
+        <v>6</v>
       </c>
       <c r="E87" t="str" cm="1">
         <f t="array" ref="E87">_xlfn.CONCAT(IF(A87="completion", "Completion", IF(A87="cassette", "Cassette", IF(A87="gemheart", "Crystal Heart", IF(A87="strawberry", _xlfn.CONCAT("Strawberry ", D87+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B87)*(regions!$B$2:$B$27=C87), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 7 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
@@ -2554,12 +2557,12 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <f>COUNTIFS($A$2:A88, A88, $B$2:B88, B88, $C$2:C88, C88) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A88, A88, $B$3:B88, B88, $C$3:C88, C88) - 1</f>
+        <v>7</v>
       </c>
       <c r="E88" t="str" cm="1">
         <f t="array" ref="E88">_xlfn.CONCAT(IF(A88="completion", "Completion", IF(A88="cassette", "Cassette", IF(A88="gemheart", "Crystal Heart", IF(A88="strawberry", _xlfn.CONCAT("Strawberry ", D88+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B88)*(regions!$B$2:$B$27=C88), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 8 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
@@ -2577,12 +2580,12 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <f>COUNTIFS($A$2:A89, A89, $B$2:B89, B89, $C$2:C89, C89) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A89, A89, $B$3:B89, B89, $C$3:C89, C89) - 1</f>
+        <v>8</v>
       </c>
       <c r="E89" t="str" cm="1">
         <f t="array" ref="E89">_xlfn.CONCAT(IF(A89="completion", "Completion", IF(A89="cassette", "Cassette", IF(A89="gemheart", "Crystal Heart", IF(A89="strawberry", _xlfn.CONCAT("Strawberry ", D89+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B89)*(regions!$B$2:$B$27=C89), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 9 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
@@ -2600,12 +2603,12 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <f>COUNTIFS($A$2:A90, A90, $B$2:B90, B90, $C$2:C90, C90) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A90, A90, $B$3:B90, B90, $C$3:C90, C90) - 1</f>
+        <v>9</v>
       </c>
       <c r="E90" t="str" cm="1">
         <f t="array" ref="E90">_xlfn.CONCAT(IF(A90="completion", "Completion", IF(A90="cassette", "Cassette", IF(A90="gemheart", "Crystal Heart", IF(A90="strawberry", _xlfn.CONCAT("Strawberry ", D90+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B90)*(regions!$B$2:$B$27=C90), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 10 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
@@ -2623,12 +2626,12 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <f>COUNTIFS($A$2:A91, A91, $B$2:B91, B91, $C$2:C91, C91) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A91, A91, $B$3:B91, B91, $C$3:C91, C91) - 1</f>
+        <v>10</v>
       </c>
       <c r="E91" t="str" cm="1">
         <f t="array" ref="E91">_xlfn.CONCAT(IF(A91="completion", "Completion", IF(A91="cassette", "Cassette", IF(A91="gemheart", "Crystal Heart", IF(A91="strawberry", _xlfn.CONCAT("Strawberry ", D91+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B91)*(regions!$B$2:$B$27=C91), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 11 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
@@ -2646,12 +2649,12 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <f>COUNTIFS($A$2:A92, A92, $B$2:B92, B92, $C$2:C92, C92) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A92, A92, $B$3:B92, B92, $C$3:C92, C92) - 1</f>
+        <v>11</v>
       </c>
       <c r="E92" t="str" cm="1">
         <f t="array" ref="E92">_xlfn.CONCAT(IF(A92="completion", "Completion", IF(A92="cassette", "Cassette", IF(A92="gemheart", "Crystal Heart", IF(A92="strawberry", _xlfn.CONCAT("Strawberry ", D92+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B92)*(regions!$B$2:$B$27=C92), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 12 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
@@ -2669,12 +2672,12 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <f>COUNTIFS($A$2:A93, A93, $B$2:B93, B93, $C$2:C93, C93) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A93, A93, $B$3:B93, B93, $C$3:C93, C93) - 1</f>
+        <v>12</v>
       </c>
       <c r="E93" t="str" cm="1">
         <f t="array" ref="E93">_xlfn.CONCAT(IF(A93="completion", "Completion", IF(A93="cassette", "Cassette", IF(A93="gemheart", "Crystal Heart", IF(A93="strawberry", _xlfn.CONCAT("Strawberry ", D93+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B93)*(regions!$B$2:$B$27=C93), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 13 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
@@ -2692,12 +2695,12 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <f>COUNTIFS($A$2:A94, A94, $B$2:B94, B94, $C$2:C94, C94) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A94, A94, $B$3:B94, B94, $C$3:C94, C94) - 1</f>
+        <v>13</v>
       </c>
       <c r="E94" t="str" cm="1">
         <f t="array" ref="E94">_xlfn.CONCAT(IF(A94="completion", "Completion", IF(A94="cassette", "Cassette", IF(A94="gemheart", "Crystal Heart", IF(A94="strawberry", _xlfn.CONCAT("Strawberry ", D94+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B94)*(regions!$B$2:$B$27=C94), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 14 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
@@ -2715,12 +2718,12 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <f>COUNTIFS($A$2:A95, A95, $B$2:B95, B95, $C$2:C95, C95) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A95, A95, $B$3:B95, B95, $C$3:C95, C95) - 1</f>
+        <v>14</v>
       </c>
       <c r="E95" t="str" cm="1">
         <f t="array" ref="E95">_xlfn.CONCAT(IF(A95="completion", "Completion", IF(A95="cassette", "Cassette", IF(A95="gemheart", "Crystal Heart", IF(A95="strawberry", _xlfn.CONCAT("Strawberry ", D95+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B95)*(regions!$B$2:$B$27=C95), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 15 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
@@ -2738,12 +2741,12 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <f>COUNTIFS($A$2:A96, A96, $B$2:B96, B96, $C$2:C96, C96) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A96, A96, $B$3:B96, B96, $C$3:C96, C96) - 1</f>
+        <v>15</v>
       </c>
       <c r="E96" t="str" cm="1">
         <f t="array" ref="E96">_xlfn.CONCAT(IF(A96="completion", "Completion", IF(A96="cassette", "Cassette", IF(A96="gemheart", "Crystal Heart", IF(A96="strawberry", _xlfn.CONCAT("Strawberry ", D96+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B96)*(regions!$B$2:$B$27=C96), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 16 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
@@ -2761,12 +2764,12 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <f>COUNTIFS($A$2:A97, A97, $B$2:B97, B97, $C$2:C97, C97) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A97, A97, $B$3:B97, B97, $C$3:C97, C97) - 1</f>
+        <v>16</v>
       </c>
       <c r="E97" t="str" cm="1">
         <f t="array" ref="E97">_xlfn.CONCAT(IF(A97="completion", "Completion", IF(A97="cassette", "Cassette", IF(A97="gemheart", "Crystal Heart", IF(A97="strawberry", _xlfn.CONCAT("Strawberry ", D97+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B97)*(regions!$B$2:$B$27=C97), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 17 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
@@ -2778,18 +2781,18 @@
         <v>6</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
-        <f>COUNTIFS($A$2:A98, A98, $B$2:B98, B98, $C$2:C98, C98) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A98, A98, $B$3:B98, B98, $C$3:C98, C98) - 1</f>
+        <v>17</v>
       </c>
       <c r="E98" t="str" cm="1">
         <f t="array" ref="E98">_xlfn.CONCAT(IF(A98="completion", "Completion", IF(A98="cassette", "Cassette", IF(A98="gemheart", "Crystal Heart", IF(A98="strawberry", _xlfn.CONCAT("Strawberry ", D98+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B98)*(regions!$B$2:$B$27=C98), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 18 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
@@ -2807,12 +2810,12 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <f>COUNTIFS($A$2:A99, A99, $B$2:B99, B99, $C$2:C99, C99) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A99, A99, $B$3:B99, B99, $C$3:C99, C99) - 1</f>
+        <v>0</v>
       </c>
       <c r="E99" t="str" cm="1">
         <f t="array" ref="E99">_xlfn.CONCAT(IF(A99="completion", "Completion", IF(A99="cassette", "Cassette", IF(A99="gemheart", "Crystal Heart", IF(A99="strawberry", _xlfn.CONCAT("Strawberry ", D99+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B99)*(regions!$B$2:$B$27=C99), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 1 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
@@ -2830,12 +2833,12 @@
         <v>0</v>
       </c>
       <c r="D100">
-        <f>COUNTIFS($A$2:A100, A100, $B$2:B100, B100, $C$2:C100, C100) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A100, A100, $B$3:B100, B100, $C$3:C100, C100) - 1</f>
+        <v>1</v>
       </c>
       <c r="E100" t="str" cm="1">
         <f t="array" ref="E100">_xlfn.CONCAT(IF(A100="completion", "Completion", IF(A100="cassette", "Cassette", IF(A100="gemheart", "Crystal Heart", IF(A100="strawberry", _xlfn.CONCAT("Strawberry ", D100+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B100)*(regions!$B$2:$B$27=C100), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 2 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
@@ -2853,12 +2856,12 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <f>COUNTIFS($A$2:A101, A101, $B$2:B101, B101, $C$2:C101, C101) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A101, A101, $B$3:B101, B101, $C$3:C101, C101) - 1</f>
+        <v>2</v>
       </c>
       <c r="E101" t="str" cm="1">
         <f t="array" ref="E101">_xlfn.CONCAT(IF(A101="completion", "Completion", IF(A101="cassette", "Cassette", IF(A101="gemheart", "Crystal Heart", IF(A101="strawberry", _xlfn.CONCAT("Strawberry ", D101+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B101)*(regions!$B$2:$B$27=C101), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 3 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
@@ -2876,12 +2879,12 @@
         <v>0</v>
       </c>
       <c r="D102">
-        <f>COUNTIFS($A$2:A102, A102, $B$2:B102, B102, $C$2:C102, C102) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A102, A102, $B$3:B102, B102, $C$3:C102, C102) - 1</f>
+        <v>3</v>
       </c>
       <c r="E102" t="str" cm="1">
         <f t="array" ref="E102">_xlfn.CONCAT(IF(A102="completion", "Completion", IF(A102="cassette", "Cassette", IF(A102="gemheart", "Crystal Heart", IF(A102="strawberry", _xlfn.CONCAT("Strawberry ", D102+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B102)*(regions!$B$2:$B$27=C102), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 4 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
@@ -2899,12 +2902,12 @@
         <v>0</v>
       </c>
       <c r="D103">
-        <f>COUNTIFS($A$2:A103, A103, $B$2:B103, B103, $C$2:C103, C103) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A103, A103, $B$3:B103, B103, $C$3:C103, C103) - 1</f>
+        <v>4</v>
       </c>
       <c r="E103" t="str" cm="1">
         <f t="array" ref="E103">_xlfn.CONCAT(IF(A103="completion", "Completion", IF(A103="cassette", "Cassette", IF(A103="gemheart", "Crystal Heart", IF(A103="strawberry", _xlfn.CONCAT("Strawberry ", D103+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B103)*(regions!$B$2:$B$27=C103), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 5 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
@@ -2922,12 +2925,12 @@
         <v>0</v>
       </c>
       <c r="D104">
-        <f>COUNTIFS($A$2:A104, A104, $B$2:B104, B104, $C$2:C104, C104) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A104, A104, $B$3:B104, B104, $C$3:C104, C104) - 1</f>
+        <v>5</v>
       </c>
       <c r="E104" t="str" cm="1">
         <f t="array" ref="E104">_xlfn.CONCAT(IF(A104="completion", "Completion", IF(A104="cassette", "Cassette", IF(A104="gemheart", "Crystal Heart", IF(A104="strawberry", _xlfn.CONCAT("Strawberry ", D104+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B104)*(regions!$B$2:$B$27=C104), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 6 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
@@ -2945,12 +2948,12 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <f>COUNTIFS($A$2:A105, A105, $B$2:B105, B105, $C$2:C105, C105) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A105, A105, $B$3:B105, B105, $C$3:C105, C105) - 1</f>
+        <v>6</v>
       </c>
       <c r="E105" t="str" cm="1">
         <f t="array" ref="E105">_xlfn.CONCAT(IF(A105="completion", "Completion", IF(A105="cassette", "Cassette", IF(A105="gemheart", "Crystal Heart", IF(A105="strawberry", _xlfn.CONCAT("Strawberry ", D105+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B105)*(regions!$B$2:$B$27=C105), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 7 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
@@ -2968,12 +2971,12 @@
         <v>0</v>
       </c>
       <c r="D106">
-        <f>COUNTIFS($A$2:A106, A106, $B$2:B106, B106, $C$2:C106, C106) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A106, A106, $B$3:B106, B106, $C$3:C106, C106) - 1</f>
+        <v>7</v>
       </c>
       <c r="E106" t="str" cm="1">
         <f t="array" ref="E106">_xlfn.CONCAT(IF(A106="completion", "Completion", IF(A106="cassette", "Cassette", IF(A106="gemheart", "Crystal Heart", IF(A106="strawberry", _xlfn.CONCAT("Strawberry ", D106+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B106)*(regions!$B$2:$B$27=C106), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 8 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
@@ -2991,12 +2994,12 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <f>COUNTIFS($A$2:A107, A107, $B$2:B107, B107, $C$2:C107, C107) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A107, A107, $B$3:B107, B107, $C$3:C107, C107) - 1</f>
+        <v>8</v>
       </c>
       <c r="E107" t="str" cm="1">
         <f t="array" ref="E107">_xlfn.CONCAT(IF(A107="completion", "Completion", IF(A107="cassette", "Cassette", IF(A107="gemheart", "Crystal Heart", IF(A107="strawberry", _xlfn.CONCAT("Strawberry ", D107+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B107)*(regions!$B$2:$B$27=C107), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 9 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
@@ -3014,12 +3017,12 @@
         <v>0</v>
       </c>
       <c r="D108">
-        <f>COUNTIFS($A$2:A108, A108, $B$2:B108, B108, $C$2:C108, C108) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A108, A108, $B$3:B108, B108, $C$3:C108, C108) - 1</f>
+        <v>9</v>
       </c>
       <c r="E108" t="str" cm="1">
         <f t="array" ref="E108">_xlfn.CONCAT(IF(A108="completion", "Completion", IF(A108="cassette", "Cassette", IF(A108="gemheart", "Crystal Heart", IF(A108="strawberry", _xlfn.CONCAT("Strawberry ", D108+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B108)*(regions!$B$2:$B$27=C108), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 10 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
@@ -3037,12 +3040,12 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <f>COUNTIFS($A$2:A109, A109, $B$2:B109, B109, $C$2:C109, C109) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A109, A109, $B$3:B109, B109, $C$3:C109, C109) - 1</f>
+        <v>10</v>
       </c>
       <c r="E109" t="str" cm="1">
         <f t="array" ref="E109">_xlfn.CONCAT(IF(A109="completion", "Completion", IF(A109="cassette", "Cassette", IF(A109="gemheart", "Crystal Heart", IF(A109="strawberry", _xlfn.CONCAT("Strawberry ", D109+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B109)*(regions!$B$2:$B$27=C109), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 11 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
@@ -3060,12 +3063,12 @@
         <v>0</v>
       </c>
       <c r="D110">
-        <f>COUNTIFS($A$2:A110, A110, $B$2:B110, B110, $C$2:C110, C110) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A110, A110, $B$3:B110, B110, $C$3:C110, C110) - 1</f>
+        <v>11</v>
       </c>
       <c r="E110" t="str" cm="1">
         <f t="array" ref="E110">_xlfn.CONCAT(IF(A110="completion", "Completion", IF(A110="cassette", "Cassette", IF(A110="gemheart", "Crystal Heart", IF(A110="strawberry", _xlfn.CONCAT("Strawberry ", D110+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B110)*(regions!$B$2:$B$27=C110), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 12 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
@@ -3083,12 +3086,12 @@
         <v>0</v>
       </c>
       <c r="D111">
-        <f>COUNTIFS($A$2:A111, A111, $B$2:B111, B111, $C$2:C111, C111) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A111, A111, $B$3:B111, B111, $C$3:C111, C111) - 1</f>
+        <v>12</v>
       </c>
       <c r="E111" t="str" cm="1">
         <f t="array" ref="E111">_xlfn.CONCAT(IF(A111="completion", "Completion", IF(A111="cassette", "Cassette", IF(A111="gemheart", "Crystal Heart", IF(A111="strawberry", _xlfn.CONCAT("Strawberry ", D111+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B111)*(regions!$B$2:$B$27=C111), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 13 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
@@ -3106,12 +3109,12 @@
         <v>0</v>
       </c>
       <c r="D112">
-        <f>COUNTIFS($A$2:A112, A112, $B$2:B112, B112, $C$2:C112, C112) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A112, A112, $B$3:B112, B112, $C$3:C112, C112) - 1</f>
+        <v>13</v>
       </c>
       <c r="E112" t="str" cm="1">
         <f t="array" ref="E112">_xlfn.CONCAT(IF(A112="completion", "Completion", IF(A112="cassette", "Cassette", IF(A112="gemheart", "Crystal Heart", IF(A112="strawberry", _xlfn.CONCAT("Strawberry ", D112+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B112)*(regions!$B$2:$B$27=C112), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 14 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
@@ -3129,12 +3132,12 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <f>COUNTIFS($A$2:A113, A113, $B$2:B113, B113, $C$2:C113, C113) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A113, A113, $B$3:B113, B113, $C$3:C113, C113) - 1</f>
+        <v>14</v>
       </c>
       <c r="E113" t="str" cm="1">
         <f t="array" ref="E113">_xlfn.CONCAT(IF(A113="completion", "Completion", IF(A113="cassette", "Cassette", IF(A113="gemheart", "Crystal Heart", IF(A113="strawberry", _xlfn.CONCAT("Strawberry ", D113+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B113)*(regions!$B$2:$B$27=C113), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 15 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
@@ -3152,12 +3155,12 @@
         <v>0</v>
       </c>
       <c r="D114">
-        <f>COUNTIFS($A$2:A114, A114, $B$2:B114, B114, $C$2:C114, C114) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A114, A114, $B$3:B114, B114, $C$3:C114, C114) - 1</f>
+        <v>15</v>
       </c>
       <c r="E114" t="str" cm="1">
         <f t="array" ref="E114">_xlfn.CONCAT(IF(A114="completion", "Completion", IF(A114="cassette", "Cassette", IF(A114="gemheart", "Crystal Heart", IF(A114="strawberry", _xlfn.CONCAT("Strawberry ", D114+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B114)*(regions!$B$2:$B$27=C114), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 16 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
@@ -3175,12 +3178,12 @@
         <v>0</v>
       </c>
       <c r="D115">
-        <f>COUNTIFS($A$2:A115, A115, $B$2:B115, B115, $C$2:C115, C115) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A115, A115, $B$3:B115, B115, $C$3:C115, C115) - 1</f>
+        <v>16</v>
       </c>
       <c r="E115" t="str" cm="1">
         <f t="array" ref="E115">_xlfn.CONCAT(IF(A115="completion", "Completion", IF(A115="cassette", "Cassette", IF(A115="gemheart", "Crystal Heart", IF(A115="strawberry", _xlfn.CONCAT("Strawberry ", D115+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B115)*(regions!$B$2:$B$27=C115), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 17 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
@@ -3198,12 +3201,12 @@
         <v>0</v>
       </c>
       <c r="D116">
-        <f>COUNTIFS($A$2:A116, A116, $B$2:B116, B116, $C$2:C116, C116) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A116, A116, $B$3:B116, B116, $C$3:C116, C116) - 1</f>
+        <v>17</v>
       </c>
       <c r="E116" t="str" cm="1">
         <f t="array" ref="E116">_xlfn.CONCAT(IF(A116="completion", "Completion", IF(A116="cassette", "Cassette", IF(A116="gemheart", "Crystal Heart", IF(A116="strawberry", _xlfn.CONCAT("Strawberry ", D116+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B116)*(regions!$B$2:$B$27=C116), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 18 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
@@ -3221,12 +3224,12 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <f>COUNTIFS($A$2:A117, A117, $B$2:B117, B117, $C$2:C117, C117) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A117, A117, $B$3:B117, B117, $C$3:C117, C117) - 1</f>
+        <v>18</v>
       </c>
       <c r="E117" t="str" cm="1">
         <f t="array" ref="E117">_xlfn.CONCAT(IF(A117="completion", "Completion", IF(A117="cassette", "Cassette", IF(A117="gemheart", "Crystal Heart", IF(A117="strawberry", _xlfn.CONCAT("Strawberry ", D117+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B117)*(regions!$B$2:$B$27=C117), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 19 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
@@ -3244,12 +3247,12 @@
         <v>0</v>
       </c>
       <c r="D118">
-        <f>COUNTIFS($A$2:A118, A118, $B$2:B118, B118, $C$2:C118, C118) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A118, A118, $B$3:B118, B118, $C$3:C118, C118) - 1</f>
+        <v>19</v>
       </c>
       <c r="E118" t="str" cm="1">
         <f t="array" ref="E118">_xlfn.CONCAT(IF(A118="completion", "Completion", IF(A118="cassette", "Cassette", IF(A118="gemheart", "Crystal Heart", IF(A118="strawberry", _xlfn.CONCAT("Strawberry ", D118+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B118)*(regions!$B$2:$B$27=C118), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 20 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="1"/>
@@ -3267,12 +3270,12 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <f>COUNTIFS($A$2:A119, A119, $B$2:B119, B119, $C$2:C119, C119) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A119, A119, $B$3:B119, B119, $C$3:C119, C119) - 1</f>
+        <v>20</v>
       </c>
       <c r="E119" t="str" cm="1">
         <f t="array" ref="E119">_xlfn.CONCAT(IF(A119="completion", "Completion", IF(A119="cassette", "Cassette", IF(A119="gemheart", "Crystal Heart", IF(A119="strawberry", _xlfn.CONCAT("Strawberry ", D119+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B119)*(regions!$B$2:$B$27=C119), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 21 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="1"/>
@@ -3290,12 +3293,12 @@
         <v>0</v>
       </c>
       <c r="D120">
-        <f>COUNTIFS($A$2:A120, A120, $B$2:B120, B120, $C$2:C120, C120) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A120, A120, $B$3:B120, B120, $C$3:C120, C120) - 1</f>
+        <v>21</v>
       </c>
       <c r="E120" t="str" cm="1">
         <f t="array" ref="E120">_xlfn.CONCAT(IF(A120="completion", "Completion", IF(A120="cassette", "Cassette", IF(A120="gemheart", "Crystal Heart", IF(A120="strawberry", _xlfn.CONCAT("Strawberry ", D120+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B120)*(regions!$B$2:$B$27=C120), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 22 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="1"/>
@@ -3313,12 +3316,12 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <f>COUNTIFS($A$2:A121, A121, $B$2:B121, B121, $C$2:C121, C121) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A121, A121, $B$3:B121, B121, $C$3:C121, C121) - 1</f>
+        <v>22</v>
       </c>
       <c r="E121" t="str" cm="1">
         <f t="array" ref="E121">_xlfn.CONCAT(IF(A121="completion", "Completion", IF(A121="cassette", "Cassette", IF(A121="gemheart", "Crystal Heart", IF(A121="strawberry", _xlfn.CONCAT("Strawberry ", D121+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B121)*(regions!$B$2:$B$27=C121), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 23 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="1"/>
@@ -3336,12 +3339,12 @@
         <v>0</v>
       </c>
       <c r="D122">
-        <f>COUNTIFS($A$2:A122, A122, $B$2:B122, B122, $C$2:C122, C122) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A122, A122, $B$3:B122, B122, $C$3:C122, C122) - 1</f>
+        <v>23</v>
       </c>
       <c r="E122" t="str" cm="1">
         <f t="array" ref="E122">_xlfn.CONCAT(IF(A122="completion", "Completion", IF(A122="cassette", "Cassette", IF(A122="gemheart", "Crystal Heart", IF(A122="strawberry", _xlfn.CONCAT("Strawberry ", D122+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B122)*(regions!$B$2:$B$27=C122), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 24 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
@@ -3353,18 +3356,18 @@
         <v>6</v>
       </c>
       <c r="B123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C123">
         <v>0</v>
       </c>
       <c r="D123">
-        <f>COUNTIFS($A$2:A123, A123, $B$2:B123, B123, $C$2:C123, C123) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A123, A123, $B$3:B123, B123, $C$3:C123, C123) - 1</f>
+        <v>24</v>
       </c>
       <c r="E123" t="str" cm="1">
         <f t="array" ref="E123">_xlfn.CONCAT(IF(A123="completion", "Completion", IF(A123="cassette", "Cassette", IF(A123="gemheart", "Crystal Heart", IF(A123="strawberry", _xlfn.CONCAT("Strawberry ", D123+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B123)*(regions!$B$2:$B$27=C123), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 25 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
@@ -3382,12 +3385,12 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <f>COUNTIFS($A$2:A124, A124, $B$2:B124, B124, $C$2:C124, C124) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A124, A124, $B$3:B124, B124, $C$3:C124, C124) - 1</f>
+        <v>0</v>
       </c>
       <c r="E124" t="str" cm="1">
         <f t="array" ref="E124">_xlfn.CONCAT(IF(A124="completion", "Completion", IF(A124="cassette", "Cassette", IF(A124="gemheart", "Crystal Heart", IF(A124="strawberry", _xlfn.CONCAT("Strawberry ", D124+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B124)*(regions!$B$2:$B$27=C124), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 1 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
@@ -3405,12 +3408,12 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <f>COUNTIFS($A$2:A125, A125, $B$2:B125, B125, $C$2:C125, C125) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A125, A125, $B$3:B125, B125, $C$3:C125, C125) - 1</f>
+        <v>1</v>
       </c>
       <c r="E125" t="str" cm="1">
         <f t="array" ref="E125">_xlfn.CONCAT(IF(A125="completion", "Completion", IF(A125="cassette", "Cassette", IF(A125="gemheart", "Crystal Heart", IF(A125="strawberry", _xlfn.CONCAT("Strawberry ", D125+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B125)*(regions!$B$2:$B$27=C125), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 2 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="1"/>
@@ -3428,12 +3431,12 @@
         <v>0</v>
       </c>
       <c r="D126">
-        <f>COUNTIFS($A$2:A126, A126, $B$2:B126, B126, $C$2:C126, C126) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A126, A126, $B$3:B126, B126, $C$3:C126, C126) - 1</f>
+        <v>2</v>
       </c>
       <c r="E126" t="str" cm="1">
         <f t="array" ref="E126">_xlfn.CONCAT(IF(A126="completion", "Completion", IF(A126="cassette", "Cassette", IF(A126="gemheart", "Crystal Heart", IF(A126="strawberry", _xlfn.CONCAT("Strawberry ", D126+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B126)*(regions!$B$2:$B$27=C126), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 3 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="1"/>
@@ -3451,12 +3454,12 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <f>COUNTIFS($A$2:A127, A127, $B$2:B127, B127, $C$2:C127, C127) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A127, A127, $B$3:B127, B127, $C$3:C127, C127) - 1</f>
+        <v>3</v>
       </c>
       <c r="E127" t="str" cm="1">
         <f t="array" ref="E127">_xlfn.CONCAT(IF(A127="completion", "Completion", IF(A127="cassette", "Cassette", IF(A127="gemheart", "Crystal Heart", IF(A127="strawberry", _xlfn.CONCAT("Strawberry ", D127+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B127)*(regions!$B$2:$B$27=C127), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 4 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="1"/>
@@ -3474,12 +3477,12 @@
         <v>0</v>
       </c>
       <c r="D128">
-        <f>COUNTIFS($A$2:A128, A128, $B$2:B128, B128, $C$2:C128, C128) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A128, A128, $B$3:B128, B128, $C$3:C128, C128) - 1</f>
+        <v>4</v>
       </c>
       <c r="E128" t="str" cm="1">
         <f t="array" ref="E128">_xlfn.CONCAT(IF(A128="completion", "Completion", IF(A128="cassette", "Cassette", IF(A128="gemheart", "Crystal Heart", IF(A128="strawberry", _xlfn.CONCAT("Strawberry ", D128+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B128)*(regions!$B$2:$B$27=C128), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 5 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
@@ -3497,12 +3500,12 @@
         <v>0</v>
       </c>
       <c r="D129">
-        <f>COUNTIFS($A$2:A129, A129, $B$2:B129, B129, $C$2:C129, C129) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A129, A129, $B$3:B129, B129, $C$3:C129, C129) - 1</f>
+        <v>5</v>
       </c>
       <c r="E129" t="str" cm="1">
         <f t="array" ref="E129">_xlfn.CONCAT(IF(A129="completion", "Completion", IF(A129="cassette", "Cassette", IF(A129="gemheart", "Crystal Heart", IF(A129="strawberry", _xlfn.CONCAT("Strawberry ", D129+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B129)*(regions!$B$2:$B$27=C129), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 6 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="1"/>
@@ -3520,15 +3523,15 @@
         <v>0</v>
       </c>
       <c r="D130">
-        <f>COUNTIFS($A$2:A130, A130, $B$2:B130, B130, $C$2:C130, C130) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A130, A130, $B$3:B130, B130, $C$3:C130, C130) - 1</f>
+        <v>6</v>
       </c>
       <c r="E130" t="str" cm="1">
         <f t="array" ref="E130">_xlfn.CONCAT(IF(A130="completion", "Completion", IF(A130="cassette", "Cassette", IF(A130="gemheart", "Crystal Heart", IF(A130="strawberry", _xlfn.CONCAT("Strawberry ", D130+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B130)*(regions!$B$2:$B$27=C130), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 7 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" ref="F130:F193" si="2">IF(A130="strawberry", "Strawberry", E130)</f>
+        <f t="shared" si="1"/>
         <v>Strawberry</v>
       </c>
     </row>
@@ -3543,15 +3546,15 @@
         <v>0</v>
       </c>
       <c r="D131">
-        <f>COUNTIFS($A$2:A131, A131, $B$2:B131, B131, $C$2:C131, C131) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A131, A131, $B$3:B131, B131, $C$3:C131, C131) - 1</f>
+        <v>7</v>
       </c>
       <c r="E131" t="str" cm="1">
         <f t="array" ref="E131">_xlfn.CONCAT(IF(A131="completion", "Completion", IF(A131="cassette", "Cassette", IF(A131="gemheart", "Crystal Heart", IF(A131="strawberry", _xlfn.CONCAT("Strawberry ", D131+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B131)*(regions!$B$2:$B$27=C131), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 8 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F131:F194" si="2">IF(A131="strawberry", "Strawberry", E131)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -3566,12 +3569,12 @@
         <v>0</v>
       </c>
       <c r="D132">
-        <f>COUNTIFS($A$2:A132, A132, $B$2:B132, B132, $C$2:C132, C132) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A132, A132, $B$3:B132, B132, $C$3:C132, C132) - 1</f>
+        <v>8</v>
       </c>
       <c r="E132" t="str" cm="1">
         <f t="array" ref="E132">_xlfn.CONCAT(IF(A132="completion", "Completion", IF(A132="cassette", "Cassette", IF(A132="gemheart", "Crystal Heart", IF(A132="strawberry", _xlfn.CONCAT("Strawberry ", D132+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B132)*(regions!$B$2:$B$27=C132), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 9 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F132" t="str">
         <f t="shared" si="2"/>
@@ -3589,12 +3592,12 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <f>COUNTIFS($A$2:A133, A133, $B$2:B133, B133, $C$2:C133, C133) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A133, A133, $B$3:B133, B133, $C$3:C133, C133) - 1</f>
+        <v>9</v>
       </c>
       <c r="E133" t="str" cm="1">
         <f t="array" ref="E133">_xlfn.CONCAT(IF(A133="completion", "Completion", IF(A133="cassette", "Cassette", IF(A133="gemheart", "Crystal Heart", IF(A133="strawberry", _xlfn.CONCAT("Strawberry ", D133+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B133)*(regions!$B$2:$B$27=C133), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 10 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="2"/>
@@ -3612,12 +3615,12 @@
         <v>0</v>
       </c>
       <c r="D134">
-        <f>COUNTIFS($A$2:A134, A134, $B$2:B134, B134, $C$2:C134, C134) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A134, A134, $B$3:B134, B134, $C$3:C134, C134) - 1</f>
+        <v>10</v>
       </c>
       <c r="E134" t="str" cm="1">
         <f t="array" ref="E134">_xlfn.CONCAT(IF(A134="completion", "Completion", IF(A134="cassette", "Cassette", IF(A134="gemheart", "Crystal Heart", IF(A134="strawberry", _xlfn.CONCAT("Strawberry ", D134+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B134)*(regions!$B$2:$B$27=C134), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 11 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F134" t="str">
         <f t="shared" si="2"/>
@@ -3635,12 +3638,12 @@
         <v>0</v>
       </c>
       <c r="D135">
-        <f>COUNTIFS($A$2:A135, A135, $B$2:B135, B135, $C$2:C135, C135) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A135, A135, $B$3:B135, B135, $C$3:C135, C135) - 1</f>
+        <v>11</v>
       </c>
       <c r="E135" t="str" cm="1">
         <f t="array" ref="E135">_xlfn.CONCAT(IF(A135="completion", "Completion", IF(A135="cassette", "Cassette", IF(A135="gemheart", "Crystal Heart", IF(A135="strawberry", _xlfn.CONCAT("Strawberry ", D135+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B135)*(regions!$B$2:$B$27=C135), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 12 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="2"/>
@@ -3658,12 +3661,12 @@
         <v>0</v>
       </c>
       <c r="D136">
-        <f>COUNTIFS($A$2:A136, A136, $B$2:B136, B136, $C$2:C136, C136) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A136, A136, $B$3:B136, B136, $C$3:C136, C136) - 1</f>
+        <v>12</v>
       </c>
       <c r="E136" t="str" cm="1">
         <f t="array" ref="E136">_xlfn.CONCAT(IF(A136="completion", "Completion", IF(A136="cassette", "Cassette", IF(A136="gemheart", "Crystal Heart", IF(A136="strawberry", _xlfn.CONCAT("Strawberry ", D136+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B136)*(regions!$B$2:$B$27=C136), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 13 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="2"/>
@@ -3681,12 +3684,12 @@
         <v>0</v>
       </c>
       <c r="D137">
-        <f>COUNTIFS($A$2:A137, A137, $B$2:B137, B137, $C$2:C137, C137) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A137, A137, $B$3:B137, B137, $C$3:C137, C137) - 1</f>
+        <v>13</v>
       </c>
       <c r="E137" t="str" cm="1">
         <f t="array" ref="E137">_xlfn.CONCAT(IF(A137="completion", "Completion", IF(A137="cassette", "Cassette", IF(A137="gemheart", "Crystal Heart", IF(A137="strawberry", _xlfn.CONCAT("Strawberry ", D137+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B137)*(regions!$B$2:$B$27=C137), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 14 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="2"/>
@@ -3704,12 +3707,12 @@
         <v>0</v>
       </c>
       <c r="D138">
-        <f>COUNTIFS($A$2:A138, A138, $B$2:B138, B138, $C$2:C138, C138) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A138, A138, $B$3:B138, B138, $C$3:C138, C138) - 1</f>
+        <v>14</v>
       </c>
       <c r="E138" t="str" cm="1">
         <f t="array" ref="E138">_xlfn.CONCAT(IF(A138="completion", "Completion", IF(A138="cassette", "Cassette", IF(A138="gemheart", "Crystal Heart", IF(A138="strawberry", _xlfn.CONCAT("Strawberry ", D138+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B138)*(regions!$B$2:$B$27=C138), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 15 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="2"/>
@@ -3727,12 +3730,12 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <f>COUNTIFS($A$2:A139, A139, $B$2:B139, B139, $C$2:C139, C139) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A139, A139, $B$3:B139, B139, $C$3:C139, C139) - 1</f>
+        <v>15</v>
       </c>
       <c r="E139" t="str" cm="1">
         <f t="array" ref="E139">_xlfn.CONCAT(IF(A139="completion", "Completion", IF(A139="cassette", "Cassette", IF(A139="gemheart", "Crystal Heart", IF(A139="strawberry", _xlfn.CONCAT("Strawberry ", D139+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B139)*(regions!$B$2:$B$27=C139), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 16 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F139" t="str">
         <f t="shared" si="2"/>
@@ -3750,12 +3753,12 @@
         <v>0</v>
       </c>
       <c r="D140">
-        <f>COUNTIFS($A$2:A140, A140, $B$2:B140, B140, $C$2:C140, C140) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A140, A140, $B$3:B140, B140, $C$3:C140, C140) - 1</f>
+        <v>16</v>
       </c>
       <c r="E140" t="str" cm="1">
         <f t="array" ref="E140">_xlfn.CONCAT(IF(A140="completion", "Completion", IF(A140="cassette", "Cassette", IF(A140="gemheart", "Crystal Heart", IF(A140="strawberry", _xlfn.CONCAT("Strawberry ", D140+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B140)*(regions!$B$2:$B$27=C140), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 17 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F140" t="str">
         <f t="shared" si="2"/>
@@ -3773,12 +3776,12 @@
         <v>0</v>
       </c>
       <c r="D141">
-        <f>COUNTIFS($A$2:A141, A141, $B$2:B141, B141, $C$2:C141, C141) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A141, A141, $B$3:B141, B141, $C$3:C141, C141) - 1</f>
+        <v>17</v>
       </c>
       <c r="E141" t="str" cm="1">
         <f t="array" ref="E141">_xlfn.CONCAT(IF(A141="completion", "Completion", IF(A141="cassette", "Cassette", IF(A141="gemheart", "Crystal Heart", IF(A141="strawberry", _xlfn.CONCAT("Strawberry ", D141+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B141)*(regions!$B$2:$B$27=C141), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 18 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="2"/>
@@ -3796,12 +3799,12 @@
         <v>0</v>
       </c>
       <c r="D142">
-        <f>COUNTIFS($A$2:A142, A142, $B$2:B142, B142, $C$2:C142, C142) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A142, A142, $B$3:B142, B142, $C$3:C142, C142) - 1</f>
+        <v>18</v>
       </c>
       <c r="E142" t="str" cm="1">
         <f t="array" ref="E142">_xlfn.CONCAT(IF(A142="completion", "Completion", IF(A142="cassette", "Cassette", IF(A142="gemheart", "Crystal Heart", IF(A142="strawberry", _xlfn.CONCAT("Strawberry ", D142+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B142)*(regions!$B$2:$B$27=C142), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 19 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="2"/>
@@ -3819,12 +3822,12 @@
         <v>0</v>
       </c>
       <c r="D143">
-        <f>COUNTIFS($A$2:A143, A143, $B$2:B143, B143, $C$2:C143, C143) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A143, A143, $B$3:B143, B143, $C$3:C143, C143) - 1</f>
+        <v>19</v>
       </c>
       <c r="E143" t="str" cm="1">
         <f t="array" ref="E143">_xlfn.CONCAT(IF(A143="completion", "Completion", IF(A143="cassette", "Cassette", IF(A143="gemheart", "Crystal Heart", IF(A143="strawberry", _xlfn.CONCAT("Strawberry ", D143+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B143)*(regions!$B$2:$B$27=C143), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 20 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="2"/>
@@ -3842,12 +3845,12 @@
         <v>0</v>
       </c>
       <c r="D144">
-        <f>COUNTIFS($A$2:A144, A144, $B$2:B144, B144, $C$2:C144, C144) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A144, A144, $B$3:B144, B144, $C$3:C144, C144) - 1</f>
+        <v>20</v>
       </c>
       <c r="E144" t="str" cm="1">
         <f t="array" ref="E144">_xlfn.CONCAT(IF(A144="completion", "Completion", IF(A144="cassette", "Cassette", IF(A144="gemheart", "Crystal Heart", IF(A144="strawberry", _xlfn.CONCAT("Strawberry ", D144+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B144)*(regions!$B$2:$B$27=C144), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 21 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="2"/>
@@ -3865,12 +3868,12 @@
         <v>0</v>
       </c>
       <c r="D145">
-        <f>COUNTIFS($A$2:A145, A145, $B$2:B145, B145, $C$2:C145, C145) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A145, A145, $B$3:B145, B145, $C$3:C145, C145) - 1</f>
+        <v>21</v>
       </c>
       <c r="E145" t="str" cm="1">
         <f t="array" ref="E145">_xlfn.CONCAT(IF(A145="completion", "Completion", IF(A145="cassette", "Cassette", IF(A145="gemheart", "Crystal Heart", IF(A145="strawberry", _xlfn.CONCAT("Strawberry ", D145+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B145)*(regions!$B$2:$B$27=C145), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 22 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="2"/>
@@ -3888,12 +3891,12 @@
         <v>0</v>
       </c>
       <c r="D146">
-        <f>COUNTIFS($A$2:A146, A146, $B$2:B146, B146, $C$2:C146, C146) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A146, A146, $B$3:B146, B146, $C$3:C146, C146) - 1</f>
+        <v>22</v>
       </c>
       <c r="E146" t="str" cm="1">
         <f t="array" ref="E146">_xlfn.CONCAT(IF(A146="completion", "Completion", IF(A146="cassette", "Cassette", IF(A146="gemheart", "Crystal Heart", IF(A146="strawberry", _xlfn.CONCAT("Strawberry ", D146+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B146)*(regions!$B$2:$B$27=C146), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 23 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="2"/>
@@ -3911,12 +3914,12 @@
         <v>0</v>
       </c>
       <c r="D147">
-        <f>COUNTIFS($A$2:A147, A147, $B$2:B147, B147, $C$2:C147, C147) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A147, A147, $B$3:B147, B147, $C$3:C147, C147) - 1</f>
+        <v>23</v>
       </c>
       <c r="E147" t="str" cm="1">
         <f t="array" ref="E147">_xlfn.CONCAT(IF(A147="completion", "Completion", IF(A147="cassette", "Cassette", IF(A147="gemheart", "Crystal Heart", IF(A147="strawberry", _xlfn.CONCAT("Strawberry ", D147+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B147)*(regions!$B$2:$B$27=C147), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 24 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F147" t="str">
         <f t="shared" si="2"/>
@@ -3934,12 +3937,12 @@
         <v>0</v>
       </c>
       <c r="D148">
-        <f>COUNTIFS($A$2:A148, A148, $B$2:B148, B148, $C$2:C148, C148) - 1</f>
-        <v>25</v>
+        <f>COUNTIFS($A$3:A148, A148, $B$3:B148, B148, $C$3:C148, C148) - 1</f>
+        <v>24</v>
       </c>
       <c r="E148" t="str" cm="1">
         <f t="array" ref="E148">_xlfn.CONCAT(IF(A148="completion", "Completion", IF(A148="cassette", "Cassette", IF(A148="gemheart", "Crystal Heart", IF(A148="strawberry", _xlfn.CONCAT("Strawberry ", D148+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B148)*(regions!$B$2:$B$27=C148), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 26 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 25 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F148" t="str">
         <f t="shared" si="2"/>
@@ -3957,12 +3960,12 @@
         <v>0</v>
       </c>
       <c r="D149">
-        <f>COUNTIFS($A$2:A149, A149, $B$2:B149, B149, $C$2:C149, C149) - 1</f>
-        <v>26</v>
+        <f>COUNTIFS($A$3:A149, A149, $B$3:B149, B149, $C$3:C149, C149) - 1</f>
+        <v>25</v>
       </c>
       <c r="E149" t="str" cm="1">
         <f t="array" ref="E149">_xlfn.CONCAT(IF(A149="completion", "Completion", IF(A149="cassette", "Cassette", IF(A149="gemheart", "Crystal Heart", IF(A149="strawberry", _xlfn.CONCAT("Strawberry ", D149+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B149)*(regions!$B$2:$B$27=C149), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 27 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 26 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F149" t="str">
         <f t="shared" si="2"/>
@@ -3980,12 +3983,12 @@
         <v>0</v>
       </c>
       <c r="D150">
-        <f>COUNTIFS($A$2:A150, A150, $B$2:B150, B150, $C$2:C150, C150) - 1</f>
-        <v>27</v>
+        <f>COUNTIFS($A$3:A150, A150, $B$3:B150, B150, $C$3:C150, C150) - 1</f>
+        <v>26</v>
       </c>
       <c r="E150" t="str" cm="1">
         <f t="array" ref="E150">_xlfn.CONCAT(IF(A150="completion", "Completion", IF(A150="cassette", "Cassette", IF(A150="gemheart", "Crystal Heart", IF(A150="strawberry", _xlfn.CONCAT("Strawberry ", D150+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B150)*(regions!$B$2:$B$27=C150), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 28 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 27 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F150" t="str">
         <f t="shared" si="2"/>
@@ -4003,12 +4006,12 @@
         <v>0</v>
       </c>
       <c r="D151">
-        <f>COUNTIFS($A$2:A151, A151, $B$2:B151, B151, $C$2:C151, C151) - 1</f>
-        <v>28</v>
+        <f>COUNTIFS($A$3:A151, A151, $B$3:B151, B151, $C$3:C151, C151) - 1</f>
+        <v>27</v>
       </c>
       <c r="E151" t="str" cm="1">
         <f t="array" ref="E151">_xlfn.CONCAT(IF(A151="completion", "Completion", IF(A151="cassette", "Cassette", IF(A151="gemheart", "Crystal Heart", IF(A151="strawberry", _xlfn.CONCAT("Strawberry ", D151+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B151)*(regions!$B$2:$B$27=C151), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 29 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 28 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F151" t="str">
         <f t="shared" si="2"/>
@@ -4020,18 +4023,18 @@
         <v>6</v>
       </c>
       <c r="B152">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152">
         <v>0</v>
       </c>
       <c r="D152">
-        <f>COUNTIFS($A$2:A152, A152, $B$2:B152, B152, $C$2:C152, C152) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A152, A152, $B$3:B152, B152, $C$3:C152, C152) - 1</f>
+        <v>28</v>
       </c>
       <c r="E152" t="str" cm="1">
         <f t="array" ref="E152">_xlfn.CONCAT(IF(A152="completion", "Completion", IF(A152="cassette", "Cassette", IF(A152="gemheart", "Crystal Heart", IF(A152="strawberry", _xlfn.CONCAT("Strawberry ", D152+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B152)*(regions!$B$2:$B$27=C152), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 29 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F152" t="str">
         <f t="shared" si="2"/>
@@ -4049,12 +4052,12 @@
         <v>0</v>
       </c>
       <c r="D153">
-        <f>COUNTIFS($A$2:A153, A153, $B$2:B153, B153, $C$2:C153, C153) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A153, A153, $B$3:B153, B153, $C$3:C153, C153) - 1</f>
+        <v>0</v>
       </c>
       <c r="E153" t="str" cm="1">
         <f t="array" ref="E153">_xlfn.CONCAT(IF(A153="completion", "Completion", IF(A153="cassette", "Cassette", IF(A153="gemheart", "Crystal Heart", IF(A153="strawberry", _xlfn.CONCAT("Strawberry ", D153+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B153)*(regions!$B$2:$B$27=C153), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 1 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F153" t="str">
         <f t="shared" si="2"/>
@@ -4072,12 +4075,12 @@
         <v>0</v>
       </c>
       <c r="D154">
-        <f>COUNTIFS($A$2:A154, A154, $B$2:B154, B154, $C$2:C154, C154) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A154, A154, $B$3:B154, B154, $C$3:C154, C154) - 1</f>
+        <v>1</v>
       </c>
       <c r="E154" t="str" cm="1">
         <f t="array" ref="E154">_xlfn.CONCAT(IF(A154="completion", "Completion", IF(A154="cassette", "Cassette", IF(A154="gemheart", "Crystal Heart", IF(A154="strawberry", _xlfn.CONCAT("Strawberry ", D154+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B154)*(regions!$B$2:$B$27=C154), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 2 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F154" t="str">
         <f t="shared" si="2"/>
@@ -4095,12 +4098,12 @@
         <v>0</v>
       </c>
       <c r="D155">
-        <f>COUNTIFS($A$2:A155, A155, $B$2:B155, B155, $C$2:C155, C155) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A155, A155, $B$3:B155, B155, $C$3:C155, C155) - 1</f>
+        <v>2</v>
       </c>
       <c r="E155" t="str" cm="1">
         <f t="array" ref="E155">_xlfn.CONCAT(IF(A155="completion", "Completion", IF(A155="cassette", "Cassette", IF(A155="gemheart", "Crystal Heart", IF(A155="strawberry", _xlfn.CONCAT("Strawberry ", D155+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B155)*(regions!$B$2:$B$27=C155), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 3 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F155" t="str">
         <f t="shared" si="2"/>
@@ -4118,12 +4121,12 @@
         <v>0</v>
       </c>
       <c r="D156">
-        <f>COUNTIFS($A$2:A156, A156, $B$2:B156, B156, $C$2:C156, C156) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A156, A156, $B$3:B156, B156, $C$3:C156, C156) - 1</f>
+        <v>3</v>
       </c>
       <c r="E156" t="str" cm="1">
         <f t="array" ref="E156">_xlfn.CONCAT(IF(A156="completion", "Completion", IF(A156="cassette", "Cassette", IF(A156="gemheart", "Crystal Heart", IF(A156="strawberry", _xlfn.CONCAT("Strawberry ", D156+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B156)*(regions!$B$2:$B$27=C156), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 4 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F156" t="str">
         <f t="shared" si="2"/>
@@ -4141,12 +4144,12 @@
         <v>0</v>
       </c>
       <c r="D157">
-        <f>COUNTIFS($A$2:A157, A157, $B$2:B157, B157, $C$2:C157, C157) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A157, A157, $B$3:B157, B157, $C$3:C157, C157) - 1</f>
+        <v>4</v>
       </c>
       <c r="E157" t="str" cm="1">
         <f t="array" ref="E157">_xlfn.CONCAT(IF(A157="completion", "Completion", IF(A157="cassette", "Cassette", IF(A157="gemheart", "Crystal Heart", IF(A157="strawberry", _xlfn.CONCAT("Strawberry ", D157+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B157)*(regions!$B$2:$B$27=C157), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 5 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="2"/>
@@ -4164,12 +4167,12 @@
         <v>0</v>
       </c>
       <c r="D158">
-        <f>COUNTIFS($A$2:A158, A158, $B$2:B158, B158, $C$2:C158, C158) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A158, A158, $B$3:B158, B158, $C$3:C158, C158) - 1</f>
+        <v>5</v>
       </c>
       <c r="E158" t="str" cm="1">
         <f t="array" ref="E158">_xlfn.CONCAT(IF(A158="completion", "Completion", IF(A158="cassette", "Cassette", IF(A158="gemheart", "Crystal Heart", IF(A158="strawberry", _xlfn.CONCAT("Strawberry ", D158+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B158)*(regions!$B$2:$B$27=C158), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 6 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="2"/>
@@ -4187,12 +4190,12 @@
         <v>0</v>
       </c>
       <c r="D159">
-        <f>COUNTIFS($A$2:A159, A159, $B$2:B159, B159, $C$2:C159, C159) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A159, A159, $B$3:B159, B159, $C$3:C159, C159) - 1</f>
+        <v>6</v>
       </c>
       <c r="E159" t="str" cm="1">
         <f t="array" ref="E159">_xlfn.CONCAT(IF(A159="completion", "Completion", IF(A159="cassette", "Cassette", IF(A159="gemheart", "Crystal Heart", IF(A159="strawberry", _xlfn.CONCAT("Strawberry ", D159+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B159)*(regions!$B$2:$B$27=C159), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 7 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="2"/>
@@ -4210,12 +4213,12 @@
         <v>0</v>
       </c>
       <c r="D160">
-        <f>COUNTIFS($A$2:A160, A160, $B$2:B160, B160, $C$2:C160, C160) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A160, A160, $B$3:B160, B160, $C$3:C160, C160) - 1</f>
+        <v>7</v>
       </c>
       <c r="E160" t="str" cm="1">
         <f t="array" ref="E160">_xlfn.CONCAT(IF(A160="completion", "Completion", IF(A160="cassette", "Cassette", IF(A160="gemheart", "Crystal Heart", IF(A160="strawberry", _xlfn.CONCAT("Strawberry ", D160+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B160)*(regions!$B$2:$B$27=C160), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 8 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F160" t="str">
         <f t="shared" si="2"/>
@@ -4233,12 +4236,12 @@
         <v>0</v>
       </c>
       <c r="D161">
-        <f>COUNTIFS($A$2:A161, A161, $B$2:B161, B161, $C$2:C161, C161) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A161, A161, $B$3:B161, B161, $C$3:C161, C161) - 1</f>
+        <v>8</v>
       </c>
       <c r="E161" t="str" cm="1">
         <f t="array" ref="E161">_xlfn.CONCAT(IF(A161="completion", "Completion", IF(A161="cassette", "Cassette", IF(A161="gemheart", "Crystal Heart", IF(A161="strawberry", _xlfn.CONCAT("Strawberry ", D161+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B161)*(regions!$B$2:$B$27=C161), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 9 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F161" t="str">
         <f t="shared" si="2"/>
@@ -4256,12 +4259,12 @@
         <v>0</v>
       </c>
       <c r="D162">
-        <f>COUNTIFS($A$2:A162, A162, $B$2:B162, B162, $C$2:C162, C162) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A162, A162, $B$3:B162, B162, $C$3:C162, C162) - 1</f>
+        <v>9</v>
       </c>
       <c r="E162" t="str" cm="1">
         <f t="array" ref="E162">_xlfn.CONCAT(IF(A162="completion", "Completion", IF(A162="cassette", "Cassette", IF(A162="gemheart", "Crystal Heart", IF(A162="strawberry", _xlfn.CONCAT("Strawberry ", D162+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B162)*(regions!$B$2:$B$27=C162), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 10 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F162" t="str">
         <f t="shared" si="2"/>
@@ -4279,12 +4282,12 @@
         <v>0</v>
       </c>
       <c r="D163">
-        <f>COUNTIFS($A$2:A163, A163, $B$2:B163, B163, $C$2:C163, C163) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A163, A163, $B$3:B163, B163, $C$3:C163, C163) - 1</f>
+        <v>10</v>
       </c>
       <c r="E163" t="str" cm="1">
         <f t="array" ref="E163">_xlfn.CONCAT(IF(A163="completion", "Completion", IF(A163="cassette", "Cassette", IF(A163="gemheart", "Crystal Heart", IF(A163="strawberry", _xlfn.CONCAT("Strawberry ", D163+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B163)*(regions!$B$2:$B$27=C163), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 11 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F163" t="str">
         <f t="shared" si="2"/>
@@ -4302,12 +4305,12 @@
         <v>0</v>
       </c>
       <c r="D164">
-        <f>COUNTIFS($A$2:A164, A164, $B$2:B164, B164, $C$2:C164, C164) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A164, A164, $B$3:B164, B164, $C$3:C164, C164) - 1</f>
+        <v>11</v>
       </c>
       <c r="E164" t="str" cm="1">
         <f t="array" ref="E164">_xlfn.CONCAT(IF(A164="completion", "Completion", IF(A164="cassette", "Cassette", IF(A164="gemheart", "Crystal Heart", IF(A164="strawberry", _xlfn.CONCAT("Strawberry ", D164+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B164)*(regions!$B$2:$B$27=C164), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 12 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="2"/>
@@ -4325,12 +4328,12 @@
         <v>0</v>
       </c>
       <c r="D165">
-        <f>COUNTIFS($A$2:A165, A165, $B$2:B165, B165, $C$2:C165, C165) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A165, A165, $B$3:B165, B165, $C$3:C165, C165) - 1</f>
+        <v>12</v>
       </c>
       <c r="E165" t="str" cm="1">
         <f t="array" ref="E165">_xlfn.CONCAT(IF(A165="completion", "Completion", IF(A165="cassette", "Cassette", IF(A165="gemheart", "Crystal Heart", IF(A165="strawberry", _xlfn.CONCAT("Strawberry ", D165+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B165)*(regions!$B$2:$B$27=C165), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 13 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F165" t="str">
         <f t="shared" si="2"/>
@@ -4348,12 +4351,12 @@
         <v>0</v>
       </c>
       <c r="D166">
-        <f>COUNTIFS($A$2:A166, A166, $B$2:B166, B166, $C$2:C166, C166) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A166, A166, $B$3:B166, B166, $C$3:C166, C166) - 1</f>
+        <v>13</v>
       </c>
       <c r="E166" t="str" cm="1">
         <f t="array" ref="E166">_xlfn.CONCAT(IF(A166="completion", "Completion", IF(A166="cassette", "Cassette", IF(A166="gemheart", "Crystal Heart", IF(A166="strawberry", _xlfn.CONCAT("Strawberry ", D166+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B166)*(regions!$B$2:$B$27=C166), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 14 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F166" t="str">
         <f t="shared" si="2"/>
@@ -4371,12 +4374,12 @@
         <v>0</v>
       </c>
       <c r="D167">
-        <f>COUNTIFS($A$2:A167, A167, $B$2:B167, B167, $C$2:C167, C167) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A167, A167, $B$3:B167, B167, $C$3:C167, C167) - 1</f>
+        <v>14</v>
       </c>
       <c r="E167" t="str" cm="1">
         <f t="array" ref="E167">_xlfn.CONCAT(IF(A167="completion", "Completion", IF(A167="cassette", "Cassette", IF(A167="gemheart", "Crystal Heart", IF(A167="strawberry", _xlfn.CONCAT("Strawberry ", D167+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B167)*(regions!$B$2:$B$27=C167), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 15 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="2"/>
@@ -4394,12 +4397,12 @@
         <v>0</v>
       </c>
       <c r="D168">
-        <f>COUNTIFS($A$2:A168, A168, $B$2:B168, B168, $C$2:C168, C168) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A168, A168, $B$3:B168, B168, $C$3:C168, C168) - 1</f>
+        <v>15</v>
       </c>
       <c r="E168" t="str" cm="1">
         <f t="array" ref="E168">_xlfn.CONCAT(IF(A168="completion", "Completion", IF(A168="cassette", "Cassette", IF(A168="gemheart", "Crystal Heart", IF(A168="strawberry", _xlfn.CONCAT("Strawberry ", D168+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B168)*(regions!$B$2:$B$27=C168), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 16 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F168" t="str">
         <f t="shared" si="2"/>
@@ -4417,12 +4420,12 @@
         <v>0</v>
       </c>
       <c r="D169">
-        <f>COUNTIFS($A$2:A169, A169, $B$2:B169, B169, $C$2:C169, C169) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A169, A169, $B$3:B169, B169, $C$3:C169, C169) - 1</f>
+        <v>16</v>
       </c>
       <c r="E169" t="str" cm="1">
         <f t="array" ref="E169">_xlfn.CONCAT(IF(A169="completion", "Completion", IF(A169="cassette", "Cassette", IF(A169="gemheart", "Crystal Heart", IF(A169="strawberry", _xlfn.CONCAT("Strawberry ", D169+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B169)*(regions!$B$2:$B$27=C169), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 17 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F169" t="str">
         <f t="shared" si="2"/>
@@ -4440,12 +4443,12 @@
         <v>0</v>
       </c>
       <c r="D170">
-        <f>COUNTIFS($A$2:A170, A170, $B$2:B170, B170, $C$2:C170, C170) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A170, A170, $B$3:B170, B170, $C$3:C170, C170) - 1</f>
+        <v>17</v>
       </c>
       <c r="E170" t="str" cm="1">
         <f t="array" ref="E170">_xlfn.CONCAT(IF(A170="completion", "Completion", IF(A170="cassette", "Cassette", IF(A170="gemheart", "Crystal Heart", IF(A170="strawberry", _xlfn.CONCAT("Strawberry ", D170+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B170)*(regions!$B$2:$B$27=C170), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 18 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F170" t="str">
         <f t="shared" si="2"/>
@@ -4463,12 +4466,12 @@
         <v>0</v>
       </c>
       <c r="D171">
-        <f>COUNTIFS($A$2:A171, A171, $B$2:B171, B171, $C$2:C171, C171) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A171, A171, $B$3:B171, B171, $C$3:C171, C171) - 1</f>
+        <v>18</v>
       </c>
       <c r="E171" t="str" cm="1">
         <f t="array" ref="E171">_xlfn.CONCAT(IF(A171="completion", "Completion", IF(A171="cassette", "Cassette", IF(A171="gemheart", "Crystal Heart", IF(A171="strawberry", _xlfn.CONCAT("Strawberry ", D171+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B171)*(regions!$B$2:$B$27=C171), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 19 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F171" t="str">
         <f t="shared" si="2"/>
@@ -4486,12 +4489,12 @@
         <v>0</v>
       </c>
       <c r="D172">
-        <f>COUNTIFS($A$2:A172, A172, $B$2:B172, B172, $C$2:C172, C172) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A172, A172, $B$3:B172, B172, $C$3:C172, C172) - 1</f>
+        <v>19</v>
       </c>
       <c r="E172" t="str" cm="1">
         <f t="array" ref="E172">_xlfn.CONCAT(IF(A172="completion", "Completion", IF(A172="cassette", "Cassette", IF(A172="gemheart", "Crystal Heart", IF(A172="strawberry", _xlfn.CONCAT("Strawberry ", D172+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B172)*(regions!$B$2:$B$27=C172), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 20 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F172" t="str">
         <f t="shared" si="2"/>
@@ -4509,12 +4512,12 @@
         <v>0</v>
       </c>
       <c r="D173">
-        <f>COUNTIFS($A$2:A173, A173, $B$2:B173, B173, $C$2:C173, C173) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A173, A173, $B$3:B173, B173, $C$3:C173, C173) - 1</f>
+        <v>20</v>
       </c>
       <c r="E173" t="str" cm="1">
         <f t="array" ref="E173">_xlfn.CONCAT(IF(A173="completion", "Completion", IF(A173="cassette", "Cassette", IF(A173="gemheart", "Crystal Heart", IF(A173="strawberry", _xlfn.CONCAT("Strawberry ", D173+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B173)*(regions!$B$2:$B$27=C173), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 21 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F173" t="str">
         <f t="shared" si="2"/>
@@ -4532,12 +4535,12 @@
         <v>0</v>
       </c>
       <c r="D174">
-        <f>COUNTIFS($A$2:A174, A174, $B$2:B174, B174, $C$2:C174, C174) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A174, A174, $B$3:B174, B174, $C$3:C174, C174) - 1</f>
+        <v>21</v>
       </c>
       <c r="E174" t="str" cm="1">
         <f t="array" ref="E174">_xlfn.CONCAT(IF(A174="completion", "Completion", IF(A174="cassette", "Cassette", IF(A174="gemheart", "Crystal Heart", IF(A174="strawberry", _xlfn.CONCAT("Strawberry ", D174+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B174)*(regions!$B$2:$B$27=C174), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 22 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F174" t="str">
         <f t="shared" si="2"/>
@@ -4555,12 +4558,12 @@
         <v>0</v>
       </c>
       <c r="D175">
-        <f>COUNTIFS($A$2:A175, A175, $B$2:B175, B175, $C$2:C175, C175) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A175, A175, $B$3:B175, B175, $C$3:C175, C175) - 1</f>
+        <v>22</v>
       </c>
       <c r="E175" t="str" cm="1">
         <f t="array" ref="E175">_xlfn.CONCAT(IF(A175="completion", "Completion", IF(A175="cassette", "Cassette", IF(A175="gemheart", "Crystal Heart", IF(A175="strawberry", _xlfn.CONCAT("Strawberry ", D175+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B175)*(regions!$B$2:$B$27=C175), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 23 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F175" t="str">
         <f t="shared" si="2"/>
@@ -4578,12 +4581,12 @@
         <v>0</v>
       </c>
       <c r="D176">
-        <f>COUNTIFS($A$2:A176, A176, $B$2:B176, B176, $C$2:C176, C176) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A176, A176, $B$3:B176, B176, $C$3:C176, C176) - 1</f>
+        <v>23</v>
       </c>
       <c r="E176" t="str" cm="1">
         <f t="array" ref="E176">_xlfn.CONCAT(IF(A176="completion", "Completion", IF(A176="cassette", "Cassette", IF(A176="gemheart", "Crystal Heart", IF(A176="strawberry", _xlfn.CONCAT("Strawberry ", D176+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B176)*(regions!$B$2:$B$27=C176), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 24 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F176" t="str">
         <f t="shared" si="2"/>
@@ -4601,12 +4604,12 @@
         <v>0</v>
       </c>
       <c r="D177">
-        <f>COUNTIFS($A$2:A177, A177, $B$2:B177, B177, $C$2:C177, C177) - 1</f>
-        <v>25</v>
+        <f>COUNTIFS($A$3:A177, A177, $B$3:B177, B177, $C$3:C177, C177) - 1</f>
+        <v>24</v>
       </c>
       <c r="E177" t="str" cm="1">
         <f t="array" ref="E177">_xlfn.CONCAT(IF(A177="completion", "Completion", IF(A177="cassette", "Cassette", IF(A177="gemheart", "Crystal Heart", IF(A177="strawberry", _xlfn.CONCAT("Strawberry ", D177+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B177)*(regions!$B$2:$B$27=C177), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 26 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 25 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="2"/>
@@ -4624,12 +4627,12 @@
         <v>0</v>
       </c>
       <c r="D178">
-        <f>COUNTIFS($A$2:A178, A178, $B$2:B178, B178, $C$2:C178, C178) - 1</f>
-        <v>26</v>
+        <f>COUNTIFS($A$3:A178, A178, $B$3:B178, B178, $C$3:C178, C178) - 1</f>
+        <v>25</v>
       </c>
       <c r="E178" t="str" cm="1">
         <f t="array" ref="E178">_xlfn.CONCAT(IF(A178="completion", "Completion", IF(A178="cassette", "Cassette", IF(A178="gemheart", "Crystal Heart", IF(A178="strawberry", _xlfn.CONCAT("Strawberry ", D178+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B178)*(regions!$B$2:$B$27=C178), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 27 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 26 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F178" t="str">
         <f t="shared" si="2"/>
@@ -4647,12 +4650,12 @@
         <v>0</v>
       </c>
       <c r="D179">
-        <f>COUNTIFS($A$2:A179, A179, $B$2:B179, B179, $C$2:C179, C179) - 1</f>
-        <v>27</v>
+        <f>COUNTIFS($A$3:A179, A179, $B$3:B179, B179, $C$3:C179, C179) - 1</f>
+        <v>26</v>
       </c>
       <c r="E179" t="str" cm="1">
         <f t="array" ref="E179">_xlfn.CONCAT(IF(A179="completion", "Completion", IF(A179="cassette", "Cassette", IF(A179="gemheart", "Crystal Heart", IF(A179="strawberry", _xlfn.CONCAT("Strawberry ", D179+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B179)*(regions!$B$2:$B$27=C179), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 28 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 27 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F179" t="str">
         <f t="shared" si="2"/>
@@ -4670,12 +4673,12 @@
         <v>0</v>
       </c>
       <c r="D180">
-        <f>COUNTIFS($A$2:A180, A180, $B$2:B180, B180, $C$2:C180, C180) - 1</f>
-        <v>28</v>
+        <f>COUNTIFS($A$3:A180, A180, $B$3:B180, B180, $C$3:C180, C180) - 1</f>
+        <v>27</v>
       </c>
       <c r="E180" t="str" cm="1">
         <f t="array" ref="E180">_xlfn.CONCAT(IF(A180="completion", "Completion", IF(A180="cassette", "Cassette", IF(A180="gemheart", "Crystal Heart", IF(A180="strawberry", _xlfn.CONCAT("Strawberry ", D180+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B180)*(regions!$B$2:$B$27=C180), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 29 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 28 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F180" t="str">
         <f t="shared" si="2"/>
@@ -4693,12 +4696,12 @@
         <v>0</v>
       </c>
       <c r="D181">
-        <f>COUNTIFS($A$2:A181, A181, $B$2:B181, B181, $C$2:C181, C181) - 1</f>
-        <v>29</v>
+        <f>COUNTIFS($A$3:A181, A181, $B$3:B181, B181, $C$3:C181, C181) - 1</f>
+        <v>28</v>
       </c>
       <c r="E181" t="str" cm="1">
         <f t="array" ref="E181">_xlfn.CONCAT(IF(A181="completion", "Completion", IF(A181="cassette", "Cassette", IF(A181="gemheart", "Crystal Heart", IF(A181="strawberry", _xlfn.CONCAT("Strawberry ", D181+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B181)*(regions!$B$2:$B$27=C181), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 30 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 29 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F181" t="str">
         <f t="shared" si="2"/>
@@ -4716,12 +4719,12 @@
         <v>0</v>
       </c>
       <c r="D182">
-        <f>COUNTIFS($A$2:A182, A182, $B$2:B182, B182, $C$2:C182, C182) - 1</f>
-        <v>30</v>
+        <f>COUNTIFS($A$3:A182, A182, $B$3:B182, B182, $C$3:C182, C182) - 1</f>
+        <v>29</v>
       </c>
       <c r="E182" t="str" cm="1">
         <f t="array" ref="E182">_xlfn.CONCAT(IF(A182="completion", "Completion", IF(A182="cassette", "Cassette", IF(A182="gemheart", "Crystal Heart", IF(A182="strawberry", _xlfn.CONCAT("Strawberry ", D182+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B182)*(regions!$B$2:$B$27=C182), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 31 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 30 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F182" t="str">
         <f t="shared" si="2"/>
@@ -4733,18 +4736,18 @@
         <v>6</v>
       </c>
       <c r="B183">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C183">
         <v>0</v>
       </c>
       <c r="D183">
-        <f>COUNTIFS($A$2:A183, A183, $B$2:B183, B183, $C$2:C183, C183) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A183, A183, $B$3:B183, B183, $C$3:C183, C183) - 1</f>
+        <v>30</v>
       </c>
       <c r="E183" t="str" cm="1">
         <f t="array" ref="E183">_xlfn.CONCAT(IF(A183="completion", "Completion", IF(A183="cassette", "Cassette", IF(A183="gemheart", "Crystal Heart", IF(A183="strawberry", _xlfn.CONCAT("Strawberry ", D183+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B183)*(regions!$B$2:$B$27=C183), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 31 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F183" t="str">
         <f t="shared" si="2"/>
@@ -4762,12 +4765,12 @@
         <v>0</v>
       </c>
       <c r="D184">
-        <f>COUNTIFS($A$2:A184, A184, $B$2:B184, B184, $C$2:C184, C184) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A184, A184, $B$3:B184, B184, $C$3:C184, C184) - 1</f>
+        <v>0</v>
       </c>
       <c r="E184" t="str" cm="1">
         <f t="array" ref="E184">_xlfn.CONCAT(IF(A184="completion", "Completion", IF(A184="cassette", "Cassette", IF(A184="gemheart", "Crystal Heart", IF(A184="strawberry", _xlfn.CONCAT("Strawberry ", D184+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B184)*(regions!$B$2:$B$27=C184), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 1 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F184" t="str">
         <f t="shared" si="2"/>
@@ -4785,12 +4788,12 @@
         <v>0</v>
       </c>
       <c r="D185">
-        <f>COUNTIFS($A$2:A185, A185, $B$2:B185, B185, $C$2:C185, C185) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A185, A185, $B$3:B185, B185, $C$3:C185, C185) - 1</f>
+        <v>1</v>
       </c>
       <c r="E185" t="str" cm="1">
         <f t="array" ref="E185">_xlfn.CONCAT(IF(A185="completion", "Completion", IF(A185="cassette", "Cassette", IF(A185="gemheart", "Crystal Heart", IF(A185="strawberry", _xlfn.CONCAT("Strawberry ", D185+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B185)*(regions!$B$2:$B$27=C185), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 2 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F185" t="str">
         <f t="shared" si="2"/>
@@ -4808,12 +4811,12 @@
         <v>0</v>
       </c>
       <c r="D186">
-        <f>COUNTIFS($A$2:A186, A186, $B$2:B186, B186, $C$2:C186, C186) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A186, A186, $B$3:B186, B186, $C$3:C186, C186) - 1</f>
+        <v>2</v>
       </c>
       <c r="E186" t="str" cm="1">
         <f t="array" ref="E186">_xlfn.CONCAT(IF(A186="completion", "Completion", IF(A186="cassette", "Cassette", IF(A186="gemheart", "Crystal Heart", IF(A186="strawberry", _xlfn.CONCAT("Strawberry ", D186+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B186)*(regions!$B$2:$B$27=C186), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 3 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F186" t="str">
         <f t="shared" si="2"/>
@@ -4831,12 +4834,12 @@
         <v>0</v>
       </c>
       <c r="D187">
-        <f>COUNTIFS($A$2:A187, A187, $B$2:B187, B187, $C$2:C187, C187) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A187, A187, $B$3:B187, B187, $C$3:C187, C187) - 1</f>
+        <v>3</v>
       </c>
       <c r="E187" t="str" cm="1">
         <f t="array" ref="E187">_xlfn.CONCAT(IF(A187="completion", "Completion", IF(A187="cassette", "Cassette", IF(A187="gemheart", "Crystal Heart", IF(A187="strawberry", _xlfn.CONCAT("Strawberry ", D187+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B187)*(regions!$B$2:$B$27=C187), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 4 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F187" t="str">
         <f t="shared" si="2"/>
@@ -4854,12 +4857,12 @@
         <v>0</v>
       </c>
       <c r="D188">
-        <f>COUNTIFS($A$2:A188, A188, $B$2:B188, B188, $C$2:C188, C188) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A188, A188, $B$3:B188, B188, $C$3:C188, C188) - 1</f>
+        <v>4</v>
       </c>
       <c r="E188" t="str" cm="1">
         <f t="array" ref="E188">_xlfn.CONCAT(IF(A188="completion", "Completion", IF(A188="cassette", "Cassette", IF(A188="gemheart", "Crystal Heart", IF(A188="strawberry", _xlfn.CONCAT("Strawberry ", D188+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B188)*(regions!$B$2:$B$27=C188), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 5 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F188" t="str">
         <f t="shared" si="2"/>
@@ -4877,12 +4880,12 @@
         <v>0</v>
       </c>
       <c r="D189">
-        <f>COUNTIFS($A$2:A189, A189, $B$2:B189, B189, $C$2:C189, C189) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A189, A189, $B$3:B189, B189, $C$3:C189, C189) - 1</f>
+        <v>5</v>
       </c>
       <c r="E189" t="str" cm="1">
         <f t="array" ref="E189">_xlfn.CONCAT(IF(A189="completion", "Completion", IF(A189="cassette", "Cassette", IF(A189="gemheart", "Crystal Heart", IF(A189="strawberry", _xlfn.CONCAT("Strawberry ", D189+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B189)*(regions!$B$2:$B$27=C189), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 6 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F189" t="str">
         <f t="shared" si="2"/>
@@ -4900,12 +4903,12 @@
         <v>0</v>
       </c>
       <c r="D190">
-        <f>COUNTIFS($A$2:A190, A190, $B$2:B190, B190, $C$2:C190, C190) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A190, A190, $B$3:B190, B190, $C$3:C190, C190) - 1</f>
+        <v>6</v>
       </c>
       <c r="E190" t="str" cm="1">
         <f t="array" ref="E190">_xlfn.CONCAT(IF(A190="completion", "Completion", IF(A190="cassette", "Cassette", IF(A190="gemheart", "Crystal Heart", IF(A190="strawberry", _xlfn.CONCAT("Strawberry ", D190+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B190)*(regions!$B$2:$B$27=C190), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 7 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F190" t="str">
         <f t="shared" si="2"/>
@@ -4923,12 +4926,12 @@
         <v>0</v>
       </c>
       <c r="D191">
-        <f>COUNTIFS($A$2:A191, A191, $B$2:B191, B191, $C$2:C191, C191) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A191, A191, $B$3:B191, B191, $C$3:C191, C191) - 1</f>
+        <v>7</v>
       </c>
       <c r="E191" t="str" cm="1">
         <f t="array" ref="E191">_xlfn.CONCAT(IF(A191="completion", "Completion", IF(A191="cassette", "Cassette", IF(A191="gemheart", "Crystal Heart", IF(A191="strawberry", _xlfn.CONCAT("Strawberry ", D191+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B191)*(regions!$B$2:$B$27=C191), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 8 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F191" t="str">
         <f t="shared" si="2"/>
@@ -4946,12 +4949,12 @@
         <v>0</v>
       </c>
       <c r="D192">
-        <f>COUNTIFS($A$2:A192, A192, $B$2:B192, B192, $C$2:C192, C192) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A192, A192, $B$3:B192, B192, $C$3:C192, C192) - 1</f>
+        <v>8</v>
       </c>
       <c r="E192" t="str" cm="1">
         <f t="array" ref="E192">_xlfn.CONCAT(IF(A192="completion", "Completion", IF(A192="cassette", "Cassette", IF(A192="gemheart", "Crystal Heart", IF(A192="strawberry", _xlfn.CONCAT("Strawberry ", D192+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B192)*(regions!$B$2:$B$27=C192), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 9 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F192" t="str">
         <f t="shared" si="2"/>
@@ -4969,12 +4972,12 @@
         <v>0</v>
       </c>
       <c r="D193">
-        <f>COUNTIFS($A$2:A193, A193, $B$2:B193, B193, $C$2:C193, C193) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A193, A193, $B$3:B193, B193, $C$3:C193, C193) - 1</f>
+        <v>9</v>
       </c>
       <c r="E193" t="str" cm="1">
         <f t="array" ref="E193">_xlfn.CONCAT(IF(A193="completion", "Completion", IF(A193="cassette", "Cassette", IF(A193="gemheart", "Crystal Heart", IF(A193="strawberry", _xlfn.CONCAT("Strawberry ", D193+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B193)*(regions!$B$2:$B$27=C193), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 10 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F193" t="str">
         <f t="shared" si="2"/>
@@ -4992,15 +4995,15 @@
         <v>0</v>
       </c>
       <c r="D194">
-        <f>COUNTIFS($A$2:A194, A194, $B$2:B194, B194, $C$2:C194, C194) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A194, A194, $B$3:B194, B194, $C$3:C194, C194) - 1</f>
+        <v>10</v>
       </c>
       <c r="E194" t="str" cm="1">
         <f t="array" ref="E194">_xlfn.CONCAT(IF(A194="completion", "Completion", IF(A194="cassette", "Cassette", IF(A194="gemheart", "Crystal Heart", IF(A194="strawberry", _xlfn.CONCAT("Strawberry ", D194+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B194)*(regions!$B$2:$B$27=C194), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 11 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F194" t="str">
-        <f t="shared" ref="F194:F234" si="3">IF(A194="strawberry", "Strawberry", E194)</f>
+        <f t="shared" si="2"/>
         <v>Strawberry</v>
       </c>
     </row>
@@ -5015,15 +5018,15 @@
         <v>0</v>
       </c>
       <c r="D195">
-        <f>COUNTIFS($A$2:A195, A195, $B$2:B195, B195, $C$2:C195, C195) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A195, A195, $B$3:B195, B195, $C$3:C195, C195) - 1</f>
+        <v>11</v>
       </c>
       <c r="E195" t="str" cm="1">
         <f t="array" ref="E195">_xlfn.CONCAT(IF(A195="completion", "Completion", IF(A195="cassette", "Cassette", IF(A195="gemheart", "Crystal Heart", IF(A195="strawberry", _xlfn.CONCAT("Strawberry ", D195+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B195)*(regions!$B$2:$B$27=C195), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 12 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F195" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F195:F235" si="3">IF(A195="strawberry", "Strawberry", E195)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -5038,12 +5041,12 @@
         <v>0</v>
       </c>
       <c r="D196">
-        <f>COUNTIFS($A$2:A196, A196, $B$2:B196, B196, $C$2:C196, C196) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A196, A196, $B$3:B196, B196, $C$3:C196, C196) - 1</f>
+        <v>12</v>
       </c>
       <c r="E196" t="str" cm="1">
         <f t="array" ref="E196">_xlfn.CONCAT(IF(A196="completion", "Completion", IF(A196="cassette", "Cassette", IF(A196="gemheart", "Crystal Heart", IF(A196="strawberry", _xlfn.CONCAT("Strawberry ", D196+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B196)*(regions!$B$2:$B$27=C196), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 13 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F196" t="str">
         <f t="shared" si="3"/>
@@ -5061,12 +5064,12 @@
         <v>0</v>
       </c>
       <c r="D197">
-        <f>COUNTIFS($A$2:A197, A197, $B$2:B197, B197, $C$2:C197, C197) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A197, A197, $B$3:B197, B197, $C$3:C197, C197) - 1</f>
+        <v>13</v>
       </c>
       <c r="E197" t="str" cm="1">
         <f t="array" ref="E197">_xlfn.CONCAT(IF(A197="completion", "Completion", IF(A197="cassette", "Cassette", IF(A197="gemheart", "Crystal Heart", IF(A197="strawberry", _xlfn.CONCAT("Strawberry ", D197+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B197)*(regions!$B$2:$B$27=C197), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 14 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F197" t="str">
         <f t="shared" si="3"/>
@@ -5084,12 +5087,12 @@
         <v>0</v>
       </c>
       <c r="D198">
-        <f>COUNTIFS($A$2:A198, A198, $B$2:B198, B198, $C$2:C198, C198) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A198, A198, $B$3:B198, B198, $C$3:C198, C198) - 1</f>
+        <v>14</v>
       </c>
       <c r="E198" t="str" cm="1">
         <f t="array" ref="E198">_xlfn.CONCAT(IF(A198="completion", "Completion", IF(A198="cassette", "Cassette", IF(A198="gemheart", "Crystal Heart", IF(A198="strawberry", _xlfn.CONCAT("Strawberry ", D198+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B198)*(regions!$B$2:$B$27=C198), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 15 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F198" t="str">
         <f t="shared" si="3"/>
@@ -5107,12 +5110,12 @@
         <v>0</v>
       </c>
       <c r="D199">
-        <f>COUNTIFS($A$2:A199, A199, $B$2:B199, B199, $C$2:C199, C199) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A199, A199, $B$3:B199, B199, $C$3:C199, C199) - 1</f>
+        <v>15</v>
       </c>
       <c r="E199" t="str" cm="1">
         <f t="array" ref="E199">_xlfn.CONCAT(IF(A199="completion", "Completion", IF(A199="cassette", "Cassette", IF(A199="gemheart", "Crystal Heart", IF(A199="strawberry", _xlfn.CONCAT("Strawberry ", D199+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B199)*(regions!$B$2:$B$27=C199), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 16 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F199" t="str">
         <f t="shared" si="3"/>
@@ -5130,12 +5133,12 @@
         <v>0</v>
       </c>
       <c r="D200">
-        <f>COUNTIFS($A$2:A200, A200, $B$2:B200, B200, $C$2:C200, C200) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A200, A200, $B$3:B200, B200, $C$3:C200, C200) - 1</f>
+        <v>16</v>
       </c>
       <c r="E200" t="str" cm="1">
         <f t="array" ref="E200">_xlfn.CONCAT(IF(A200="completion", "Completion", IF(A200="cassette", "Cassette", IF(A200="gemheart", "Crystal Heart", IF(A200="strawberry", _xlfn.CONCAT("Strawberry ", D200+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B200)*(regions!$B$2:$B$27=C200), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 17 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F200" t="str">
         <f t="shared" si="3"/>
@@ -5153,12 +5156,12 @@
         <v>0</v>
       </c>
       <c r="D201">
-        <f>COUNTIFS($A$2:A201, A201, $B$2:B201, B201, $C$2:C201, C201) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A201, A201, $B$3:B201, B201, $C$3:C201, C201) - 1</f>
+        <v>17</v>
       </c>
       <c r="E201" t="str" cm="1">
         <f t="array" ref="E201">_xlfn.CONCAT(IF(A201="completion", "Completion", IF(A201="cassette", "Cassette", IF(A201="gemheart", "Crystal Heart", IF(A201="strawberry", _xlfn.CONCAT("Strawberry ", D201+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B201)*(regions!$B$2:$B$27=C201), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 18 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F201" t="str">
         <f t="shared" si="3"/>
@@ -5176,12 +5179,12 @@
         <v>0</v>
       </c>
       <c r="D202">
-        <f>COUNTIFS($A$2:A202, A202, $B$2:B202, B202, $C$2:C202, C202) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A202, A202, $B$3:B202, B202, $C$3:C202, C202) - 1</f>
+        <v>18</v>
       </c>
       <c r="E202" t="str" cm="1">
         <f t="array" ref="E202">_xlfn.CONCAT(IF(A202="completion", "Completion", IF(A202="cassette", "Cassette", IF(A202="gemheart", "Crystal Heart", IF(A202="strawberry", _xlfn.CONCAT("Strawberry ", D202+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B202)*(regions!$B$2:$B$27=C202), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 19 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F202" t="str">
         <f t="shared" si="3"/>
@@ -5199,12 +5202,12 @@
         <v>0</v>
       </c>
       <c r="D203">
-        <f>COUNTIFS($A$2:A203, A203, $B$2:B203, B203, $C$2:C203, C203) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A203, A203, $B$3:B203, B203, $C$3:C203, C203) - 1</f>
+        <v>19</v>
       </c>
       <c r="E203" t="str" cm="1">
         <f t="array" ref="E203">_xlfn.CONCAT(IF(A203="completion", "Completion", IF(A203="cassette", "Cassette", IF(A203="gemheart", "Crystal Heart", IF(A203="strawberry", _xlfn.CONCAT("Strawberry ", D203+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B203)*(regions!$B$2:$B$27=C203), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 20 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F203" t="str">
         <f t="shared" si="3"/>
@@ -5222,12 +5225,12 @@
         <v>0</v>
       </c>
       <c r="D204">
-        <f>COUNTIFS($A$2:A204, A204, $B$2:B204, B204, $C$2:C204, C204) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A204, A204, $B$3:B204, B204, $C$3:C204, C204) - 1</f>
+        <v>20</v>
       </c>
       <c r="E204" t="str" cm="1">
         <f t="array" ref="E204">_xlfn.CONCAT(IF(A204="completion", "Completion", IF(A204="cassette", "Cassette", IF(A204="gemheart", "Crystal Heart", IF(A204="strawberry", _xlfn.CONCAT("Strawberry ", D204+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B204)*(regions!$B$2:$B$27=C204), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 21 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F204" t="str">
         <f t="shared" si="3"/>
@@ -5245,12 +5248,12 @@
         <v>0</v>
       </c>
       <c r="D205">
-        <f>COUNTIFS($A$2:A205, A205, $B$2:B205, B205, $C$2:C205, C205) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A205, A205, $B$3:B205, B205, $C$3:C205, C205) - 1</f>
+        <v>21</v>
       </c>
       <c r="E205" t="str" cm="1">
         <f t="array" ref="E205">_xlfn.CONCAT(IF(A205="completion", "Completion", IF(A205="cassette", "Cassette", IF(A205="gemheart", "Crystal Heart", IF(A205="strawberry", _xlfn.CONCAT("Strawberry ", D205+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B205)*(regions!$B$2:$B$27=C205), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 22 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F205" t="str">
         <f t="shared" si="3"/>
@@ -5268,12 +5271,12 @@
         <v>0</v>
       </c>
       <c r="D206">
-        <f>COUNTIFS($A$2:A206, A206, $B$2:B206, B206, $C$2:C206, C206) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A206, A206, $B$3:B206, B206, $C$3:C206, C206) - 1</f>
+        <v>22</v>
       </c>
       <c r="E206" t="str" cm="1">
         <f t="array" ref="E206">_xlfn.CONCAT(IF(A206="completion", "Completion", IF(A206="cassette", "Cassette", IF(A206="gemheart", "Crystal Heart", IF(A206="strawberry", _xlfn.CONCAT("Strawberry ", D206+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B206)*(regions!$B$2:$B$27=C206), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 23 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F206" t="str">
         <f t="shared" si="3"/>
@@ -5291,12 +5294,12 @@
         <v>0</v>
       </c>
       <c r="D207">
-        <f>COUNTIFS($A$2:A207, A207, $B$2:B207, B207, $C$2:C207, C207) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A207, A207, $B$3:B207, B207, $C$3:C207, C207) - 1</f>
+        <v>23</v>
       </c>
       <c r="E207" t="str" cm="1">
         <f t="array" ref="E207">_xlfn.CONCAT(IF(A207="completion", "Completion", IF(A207="cassette", "Cassette", IF(A207="gemheart", "Crystal Heart", IF(A207="strawberry", _xlfn.CONCAT("Strawberry ", D207+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B207)*(regions!$B$2:$B$27=C207), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 24 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F207" t="str">
         <f t="shared" si="3"/>
@@ -5314,12 +5317,12 @@
         <v>0</v>
       </c>
       <c r="D208">
-        <f>COUNTIFS($A$2:A208, A208, $B$2:B208, B208, $C$2:C208, C208) - 1</f>
-        <v>25</v>
+        <f>COUNTIFS($A$3:A208, A208, $B$3:B208, B208, $C$3:C208, C208) - 1</f>
+        <v>24</v>
       </c>
       <c r="E208" t="str" cm="1">
         <f t="array" ref="E208">_xlfn.CONCAT(IF(A208="completion", "Completion", IF(A208="cassette", "Cassette", IF(A208="gemheart", "Crystal Heart", IF(A208="strawberry", _xlfn.CONCAT("Strawberry ", D208+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B208)*(regions!$B$2:$B$27=C208), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 26 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 25 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F208" t="str">
         <f t="shared" si="3"/>
@@ -5337,12 +5340,12 @@
         <v>0</v>
       </c>
       <c r="D209">
-        <f>COUNTIFS($A$2:A209, A209, $B$2:B209, B209, $C$2:C209, C209) - 1</f>
-        <v>26</v>
+        <f>COUNTIFS($A$3:A209, A209, $B$3:B209, B209, $C$3:C209, C209) - 1</f>
+        <v>25</v>
       </c>
       <c r="E209" t="str" cm="1">
         <f t="array" ref="E209">_xlfn.CONCAT(IF(A209="completion", "Completion", IF(A209="cassette", "Cassette", IF(A209="gemheart", "Crystal Heart", IF(A209="strawberry", _xlfn.CONCAT("Strawberry ", D209+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B209)*(regions!$B$2:$B$27=C209), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 27 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 26 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F209" t="str">
         <f t="shared" si="3"/>
@@ -5360,12 +5363,12 @@
         <v>0</v>
       </c>
       <c r="D210">
-        <f>COUNTIFS($A$2:A210, A210, $B$2:B210, B210, $C$2:C210, C210) - 1</f>
-        <v>27</v>
+        <f>COUNTIFS($A$3:A210, A210, $B$3:B210, B210, $C$3:C210, C210) - 1</f>
+        <v>26</v>
       </c>
       <c r="E210" t="str" cm="1">
         <f t="array" ref="E210">_xlfn.CONCAT(IF(A210="completion", "Completion", IF(A210="cassette", "Cassette", IF(A210="gemheart", "Crystal Heart", IF(A210="strawberry", _xlfn.CONCAT("Strawberry ", D210+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B210)*(regions!$B$2:$B$27=C210), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 28 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 27 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F210" t="str">
         <f t="shared" si="3"/>
@@ -5383,12 +5386,12 @@
         <v>0</v>
       </c>
       <c r="D211">
-        <f>COUNTIFS($A$2:A211, A211, $B$2:B211, B211, $C$2:C211, C211) - 1</f>
-        <v>28</v>
+        <f>COUNTIFS($A$3:A211, A211, $B$3:B211, B211, $C$3:C211, C211) - 1</f>
+        <v>27</v>
       </c>
       <c r="E211" t="str" cm="1">
         <f t="array" ref="E211">_xlfn.CONCAT(IF(A211="completion", "Completion", IF(A211="cassette", "Cassette", IF(A211="gemheart", "Crystal Heart", IF(A211="strawberry", _xlfn.CONCAT("Strawberry ", D211+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B211)*(regions!$B$2:$B$27=C211), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 29 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 28 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F211" t="str">
         <f t="shared" si="3"/>
@@ -5406,12 +5409,12 @@
         <v>0</v>
       </c>
       <c r="D212">
-        <f>COUNTIFS($A$2:A212, A212, $B$2:B212, B212, $C$2:C212, C212) - 1</f>
-        <v>29</v>
+        <f>COUNTIFS($A$3:A212, A212, $B$3:B212, B212, $C$3:C212, C212) - 1</f>
+        <v>28</v>
       </c>
       <c r="E212" t="str" cm="1">
         <f t="array" ref="E212">_xlfn.CONCAT(IF(A212="completion", "Completion", IF(A212="cassette", "Cassette", IF(A212="gemheart", "Crystal Heart", IF(A212="strawberry", _xlfn.CONCAT("Strawberry ", D212+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B212)*(regions!$B$2:$B$27=C212), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 30 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 29 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F212" t="str">
         <f t="shared" si="3"/>
@@ -5429,12 +5432,12 @@
         <v>0</v>
       </c>
       <c r="D213">
-        <f>COUNTIFS($A$2:A213, A213, $B$2:B213, B213, $C$2:C213, C213) - 1</f>
-        <v>30</v>
+        <f>COUNTIFS($A$3:A213, A213, $B$3:B213, B213, $C$3:C213, C213) - 1</f>
+        <v>29</v>
       </c>
       <c r="E213" t="str" cm="1">
         <f t="array" ref="E213">_xlfn.CONCAT(IF(A213="completion", "Completion", IF(A213="cassette", "Cassette", IF(A213="gemheart", "Crystal Heart", IF(A213="strawberry", _xlfn.CONCAT("Strawberry ", D213+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B213)*(regions!$B$2:$B$27=C213), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 31 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 30 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F213" t="str">
         <f t="shared" si="3"/>
@@ -5452,12 +5455,12 @@
         <v>0</v>
       </c>
       <c r="D214">
-        <f>COUNTIFS($A$2:A214, A214, $B$2:B214, B214, $C$2:C214, C214) - 1</f>
-        <v>31</v>
+        <f>COUNTIFS($A$3:A214, A214, $B$3:B214, B214, $C$3:C214, C214) - 1</f>
+        <v>30</v>
       </c>
       <c r="E214" t="str" cm="1">
         <f t="array" ref="E214">_xlfn.CONCAT(IF(A214="completion", "Completion", IF(A214="cassette", "Cassette", IF(A214="gemheart", "Crystal Heart", IF(A214="strawberry", _xlfn.CONCAT("Strawberry ", D214+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B214)*(regions!$B$2:$B$27=C214), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 32 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 31 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F214" t="str">
         <f t="shared" si="3"/>
@@ -5475,12 +5478,12 @@
         <v>0</v>
       </c>
       <c r="D215">
-        <f>COUNTIFS($A$2:A215, A215, $B$2:B215, B215, $C$2:C215, C215) - 1</f>
-        <v>32</v>
+        <f>COUNTIFS($A$3:A215, A215, $B$3:B215, B215, $C$3:C215, C215) - 1</f>
+        <v>31</v>
       </c>
       <c r="E215" t="str" cm="1">
         <f t="array" ref="E215">_xlfn.CONCAT(IF(A215="completion", "Completion", IF(A215="cassette", "Cassette", IF(A215="gemheart", "Crystal Heart", IF(A215="strawberry", _xlfn.CONCAT("Strawberry ", D215+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B215)*(regions!$B$2:$B$27=C215), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 33 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 32 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F215" t="str">
         <f t="shared" si="3"/>
@@ -5498,12 +5501,12 @@
         <v>0</v>
       </c>
       <c r="D216">
-        <f>COUNTIFS($A$2:A216, A216, $B$2:B216, B216, $C$2:C216, C216) - 1</f>
-        <v>33</v>
+        <f>COUNTIFS($A$3:A216, A216, $B$3:B216, B216, $C$3:C216, C216) - 1</f>
+        <v>32</v>
       </c>
       <c r="E216" t="str" cm="1">
         <f t="array" ref="E216">_xlfn.CONCAT(IF(A216="completion", "Completion", IF(A216="cassette", "Cassette", IF(A216="gemheart", "Crystal Heart", IF(A216="strawberry", _xlfn.CONCAT("Strawberry ", D216+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B216)*(regions!$B$2:$B$27=C216), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 34 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 33 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F216" t="str">
         <f t="shared" si="3"/>
@@ -5521,12 +5524,12 @@
         <v>0</v>
       </c>
       <c r="D217">
-        <f>COUNTIFS($A$2:A217, A217, $B$2:B217, B217, $C$2:C217, C217) - 1</f>
-        <v>34</v>
+        <f>COUNTIFS($A$3:A217, A217, $B$3:B217, B217, $C$3:C217, C217) - 1</f>
+        <v>33</v>
       </c>
       <c r="E217" t="str" cm="1">
         <f t="array" ref="E217">_xlfn.CONCAT(IF(A217="completion", "Completion", IF(A217="cassette", "Cassette", IF(A217="gemheart", "Crystal Heart", IF(A217="strawberry", _xlfn.CONCAT("Strawberry ", D217+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B217)*(regions!$B$2:$B$27=C217), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 35 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 34 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F217" t="str">
         <f t="shared" si="3"/>
@@ -5544,12 +5547,12 @@
         <v>0</v>
       </c>
       <c r="D218">
-        <f>COUNTIFS($A$2:A218, A218, $B$2:B218, B218, $C$2:C218, C218) - 1</f>
-        <v>35</v>
+        <f>COUNTIFS($A$3:A218, A218, $B$3:B218, B218, $C$3:C218, C218) - 1</f>
+        <v>34</v>
       </c>
       <c r="E218" t="str" cm="1">
         <f t="array" ref="E218">_xlfn.CONCAT(IF(A218="completion", "Completion", IF(A218="cassette", "Cassette", IF(A218="gemheart", "Crystal Heart", IF(A218="strawberry", _xlfn.CONCAT("Strawberry ", D218+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B218)*(regions!$B$2:$B$27=C218), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 36 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 35 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F218" t="str">
         <f t="shared" si="3"/>
@@ -5567,12 +5570,12 @@
         <v>0</v>
       </c>
       <c r="D219">
-        <f>COUNTIFS($A$2:A219, A219, $B$2:B219, B219, $C$2:C219, C219) - 1</f>
-        <v>36</v>
+        <f>COUNTIFS($A$3:A219, A219, $B$3:B219, B219, $C$3:C219, C219) - 1</f>
+        <v>35</v>
       </c>
       <c r="E219" t="str" cm="1">
         <f t="array" ref="E219">_xlfn.CONCAT(IF(A219="completion", "Completion", IF(A219="cassette", "Cassette", IF(A219="gemheart", "Crystal Heart", IF(A219="strawberry", _xlfn.CONCAT("Strawberry ", D219+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B219)*(regions!$B$2:$B$27=C219), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 37 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 36 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F219" t="str">
         <f t="shared" si="3"/>
@@ -5590,12 +5593,12 @@
         <v>0</v>
       </c>
       <c r="D220">
-        <f>COUNTIFS($A$2:A220, A220, $B$2:B220, B220, $C$2:C220, C220) - 1</f>
-        <v>37</v>
+        <f>COUNTIFS($A$3:A220, A220, $B$3:B220, B220, $C$3:C220, C220) - 1</f>
+        <v>36</v>
       </c>
       <c r="E220" t="str" cm="1">
         <f t="array" ref="E220">_xlfn.CONCAT(IF(A220="completion", "Completion", IF(A220="cassette", "Cassette", IF(A220="gemheart", "Crystal Heart", IF(A220="strawberry", _xlfn.CONCAT("Strawberry ", D220+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B220)*(regions!$B$2:$B$27=C220), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 38 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 37 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F220" t="str">
         <f t="shared" si="3"/>
@@ -5613,12 +5616,12 @@
         <v>0</v>
       </c>
       <c r="D221">
-        <f>COUNTIFS($A$2:A221, A221, $B$2:B221, B221, $C$2:C221, C221) - 1</f>
-        <v>38</v>
+        <f>COUNTIFS($A$3:A221, A221, $B$3:B221, B221, $C$3:C221, C221) - 1</f>
+        <v>37</v>
       </c>
       <c r="E221" t="str" cm="1">
         <f t="array" ref="E221">_xlfn.CONCAT(IF(A221="completion", "Completion", IF(A221="cassette", "Cassette", IF(A221="gemheart", "Crystal Heart", IF(A221="strawberry", _xlfn.CONCAT("Strawberry ", D221+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B221)*(regions!$B$2:$B$27=C221), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 39 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 38 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F221" t="str">
         <f t="shared" si="3"/>
@@ -5636,12 +5639,12 @@
         <v>0</v>
       </c>
       <c r="D222">
-        <f>COUNTIFS($A$2:A222, A222, $B$2:B222, B222, $C$2:C222, C222) - 1</f>
-        <v>39</v>
+        <f>COUNTIFS($A$3:A222, A222, $B$3:B222, B222, $C$3:C222, C222) - 1</f>
+        <v>38</v>
       </c>
       <c r="E222" t="str" cm="1">
         <f t="array" ref="E222">_xlfn.CONCAT(IF(A222="completion", "Completion", IF(A222="cassette", "Cassette", IF(A222="gemheart", "Crystal Heart", IF(A222="strawberry", _xlfn.CONCAT("Strawberry ", D222+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B222)*(regions!$B$2:$B$27=C222), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 40 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 39 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F222" t="str">
         <f t="shared" si="3"/>
@@ -5659,12 +5662,12 @@
         <v>0</v>
       </c>
       <c r="D223">
-        <f>COUNTIFS($A$2:A223, A223, $B$2:B223, B223, $C$2:C223, C223) - 1</f>
-        <v>40</v>
+        <f>COUNTIFS($A$3:A223, A223, $B$3:B223, B223, $C$3:C223, C223) - 1</f>
+        <v>39</v>
       </c>
       <c r="E223" t="str" cm="1">
         <f t="array" ref="E223">_xlfn.CONCAT(IF(A223="completion", "Completion", IF(A223="cassette", "Cassette", IF(A223="gemheart", "Crystal Heart", IF(A223="strawberry", _xlfn.CONCAT("Strawberry ", D223+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B223)*(regions!$B$2:$B$27=C223), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 41 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 40 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F223" t="str">
         <f t="shared" si="3"/>
@@ -5682,12 +5685,12 @@
         <v>0</v>
       </c>
       <c r="D224">
-        <f>COUNTIFS($A$2:A224, A224, $B$2:B224, B224, $C$2:C224, C224) - 1</f>
-        <v>41</v>
+        <f>COUNTIFS($A$3:A224, A224, $B$3:B224, B224, $C$3:C224, C224) - 1</f>
+        <v>40</v>
       </c>
       <c r="E224" t="str" cm="1">
         <f t="array" ref="E224">_xlfn.CONCAT(IF(A224="completion", "Completion", IF(A224="cassette", "Cassette", IF(A224="gemheart", "Crystal Heart", IF(A224="strawberry", _xlfn.CONCAT("Strawberry ", D224+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B224)*(regions!$B$2:$B$27=C224), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 42 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 41 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F224" t="str">
         <f t="shared" si="3"/>
@@ -5705,12 +5708,12 @@
         <v>0</v>
       </c>
       <c r="D225">
-        <f>COUNTIFS($A$2:A225, A225, $B$2:B225, B225, $C$2:C225, C225) - 1</f>
-        <v>42</v>
+        <f>COUNTIFS($A$3:A225, A225, $B$3:B225, B225, $C$3:C225, C225) - 1</f>
+        <v>41</v>
       </c>
       <c r="E225" t="str" cm="1">
         <f t="array" ref="E225">_xlfn.CONCAT(IF(A225="completion", "Completion", IF(A225="cassette", "Cassette", IF(A225="gemheart", "Crystal Heart", IF(A225="strawberry", _xlfn.CONCAT("Strawberry ", D225+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B225)*(regions!$B$2:$B$27=C225), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 43 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 42 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F225" t="str">
         <f t="shared" si="3"/>
@@ -5728,12 +5731,12 @@
         <v>0</v>
       </c>
       <c r="D226">
-        <f>COUNTIFS($A$2:A226, A226, $B$2:B226, B226, $C$2:C226, C226) - 1</f>
-        <v>43</v>
+        <f>COUNTIFS($A$3:A226, A226, $B$3:B226, B226, $C$3:C226, C226) - 1</f>
+        <v>42</v>
       </c>
       <c r="E226" t="str" cm="1">
         <f t="array" ref="E226">_xlfn.CONCAT(IF(A226="completion", "Completion", IF(A226="cassette", "Cassette", IF(A226="gemheart", "Crystal Heart", IF(A226="strawberry", _xlfn.CONCAT("Strawberry ", D226+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B226)*(regions!$B$2:$B$27=C226), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 44 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 43 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F226" t="str">
         <f t="shared" si="3"/>
@@ -5751,12 +5754,12 @@
         <v>0</v>
       </c>
       <c r="D227">
-        <f>COUNTIFS($A$2:A227, A227, $B$2:B227, B227, $C$2:C227, C227) - 1</f>
-        <v>44</v>
+        <f>COUNTIFS($A$3:A227, A227, $B$3:B227, B227, $C$3:C227, C227) - 1</f>
+        <v>43</v>
       </c>
       <c r="E227" t="str" cm="1">
         <f t="array" ref="E227">_xlfn.CONCAT(IF(A227="completion", "Completion", IF(A227="cassette", "Cassette", IF(A227="gemheart", "Crystal Heart", IF(A227="strawberry", _xlfn.CONCAT("Strawberry ", D227+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B227)*(regions!$B$2:$B$27=C227), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 45 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 44 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F227" t="str">
         <f t="shared" si="3"/>
@@ -5774,12 +5777,12 @@
         <v>0</v>
       </c>
       <c r="D228">
-        <f>COUNTIFS($A$2:A228, A228, $B$2:B228, B228, $C$2:C228, C228) - 1</f>
-        <v>45</v>
+        <f>COUNTIFS($A$3:A228, A228, $B$3:B228, B228, $C$3:C228, C228) - 1</f>
+        <v>44</v>
       </c>
       <c r="E228" t="str" cm="1">
         <f t="array" ref="E228">_xlfn.CONCAT(IF(A228="completion", "Completion", IF(A228="cassette", "Cassette", IF(A228="gemheart", "Crystal Heart", IF(A228="strawberry", _xlfn.CONCAT("Strawberry ", D228+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B228)*(regions!$B$2:$B$27=C228), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 46 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 45 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F228" t="str">
         <f t="shared" si="3"/>
@@ -5797,12 +5800,12 @@
         <v>0</v>
       </c>
       <c r="D229">
-        <f>COUNTIFS($A$2:A229, A229, $B$2:B229, B229, $C$2:C229, C229) - 1</f>
-        <v>46</v>
+        <f>COUNTIFS($A$3:A229, A229, $B$3:B229, B229, $C$3:C229, C229) - 1</f>
+        <v>45</v>
       </c>
       <c r="E229" t="str" cm="1">
         <f t="array" ref="E229">_xlfn.CONCAT(IF(A229="completion", "Completion", IF(A229="cassette", "Cassette", IF(A229="gemheart", "Crystal Heart", IF(A229="strawberry", _xlfn.CONCAT("Strawberry ", D229+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B229)*(regions!$B$2:$B$27=C229), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 47 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 46 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F229" t="str">
         <f t="shared" si="3"/>
@@ -5814,18 +5817,18 @@
         <v>6</v>
       </c>
       <c r="B230">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C230">
         <v>0</v>
       </c>
       <c r="D230">
-        <f>COUNTIFS($A$2:A230, A230, $B$2:B230, B230, $C$2:C230, C230) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A230, A230, $B$3:B230, B230, $C$3:C230, C230) - 1</f>
+        <v>46</v>
       </c>
       <c r="E230" t="str" cm="1">
         <f t="array" ref="E230">_xlfn.CONCAT(IF(A230="completion", "Completion", IF(A230="cassette", "Cassette", IF(A230="gemheart", "Crystal Heart", IF(A230="strawberry", _xlfn.CONCAT("Strawberry ", D230+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B230)*(regions!$B$2:$B$27=C230), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 47 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F230" t="str">
         <f t="shared" si="3"/>
@@ -5843,12 +5846,12 @@
         <v>0</v>
       </c>
       <c r="D231">
-        <f>COUNTIFS($A$2:A231, A231, $B$2:B231, B231, $C$2:C231, C231) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A231, A231, $B$3:B231, B231, $C$3:C231, C231) - 1</f>
+        <v>0</v>
       </c>
       <c r="E231" t="str" cm="1">
         <f t="array" ref="E231">_xlfn.CONCAT(IF(A231="completion", "Completion", IF(A231="cassette", "Cassette", IF(A231="gemheart", "Crystal Heart", IF(A231="strawberry", _xlfn.CONCAT("Strawberry ", D231+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B231)*(regions!$B$2:$B$27=C231), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 1 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F231" t="str">
         <f t="shared" si="3"/>
@@ -5866,12 +5869,12 @@
         <v>0</v>
       </c>
       <c r="D232">
-        <f>COUNTIFS($A$2:A232, A232, $B$2:B232, B232, $C$2:C232, C232) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A232, A232, $B$3:B232, B232, $C$3:C232, C232) - 1</f>
+        <v>1</v>
       </c>
       <c r="E232" t="str" cm="1">
         <f t="array" ref="E232">_xlfn.CONCAT(IF(A232="completion", "Completion", IF(A232="cassette", "Cassette", IF(A232="gemheart", "Crystal Heart", IF(A232="strawberry", _xlfn.CONCAT("Strawberry ", D232+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B232)*(regions!$B$2:$B$27=C232), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 2 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F232" t="str">
         <f t="shared" si="3"/>
@@ -5889,12 +5892,12 @@
         <v>0</v>
       </c>
       <c r="D233">
-        <f>COUNTIFS($A$2:A233, A233, $B$2:B233, B233, $C$2:C233, C233) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A233, A233, $B$3:B233, B233, $C$3:C233, C233) - 1</f>
+        <v>2</v>
       </c>
       <c r="E233" t="str" cm="1">
         <f t="array" ref="E233">_xlfn.CONCAT(IF(A233="completion", "Completion", IF(A233="cassette", "Cassette", IF(A233="gemheart", "Crystal Heart", IF(A233="strawberry", _xlfn.CONCAT("Strawberry ", D233+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B233)*(regions!$B$2:$B$27=C233), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 3 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F233" t="str">
         <f t="shared" si="3"/>
@@ -5912,14 +5915,37 @@
         <v>0</v>
       </c>
       <c r="D234">
-        <f>COUNTIFS($A$2:A234, A234, $B$2:B234, B234, $C$2:C234, C234) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A234, A234, $B$3:B234, B234, $C$3:C234, C234) - 1</f>
+        <v>3</v>
       </c>
       <c r="E234" t="str" cm="1">
         <f t="array" ref="E234">_xlfn.CONCAT(IF(A234="completion", "Completion", IF(A234="cassette", "Cassette", IF(A234="gemheart", "Crystal Heart", IF(A234="strawberry", _xlfn.CONCAT("Strawberry ", D234+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B234)*(regions!$B$2:$B$27=C234), regions!$C$2:$C$27, "", 0, 1), ")")</f>
+        <v>Strawberry 4 (Chapter 8: Core A-Side)</v>
+      </c>
+      <c r="F234" t="str">
+        <f t="shared" si="3"/>
+        <v>Strawberry</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>6</v>
+      </c>
+      <c r="B235">
+        <v>9</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235">
+        <f>COUNTIFS($A$3:A235, A235, $B$3:B235, B235, $C$3:C235, C235) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="E235" t="str" cm="1">
+        <f t="array" ref="E235">_xlfn.CONCAT(IF(A235="completion", "Completion", IF(A235="cassette", "Cassette", IF(A235="gemheart", "Crystal Heart", IF(A235="strawberry", _xlfn.CONCAT("Strawberry ", D235+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B235)*(regions!$B$2:$B$27=C235), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 8: Core A-Side)</v>
       </c>
-      <c r="F234" t="str">
+      <c r="F235" t="str">
         <f t="shared" si="3"/>
         <v>Strawberry</v>
       </c>
@@ -5934,7 +5960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1A1AF2-907D-41B3-B0A4-149E1E23A84D}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
General overhaul post-0.3.0 (#6)
* Fixed bug with C-Side region access

* Bumped version requirement

* Fixed level requirement maximum to include Epilogue

* Converted Celeste world to use dependency injection for handling different progressions

* Fixed bug where options_dataclass was not set correctly

* Fixed issue with relative referencing

* Fixed more issues with relative referencing

* Changed extraneous items to filler rather than useful

* Prettified JSON
</commit_message>
<xml_diff>
--- a/worlds/celeste/data/items.xlsx
+++ b/worlds/celeste/data/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Archipelago\worlds\celeste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D73B774-C4CE-42B9-80B0-DD5C3012104C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB511E2F-18EF-413B-9DBB-A860AE52C27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="0" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{C0CD6F56-D694-4BE6-8516-FA8CA6FB3D5E}"/>
+    <workbookView xWindow="-30828" yWindow="0" windowWidth="30936" windowHeight="16896" xr2:uid="{C0CD6F56-D694-4BE6-8516-FA8CA6FB3D5E}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="39">
   <si>
     <t>level</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>region_name</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>Victory (Celeste)</t>
   </si>
 </sst>
 </file>
@@ -530,11 +536,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A95FA-F51A-42F8-84DA-309114F88AAA}">
-  <dimension ref="A1:F234"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,25 +573,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>COUNTIFS($A$2:A2, A2, $B$2:B2, B2, $C$2:C2, C2) - 1</f>
-        <v>0</v>
-      </c>
-      <c r="E2" t="str" cm="1">
-        <f t="array" ref="E2">_xlfn.CONCAT(IF(A2="completion", "Completion", IF(A2="cassette", "Cassette", IF(A2="gemheart", "Crystal Heart", IF(A2="strawberry", _xlfn.CONCAT("Strawberry ", D2+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B2)*(regions!$B$2:$B$27=C2), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F65" si="0">IF(A2="strawberry", "Strawberry", E2)</f>
-        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -593,22 +596,22 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f>COUNTIFS($A$2:A3, A3, $B$2:B3, B3, $C$2:C3, C3) - 1</f>
+        <f>COUNTIFS($A$3:A3, A3, $B$3:B3, B3, $C$3:C3, C3) - 1</f>
         <v>0</v>
       </c>
       <c r="E3" t="str" cm="1">
         <f t="array" ref="E3">_xlfn.CONCAT(IF(A3="completion", "Completion", IF(A3="cassette", "Cassette", IF(A3="gemheart", "Crystal Heart", IF(A3="strawberry", _xlfn.CONCAT("Strawberry ", D3+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B3)*(regions!$B$2:$B$27=C3), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 2: Old Site A-Side)</v>
+        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>Cassette (Chapter 2: Old Site A-Side)</v>
+        <f t="shared" ref="F3:F66" si="0">IF(A3="strawberry", "Strawberry", E3)</f>
+        <v>Cassette (Chapter 1: Forsaken City A-Side)</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -616,22 +619,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f>COUNTIFS($A$2:A4, A4, $B$2:B4, B4, $C$2:C4, C4) - 1</f>
+        <f>COUNTIFS($A$3:A4, A4, $B$3:B4, B4, $C$3:C4, C4) - 1</f>
         <v>0</v>
       </c>
       <c r="E4" t="str" cm="1">
         <f t="array" ref="E4">_xlfn.CONCAT(IF(A4="completion", "Completion", IF(A4="cassette", "Cassette", IF(A4="gemheart", "Crystal Heart", IF(A4="strawberry", _xlfn.CONCAT("Strawberry ", D4+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B4)*(regions!$B$2:$B$27=C4), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Cassette (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Cassette (Chapter 2: Old Site A-Side)</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -639,22 +642,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <f>COUNTIFS($A$2:A5, A5, $B$2:B5, B5, $C$2:C5, C5) - 1</f>
+        <f>COUNTIFS($A$3:A5, A5, $B$3:B5, B5, $C$3:C5, C5) - 1</f>
         <v>0</v>
       </c>
       <c r="E5" t="str" cm="1">
         <f t="array" ref="E5">_xlfn.CONCAT(IF(A5="completion", "Completion", IF(A5="cassette", "Cassette", IF(A5="gemheart", "Crystal Heart", IF(A5="strawberry", _xlfn.CONCAT("Strawberry ", D5+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B5)*(regions!$B$2:$B$27=C5), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Cassette (Chapter 3: Celestial Resort A-Side)</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -662,22 +665,22 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <f>COUNTIFS($A$2:A6, A6, $B$2:B6, B6, $C$2:C6, C6) - 1</f>
+        <f>COUNTIFS($A$3:A6, A6, $B$3:B6, B6, $C$3:C6, C6) - 1</f>
         <v>0</v>
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.CONCAT(IF(A6="completion", "Completion", IF(A6="cassette", "Cassette", IF(A6="gemheart", "Crystal Heart", IF(A6="strawberry", _xlfn.CONCAT("Strawberry ", D6+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B6)*(regions!$B$2:$B$27=C6), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Cassette (Chapter 4: Golden Ridge A-Side)</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -685,22 +688,22 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f>COUNTIFS($A$2:A7, A7, $B$2:B7, B7, $C$2:C7, C7) - 1</f>
+        <f>COUNTIFS($A$3:A7, A7, $B$3:B7, B7, $C$3:C7, C7) - 1</f>
         <v>0</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xlfn.CONCAT(IF(A7="completion", "Completion", IF(A7="cassette", "Cassette", IF(A7="gemheart", "Crystal Heart", IF(A7="strawberry", _xlfn.CONCAT("Strawberry ", D7+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B7)*(regions!$B$2:$B$27=C7), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 6: Reflection A-Side)</v>
+        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 6: Reflection A-Side)</v>
+        <v>Cassette (Chapter 5: Mirror Temple A-Side)</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -708,22 +711,22 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <f>COUNTIFS($A$2:A8, A8, $B$2:B8, B8, $C$2:C8, C8) - 1</f>
+        <f>COUNTIFS($A$3:A8, A8, $B$3:B8, B8, $C$3:C8, C8) - 1</f>
         <v>0</v>
       </c>
       <c r="E8" t="str" cm="1">
         <f t="array" ref="E8">_xlfn.CONCAT(IF(A8="completion", "Completion", IF(A8="cassette", "Cassette", IF(A8="gemheart", "Crystal Heart", IF(A8="strawberry", _xlfn.CONCAT("Strawberry ", D8+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B8)*(regions!$B$2:$B$27=C8), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 7: The Summit A-Side)</v>
+        <v>Cassette (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 7: The Summit A-Side)</v>
+        <v>Cassette (Chapter 6: Reflection A-Side)</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -731,45 +734,45 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <f>COUNTIFS($A$2:A9, A9, $B$2:B9, B9, $C$2:C9, C9) - 1</f>
+        <f>COUNTIFS($A$3:A9, A9, $B$3:B9, B9, $C$3:C9, C9) - 1</f>
         <v>0</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xlfn.CONCAT(IF(A9="completion", "Completion", IF(A9="cassette", "Cassette", IF(A9="gemheart", "Crystal Heart", IF(A9="strawberry", _xlfn.CONCAT("Strawberry ", D9+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B9)*(regions!$B$2:$B$27=C9), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Cassette (Chapter 8: Core A-Side)</v>
+        <v>Cassette (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>Cassette (Chapter 8: Core A-Side)</v>
+        <v>Cassette (Chapter 7: The Summit A-Side)</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <f>COUNTIFS($A$2:A10, A10, $B$2:B10, B10, $C$2:C10, C10) - 1</f>
+        <f>COUNTIFS($A$3:A10, A10, $B$3:B10, B10, $C$3:C10, C10) - 1</f>
         <v>0</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10">_xlfn.CONCAT(IF(A10="completion", "Completion", IF(A10="cassette", "Cassette", IF(A10="gemheart", "Crystal Heart", IF(A10="strawberry", _xlfn.CONCAT("Strawberry ", D10+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B10)*(regions!$B$2:$B$27=C10), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
+        <v>Cassette (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
+        <v>Cassette (Chapter 8: Core A-Side)</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,22 +780,22 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <f>COUNTIFS($A$2:A11, A11, $B$2:B11, B11, $C$2:C11, C11) - 1</f>
+        <f>COUNTIFS($A$3:A11, A11, $B$3:B11, B11, $C$3:C11, C11) - 1</f>
         <v>0</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xlfn.CONCAT(IF(A11="completion", "Completion", IF(A11="cassette", "Cassette", IF(A11="gemheart", "Crystal Heart", IF(A11="strawberry", _xlfn.CONCAT("Strawberry ", D11+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B11)*(regions!$B$2:$B$27=C11), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 2: Old Site A-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 2: Old Site A-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City A-Side)</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -800,22 +803,22 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <f>COUNTIFS($A$2:A12, A12, $B$2:B12, B12, $C$2:C12, C12) - 1</f>
+        <f>COUNTIFS($A$3:A12, A12, $B$3:B12, B12, $C$3:C12, C12) - 1</f>
         <v>0</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" ref="E12">_xlfn.CONCAT(IF(A12="completion", "Completion", IF(A12="cassette", "Cassette", IF(A12="gemheart", "Crystal Heart", IF(A12="strawberry", _xlfn.CONCAT("Strawberry ", D12+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B12)*(regions!$B$2:$B$27=C12), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Completion (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Completion (Chapter 2: Old Site A-Side)</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,22 +826,22 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <f>COUNTIFS($A$2:A13, A13, $B$2:B13, B13, $C$2:C13, C13) - 1</f>
+        <f>COUNTIFS($A$3:A13, A13, $B$3:B13, B13, $C$3:C13, C13) - 1</f>
         <v>0</v>
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xlfn.CONCAT(IF(A13="completion", "Completion", IF(A13="cassette", "Cassette", IF(A13="gemheart", "Crystal Heart", IF(A13="strawberry", _xlfn.CONCAT("Strawberry ", D13+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B13)*(regions!$B$2:$B$27=C13), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort A-Side)</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -846,22 +849,22 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <f>COUNTIFS($A$2:A14, A14, $B$2:B14, B14, $C$2:C14, C14) - 1</f>
+        <f>COUNTIFS($A$3:A14, A14, $B$3:B14, B14, $C$3:C14, C14) - 1</f>
         <v>0</v>
       </c>
       <c r="E14" t="str" cm="1">
         <f t="array" ref="E14">_xlfn.CONCAT(IF(A14="completion", "Completion", IF(A14="cassette", "Cassette", IF(A14="gemheart", "Crystal Heart", IF(A14="strawberry", _xlfn.CONCAT("Strawberry ", D14+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B14)*(regions!$B$2:$B$27=C14), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge A-Side)</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -869,22 +872,22 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f>COUNTIFS($A$2:A15, A15, $B$2:B15, B15, $C$2:C15, C15) - 1</f>
+        <f>COUNTIFS($A$3:A15, A15, $B$3:B15, B15, $C$3:C15, C15) - 1</f>
         <v>0</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xlfn.CONCAT(IF(A15="completion", "Completion", IF(A15="cassette", "Cassette", IF(A15="gemheart", "Crystal Heart", IF(A15="strawberry", _xlfn.CONCAT("Strawberry ", D15+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B15)*(regions!$B$2:$B$27=C15), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 6: Reflection A-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 6: Reflection A-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple A-Side)</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -892,22 +895,22 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f>COUNTIFS($A$2:A16, A16, $B$2:B16, B16, $C$2:C16, C16) - 1</f>
+        <f>COUNTIFS($A$3:A16, A16, $B$3:B16, B16, $C$3:C16, C16) - 1</f>
         <v>0</v>
       </c>
       <c r="E16" t="str" cm="1">
         <f t="array" ref="E16">_xlfn.CONCAT(IF(A16="completion", "Completion", IF(A16="cassette", "Cassette", IF(A16="gemheart", "Crystal Heart", IF(A16="strawberry", _xlfn.CONCAT("Strawberry ", D16+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B16)*(regions!$B$2:$B$27=C16), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 7: The Summit A-Side)</v>
+        <v>Completion (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 7: The Summit A-Side)</v>
+        <v>Completion (Chapter 6: Reflection A-Side)</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,22 +918,22 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f>COUNTIFS($A$2:A17, A17, $B$2:B17, B17, $C$2:C17, C17) - 1</f>
+        <f>COUNTIFS($A$3:A17, A17, $B$3:B17, B17, $C$3:C17, C17) - 1</f>
         <v>0</v>
       </c>
       <c r="E17" t="str" cm="1">
         <f t="array" ref="E17">_xlfn.CONCAT(IF(A17="completion", "Completion", IF(A17="cassette", "Cassette", IF(A17="gemheart", "Crystal Heart", IF(A17="strawberry", _xlfn.CONCAT("Strawberry ", D17+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B17)*(regions!$B$2:$B$27=C17), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Epilogue)</v>
+        <v>Completion (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Epilogue)</v>
+        <v>Completion (Chapter 7: The Summit A-Side)</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -938,22 +941,22 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <f>COUNTIFS($A$2:A18, A18, $B$2:B18, B18, $C$2:C18, C18) - 1</f>
+        <f>COUNTIFS($A$3:A18, A18, $B$3:B18, B18, $C$3:C18, C18) - 1</f>
         <v>0</v>
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" ref="E18">_xlfn.CONCAT(IF(A18="completion", "Completion", IF(A18="cassette", "Cassette", IF(A18="gemheart", "Crystal Heart", IF(A18="strawberry", _xlfn.CONCAT("Strawberry ", D18+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B18)*(regions!$B$2:$B$27=C18), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 8: Core A-Side)</v>
+        <v>Completion (Epilogue)</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 8: Core A-Side)</v>
+        <v>Completion (Epilogue)</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,22 +964,22 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f>COUNTIFS($A$2:A19, A19, $B$2:B19, B19, $C$2:C19, C19) - 1</f>
+        <f>COUNTIFS($A$3:A19, A19, $B$3:B19, B19, $C$3:C19, C19) - 1</f>
         <v>0</v>
       </c>
       <c r="E19" t="str" cm="1">
         <f t="array" ref="E19">_xlfn.CONCAT(IF(A19="completion", "Completion", IF(A19="cassette", "Cassette", IF(A19="gemheart", "Crystal Heart", IF(A19="strawberry", _xlfn.CONCAT("Strawberry ", D19+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B19)*(regions!$B$2:$B$27=C19), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 9: Farewell A-Side)</v>
+        <v>Completion (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 9: Farewell A-Side)</v>
+        <v>Completion (Chapter 8: Core A-Side)</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -984,22 +987,22 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f>COUNTIFS($A$2:A20, A20, $B$2:B20, B20, $C$2:C20, C20) - 1</f>
+        <f>COUNTIFS($A$3:A20, A20, $B$3:B20, B20, $C$3:C20, C20) - 1</f>
         <v>0</v>
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.CONCAT(IF(A20="completion", "Completion", IF(A20="cassette", "Cassette", IF(A20="gemheart", "Crystal Heart", IF(A20="strawberry", _xlfn.CONCAT("Strawberry ", D20+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B20)*(regions!$B$2:$B$27=C20), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
+        <v>Completion (Chapter 9: Farewell A-Side)</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
+        <v>Completion (Chapter 9: Farewell A-Side)</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1007,22 +1010,22 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <f>COUNTIFS($A$2:A21, A21, $B$2:B21, B21, $C$2:C21, C21) - 1</f>
+        <f>COUNTIFS($A$3:A21, A21, $B$3:B21, B21, $C$3:C21, C21) - 1</f>
         <v>0</v>
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.CONCAT(IF(A21="completion", "Completion", IF(A21="cassette", "Cassette", IF(A21="gemheart", "Crystal Heart", IF(A21="strawberry", _xlfn.CONCAT("Strawberry ", D21+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B21)*(regions!$B$2:$B$27=C21), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 2: Old Site B-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 2: Old Site B-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City B-Side)</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,22 +1033,22 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <f>COUNTIFS($A$2:A22, A22, $B$2:B22, B22, $C$2:C22, C22) - 1</f>
+        <f>COUNTIFS($A$3:A22, A22, $B$3:B22, B22, $C$3:C22, C22) - 1</f>
         <v>0</v>
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.CONCAT(IF(A22="completion", "Completion", IF(A22="cassette", "Cassette", IF(A22="gemheart", "Crystal Heart", IF(A22="strawberry", _xlfn.CONCAT("Strawberry ", D22+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B22)*(regions!$B$2:$B$27=C22), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Completion (Chapter 2: Old Site B-Side)</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Completion (Chapter 2: Old Site B-Side)</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1053,22 +1056,22 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <f>COUNTIFS($A$2:A23, A23, $B$2:B23, B23, $C$2:C23, C23) - 1</f>
+        <f>COUNTIFS($A$3:A23, A23, $B$3:B23, B23, $C$3:C23, C23) - 1</f>
         <v>0</v>
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.CONCAT(IF(A23="completion", "Completion", IF(A23="cassette", "Cassette", IF(A23="gemheart", "Crystal Heart", IF(A23="strawberry", _xlfn.CONCAT("Strawberry ", D23+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B23)*(regions!$B$2:$B$27=C23), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort B-Side)</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1076,22 +1079,22 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <f>COUNTIFS($A$2:A24, A24, $B$2:B24, B24, $C$2:C24, C24) - 1</f>
+        <f>COUNTIFS($A$3:A24, A24, $B$3:B24, B24, $C$3:C24, C24) - 1</f>
         <v>0</v>
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.CONCAT(IF(A24="completion", "Completion", IF(A24="cassette", "Cassette", IF(A24="gemheart", "Crystal Heart", IF(A24="strawberry", _xlfn.CONCAT("Strawberry ", D24+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B24)*(regions!$B$2:$B$27=C24), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge B-Side)</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1099,22 +1102,22 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <f>COUNTIFS($A$2:A25, A25, $B$2:B25, B25, $C$2:C25, C25) - 1</f>
+        <f>COUNTIFS($A$3:A25, A25, $B$3:B25, B25, $C$3:C25, C25) - 1</f>
         <v>0</v>
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.CONCAT(IF(A25="completion", "Completion", IF(A25="cassette", "Cassette", IF(A25="gemheart", "Crystal Heart", IF(A25="strawberry", _xlfn.CONCAT("Strawberry ", D25+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B25)*(regions!$B$2:$B$27=C25), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 6: Reflection B-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 6: Reflection B-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple B-Side)</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1122,22 +1125,22 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <f>COUNTIFS($A$2:A26, A26, $B$2:B26, B26, $C$2:C26, C26) - 1</f>
+        <f>COUNTIFS($A$3:A26, A26, $B$3:B26, B26, $C$3:C26, C26) - 1</f>
         <v>0</v>
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.CONCAT(IF(A26="completion", "Completion", IF(A26="cassette", "Cassette", IF(A26="gemheart", "Crystal Heart", IF(A26="strawberry", _xlfn.CONCAT("Strawberry ", D26+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B26)*(regions!$B$2:$B$27=C26), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 7: The Summit B-Side)</v>
+        <v>Completion (Chapter 6: Reflection B-Side)</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 7: The Summit B-Side)</v>
+        <v>Completion (Chapter 6: Reflection B-Side)</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1145,22 +1148,22 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <f>COUNTIFS($A$2:A27, A27, $B$2:B27, B27, $C$2:C27, C27) - 1</f>
+        <f>COUNTIFS($A$3:A27, A27, $B$3:B27, B27, $C$3:C27, C27) - 1</f>
         <v>0</v>
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.CONCAT(IF(A27="completion", "Completion", IF(A27="cassette", "Cassette", IF(A27="gemheart", "Crystal Heart", IF(A27="strawberry", _xlfn.CONCAT("Strawberry ", D27+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B27)*(regions!$B$2:$B$27=C27), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 8: Core B-Side)</v>
+        <v>Completion (Chapter 7: The Summit B-Side)</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 8: Core B-Side)</v>
+        <v>Completion (Chapter 7: The Summit B-Side)</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1168,22 +1171,22 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <f>COUNTIFS($A$2:A28, A28, $B$2:B28, B28, $C$2:C28, C28) - 1</f>
+        <f>COUNTIFS($A$3:A28, A28, $B$3:B28, B28, $C$3:C28, C28) - 1</f>
         <v>0</v>
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.CONCAT(IF(A28="completion", "Completion", IF(A28="cassette", "Cassette", IF(A28="gemheart", "Crystal Heart", IF(A28="strawberry", _xlfn.CONCAT("Strawberry ", D28+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B28)*(regions!$B$2:$B$27=C28), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
+        <v>Completion (Chapter 8: Core B-Side)</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
+        <v>Completion (Chapter 8: Core B-Side)</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,22 +1194,22 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29">
-        <f>COUNTIFS($A$2:A29, A29, $B$2:B29, B29, $C$2:C29, C29) - 1</f>
+        <f>COUNTIFS($A$3:A29, A29, $B$3:B29, B29, $C$3:C29, C29) - 1</f>
         <v>0</v>
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.CONCAT(IF(A29="completion", "Completion", IF(A29="cassette", "Cassette", IF(A29="gemheart", "Crystal Heart", IF(A29="strawberry", _xlfn.CONCAT("Strawberry ", D29+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B29)*(regions!$B$2:$B$27=C29), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 2: Old Site C-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 2: Old Site C-Side)</v>
+        <v>Completion (Chapter 1: Forsaken City C-Side)</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1214,22 +1217,22 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30">
-        <f>COUNTIFS($A$2:A30, A30, $B$2:B30, B30, $C$2:C30, C30) - 1</f>
+        <f>COUNTIFS($A$3:A30, A30, $B$3:B30, B30, $C$3:C30, C30) - 1</f>
         <v>0</v>
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.CONCAT(IF(A30="completion", "Completion", IF(A30="cassette", "Cassette", IF(A30="gemheart", "Crystal Heart", IF(A30="strawberry", _xlfn.CONCAT("Strawberry ", D30+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B30)*(regions!$B$2:$B$27=C30), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Completion (Chapter 2: Old Site C-Side)</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Completion (Chapter 2: Old Site C-Side)</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,22 +1240,22 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31">
-        <f>COUNTIFS($A$2:A31, A31, $B$2:B31, B31, $C$2:C31, C31) - 1</f>
+        <f>COUNTIFS($A$3:A31, A31, $B$3:B31, B31, $C$3:C31, C31) - 1</f>
         <v>0</v>
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.CONCAT(IF(A31="completion", "Completion", IF(A31="cassette", "Cassette", IF(A31="gemheart", "Crystal Heart", IF(A31="strawberry", _xlfn.CONCAT("Strawberry ", D31+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B31)*(regions!$B$2:$B$27=C31), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Completion (Chapter 3: Celestial Resort C-Side)</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1260,22 +1263,22 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32">
-        <f>COUNTIFS($A$2:A32, A32, $B$2:B32, B32, $C$2:C32, C32) - 1</f>
+        <f>COUNTIFS($A$3:A32, A32, $B$3:B32, B32, $C$3:C32, C32) - 1</f>
         <v>0</v>
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.CONCAT(IF(A32="completion", "Completion", IF(A32="cassette", "Cassette", IF(A32="gemheart", "Crystal Heart", IF(A32="strawberry", _xlfn.CONCAT("Strawberry ", D32+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B32)*(regions!$B$2:$B$27=C32), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Completion (Chapter 4: Golden Ridge C-Side)</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1283,22 +1286,22 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33">
-        <f>COUNTIFS($A$2:A33, A33, $B$2:B33, B33, $C$2:C33, C33) - 1</f>
+        <f>COUNTIFS($A$3:A33, A33, $B$3:B33, B33, $C$3:C33, C33) - 1</f>
         <v>0</v>
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.CONCAT(IF(A33="completion", "Completion", IF(A33="cassette", "Cassette", IF(A33="gemheart", "Crystal Heart", IF(A33="strawberry", _xlfn.CONCAT("Strawberry ", D33+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B33)*(regions!$B$2:$B$27=C33), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 6: Reflection C-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 6: Reflection C-Side)</v>
+        <v>Completion (Chapter 5: Mirror Temple C-Side)</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1306,22 +1309,22 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <f>COUNTIFS($A$2:A34, A34, $B$2:B34, B34, $C$2:C34, C34) - 1</f>
+        <f>COUNTIFS($A$3:A34, A34, $B$3:B34, B34, $C$3:C34, C34) - 1</f>
         <v>0</v>
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.CONCAT(IF(A34="completion", "Completion", IF(A34="cassette", "Cassette", IF(A34="gemheart", "Crystal Heart", IF(A34="strawberry", _xlfn.CONCAT("Strawberry ", D34+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B34)*(regions!$B$2:$B$27=C34), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 7: The Summit C-Side)</v>
+        <v>Completion (Chapter 6: Reflection C-Side)</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 7: The Summit C-Side)</v>
+        <v>Completion (Chapter 6: Reflection C-Side)</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1329,45 +1332,45 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35">
-        <f>COUNTIFS($A$2:A35, A35, $B$2:B35, B35, $C$2:C35, C35) - 1</f>
+        <f>COUNTIFS($A$3:A35, A35, $B$3:B35, B35, $C$3:C35, C35) - 1</f>
         <v>0</v>
       </c>
       <c r="E35" t="str" cm="1">
         <f t="array" ref="E35">_xlfn.CONCAT(IF(A35="completion", "Completion", IF(A35="cassette", "Cassette", IF(A35="gemheart", "Crystal Heart", IF(A35="strawberry", _xlfn.CONCAT("Strawberry ", D35+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B35)*(regions!$B$2:$B$27=C35), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Completion (Chapter 8: Core C-Side)</v>
+        <v>Completion (Chapter 7: The Summit C-Side)</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>Completion (Chapter 8: Core C-Side)</v>
+        <v>Completion (Chapter 7: The Summit C-Side)</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <f>COUNTIFS($A$2:A36, A36, $B$2:B36, B36, $C$2:C36, C36) - 1</f>
+        <f>COUNTIFS($A$3:A36, A36, $B$3:B36, B36, $C$3:C36, C36) - 1</f>
         <v>0</v>
       </c>
       <c r="E36" t="str" cm="1">
         <f t="array" ref="E36">_xlfn.CONCAT(IF(A36="completion", "Completion", IF(A36="cassette", "Cassette", IF(A36="gemheart", "Crystal Heart", IF(A36="strawberry", _xlfn.CONCAT("Strawberry ", D36+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B36)*(regions!$B$2:$B$27=C36), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
+        <v>Completion (Chapter 8: Core C-Side)</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
+        <v>Completion (Chapter 8: Core C-Side)</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1375,22 +1378,22 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <f>COUNTIFS($A$2:A37, A37, $B$2:B37, B37, $C$2:C37, C37) - 1</f>
+        <f>COUNTIFS($A$3:A37, A37, $B$3:B37, B37, $C$3:C37, C37) - 1</f>
         <v>0</v>
       </c>
       <c r="E37" t="str" cm="1">
         <f t="array" ref="E37">_xlfn.CONCAT(IF(A37="completion", "Completion", IF(A37="cassette", "Cassette", IF(A37="gemheart", "Crystal Heart", IF(A37="strawberry", _xlfn.CONCAT("Strawberry ", D37+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B37)*(regions!$B$2:$B$27=C37), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City A-Side)</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1398,22 +1401,22 @@
         <v>5</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <f>COUNTIFS($A$2:A38, A38, $B$2:B38, B38, $C$2:C38, C38) - 1</f>
+        <f>COUNTIFS($A$3:A38, A38, $B$3:B38, B38, $C$3:C38, C38) - 1</f>
         <v>0</v>
       </c>
       <c r="E38" t="str" cm="1">
         <f t="array" ref="E38">_xlfn.CONCAT(IF(A38="completion", "Completion", IF(A38="cassette", "Cassette", IF(A38="gemheart", "Crystal Heart", IF(A38="strawberry", _xlfn.CONCAT("Strawberry ", D38+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B38)*(regions!$B$2:$B$27=C38), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site A-Side)</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1421,22 +1424,22 @@
         <v>5</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <f>COUNTIFS($A$2:A39, A39, $B$2:B39, B39, $C$2:C39, C39) - 1</f>
+        <f>COUNTIFS($A$3:A39, A39, $B$3:B39, B39, $C$3:C39, C39) - 1</f>
         <v>0</v>
       </c>
       <c r="E39" t="str" cm="1">
         <f t="array" ref="E39">_xlfn.CONCAT(IF(A39="completion", "Completion", IF(A39="cassette", "Cassette", IF(A39="gemheart", "Crystal Heart", IF(A39="strawberry", _xlfn.CONCAT("Strawberry ", D39+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B39)*(regions!$B$2:$B$27=C39), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort A-Side)</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1444,22 +1447,22 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <f>COUNTIFS($A$2:A40, A40, $B$2:B40, B40, $C$2:C40, C40) - 1</f>
+        <f>COUNTIFS($A$3:A40, A40, $B$3:B40, B40, $C$3:C40, C40) - 1</f>
         <v>0</v>
       </c>
       <c r="E40" t="str" cm="1">
         <f t="array" ref="E40">_xlfn.CONCAT(IF(A40="completion", "Completion", IF(A40="cassette", "Cassette", IF(A40="gemheart", "Crystal Heart", IF(A40="strawberry", _xlfn.CONCAT("Strawberry ", D40+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B40)*(regions!$B$2:$B$27=C40), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge A-Side)</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1467,22 +1470,22 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <f>COUNTIFS($A$2:A41, A41, $B$2:B41, B41, $C$2:C41, C41) - 1</f>
+        <f>COUNTIFS($A$3:A41, A41, $B$3:B41, B41, $C$3:C41, C41) - 1</f>
         <v>0</v>
       </c>
       <c r="E41" t="str" cm="1">
         <f t="array" ref="E41">_xlfn.CONCAT(IF(A41="completion", "Completion", IF(A41="cassette", "Cassette", IF(A41="gemheart", "Crystal Heart", IF(A41="strawberry", _xlfn.CONCAT("Strawberry ", D41+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B41)*(regions!$B$2:$B$27=C41), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple A-Side)</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1490,22 +1493,22 @@
         <v>5</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <f>COUNTIFS($A$2:A42, A42, $B$2:B42, B42, $C$2:C42, C42) - 1</f>
+        <f>COUNTIFS($A$3:A42, A42, $B$3:B42, B42, $C$3:C42, C42) - 1</f>
         <v>0</v>
       </c>
       <c r="E42" t="str" cm="1">
         <f t="array" ref="E42">_xlfn.CONCAT(IF(A42="completion", "Completion", IF(A42="cassette", "Cassette", IF(A42="gemheart", "Crystal Heart", IF(A42="strawberry", _xlfn.CONCAT("Strawberry ", D42+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B42)*(regions!$B$2:$B$27=C42), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection A-Side)</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,22 +1516,22 @@
         <v>5</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <f>COUNTIFS($A$2:A43, A43, $B$2:B43, B43, $C$2:C43, C43) - 1</f>
+        <f>COUNTIFS($A$3:A43, A43, $B$3:B43, B43, $C$3:C43, C43) - 1</f>
         <v>0</v>
       </c>
       <c r="E43" t="str" cm="1">
         <f t="array" ref="E43">_xlfn.CONCAT(IF(A43="completion", "Completion", IF(A43="cassette", "Cassette", IF(A43="gemheart", "Crystal Heart", IF(A43="strawberry", _xlfn.CONCAT("Strawberry ", D43+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B43)*(regions!$B$2:$B$27=C43), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit A-Side)</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1536,22 +1539,22 @@
         <v>5</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <f>COUNTIFS($A$2:A44, A44, $B$2:B44, B44, $C$2:C44, C44) - 1</f>
+        <f>COUNTIFS($A$3:A44, A44, $B$3:B44, B44, $C$3:C44, C44) - 1</f>
         <v>0</v>
       </c>
       <c r="E44" t="str" cm="1">
         <f t="array" ref="E44">_xlfn.CONCAT(IF(A44="completion", "Completion", IF(A44="cassette", "Cassette", IF(A44="gemheart", "Crystal Heart", IF(A44="strawberry", _xlfn.CONCAT("Strawberry ", D44+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B44)*(regions!$B$2:$B$27=C44), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core A-Side)</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1559,22 +1562,22 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <f>COUNTIFS($A$2:A45, A45, $B$2:B45, B45, $C$2:C45, C45) - 1</f>
+        <f>COUNTIFS($A$3:A45, A45, $B$3:B45, B45, $C$3:C45, C45) - 1</f>
         <v>0</v>
       </c>
       <c r="E45" t="str" cm="1">
         <f t="array" ref="E45">_xlfn.CONCAT(IF(A45="completion", "Completion", IF(A45="cassette", "Cassette", IF(A45="gemheart", "Crystal Heart", IF(A45="strawberry", _xlfn.CONCAT("Strawberry ", D45+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B45)*(regions!$B$2:$B$27=C45), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City B-Side)</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1582,22 +1585,22 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <f>COUNTIFS($A$2:A46, A46, $B$2:B46, B46, $C$2:C46, C46) - 1</f>
+        <f>COUNTIFS($A$3:A46, A46, $B$3:B46, B46, $C$3:C46, C46) - 1</f>
         <v>0</v>
       </c>
       <c r="E46" t="str" cm="1">
         <f t="array" ref="E46">_xlfn.CONCAT(IF(A46="completion", "Completion", IF(A46="cassette", "Cassette", IF(A46="gemheart", "Crystal Heart", IF(A46="strawberry", _xlfn.CONCAT("Strawberry ", D46+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B46)*(regions!$B$2:$B$27=C46), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site B-Side)</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1605,22 +1608,22 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <f>COUNTIFS($A$2:A47, A47, $B$2:B47, B47, $C$2:C47, C47) - 1</f>
+        <f>COUNTIFS($A$3:A47, A47, $B$3:B47, B47, $C$3:C47, C47) - 1</f>
         <v>0</v>
       </c>
       <c r="E47" t="str" cm="1">
         <f t="array" ref="E47">_xlfn.CONCAT(IF(A47="completion", "Completion", IF(A47="cassette", "Cassette", IF(A47="gemheart", "Crystal Heart", IF(A47="strawberry", _xlfn.CONCAT("Strawberry ", D47+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B47)*(regions!$B$2:$B$27=C47), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort B-Side)</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1628,22 +1631,22 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <f>COUNTIFS($A$2:A48, A48, $B$2:B48, B48, $C$2:C48, C48) - 1</f>
+        <f>COUNTIFS($A$3:A48, A48, $B$3:B48, B48, $C$3:C48, C48) - 1</f>
         <v>0</v>
       </c>
       <c r="E48" t="str" cm="1">
         <f t="array" ref="E48">_xlfn.CONCAT(IF(A48="completion", "Completion", IF(A48="cassette", "Cassette", IF(A48="gemheart", "Crystal Heart", IF(A48="strawberry", _xlfn.CONCAT("Strawberry ", D48+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B48)*(regions!$B$2:$B$27=C48), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge B-Side)</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,22 +1654,22 @@
         <v>5</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <f>COUNTIFS($A$2:A49, A49, $B$2:B49, B49, $C$2:C49, C49) - 1</f>
+        <f>COUNTIFS($A$3:A49, A49, $B$3:B49, B49, $C$3:C49, C49) - 1</f>
         <v>0</v>
       </c>
       <c r="E49" t="str" cm="1">
         <f t="array" ref="E49">_xlfn.CONCAT(IF(A49="completion", "Completion", IF(A49="cassette", "Cassette", IF(A49="gemheart", "Crystal Heart", IF(A49="strawberry", _xlfn.CONCAT("Strawberry ", D49+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B49)*(regions!$B$2:$B$27=C49), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple B-Side)</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1674,22 +1677,22 @@
         <v>5</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <f>COUNTIFS($A$2:A50, A50, $B$2:B50, B50, $C$2:C50, C50) - 1</f>
+        <f>COUNTIFS($A$3:A50, A50, $B$3:B50, B50, $C$3:C50, C50) - 1</f>
         <v>0</v>
       </c>
       <c r="E50" t="str" cm="1">
         <f t="array" ref="E50">_xlfn.CONCAT(IF(A50="completion", "Completion", IF(A50="cassette", "Cassette", IF(A50="gemheart", "Crystal Heart", IF(A50="strawberry", _xlfn.CONCAT("Strawberry ", D50+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B50)*(regions!$B$2:$B$27=C50), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection B-Side)</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1697,22 +1700,22 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <f>COUNTIFS($A$2:A51, A51, $B$2:B51, B51, $C$2:C51, C51) - 1</f>
+        <f>COUNTIFS($A$3:A51, A51, $B$3:B51, B51, $C$3:C51, C51) - 1</f>
         <v>0</v>
       </c>
       <c r="E51" t="str" cm="1">
         <f t="array" ref="E51">_xlfn.CONCAT(IF(A51="completion", "Completion", IF(A51="cassette", "Cassette", IF(A51="gemheart", "Crystal Heart", IF(A51="strawberry", _xlfn.CONCAT("Strawberry ", D51+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B51)*(regions!$B$2:$B$27=C51), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit B-Side)</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1720,22 +1723,22 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <f>COUNTIFS($A$2:A52, A52, $B$2:B52, B52, $C$2:C52, C52) - 1</f>
+        <f>COUNTIFS($A$3:A52, A52, $B$3:B52, B52, $C$3:C52, C52) - 1</f>
         <v>0</v>
       </c>
       <c r="E52" t="str" cm="1">
         <f t="array" ref="E52">_xlfn.CONCAT(IF(A52="completion", "Completion", IF(A52="cassette", "Cassette", IF(A52="gemheart", "Crystal Heart", IF(A52="strawberry", _xlfn.CONCAT("Strawberry ", D52+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B52)*(regions!$B$2:$B$27=C52), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core B-Side)</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1743,22 +1746,22 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <f>COUNTIFS($A$2:A53, A53, $B$2:B53, B53, $C$2:C53, C53) - 1</f>
+        <f>COUNTIFS($A$3:A53, A53, $B$3:B53, B53, $C$3:C53, C53) - 1</f>
         <v>0</v>
       </c>
       <c r="E53" t="str" cm="1">
         <f t="array" ref="E53">_xlfn.CONCAT(IF(A53="completion", "Completion", IF(A53="cassette", "Cassette", IF(A53="gemheart", "Crystal Heart", IF(A53="strawberry", _xlfn.CONCAT("Strawberry ", D53+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B53)*(regions!$B$2:$B$27=C53), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
+        <v>Crystal Heart (Chapter 1: Forsaken City C-Side)</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,22 +1769,22 @@
         <v>5</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54">
-        <f>COUNTIFS($A$2:A54, A54, $B$2:B54, B54, $C$2:C54, C54) - 1</f>
+        <f>COUNTIFS($A$3:A54, A54, $B$3:B54, B54, $C$3:C54, C54) - 1</f>
         <v>0</v>
       </c>
       <c r="E54" t="str" cm="1">
         <f t="array" ref="E54">_xlfn.CONCAT(IF(A54="completion", "Completion", IF(A54="cassette", "Cassette", IF(A54="gemheart", "Crystal Heart", IF(A54="strawberry", _xlfn.CONCAT("Strawberry ", D54+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B54)*(regions!$B$2:$B$27=C54), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
+        <v>Crystal Heart (Chapter 2: Old Site C-Side)</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1789,22 +1792,22 @@
         <v>5</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C55">
         <v>2</v>
       </c>
       <c r="D55">
-        <f>COUNTIFS($A$2:A55, A55, $B$2:B55, B55, $C$2:C55, C55) - 1</f>
+        <f>COUNTIFS($A$3:A55, A55, $B$3:B55, B55, $C$3:C55, C55) - 1</f>
         <v>0</v>
       </c>
       <c r="E55" t="str" cm="1">
         <f t="array" ref="E55">_xlfn.CONCAT(IF(A55="completion", "Completion", IF(A55="cassette", "Cassette", IF(A55="gemheart", "Crystal Heart", IF(A55="strawberry", _xlfn.CONCAT("Strawberry ", D55+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B55)*(regions!$B$2:$B$27=C55), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
+        <v>Crystal Heart (Chapter 3: Celestial Resort C-Side)</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1812,22 +1815,22 @@
         <v>5</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
       <c r="D56">
-        <f>COUNTIFS($A$2:A56, A56, $B$2:B56, B56, $C$2:C56, C56) - 1</f>
+        <f>COUNTIFS($A$3:A56, A56, $B$3:B56, B56, $C$3:C56, C56) - 1</f>
         <v>0</v>
       </c>
       <c r="E56" t="str" cm="1">
         <f t="array" ref="E56">_xlfn.CONCAT(IF(A56="completion", "Completion", IF(A56="cassette", "Cassette", IF(A56="gemheart", "Crystal Heart", IF(A56="strawberry", _xlfn.CONCAT("Strawberry ", D56+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B56)*(regions!$B$2:$B$27=C56), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
+        <v>Crystal Heart (Chapter 4: Golden Ridge C-Side)</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1835,22 +1838,22 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="D57">
-        <f>COUNTIFS($A$2:A57, A57, $B$2:B57, B57, $C$2:C57, C57) - 1</f>
+        <f>COUNTIFS($A$3:A57, A57, $B$3:B57, B57, $C$3:C57, C57) - 1</f>
         <v>0</v>
       </c>
       <c r="E57" t="str" cm="1">
         <f t="array" ref="E57">_xlfn.CONCAT(IF(A57="completion", "Completion", IF(A57="cassette", "Cassette", IF(A57="gemheart", "Crystal Heart", IF(A57="strawberry", _xlfn.CONCAT("Strawberry ", D57+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B57)*(regions!$B$2:$B$27=C57), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
+        <v>Crystal Heart (Chapter 5: Mirror Temple C-Side)</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1858,22 +1861,22 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58">
         <v>2</v>
       </c>
       <c r="D58">
-        <f>COUNTIFS($A$2:A58, A58, $B$2:B58, B58, $C$2:C58, C58) - 1</f>
+        <f>COUNTIFS($A$3:A58, A58, $B$3:B58, B58, $C$3:C58, C58) - 1</f>
         <v>0</v>
       </c>
       <c r="E58" t="str" cm="1">
         <f t="array" ref="E58">_xlfn.CONCAT(IF(A58="completion", "Completion", IF(A58="cassette", "Cassette", IF(A58="gemheart", "Crystal Heart", IF(A58="strawberry", _xlfn.CONCAT("Strawberry ", D58+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B58)*(regions!$B$2:$B$27=C58), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
+        <v>Crystal Heart (Chapter 6: Reflection C-Side)</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1881,45 +1884,45 @@
         <v>5</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59">
-        <f>COUNTIFS($A$2:A59, A59, $B$2:B59, B59, $C$2:C59, C59) - 1</f>
+        <f>COUNTIFS($A$3:A59, A59, $B$3:B59, B59, $C$3:C59, C59) - 1</f>
         <v>0</v>
       </c>
       <c r="E59" t="str" cm="1">
         <f t="array" ref="E59">_xlfn.CONCAT(IF(A59="completion", "Completion", IF(A59="cassette", "Cassette", IF(A59="gemheart", "Crystal Heart", IF(A59="strawberry", _xlfn.CONCAT("Strawberry ", D59+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B59)*(regions!$B$2:$B$27=C59), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
+        <v>Crystal Heart (Chapter 7: The Summit C-Side)</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60">
-        <f>COUNTIFS($A$2:A60, A60, $B$2:B60, B60, $C$2:C60, C60) - 1</f>
+        <f>COUNTIFS($A$3:A60, A60, $B$3:B60, B60, $C$3:C60, C60) - 1</f>
         <v>0</v>
       </c>
       <c r="E60" t="str" cm="1">
         <f t="array" ref="E60">_xlfn.CONCAT(IF(A60="completion", "Completion", IF(A60="cassette", "Cassette", IF(A60="gemheart", "Crystal Heart", IF(A60="strawberry", _xlfn.CONCAT("Strawberry ", D60+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B60)*(regions!$B$2:$B$27=C60), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>Strawberry</v>
+        <v>Crystal Heart (Chapter 8: Core C-Side)</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1933,12 +1936,12 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <f>COUNTIFS($A$2:A61, A61, $B$2:B61, B61, $C$2:C61, C61) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A61, A61, $B$3:B61, B61, $C$3:C61, C61) - 1</f>
+        <v>0</v>
       </c>
       <c r="E61" t="str" cm="1">
         <f t="array" ref="E61">_xlfn.CONCAT(IF(A61="completion", "Completion", IF(A61="cassette", "Cassette", IF(A61="gemheart", "Crystal Heart", IF(A61="strawberry", _xlfn.CONCAT("Strawberry ", D61+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B61)*(regions!$B$2:$B$27=C61), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 1 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
@@ -1956,12 +1959,12 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <f>COUNTIFS($A$2:A62, A62, $B$2:B62, B62, $C$2:C62, C62) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A62, A62, $B$3:B62, B62, $C$3:C62, C62) - 1</f>
+        <v>1</v>
       </c>
       <c r="E62" t="str" cm="1">
         <f t="array" ref="E62">_xlfn.CONCAT(IF(A62="completion", "Completion", IF(A62="cassette", "Cassette", IF(A62="gemheart", "Crystal Heart", IF(A62="strawberry", _xlfn.CONCAT("Strawberry ", D62+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B62)*(regions!$B$2:$B$27=C62), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 2 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
@@ -1979,12 +1982,12 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <f>COUNTIFS($A$2:A63, A63, $B$2:B63, B63, $C$2:C63, C63) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A63, A63, $B$3:B63, B63, $C$3:C63, C63) - 1</f>
+        <v>2</v>
       </c>
       <c r="E63" t="str" cm="1">
         <f t="array" ref="E63">_xlfn.CONCAT(IF(A63="completion", "Completion", IF(A63="cassette", "Cassette", IF(A63="gemheart", "Crystal Heart", IF(A63="strawberry", _xlfn.CONCAT("Strawberry ", D63+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B63)*(regions!$B$2:$B$27=C63), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 3 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
@@ -2002,12 +2005,12 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <f>COUNTIFS($A$2:A64, A64, $B$2:B64, B64, $C$2:C64, C64) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A64, A64, $B$3:B64, B64, $C$3:C64, C64) - 1</f>
+        <v>3</v>
       </c>
       <c r="E64" t="str" cm="1">
         <f t="array" ref="E64">_xlfn.CONCAT(IF(A64="completion", "Completion", IF(A64="cassette", "Cassette", IF(A64="gemheart", "Crystal Heart", IF(A64="strawberry", _xlfn.CONCAT("Strawberry ", D64+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B64)*(regions!$B$2:$B$27=C64), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 4 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
@@ -2025,12 +2028,12 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <f>COUNTIFS($A$2:A65, A65, $B$2:B65, B65, $C$2:C65, C65) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A65, A65, $B$3:B65, B65, $C$3:C65, C65) - 1</f>
+        <v>4</v>
       </c>
       <c r="E65" t="str" cm="1">
         <f t="array" ref="E65">_xlfn.CONCAT(IF(A65="completion", "Completion", IF(A65="cassette", "Cassette", IF(A65="gemheart", "Crystal Heart", IF(A65="strawberry", _xlfn.CONCAT("Strawberry ", D65+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B65)*(regions!$B$2:$B$27=C65), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 5 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
@@ -2048,15 +2051,15 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <f>COUNTIFS($A$2:A66, A66, $B$2:B66, B66, $C$2:C66, C66) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A66, A66, $B$3:B66, B66, $C$3:C66, C66) - 1</f>
+        <v>5</v>
       </c>
       <c r="E66" t="str" cm="1">
         <f t="array" ref="E66">_xlfn.CONCAT(IF(A66="completion", "Completion", IF(A66="cassette", "Cassette", IF(A66="gemheart", "Crystal Heart", IF(A66="strawberry", _xlfn.CONCAT("Strawberry ", D66+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B66)*(regions!$B$2:$B$27=C66), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 6 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F129" si="1">IF(A66="strawberry", "Strawberry", E66)</f>
+        <f t="shared" si="0"/>
         <v>Strawberry</v>
       </c>
     </row>
@@ -2071,15 +2074,15 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <f>COUNTIFS($A$2:A67, A67, $B$2:B67, B67, $C$2:C67, C67) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A67, A67, $B$3:B67, B67, $C$3:C67, C67) - 1</f>
+        <v>6</v>
       </c>
       <c r="E67" t="str" cm="1">
         <f t="array" ref="E67">_xlfn.CONCAT(IF(A67="completion", "Completion", IF(A67="cassette", "Cassette", IF(A67="gemheart", "Crystal Heart", IF(A67="strawberry", _xlfn.CONCAT("Strawberry ", D67+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B67)*(regions!$B$2:$B$27=C67), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 7 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F67:F130" si="1">IF(A67="strawberry", "Strawberry", E67)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -2094,12 +2097,12 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <f>COUNTIFS($A$2:A68, A68, $B$2:B68, B68, $C$2:C68, C68) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A68, A68, $B$3:B68, B68, $C$3:C68, C68) - 1</f>
+        <v>7</v>
       </c>
       <c r="E68" t="str" cm="1">
         <f t="array" ref="E68">_xlfn.CONCAT(IF(A68="completion", "Completion", IF(A68="cassette", "Cassette", IF(A68="gemheart", "Crystal Heart", IF(A68="strawberry", _xlfn.CONCAT("Strawberry ", D68+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B68)*(regions!$B$2:$B$27=C68), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 8 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
@@ -2117,12 +2120,12 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f>COUNTIFS($A$2:A69, A69, $B$2:B69, B69, $C$2:C69, C69) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A69, A69, $B$3:B69, B69, $C$3:C69, C69) - 1</f>
+        <v>8</v>
       </c>
       <c r="E69" t="str" cm="1">
         <f t="array" ref="E69">_xlfn.CONCAT(IF(A69="completion", "Completion", IF(A69="cassette", "Cassette", IF(A69="gemheart", "Crystal Heart", IF(A69="strawberry", _xlfn.CONCAT("Strawberry ", D69+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B69)*(regions!$B$2:$B$27=C69), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 9 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
@@ -2140,12 +2143,12 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f>COUNTIFS($A$2:A70, A70, $B$2:B70, B70, $C$2:C70, C70) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A70, A70, $B$3:B70, B70, $C$3:C70, C70) - 1</f>
+        <v>9</v>
       </c>
       <c r="E70" t="str" cm="1">
         <f t="array" ref="E70">_xlfn.CONCAT(IF(A70="completion", "Completion", IF(A70="cassette", "Cassette", IF(A70="gemheart", "Crystal Heart", IF(A70="strawberry", _xlfn.CONCAT("Strawberry ", D70+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B70)*(regions!$B$2:$B$27=C70), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 10 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
@@ -2163,12 +2166,12 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <f>COUNTIFS($A$2:A71, A71, $B$2:B71, B71, $C$2:C71, C71) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A71, A71, $B$3:B71, B71, $C$3:C71, C71) - 1</f>
+        <v>10</v>
       </c>
       <c r="E71" t="str" cm="1">
         <f t="array" ref="E71">_xlfn.CONCAT(IF(A71="completion", "Completion", IF(A71="cassette", "Cassette", IF(A71="gemheart", "Crystal Heart", IF(A71="strawberry", _xlfn.CONCAT("Strawberry ", D71+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B71)*(regions!$B$2:$B$27=C71), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 11 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
@@ -2186,12 +2189,12 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f>COUNTIFS($A$2:A72, A72, $B$2:B72, B72, $C$2:C72, C72) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A72, A72, $B$3:B72, B72, $C$3:C72, C72) - 1</f>
+        <v>11</v>
       </c>
       <c r="E72" t="str" cm="1">
         <f t="array" ref="E72">_xlfn.CONCAT(IF(A72="completion", "Completion", IF(A72="cassette", "Cassette", IF(A72="gemheart", "Crystal Heart", IF(A72="strawberry", _xlfn.CONCAT("Strawberry ", D72+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B72)*(regions!$B$2:$B$27=C72), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 12 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
@@ -2209,12 +2212,12 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <f>COUNTIFS($A$2:A73, A73, $B$2:B73, B73, $C$2:C73, C73) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A73, A73, $B$3:B73, B73, $C$3:C73, C73) - 1</f>
+        <v>12</v>
       </c>
       <c r="E73" t="str" cm="1">
         <f t="array" ref="E73">_xlfn.CONCAT(IF(A73="completion", "Completion", IF(A73="cassette", "Cassette", IF(A73="gemheart", "Crystal Heart", IF(A73="strawberry", _xlfn.CONCAT("Strawberry ", D73+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B73)*(regions!$B$2:$B$27=C73), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 13 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
@@ -2232,12 +2235,12 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <f>COUNTIFS($A$2:A74, A74, $B$2:B74, B74, $C$2:C74, C74) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A74, A74, $B$3:B74, B74, $C$3:C74, C74) - 1</f>
+        <v>13</v>
       </c>
       <c r="E74" t="str" cm="1">
         <f t="array" ref="E74">_xlfn.CONCAT(IF(A74="completion", "Completion", IF(A74="cassette", "Cassette", IF(A74="gemheart", "Crystal Heart", IF(A74="strawberry", _xlfn.CONCAT("Strawberry ", D74+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B74)*(regions!$B$2:$B$27=C74), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 14 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
@@ -2255,12 +2258,12 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <f>COUNTIFS($A$2:A75, A75, $B$2:B75, B75, $C$2:C75, C75) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A75, A75, $B$3:B75, B75, $C$3:C75, C75) - 1</f>
+        <v>14</v>
       </c>
       <c r="E75" t="str" cm="1">
         <f t="array" ref="E75">_xlfn.CONCAT(IF(A75="completion", "Completion", IF(A75="cassette", "Cassette", IF(A75="gemheart", "Crystal Heart", IF(A75="strawberry", _xlfn.CONCAT("Strawberry ", D75+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B75)*(regions!$B$2:$B$27=C75), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 15 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
@@ -2278,12 +2281,12 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <f>COUNTIFS($A$2:A76, A76, $B$2:B76, B76, $C$2:C76, C76) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A76, A76, $B$3:B76, B76, $C$3:C76, C76) - 1</f>
+        <v>15</v>
       </c>
       <c r="E76" t="str" cm="1">
         <f t="array" ref="E76">_xlfn.CONCAT(IF(A76="completion", "Completion", IF(A76="cassette", "Cassette", IF(A76="gemheart", "Crystal Heart", IF(A76="strawberry", _xlfn.CONCAT("Strawberry ", D76+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B76)*(regions!$B$2:$B$27=C76), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 16 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
@@ -2301,12 +2304,12 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <f>COUNTIFS($A$2:A77, A77, $B$2:B77, B77, $C$2:C77, C77) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A77, A77, $B$3:B77, B77, $C$3:C77, C77) - 1</f>
+        <v>16</v>
       </c>
       <c r="E77" t="str" cm="1">
         <f t="array" ref="E77">_xlfn.CONCAT(IF(A77="completion", "Completion", IF(A77="cassette", "Cassette", IF(A77="gemheart", "Crystal Heart", IF(A77="strawberry", _xlfn.CONCAT("Strawberry ", D77+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B77)*(regions!$B$2:$B$27=C77), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 17 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
@@ -2324,12 +2327,12 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <f>COUNTIFS($A$2:A78, A78, $B$2:B78, B78, $C$2:C78, C78) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A78, A78, $B$3:B78, B78, $C$3:C78, C78) - 1</f>
+        <v>17</v>
       </c>
       <c r="E78" t="str" cm="1">
         <f t="array" ref="E78">_xlfn.CONCAT(IF(A78="completion", "Completion", IF(A78="cassette", "Cassette", IF(A78="gemheart", "Crystal Heart", IF(A78="strawberry", _xlfn.CONCAT("Strawberry ", D78+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B78)*(regions!$B$2:$B$27=C78), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 18 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
@@ -2347,12 +2350,12 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <f>COUNTIFS($A$2:A79, A79, $B$2:B79, B79, $C$2:C79, C79) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A79, A79, $B$3:B79, B79, $C$3:C79, C79) - 1</f>
+        <v>18</v>
       </c>
       <c r="E79" t="str" cm="1">
         <f t="array" ref="E79">_xlfn.CONCAT(IF(A79="completion", "Completion", IF(A79="cassette", "Cassette", IF(A79="gemheart", "Crystal Heart", IF(A79="strawberry", _xlfn.CONCAT("Strawberry ", D79+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B79)*(regions!$B$2:$B$27=C79), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 1: Forsaken City A-Side)</v>
+        <v>Strawberry 19 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
@@ -2364,18 +2367,18 @@
         <v>6</v>
       </c>
       <c r="B80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <f>COUNTIFS($A$2:A80, A80, $B$2:B80, B80, $C$2:C80, C80) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A80, A80, $B$3:B80, B80, $C$3:C80, C80) - 1</f>
+        <v>19</v>
       </c>
       <c r="E80" t="str" cm="1">
         <f t="array" ref="E80">_xlfn.CONCAT(IF(A80="completion", "Completion", IF(A80="cassette", "Cassette", IF(A80="gemheart", "Crystal Heart", IF(A80="strawberry", _xlfn.CONCAT("Strawberry ", D80+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B80)*(regions!$B$2:$B$27=C80), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 20 (Chapter 1: Forsaken City A-Side)</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
@@ -2393,12 +2396,12 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <f>COUNTIFS($A$2:A81, A81, $B$2:B81, B81, $C$2:C81, C81) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A81, A81, $B$3:B81, B81, $C$3:C81, C81) - 1</f>
+        <v>0</v>
       </c>
       <c r="E81" t="str" cm="1">
         <f t="array" ref="E81">_xlfn.CONCAT(IF(A81="completion", "Completion", IF(A81="cassette", "Cassette", IF(A81="gemheart", "Crystal Heart", IF(A81="strawberry", _xlfn.CONCAT("Strawberry ", D81+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B81)*(regions!$B$2:$B$27=C81), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 1 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
@@ -2416,12 +2419,12 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <f>COUNTIFS($A$2:A82, A82, $B$2:B82, B82, $C$2:C82, C82) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A82, A82, $B$3:B82, B82, $C$3:C82, C82) - 1</f>
+        <v>1</v>
       </c>
       <c r="E82" t="str" cm="1">
         <f t="array" ref="E82">_xlfn.CONCAT(IF(A82="completion", "Completion", IF(A82="cassette", "Cassette", IF(A82="gemheart", "Crystal Heart", IF(A82="strawberry", _xlfn.CONCAT("Strawberry ", D82+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B82)*(regions!$B$2:$B$27=C82), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 2 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
@@ -2439,12 +2442,12 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <f>COUNTIFS($A$2:A83, A83, $B$2:B83, B83, $C$2:C83, C83) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A83, A83, $B$3:B83, B83, $C$3:C83, C83) - 1</f>
+        <v>2</v>
       </c>
       <c r="E83" t="str" cm="1">
         <f t="array" ref="E83">_xlfn.CONCAT(IF(A83="completion", "Completion", IF(A83="cassette", "Cassette", IF(A83="gemheart", "Crystal Heart", IF(A83="strawberry", _xlfn.CONCAT("Strawberry ", D83+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B83)*(regions!$B$2:$B$27=C83), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 3 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
@@ -2462,12 +2465,12 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <f>COUNTIFS($A$2:A84, A84, $B$2:B84, B84, $C$2:C84, C84) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A84, A84, $B$3:B84, B84, $C$3:C84, C84) - 1</f>
+        <v>3</v>
       </c>
       <c r="E84" t="str" cm="1">
         <f t="array" ref="E84">_xlfn.CONCAT(IF(A84="completion", "Completion", IF(A84="cassette", "Cassette", IF(A84="gemheart", "Crystal Heart", IF(A84="strawberry", _xlfn.CONCAT("Strawberry ", D84+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B84)*(regions!$B$2:$B$27=C84), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 4 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
@@ -2485,12 +2488,12 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <f>COUNTIFS($A$2:A85, A85, $B$2:B85, B85, $C$2:C85, C85) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A85, A85, $B$3:B85, B85, $C$3:C85, C85) - 1</f>
+        <v>4</v>
       </c>
       <c r="E85" t="str" cm="1">
         <f t="array" ref="E85">_xlfn.CONCAT(IF(A85="completion", "Completion", IF(A85="cassette", "Cassette", IF(A85="gemheart", "Crystal Heart", IF(A85="strawberry", _xlfn.CONCAT("Strawberry ", D85+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B85)*(regions!$B$2:$B$27=C85), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 5 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
@@ -2508,12 +2511,12 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <f>COUNTIFS($A$2:A86, A86, $B$2:B86, B86, $C$2:C86, C86) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A86, A86, $B$3:B86, B86, $C$3:C86, C86) - 1</f>
+        <v>5</v>
       </c>
       <c r="E86" t="str" cm="1">
         <f t="array" ref="E86">_xlfn.CONCAT(IF(A86="completion", "Completion", IF(A86="cassette", "Cassette", IF(A86="gemheart", "Crystal Heart", IF(A86="strawberry", _xlfn.CONCAT("Strawberry ", D86+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B86)*(regions!$B$2:$B$27=C86), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 6 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
@@ -2531,12 +2534,12 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <f>COUNTIFS($A$2:A87, A87, $B$2:B87, B87, $C$2:C87, C87) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A87, A87, $B$3:B87, B87, $C$3:C87, C87) - 1</f>
+        <v>6</v>
       </c>
       <c r="E87" t="str" cm="1">
         <f t="array" ref="E87">_xlfn.CONCAT(IF(A87="completion", "Completion", IF(A87="cassette", "Cassette", IF(A87="gemheart", "Crystal Heart", IF(A87="strawberry", _xlfn.CONCAT("Strawberry ", D87+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B87)*(regions!$B$2:$B$27=C87), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 7 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
@@ -2554,12 +2557,12 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <f>COUNTIFS($A$2:A88, A88, $B$2:B88, B88, $C$2:C88, C88) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A88, A88, $B$3:B88, B88, $C$3:C88, C88) - 1</f>
+        <v>7</v>
       </c>
       <c r="E88" t="str" cm="1">
         <f t="array" ref="E88">_xlfn.CONCAT(IF(A88="completion", "Completion", IF(A88="cassette", "Cassette", IF(A88="gemheart", "Crystal Heart", IF(A88="strawberry", _xlfn.CONCAT("Strawberry ", D88+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B88)*(regions!$B$2:$B$27=C88), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 8 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
@@ -2577,12 +2580,12 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <f>COUNTIFS($A$2:A89, A89, $B$2:B89, B89, $C$2:C89, C89) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A89, A89, $B$3:B89, B89, $C$3:C89, C89) - 1</f>
+        <v>8</v>
       </c>
       <c r="E89" t="str" cm="1">
         <f t="array" ref="E89">_xlfn.CONCAT(IF(A89="completion", "Completion", IF(A89="cassette", "Cassette", IF(A89="gemheart", "Crystal Heart", IF(A89="strawberry", _xlfn.CONCAT("Strawberry ", D89+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B89)*(regions!$B$2:$B$27=C89), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 9 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
@@ -2600,12 +2603,12 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <f>COUNTIFS($A$2:A90, A90, $B$2:B90, B90, $C$2:C90, C90) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A90, A90, $B$3:B90, B90, $C$3:C90, C90) - 1</f>
+        <v>9</v>
       </c>
       <c r="E90" t="str" cm="1">
         <f t="array" ref="E90">_xlfn.CONCAT(IF(A90="completion", "Completion", IF(A90="cassette", "Cassette", IF(A90="gemheart", "Crystal Heart", IF(A90="strawberry", _xlfn.CONCAT("Strawberry ", D90+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B90)*(regions!$B$2:$B$27=C90), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 10 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
@@ -2623,12 +2626,12 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <f>COUNTIFS($A$2:A91, A91, $B$2:B91, B91, $C$2:C91, C91) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A91, A91, $B$3:B91, B91, $C$3:C91, C91) - 1</f>
+        <v>10</v>
       </c>
       <c r="E91" t="str" cm="1">
         <f t="array" ref="E91">_xlfn.CONCAT(IF(A91="completion", "Completion", IF(A91="cassette", "Cassette", IF(A91="gemheart", "Crystal Heart", IF(A91="strawberry", _xlfn.CONCAT("Strawberry ", D91+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B91)*(regions!$B$2:$B$27=C91), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 11 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
@@ -2646,12 +2649,12 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <f>COUNTIFS($A$2:A92, A92, $B$2:B92, B92, $C$2:C92, C92) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A92, A92, $B$3:B92, B92, $C$3:C92, C92) - 1</f>
+        <v>11</v>
       </c>
       <c r="E92" t="str" cm="1">
         <f t="array" ref="E92">_xlfn.CONCAT(IF(A92="completion", "Completion", IF(A92="cassette", "Cassette", IF(A92="gemheart", "Crystal Heart", IF(A92="strawberry", _xlfn.CONCAT("Strawberry ", D92+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B92)*(regions!$B$2:$B$27=C92), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 12 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
@@ -2669,12 +2672,12 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <f>COUNTIFS($A$2:A93, A93, $B$2:B93, B93, $C$2:C93, C93) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A93, A93, $B$3:B93, B93, $C$3:C93, C93) - 1</f>
+        <v>12</v>
       </c>
       <c r="E93" t="str" cm="1">
         <f t="array" ref="E93">_xlfn.CONCAT(IF(A93="completion", "Completion", IF(A93="cassette", "Cassette", IF(A93="gemheart", "Crystal Heart", IF(A93="strawberry", _xlfn.CONCAT("Strawberry ", D93+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B93)*(regions!$B$2:$B$27=C93), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 13 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
@@ -2692,12 +2695,12 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <f>COUNTIFS($A$2:A94, A94, $B$2:B94, B94, $C$2:C94, C94) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A94, A94, $B$3:B94, B94, $C$3:C94, C94) - 1</f>
+        <v>13</v>
       </c>
       <c r="E94" t="str" cm="1">
         <f t="array" ref="E94">_xlfn.CONCAT(IF(A94="completion", "Completion", IF(A94="cassette", "Cassette", IF(A94="gemheart", "Crystal Heart", IF(A94="strawberry", _xlfn.CONCAT("Strawberry ", D94+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B94)*(regions!$B$2:$B$27=C94), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 14 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
@@ -2715,12 +2718,12 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <f>COUNTIFS($A$2:A95, A95, $B$2:B95, B95, $C$2:C95, C95) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A95, A95, $B$3:B95, B95, $C$3:C95, C95) - 1</f>
+        <v>14</v>
       </c>
       <c r="E95" t="str" cm="1">
         <f t="array" ref="E95">_xlfn.CONCAT(IF(A95="completion", "Completion", IF(A95="cassette", "Cassette", IF(A95="gemheart", "Crystal Heart", IF(A95="strawberry", _xlfn.CONCAT("Strawberry ", D95+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B95)*(regions!$B$2:$B$27=C95), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 15 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
@@ -2738,12 +2741,12 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <f>COUNTIFS($A$2:A96, A96, $B$2:B96, B96, $C$2:C96, C96) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A96, A96, $B$3:B96, B96, $C$3:C96, C96) - 1</f>
+        <v>15</v>
       </c>
       <c r="E96" t="str" cm="1">
         <f t="array" ref="E96">_xlfn.CONCAT(IF(A96="completion", "Completion", IF(A96="cassette", "Cassette", IF(A96="gemheart", "Crystal Heart", IF(A96="strawberry", _xlfn.CONCAT("Strawberry ", D96+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B96)*(regions!$B$2:$B$27=C96), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 16 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
@@ -2761,12 +2764,12 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <f>COUNTIFS($A$2:A97, A97, $B$2:B97, B97, $C$2:C97, C97) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A97, A97, $B$3:B97, B97, $C$3:C97, C97) - 1</f>
+        <v>16</v>
       </c>
       <c r="E97" t="str" cm="1">
         <f t="array" ref="E97">_xlfn.CONCAT(IF(A97="completion", "Completion", IF(A97="cassette", "Cassette", IF(A97="gemheart", "Crystal Heart", IF(A97="strawberry", _xlfn.CONCAT("Strawberry ", D97+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B97)*(regions!$B$2:$B$27=C97), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 2: Old Site A-Side)</v>
+        <v>Strawberry 17 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
@@ -2778,18 +2781,18 @@
         <v>6</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
-        <f>COUNTIFS($A$2:A98, A98, $B$2:B98, B98, $C$2:C98, C98) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A98, A98, $B$3:B98, B98, $C$3:C98, C98) - 1</f>
+        <v>17</v>
       </c>
       <c r="E98" t="str" cm="1">
         <f t="array" ref="E98">_xlfn.CONCAT(IF(A98="completion", "Completion", IF(A98="cassette", "Cassette", IF(A98="gemheart", "Crystal Heart", IF(A98="strawberry", _xlfn.CONCAT("Strawberry ", D98+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B98)*(regions!$B$2:$B$27=C98), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 18 (Chapter 2: Old Site A-Side)</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
@@ -2807,12 +2810,12 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <f>COUNTIFS($A$2:A99, A99, $B$2:B99, B99, $C$2:C99, C99) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A99, A99, $B$3:B99, B99, $C$3:C99, C99) - 1</f>
+        <v>0</v>
       </c>
       <c r="E99" t="str" cm="1">
         <f t="array" ref="E99">_xlfn.CONCAT(IF(A99="completion", "Completion", IF(A99="cassette", "Cassette", IF(A99="gemheart", "Crystal Heart", IF(A99="strawberry", _xlfn.CONCAT("Strawberry ", D99+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B99)*(regions!$B$2:$B$27=C99), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 1 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
@@ -2830,12 +2833,12 @@
         <v>0</v>
       </c>
       <c r="D100">
-        <f>COUNTIFS($A$2:A100, A100, $B$2:B100, B100, $C$2:C100, C100) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A100, A100, $B$3:B100, B100, $C$3:C100, C100) - 1</f>
+        <v>1</v>
       </c>
       <c r="E100" t="str" cm="1">
         <f t="array" ref="E100">_xlfn.CONCAT(IF(A100="completion", "Completion", IF(A100="cassette", "Cassette", IF(A100="gemheart", "Crystal Heart", IF(A100="strawberry", _xlfn.CONCAT("Strawberry ", D100+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B100)*(regions!$B$2:$B$27=C100), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 2 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
@@ -2853,12 +2856,12 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <f>COUNTIFS($A$2:A101, A101, $B$2:B101, B101, $C$2:C101, C101) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A101, A101, $B$3:B101, B101, $C$3:C101, C101) - 1</f>
+        <v>2</v>
       </c>
       <c r="E101" t="str" cm="1">
         <f t="array" ref="E101">_xlfn.CONCAT(IF(A101="completion", "Completion", IF(A101="cassette", "Cassette", IF(A101="gemheart", "Crystal Heart", IF(A101="strawberry", _xlfn.CONCAT("Strawberry ", D101+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B101)*(regions!$B$2:$B$27=C101), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 3 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
@@ -2876,12 +2879,12 @@
         <v>0</v>
       </c>
       <c r="D102">
-        <f>COUNTIFS($A$2:A102, A102, $B$2:B102, B102, $C$2:C102, C102) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A102, A102, $B$3:B102, B102, $C$3:C102, C102) - 1</f>
+        <v>3</v>
       </c>
       <c r="E102" t="str" cm="1">
         <f t="array" ref="E102">_xlfn.CONCAT(IF(A102="completion", "Completion", IF(A102="cassette", "Cassette", IF(A102="gemheart", "Crystal Heart", IF(A102="strawberry", _xlfn.CONCAT("Strawberry ", D102+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B102)*(regions!$B$2:$B$27=C102), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 4 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
@@ -2899,12 +2902,12 @@
         <v>0</v>
       </c>
       <c r="D103">
-        <f>COUNTIFS($A$2:A103, A103, $B$2:B103, B103, $C$2:C103, C103) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A103, A103, $B$3:B103, B103, $C$3:C103, C103) - 1</f>
+        <v>4</v>
       </c>
       <c r="E103" t="str" cm="1">
         <f t="array" ref="E103">_xlfn.CONCAT(IF(A103="completion", "Completion", IF(A103="cassette", "Cassette", IF(A103="gemheart", "Crystal Heart", IF(A103="strawberry", _xlfn.CONCAT("Strawberry ", D103+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B103)*(regions!$B$2:$B$27=C103), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 5 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
@@ -2922,12 +2925,12 @@
         <v>0</v>
       </c>
       <c r="D104">
-        <f>COUNTIFS($A$2:A104, A104, $B$2:B104, B104, $C$2:C104, C104) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A104, A104, $B$3:B104, B104, $C$3:C104, C104) - 1</f>
+        <v>5</v>
       </c>
       <c r="E104" t="str" cm="1">
         <f t="array" ref="E104">_xlfn.CONCAT(IF(A104="completion", "Completion", IF(A104="cassette", "Cassette", IF(A104="gemheart", "Crystal Heart", IF(A104="strawberry", _xlfn.CONCAT("Strawberry ", D104+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B104)*(regions!$B$2:$B$27=C104), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 6 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
@@ -2945,12 +2948,12 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <f>COUNTIFS($A$2:A105, A105, $B$2:B105, B105, $C$2:C105, C105) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A105, A105, $B$3:B105, B105, $C$3:C105, C105) - 1</f>
+        <v>6</v>
       </c>
       <c r="E105" t="str" cm="1">
         <f t="array" ref="E105">_xlfn.CONCAT(IF(A105="completion", "Completion", IF(A105="cassette", "Cassette", IF(A105="gemheart", "Crystal Heart", IF(A105="strawberry", _xlfn.CONCAT("Strawberry ", D105+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B105)*(regions!$B$2:$B$27=C105), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 7 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
@@ -2968,12 +2971,12 @@
         <v>0</v>
       </c>
       <c r="D106">
-        <f>COUNTIFS($A$2:A106, A106, $B$2:B106, B106, $C$2:C106, C106) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A106, A106, $B$3:B106, B106, $C$3:C106, C106) - 1</f>
+        <v>7</v>
       </c>
       <c r="E106" t="str" cm="1">
         <f t="array" ref="E106">_xlfn.CONCAT(IF(A106="completion", "Completion", IF(A106="cassette", "Cassette", IF(A106="gemheart", "Crystal Heart", IF(A106="strawberry", _xlfn.CONCAT("Strawberry ", D106+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B106)*(regions!$B$2:$B$27=C106), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 8 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
@@ -2991,12 +2994,12 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <f>COUNTIFS($A$2:A107, A107, $B$2:B107, B107, $C$2:C107, C107) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A107, A107, $B$3:B107, B107, $C$3:C107, C107) - 1</f>
+        <v>8</v>
       </c>
       <c r="E107" t="str" cm="1">
         <f t="array" ref="E107">_xlfn.CONCAT(IF(A107="completion", "Completion", IF(A107="cassette", "Cassette", IF(A107="gemheart", "Crystal Heart", IF(A107="strawberry", _xlfn.CONCAT("Strawberry ", D107+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B107)*(regions!$B$2:$B$27=C107), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 9 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
@@ -3014,12 +3017,12 @@
         <v>0</v>
       </c>
       <c r="D108">
-        <f>COUNTIFS($A$2:A108, A108, $B$2:B108, B108, $C$2:C108, C108) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A108, A108, $B$3:B108, B108, $C$3:C108, C108) - 1</f>
+        <v>9</v>
       </c>
       <c r="E108" t="str" cm="1">
         <f t="array" ref="E108">_xlfn.CONCAT(IF(A108="completion", "Completion", IF(A108="cassette", "Cassette", IF(A108="gemheart", "Crystal Heart", IF(A108="strawberry", _xlfn.CONCAT("Strawberry ", D108+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B108)*(regions!$B$2:$B$27=C108), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 10 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
@@ -3037,12 +3040,12 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <f>COUNTIFS($A$2:A109, A109, $B$2:B109, B109, $C$2:C109, C109) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A109, A109, $B$3:B109, B109, $C$3:C109, C109) - 1</f>
+        <v>10</v>
       </c>
       <c r="E109" t="str" cm="1">
         <f t="array" ref="E109">_xlfn.CONCAT(IF(A109="completion", "Completion", IF(A109="cassette", "Cassette", IF(A109="gemheart", "Crystal Heart", IF(A109="strawberry", _xlfn.CONCAT("Strawberry ", D109+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B109)*(regions!$B$2:$B$27=C109), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 11 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
@@ -3060,12 +3063,12 @@
         <v>0</v>
       </c>
       <c r="D110">
-        <f>COUNTIFS($A$2:A110, A110, $B$2:B110, B110, $C$2:C110, C110) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A110, A110, $B$3:B110, B110, $C$3:C110, C110) - 1</f>
+        <v>11</v>
       </c>
       <c r="E110" t="str" cm="1">
         <f t="array" ref="E110">_xlfn.CONCAT(IF(A110="completion", "Completion", IF(A110="cassette", "Cassette", IF(A110="gemheart", "Crystal Heart", IF(A110="strawberry", _xlfn.CONCAT("Strawberry ", D110+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B110)*(regions!$B$2:$B$27=C110), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 12 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
@@ -3083,12 +3086,12 @@
         <v>0</v>
       </c>
       <c r="D111">
-        <f>COUNTIFS($A$2:A111, A111, $B$2:B111, B111, $C$2:C111, C111) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A111, A111, $B$3:B111, B111, $C$3:C111, C111) - 1</f>
+        <v>12</v>
       </c>
       <c r="E111" t="str" cm="1">
         <f t="array" ref="E111">_xlfn.CONCAT(IF(A111="completion", "Completion", IF(A111="cassette", "Cassette", IF(A111="gemheart", "Crystal Heart", IF(A111="strawberry", _xlfn.CONCAT("Strawberry ", D111+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B111)*(regions!$B$2:$B$27=C111), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 13 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
@@ -3106,12 +3109,12 @@
         <v>0</v>
       </c>
       <c r="D112">
-        <f>COUNTIFS($A$2:A112, A112, $B$2:B112, B112, $C$2:C112, C112) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A112, A112, $B$3:B112, B112, $C$3:C112, C112) - 1</f>
+        <v>13</v>
       </c>
       <c r="E112" t="str" cm="1">
         <f t="array" ref="E112">_xlfn.CONCAT(IF(A112="completion", "Completion", IF(A112="cassette", "Cassette", IF(A112="gemheart", "Crystal Heart", IF(A112="strawberry", _xlfn.CONCAT("Strawberry ", D112+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B112)*(regions!$B$2:$B$27=C112), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 14 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
@@ -3129,12 +3132,12 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <f>COUNTIFS($A$2:A113, A113, $B$2:B113, B113, $C$2:C113, C113) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A113, A113, $B$3:B113, B113, $C$3:C113, C113) - 1</f>
+        <v>14</v>
       </c>
       <c r="E113" t="str" cm="1">
         <f t="array" ref="E113">_xlfn.CONCAT(IF(A113="completion", "Completion", IF(A113="cassette", "Cassette", IF(A113="gemheart", "Crystal Heart", IF(A113="strawberry", _xlfn.CONCAT("Strawberry ", D113+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B113)*(regions!$B$2:$B$27=C113), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 15 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
@@ -3152,12 +3155,12 @@
         <v>0</v>
       </c>
       <c r="D114">
-        <f>COUNTIFS($A$2:A114, A114, $B$2:B114, B114, $C$2:C114, C114) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A114, A114, $B$3:B114, B114, $C$3:C114, C114) - 1</f>
+        <v>15</v>
       </c>
       <c r="E114" t="str" cm="1">
         <f t="array" ref="E114">_xlfn.CONCAT(IF(A114="completion", "Completion", IF(A114="cassette", "Cassette", IF(A114="gemheart", "Crystal Heart", IF(A114="strawberry", _xlfn.CONCAT("Strawberry ", D114+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B114)*(regions!$B$2:$B$27=C114), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 16 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
@@ -3175,12 +3178,12 @@
         <v>0</v>
       </c>
       <c r="D115">
-        <f>COUNTIFS($A$2:A115, A115, $B$2:B115, B115, $C$2:C115, C115) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A115, A115, $B$3:B115, B115, $C$3:C115, C115) - 1</f>
+        <v>16</v>
       </c>
       <c r="E115" t="str" cm="1">
         <f t="array" ref="E115">_xlfn.CONCAT(IF(A115="completion", "Completion", IF(A115="cassette", "Cassette", IF(A115="gemheart", "Crystal Heart", IF(A115="strawberry", _xlfn.CONCAT("Strawberry ", D115+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B115)*(regions!$B$2:$B$27=C115), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 17 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
@@ -3198,12 +3201,12 @@
         <v>0</v>
       </c>
       <c r="D116">
-        <f>COUNTIFS($A$2:A116, A116, $B$2:B116, B116, $C$2:C116, C116) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A116, A116, $B$3:B116, B116, $C$3:C116, C116) - 1</f>
+        <v>17</v>
       </c>
       <c r="E116" t="str" cm="1">
         <f t="array" ref="E116">_xlfn.CONCAT(IF(A116="completion", "Completion", IF(A116="cassette", "Cassette", IF(A116="gemheart", "Crystal Heart", IF(A116="strawberry", _xlfn.CONCAT("Strawberry ", D116+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B116)*(regions!$B$2:$B$27=C116), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 18 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
@@ -3221,12 +3224,12 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <f>COUNTIFS($A$2:A117, A117, $B$2:B117, B117, $C$2:C117, C117) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A117, A117, $B$3:B117, B117, $C$3:C117, C117) - 1</f>
+        <v>18</v>
       </c>
       <c r="E117" t="str" cm="1">
         <f t="array" ref="E117">_xlfn.CONCAT(IF(A117="completion", "Completion", IF(A117="cassette", "Cassette", IF(A117="gemheart", "Crystal Heart", IF(A117="strawberry", _xlfn.CONCAT("Strawberry ", D117+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B117)*(regions!$B$2:$B$27=C117), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 19 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
@@ -3244,12 +3247,12 @@
         <v>0</v>
       </c>
       <c r="D118">
-        <f>COUNTIFS($A$2:A118, A118, $B$2:B118, B118, $C$2:C118, C118) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A118, A118, $B$3:B118, B118, $C$3:C118, C118) - 1</f>
+        <v>19</v>
       </c>
       <c r="E118" t="str" cm="1">
         <f t="array" ref="E118">_xlfn.CONCAT(IF(A118="completion", "Completion", IF(A118="cassette", "Cassette", IF(A118="gemheart", "Crystal Heart", IF(A118="strawberry", _xlfn.CONCAT("Strawberry ", D118+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B118)*(regions!$B$2:$B$27=C118), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 20 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="1"/>
@@ -3267,12 +3270,12 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <f>COUNTIFS($A$2:A119, A119, $B$2:B119, B119, $C$2:C119, C119) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A119, A119, $B$3:B119, B119, $C$3:C119, C119) - 1</f>
+        <v>20</v>
       </c>
       <c r="E119" t="str" cm="1">
         <f t="array" ref="E119">_xlfn.CONCAT(IF(A119="completion", "Completion", IF(A119="cassette", "Cassette", IF(A119="gemheart", "Crystal Heart", IF(A119="strawberry", _xlfn.CONCAT("Strawberry ", D119+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B119)*(regions!$B$2:$B$27=C119), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 21 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="1"/>
@@ -3290,12 +3293,12 @@
         <v>0</v>
       </c>
       <c r="D120">
-        <f>COUNTIFS($A$2:A120, A120, $B$2:B120, B120, $C$2:C120, C120) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A120, A120, $B$3:B120, B120, $C$3:C120, C120) - 1</f>
+        <v>21</v>
       </c>
       <c r="E120" t="str" cm="1">
         <f t="array" ref="E120">_xlfn.CONCAT(IF(A120="completion", "Completion", IF(A120="cassette", "Cassette", IF(A120="gemheart", "Crystal Heart", IF(A120="strawberry", _xlfn.CONCAT("Strawberry ", D120+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B120)*(regions!$B$2:$B$27=C120), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 22 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="1"/>
@@ -3313,12 +3316,12 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <f>COUNTIFS($A$2:A121, A121, $B$2:B121, B121, $C$2:C121, C121) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A121, A121, $B$3:B121, B121, $C$3:C121, C121) - 1</f>
+        <v>22</v>
       </c>
       <c r="E121" t="str" cm="1">
         <f t="array" ref="E121">_xlfn.CONCAT(IF(A121="completion", "Completion", IF(A121="cassette", "Cassette", IF(A121="gemheart", "Crystal Heart", IF(A121="strawberry", _xlfn.CONCAT("Strawberry ", D121+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B121)*(regions!$B$2:$B$27=C121), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 23 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="1"/>
@@ -3336,12 +3339,12 @@
         <v>0</v>
       </c>
       <c r="D122">
-        <f>COUNTIFS($A$2:A122, A122, $B$2:B122, B122, $C$2:C122, C122) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A122, A122, $B$3:B122, B122, $C$3:C122, C122) - 1</f>
+        <v>23</v>
       </c>
       <c r="E122" t="str" cm="1">
         <f t="array" ref="E122">_xlfn.CONCAT(IF(A122="completion", "Completion", IF(A122="cassette", "Cassette", IF(A122="gemheart", "Crystal Heart", IF(A122="strawberry", _xlfn.CONCAT("Strawberry ", D122+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B122)*(regions!$B$2:$B$27=C122), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 3: Celestial Resort A-Side)</v>
+        <v>Strawberry 24 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
@@ -3353,18 +3356,18 @@
         <v>6</v>
       </c>
       <c r="B123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C123">
         <v>0</v>
       </c>
       <c r="D123">
-        <f>COUNTIFS($A$2:A123, A123, $B$2:B123, B123, $C$2:C123, C123) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A123, A123, $B$3:B123, B123, $C$3:C123, C123) - 1</f>
+        <v>24</v>
       </c>
       <c r="E123" t="str" cm="1">
         <f t="array" ref="E123">_xlfn.CONCAT(IF(A123="completion", "Completion", IF(A123="cassette", "Cassette", IF(A123="gemheart", "Crystal Heart", IF(A123="strawberry", _xlfn.CONCAT("Strawberry ", D123+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B123)*(regions!$B$2:$B$27=C123), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 25 (Chapter 3: Celestial Resort A-Side)</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
@@ -3382,12 +3385,12 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <f>COUNTIFS($A$2:A124, A124, $B$2:B124, B124, $C$2:C124, C124) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A124, A124, $B$3:B124, B124, $C$3:C124, C124) - 1</f>
+        <v>0</v>
       </c>
       <c r="E124" t="str" cm="1">
         <f t="array" ref="E124">_xlfn.CONCAT(IF(A124="completion", "Completion", IF(A124="cassette", "Cassette", IF(A124="gemheart", "Crystal Heart", IF(A124="strawberry", _xlfn.CONCAT("Strawberry ", D124+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B124)*(regions!$B$2:$B$27=C124), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 1 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
@@ -3405,12 +3408,12 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <f>COUNTIFS($A$2:A125, A125, $B$2:B125, B125, $C$2:C125, C125) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A125, A125, $B$3:B125, B125, $C$3:C125, C125) - 1</f>
+        <v>1</v>
       </c>
       <c r="E125" t="str" cm="1">
         <f t="array" ref="E125">_xlfn.CONCAT(IF(A125="completion", "Completion", IF(A125="cassette", "Cassette", IF(A125="gemheart", "Crystal Heart", IF(A125="strawberry", _xlfn.CONCAT("Strawberry ", D125+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B125)*(regions!$B$2:$B$27=C125), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 2 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="1"/>
@@ -3428,12 +3431,12 @@
         <v>0</v>
       </c>
       <c r="D126">
-        <f>COUNTIFS($A$2:A126, A126, $B$2:B126, B126, $C$2:C126, C126) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A126, A126, $B$3:B126, B126, $C$3:C126, C126) - 1</f>
+        <v>2</v>
       </c>
       <c r="E126" t="str" cm="1">
         <f t="array" ref="E126">_xlfn.CONCAT(IF(A126="completion", "Completion", IF(A126="cassette", "Cassette", IF(A126="gemheart", "Crystal Heart", IF(A126="strawberry", _xlfn.CONCAT("Strawberry ", D126+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B126)*(regions!$B$2:$B$27=C126), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 3 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="1"/>
@@ -3451,12 +3454,12 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <f>COUNTIFS($A$2:A127, A127, $B$2:B127, B127, $C$2:C127, C127) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A127, A127, $B$3:B127, B127, $C$3:C127, C127) - 1</f>
+        <v>3</v>
       </c>
       <c r="E127" t="str" cm="1">
         <f t="array" ref="E127">_xlfn.CONCAT(IF(A127="completion", "Completion", IF(A127="cassette", "Cassette", IF(A127="gemheart", "Crystal Heart", IF(A127="strawberry", _xlfn.CONCAT("Strawberry ", D127+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B127)*(regions!$B$2:$B$27=C127), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 4 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="1"/>
@@ -3474,12 +3477,12 @@
         <v>0</v>
       </c>
       <c r="D128">
-        <f>COUNTIFS($A$2:A128, A128, $B$2:B128, B128, $C$2:C128, C128) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A128, A128, $B$3:B128, B128, $C$3:C128, C128) - 1</f>
+        <v>4</v>
       </c>
       <c r="E128" t="str" cm="1">
         <f t="array" ref="E128">_xlfn.CONCAT(IF(A128="completion", "Completion", IF(A128="cassette", "Cassette", IF(A128="gemheart", "Crystal Heart", IF(A128="strawberry", _xlfn.CONCAT("Strawberry ", D128+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B128)*(regions!$B$2:$B$27=C128), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 5 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
@@ -3497,12 +3500,12 @@
         <v>0</v>
       </c>
       <c r="D129">
-        <f>COUNTIFS($A$2:A129, A129, $B$2:B129, B129, $C$2:C129, C129) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A129, A129, $B$3:B129, B129, $C$3:C129, C129) - 1</f>
+        <v>5</v>
       </c>
       <c r="E129" t="str" cm="1">
         <f t="array" ref="E129">_xlfn.CONCAT(IF(A129="completion", "Completion", IF(A129="cassette", "Cassette", IF(A129="gemheart", "Crystal Heart", IF(A129="strawberry", _xlfn.CONCAT("Strawberry ", D129+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B129)*(regions!$B$2:$B$27=C129), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 6 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="1"/>
@@ -3520,15 +3523,15 @@
         <v>0</v>
       </c>
       <c r="D130">
-        <f>COUNTIFS($A$2:A130, A130, $B$2:B130, B130, $C$2:C130, C130) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A130, A130, $B$3:B130, B130, $C$3:C130, C130) - 1</f>
+        <v>6</v>
       </c>
       <c r="E130" t="str" cm="1">
         <f t="array" ref="E130">_xlfn.CONCAT(IF(A130="completion", "Completion", IF(A130="cassette", "Cassette", IF(A130="gemheart", "Crystal Heart", IF(A130="strawberry", _xlfn.CONCAT("Strawberry ", D130+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B130)*(regions!$B$2:$B$27=C130), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 7 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" ref="F130:F193" si="2">IF(A130="strawberry", "Strawberry", E130)</f>
+        <f t="shared" si="1"/>
         <v>Strawberry</v>
       </c>
     </row>
@@ -3543,15 +3546,15 @@
         <v>0</v>
       </c>
       <c r="D131">
-        <f>COUNTIFS($A$2:A131, A131, $B$2:B131, B131, $C$2:C131, C131) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A131, A131, $B$3:B131, B131, $C$3:C131, C131) - 1</f>
+        <v>7</v>
       </c>
       <c r="E131" t="str" cm="1">
         <f t="array" ref="E131">_xlfn.CONCAT(IF(A131="completion", "Completion", IF(A131="cassette", "Cassette", IF(A131="gemheart", "Crystal Heart", IF(A131="strawberry", _xlfn.CONCAT("Strawberry ", D131+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B131)*(regions!$B$2:$B$27=C131), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 8 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F131:F194" si="2">IF(A131="strawberry", "Strawberry", E131)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -3566,12 +3569,12 @@
         <v>0</v>
       </c>
       <c r="D132">
-        <f>COUNTIFS($A$2:A132, A132, $B$2:B132, B132, $C$2:C132, C132) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A132, A132, $B$3:B132, B132, $C$3:C132, C132) - 1</f>
+        <v>8</v>
       </c>
       <c r="E132" t="str" cm="1">
         <f t="array" ref="E132">_xlfn.CONCAT(IF(A132="completion", "Completion", IF(A132="cassette", "Cassette", IF(A132="gemheart", "Crystal Heart", IF(A132="strawberry", _xlfn.CONCAT("Strawberry ", D132+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B132)*(regions!$B$2:$B$27=C132), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 9 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F132" t="str">
         <f t="shared" si="2"/>
@@ -3589,12 +3592,12 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <f>COUNTIFS($A$2:A133, A133, $B$2:B133, B133, $C$2:C133, C133) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A133, A133, $B$3:B133, B133, $C$3:C133, C133) - 1</f>
+        <v>9</v>
       </c>
       <c r="E133" t="str" cm="1">
         <f t="array" ref="E133">_xlfn.CONCAT(IF(A133="completion", "Completion", IF(A133="cassette", "Cassette", IF(A133="gemheart", "Crystal Heart", IF(A133="strawberry", _xlfn.CONCAT("Strawberry ", D133+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B133)*(regions!$B$2:$B$27=C133), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 10 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="2"/>
@@ -3612,12 +3615,12 @@
         <v>0</v>
       </c>
       <c r="D134">
-        <f>COUNTIFS($A$2:A134, A134, $B$2:B134, B134, $C$2:C134, C134) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A134, A134, $B$3:B134, B134, $C$3:C134, C134) - 1</f>
+        <v>10</v>
       </c>
       <c r="E134" t="str" cm="1">
         <f t="array" ref="E134">_xlfn.CONCAT(IF(A134="completion", "Completion", IF(A134="cassette", "Cassette", IF(A134="gemheart", "Crystal Heart", IF(A134="strawberry", _xlfn.CONCAT("Strawberry ", D134+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B134)*(regions!$B$2:$B$27=C134), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 11 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F134" t="str">
         <f t="shared" si="2"/>
@@ -3635,12 +3638,12 @@
         <v>0</v>
       </c>
       <c r="D135">
-        <f>COUNTIFS($A$2:A135, A135, $B$2:B135, B135, $C$2:C135, C135) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A135, A135, $B$3:B135, B135, $C$3:C135, C135) - 1</f>
+        <v>11</v>
       </c>
       <c r="E135" t="str" cm="1">
         <f t="array" ref="E135">_xlfn.CONCAT(IF(A135="completion", "Completion", IF(A135="cassette", "Cassette", IF(A135="gemheart", "Crystal Heart", IF(A135="strawberry", _xlfn.CONCAT("Strawberry ", D135+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B135)*(regions!$B$2:$B$27=C135), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 12 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="2"/>
@@ -3658,12 +3661,12 @@
         <v>0</v>
       </c>
       <c r="D136">
-        <f>COUNTIFS($A$2:A136, A136, $B$2:B136, B136, $C$2:C136, C136) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A136, A136, $B$3:B136, B136, $C$3:C136, C136) - 1</f>
+        <v>12</v>
       </c>
       <c r="E136" t="str" cm="1">
         <f t="array" ref="E136">_xlfn.CONCAT(IF(A136="completion", "Completion", IF(A136="cassette", "Cassette", IF(A136="gemheart", "Crystal Heart", IF(A136="strawberry", _xlfn.CONCAT("Strawberry ", D136+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B136)*(regions!$B$2:$B$27=C136), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 13 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="2"/>
@@ -3681,12 +3684,12 @@
         <v>0</v>
       </c>
       <c r="D137">
-        <f>COUNTIFS($A$2:A137, A137, $B$2:B137, B137, $C$2:C137, C137) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A137, A137, $B$3:B137, B137, $C$3:C137, C137) - 1</f>
+        <v>13</v>
       </c>
       <c r="E137" t="str" cm="1">
         <f t="array" ref="E137">_xlfn.CONCAT(IF(A137="completion", "Completion", IF(A137="cassette", "Cassette", IF(A137="gemheart", "Crystal Heart", IF(A137="strawberry", _xlfn.CONCAT("Strawberry ", D137+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B137)*(regions!$B$2:$B$27=C137), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 14 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="2"/>
@@ -3704,12 +3707,12 @@
         <v>0</v>
       </c>
       <c r="D138">
-        <f>COUNTIFS($A$2:A138, A138, $B$2:B138, B138, $C$2:C138, C138) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A138, A138, $B$3:B138, B138, $C$3:C138, C138) - 1</f>
+        <v>14</v>
       </c>
       <c r="E138" t="str" cm="1">
         <f t="array" ref="E138">_xlfn.CONCAT(IF(A138="completion", "Completion", IF(A138="cassette", "Cassette", IF(A138="gemheart", "Crystal Heart", IF(A138="strawberry", _xlfn.CONCAT("Strawberry ", D138+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B138)*(regions!$B$2:$B$27=C138), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 15 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="2"/>
@@ -3727,12 +3730,12 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <f>COUNTIFS($A$2:A139, A139, $B$2:B139, B139, $C$2:C139, C139) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A139, A139, $B$3:B139, B139, $C$3:C139, C139) - 1</f>
+        <v>15</v>
       </c>
       <c r="E139" t="str" cm="1">
         <f t="array" ref="E139">_xlfn.CONCAT(IF(A139="completion", "Completion", IF(A139="cassette", "Cassette", IF(A139="gemheart", "Crystal Heart", IF(A139="strawberry", _xlfn.CONCAT("Strawberry ", D139+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B139)*(regions!$B$2:$B$27=C139), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 16 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F139" t="str">
         <f t="shared" si="2"/>
@@ -3750,12 +3753,12 @@
         <v>0</v>
       </c>
       <c r="D140">
-        <f>COUNTIFS($A$2:A140, A140, $B$2:B140, B140, $C$2:C140, C140) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A140, A140, $B$3:B140, B140, $C$3:C140, C140) - 1</f>
+        <v>16</v>
       </c>
       <c r="E140" t="str" cm="1">
         <f t="array" ref="E140">_xlfn.CONCAT(IF(A140="completion", "Completion", IF(A140="cassette", "Cassette", IF(A140="gemheart", "Crystal Heart", IF(A140="strawberry", _xlfn.CONCAT("Strawberry ", D140+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B140)*(regions!$B$2:$B$27=C140), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 17 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F140" t="str">
         <f t="shared" si="2"/>
@@ -3773,12 +3776,12 @@
         <v>0</v>
       </c>
       <c r="D141">
-        <f>COUNTIFS($A$2:A141, A141, $B$2:B141, B141, $C$2:C141, C141) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A141, A141, $B$3:B141, B141, $C$3:C141, C141) - 1</f>
+        <v>17</v>
       </c>
       <c r="E141" t="str" cm="1">
         <f t="array" ref="E141">_xlfn.CONCAT(IF(A141="completion", "Completion", IF(A141="cassette", "Cassette", IF(A141="gemheart", "Crystal Heart", IF(A141="strawberry", _xlfn.CONCAT("Strawberry ", D141+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B141)*(regions!$B$2:$B$27=C141), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 18 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="2"/>
@@ -3796,12 +3799,12 @@
         <v>0</v>
       </c>
       <c r="D142">
-        <f>COUNTIFS($A$2:A142, A142, $B$2:B142, B142, $C$2:C142, C142) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A142, A142, $B$3:B142, B142, $C$3:C142, C142) - 1</f>
+        <v>18</v>
       </c>
       <c r="E142" t="str" cm="1">
         <f t="array" ref="E142">_xlfn.CONCAT(IF(A142="completion", "Completion", IF(A142="cassette", "Cassette", IF(A142="gemheart", "Crystal Heart", IF(A142="strawberry", _xlfn.CONCAT("Strawberry ", D142+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B142)*(regions!$B$2:$B$27=C142), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 19 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="2"/>
@@ -3819,12 +3822,12 @@
         <v>0</v>
       </c>
       <c r="D143">
-        <f>COUNTIFS($A$2:A143, A143, $B$2:B143, B143, $C$2:C143, C143) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A143, A143, $B$3:B143, B143, $C$3:C143, C143) - 1</f>
+        <v>19</v>
       </c>
       <c r="E143" t="str" cm="1">
         <f t="array" ref="E143">_xlfn.CONCAT(IF(A143="completion", "Completion", IF(A143="cassette", "Cassette", IF(A143="gemheart", "Crystal Heart", IF(A143="strawberry", _xlfn.CONCAT("Strawberry ", D143+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B143)*(regions!$B$2:$B$27=C143), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 20 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="2"/>
@@ -3842,12 +3845,12 @@
         <v>0</v>
       </c>
       <c r="D144">
-        <f>COUNTIFS($A$2:A144, A144, $B$2:B144, B144, $C$2:C144, C144) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A144, A144, $B$3:B144, B144, $C$3:C144, C144) - 1</f>
+        <v>20</v>
       </c>
       <c r="E144" t="str" cm="1">
         <f t="array" ref="E144">_xlfn.CONCAT(IF(A144="completion", "Completion", IF(A144="cassette", "Cassette", IF(A144="gemheart", "Crystal Heart", IF(A144="strawberry", _xlfn.CONCAT("Strawberry ", D144+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B144)*(regions!$B$2:$B$27=C144), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 21 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="2"/>
@@ -3865,12 +3868,12 @@
         <v>0</v>
       </c>
       <c r="D145">
-        <f>COUNTIFS($A$2:A145, A145, $B$2:B145, B145, $C$2:C145, C145) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A145, A145, $B$3:B145, B145, $C$3:C145, C145) - 1</f>
+        <v>21</v>
       </c>
       <c r="E145" t="str" cm="1">
         <f t="array" ref="E145">_xlfn.CONCAT(IF(A145="completion", "Completion", IF(A145="cassette", "Cassette", IF(A145="gemheart", "Crystal Heart", IF(A145="strawberry", _xlfn.CONCAT("Strawberry ", D145+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B145)*(regions!$B$2:$B$27=C145), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 22 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="2"/>
@@ -3888,12 +3891,12 @@
         <v>0</v>
       </c>
       <c r="D146">
-        <f>COUNTIFS($A$2:A146, A146, $B$2:B146, B146, $C$2:C146, C146) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A146, A146, $B$3:B146, B146, $C$3:C146, C146) - 1</f>
+        <v>22</v>
       </c>
       <c r="E146" t="str" cm="1">
         <f t="array" ref="E146">_xlfn.CONCAT(IF(A146="completion", "Completion", IF(A146="cassette", "Cassette", IF(A146="gemheart", "Crystal Heart", IF(A146="strawberry", _xlfn.CONCAT("Strawberry ", D146+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B146)*(regions!$B$2:$B$27=C146), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 23 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="2"/>
@@ -3911,12 +3914,12 @@
         <v>0</v>
       </c>
       <c r="D147">
-        <f>COUNTIFS($A$2:A147, A147, $B$2:B147, B147, $C$2:C147, C147) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A147, A147, $B$3:B147, B147, $C$3:C147, C147) - 1</f>
+        <v>23</v>
       </c>
       <c r="E147" t="str" cm="1">
         <f t="array" ref="E147">_xlfn.CONCAT(IF(A147="completion", "Completion", IF(A147="cassette", "Cassette", IF(A147="gemheart", "Crystal Heart", IF(A147="strawberry", _xlfn.CONCAT("Strawberry ", D147+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B147)*(regions!$B$2:$B$27=C147), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 24 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F147" t="str">
         <f t="shared" si="2"/>
@@ -3934,12 +3937,12 @@
         <v>0</v>
       </c>
       <c r="D148">
-        <f>COUNTIFS($A$2:A148, A148, $B$2:B148, B148, $C$2:C148, C148) - 1</f>
-        <v>25</v>
+        <f>COUNTIFS($A$3:A148, A148, $B$3:B148, B148, $C$3:C148, C148) - 1</f>
+        <v>24</v>
       </c>
       <c r="E148" t="str" cm="1">
         <f t="array" ref="E148">_xlfn.CONCAT(IF(A148="completion", "Completion", IF(A148="cassette", "Cassette", IF(A148="gemheart", "Crystal Heart", IF(A148="strawberry", _xlfn.CONCAT("Strawberry ", D148+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B148)*(regions!$B$2:$B$27=C148), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 26 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 25 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F148" t="str">
         <f t="shared" si="2"/>
@@ -3957,12 +3960,12 @@
         <v>0</v>
       </c>
       <c r="D149">
-        <f>COUNTIFS($A$2:A149, A149, $B$2:B149, B149, $C$2:C149, C149) - 1</f>
-        <v>26</v>
+        <f>COUNTIFS($A$3:A149, A149, $B$3:B149, B149, $C$3:C149, C149) - 1</f>
+        <v>25</v>
       </c>
       <c r="E149" t="str" cm="1">
         <f t="array" ref="E149">_xlfn.CONCAT(IF(A149="completion", "Completion", IF(A149="cassette", "Cassette", IF(A149="gemheart", "Crystal Heart", IF(A149="strawberry", _xlfn.CONCAT("Strawberry ", D149+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B149)*(regions!$B$2:$B$27=C149), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 27 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 26 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F149" t="str">
         <f t="shared" si="2"/>
@@ -3980,12 +3983,12 @@
         <v>0</v>
       </c>
       <c r="D150">
-        <f>COUNTIFS($A$2:A150, A150, $B$2:B150, B150, $C$2:C150, C150) - 1</f>
-        <v>27</v>
+        <f>COUNTIFS($A$3:A150, A150, $B$3:B150, B150, $C$3:C150, C150) - 1</f>
+        <v>26</v>
       </c>
       <c r="E150" t="str" cm="1">
         <f t="array" ref="E150">_xlfn.CONCAT(IF(A150="completion", "Completion", IF(A150="cassette", "Cassette", IF(A150="gemheart", "Crystal Heart", IF(A150="strawberry", _xlfn.CONCAT("Strawberry ", D150+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B150)*(regions!$B$2:$B$27=C150), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 28 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 27 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F150" t="str">
         <f t="shared" si="2"/>
@@ -4003,12 +4006,12 @@
         <v>0</v>
       </c>
       <c r="D151">
-        <f>COUNTIFS($A$2:A151, A151, $B$2:B151, B151, $C$2:C151, C151) - 1</f>
-        <v>28</v>
+        <f>COUNTIFS($A$3:A151, A151, $B$3:B151, B151, $C$3:C151, C151) - 1</f>
+        <v>27</v>
       </c>
       <c r="E151" t="str" cm="1">
         <f t="array" ref="E151">_xlfn.CONCAT(IF(A151="completion", "Completion", IF(A151="cassette", "Cassette", IF(A151="gemheart", "Crystal Heart", IF(A151="strawberry", _xlfn.CONCAT("Strawberry ", D151+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B151)*(regions!$B$2:$B$27=C151), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 29 (Chapter 4: Golden Ridge A-Side)</v>
+        <v>Strawberry 28 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F151" t="str">
         <f t="shared" si="2"/>
@@ -4020,18 +4023,18 @@
         <v>6</v>
       </c>
       <c r="B152">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152">
         <v>0</v>
       </c>
       <c r="D152">
-        <f>COUNTIFS($A$2:A152, A152, $B$2:B152, B152, $C$2:C152, C152) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A152, A152, $B$3:B152, B152, $C$3:C152, C152) - 1</f>
+        <v>28</v>
       </c>
       <c r="E152" t="str" cm="1">
         <f t="array" ref="E152">_xlfn.CONCAT(IF(A152="completion", "Completion", IF(A152="cassette", "Cassette", IF(A152="gemheart", "Crystal Heart", IF(A152="strawberry", _xlfn.CONCAT("Strawberry ", D152+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B152)*(regions!$B$2:$B$27=C152), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 29 (Chapter 4: Golden Ridge A-Side)</v>
       </c>
       <c r="F152" t="str">
         <f t="shared" si="2"/>
@@ -4049,12 +4052,12 @@
         <v>0</v>
       </c>
       <c r="D153">
-        <f>COUNTIFS($A$2:A153, A153, $B$2:B153, B153, $C$2:C153, C153) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A153, A153, $B$3:B153, B153, $C$3:C153, C153) - 1</f>
+        <v>0</v>
       </c>
       <c r="E153" t="str" cm="1">
         <f t="array" ref="E153">_xlfn.CONCAT(IF(A153="completion", "Completion", IF(A153="cassette", "Cassette", IF(A153="gemheart", "Crystal Heart", IF(A153="strawberry", _xlfn.CONCAT("Strawberry ", D153+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B153)*(regions!$B$2:$B$27=C153), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 1 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F153" t="str">
         <f t="shared" si="2"/>
@@ -4072,12 +4075,12 @@
         <v>0</v>
       </c>
       <c r="D154">
-        <f>COUNTIFS($A$2:A154, A154, $B$2:B154, B154, $C$2:C154, C154) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A154, A154, $B$3:B154, B154, $C$3:C154, C154) - 1</f>
+        <v>1</v>
       </c>
       <c r="E154" t="str" cm="1">
         <f t="array" ref="E154">_xlfn.CONCAT(IF(A154="completion", "Completion", IF(A154="cassette", "Cassette", IF(A154="gemheart", "Crystal Heart", IF(A154="strawberry", _xlfn.CONCAT("Strawberry ", D154+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B154)*(regions!$B$2:$B$27=C154), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 2 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F154" t="str">
         <f t="shared" si="2"/>
@@ -4095,12 +4098,12 @@
         <v>0</v>
       </c>
       <c r="D155">
-        <f>COUNTIFS($A$2:A155, A155, $B$2:B155, B155, $C$2:C155, C155) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A155, A155, $B$3:B155, B155, $C$3:C155, C155) - 1</f>
+        <v>2</v>
       </c>
       <c r="E155" t="str" cm="1">
         <f t="array" ref="E155">_xlfn.CONCAT(IF(A155="completion", "Completion", IF(A155="cassette", "Cassette", IF(A155="gemheart", "Crystal Heart", IF(A155="strawberry", _xlfn.CONCAT("Strawberry ", D155+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B155)*(regions!$B$2:$B$27=C155), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 3 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F155" t="str">
         <f t="shared" si="2"/>
@@ -4118,12 +4121,12 @@
         <v>0</v>
       </c>
       <c r="D156">
-        <f>COUNTIFS($A$2:A156, A156, $B$2:B156, B156, $C$2:C156, C156) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A156, A156, $B$3:B156, B156, $C$3:C156, C156) - 1</f>
+        <v>3</v>
       </c>
       <c r="E156" t="str" cm="1">
         <f t="array" ref="E156">_xlfn.CONCAT(IF(A156="completion", "Completion", IF(A156="cassette", "Cassette", IF(A156="gemheart", "Crystal Heart", IF(A156="strawberry", _xlfn.CONCAT("Strawberry ", D156+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B156)*(regions!$B$2:$B$27=C156), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 4 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F156" t="str">
         <f t="shared" si="2"/>
@@ -4141,12 +4144,12 @@
         <v>0</v>
       </c>
       <c r="D157">
-        <f>COUNTIFS($A$2:A157, A157, $B$2:B157, B157, $C$2:C157, C157) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A157, A157, $B$3:B157, B157, $C$3:C157, C157) - 1</f>
+        <v>4</v>
       </c>
       <c r="E157" t="str" cm="1">
         <f t="array" ref="E157">_xlfn.CONCAT(IF(A157="completion", "Completion", IF(A157="cassette", "Cassette", IF(A157="gemheart", "Crystal Heart", IF(A157="strawberry", _xlfn.CONCAT("Strawberry ", D157+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B157)*(regions!$B$2:$B$27=C157), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 5 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="2"/>
@@ -4164,12 +4167,12 @@
         <v>0</v>
       </c>
       <c r="D158">
-        <f>COUNTIFS($A$2:A158, A158, $B$2:B158, B158, $C$2:C158, C158) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A158, A158, $B$3:B158, B158, $C$3:C158, C158) - 1</f>
+        <v>5</v>
       </c>
       <c r="E158" t="str" cm="1">
         <f t="array" ref="E158">_xlfn.CONCAT(IF(A158="completion", "Completion", IF(A158="cassette", "Cassette", IF(A158="gemheart", "Crystal Heart", IF(A158="strawberry", _xlfn.CONCAT("Strawberry ", D158+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B158)*(regions!$B$2:$B$27=C158), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 6 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="2"/>
@@ -4187,12 +4190,12 @@
         <v>0</v>
       </c>
       <c r="D159">
-        <f>COUNTIFS($A$2:A159, A159, $B$2:B159, B159, $C$2:C159, C159) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A159, A159, $B$3:B159, B159, $C$3:C159, C159) - 1</f>
+        <v>6</v>
       </c>
       <c r="E159" t="str" cm="1">
         <f t="array" ref="E159">_xlfn.CONCAT(IF(A159="completion", "Completion", IF(A159="cassette", "Cassette", IF(A159="gemheart", "Crystal Heart", IF(A159="strawberry", _xlfn.CONCAT("Strawberry ", D159+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B159)*(regions!$B$2:$B$27=C159), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 7 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="2"/>
@@ -4210,12 +4213,12 @@
         <v>0</v>
       </c>
       <c r="D160">
-        <f>COUNTIFS($A$2:A160, A160, $B$2:B160, B160, $C$2:C160, C160) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A160, A160, $B$3:B160, B160, $C$3:C160, C160) - 1</f>
+        <v>7</v>
       </c>
       <c r="E160" t="str" cm="1">
         <f t="array" ref="E160">_xlfn.CONCAT(IF(A160="completion", "Completion", IF(A160="cassette", "Cassette", IF(A160="gemheart", "Crystal Heart", IF(A160="strawberry", _xlfn.CONCAT("Strawberry ", D160+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B160)*(regions!$B$2:$B$27=C160), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 8 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F160" t="str">
         <f t="shared" si="2"/>
@@ -4233,12 +4236,12 @@
         <v>0</v>
       </c>
       <c r="D161">
-        <f>COUNTIFS($A$2:A161, A161, $B$2:B161, B161, $C$2:C161, C161) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A161, A161, $B$3:B161, B161, $C$3:C161, C161) - 1</f>
+        <v>8</v>
       </c>
       <c r="E161" t="str" cm="1">
         <f t="array" ref="E161">_xlfn.CONCAT(IF(A161="completion", "Completion", IF(A161="cassette", "Cassette", IF(A161="gemheart", "Crystal Heart", IF(A161="strawberry", _xlfn.CONCAT("Strawberry ", D161+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B161)*(regions!$B$2:$B$27=C161), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 9 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F161" t="str">
         <f t="shared" si="2"/>
@@ -4256,12 +4259,12 @@
         <v>0</v>
       </c>
       <c r="D162">
-        <f>COUNTIFS($A$2:A162, A162, $B$2:B162, B162, $C$2:C162, C162) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A162, A162, $B$3:B162, B162, $C$3:C162, C162) - 1</f>
+        <v>9</v>
       </c>
       <c r="E162" t="str" cm="1">
         <f t="array" ref="E162">_xlfn.CONCAT(IF(A162="completion", "Completion", IF(A162="cassette", "Cassette", IF(A162="gemheart", "Crystal Heart", IF(A162="strawberry", _xlfn.CONCAT("Strawberry ", D162+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B162)*(regions!$B$2:$B$27=C162), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 10 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F162" t="str">
         <f t="shared" si="2"/>
@@ -4279,12 +4282,12 @@
         <v>0</v>
       </c>
       <c r="D163">
-        <f>COUNTIFS($A$2:A163, A163, $B$2:B163, B163, $C$2:C163, C163) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A163, A163, $B$3:B163, B163, $C$3:C163, C163) - 1</f>
+        <v>10</v>
       </c>
       <c r="E163" t="str" cm="1">
         <f t="array" ref="E163">_xlfn.CONCAT(IF(A163="completion", "Completion", IF(A163="cassette", "Cassette", IF(A163="gemheart", "Crystal Heart", IF(A163="strawberry", _xlfn.CONCAT("Strawberry ", D163+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B163)*(regions!$B$2:$B$27=C163), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 11 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F163" t="str">
         <f t="shared" si="2"/>
@@ -4302,12 +4305,12 @@
         <v>0</v>
       </c>
       <c r="D164">
-        <f>COUNTIFS($A$2:A164, A164, $B$2:B164, B164, $C$2:C164, C164) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A164, A164, $B$3:B164, B164, $C$3:C164, C164) - 1</f>
+        <v>11</v>
       </c>
       <c r="E164" t="str" cm="1">
         <f t="array" ref="E164">_xlfn.CONCAT(IF(A164="completion", "Completion", IF(A164="cassette", "Cassette", IF(A164="gemheart", "Crystal Heart", IF(A164="strawberry", _xlfn.CONCAT("Strawberry ", D164+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B164)*(regions!$B$2:$B$27=C164), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 12 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="2"/>
@@ -4325,12 +4328,12 @@
         <v>0</v>
       </c>
       <c r="D165">
-        <f>COUNTIFS($A$2:A165, A165, $B$2:B165, B165, $C$2:C165, C165) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A165, A165, $B$3:B165, B165, $C$3:C165, C165) - 1</f>
+        <v>12</v>
       </c>
       <c r="E165" t="str" cm="1">
         <f t="array" ref="E165">_xlfn.CONCAT(IF(A165="completion", "Completion", IF(A165="cassette", "Cassette", IF(A165="gemheart", "Crystal Heart", IF(A165="strawberry", _xlfn.CONCAT("Strawberry ", D165+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B165)*(regions!$B$2:$B$27=C165), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 13 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F165" t="str">
         <f t="shared" si="2"/>
@@ -4348,12 +4351,12 @@
         <v>0</v>
       </c>
       <c r="D166">
-        <f>COUNTIFS($A$2:A166, A166, $B$2:B166, B166, $C$2:C166, C166) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A166, A166, $B$3:B166, B166, $C$3:C166, C166) - 1</f>
+        <v>13</v>
       </c>
       <c r="E166" t="str" cm="1">
         <f t="array" ref="E166">_xlfn.CONCAT(IF(A166="completion", "Completion", IF(A166="cassette", "Cassette", IF(A166="gemheart", "Crystal Heart", IF(A166="strawberry", _xlfn.CONCAT("Strawberry ", D166+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B166)*(regions!$B$2:$B$27=C166), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 14 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F166" t="str">
         <f t="shared" si="2"/>
@@ -4371,12 +4374,12 @@
         <v>0</v>
       </c>
       <c r="D167">
-        <f>COUNTIFS($A$2:A167, A167, $B$2:B167, B167, $C$2:C167, C167) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A167, A167, $B$3:B167, B167, $C$3:C167, C167) - 1</f>
+        <v>14</v>
       </c>
       <c r="E167" t="str" cm="1">
         <f t="array" ref="E167">_xlfn.CONCAT(IF(A167="completion", "Completion", IF(A167="cassette", "Cassette", IF(A167="gemheart", "Crystal Heart", IF(A167="strawberry", _xlfn.CONCAT("Strawberry ", D167+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B167)*(regions!$B$2:$B$27=C167), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 15 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="2"/>
@@ -4394,12 +4397,12 @@
         <v>0</v>
       </c>
       <c r="D168">
-        <f>COUNTIFS($A$2:A168, A168, $B$2:B168, B168, $C$2:C168, C168) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A168, A168, $B$3:B168, B168, $C$3:C168, C168) - 1</f>
+        <v>15</v>
       </c>
       <c r="E168" t="str" cm="1">
         <f t="array" ref="E168">_xlfn.CONCAT(IF(A168="completion", "Completion", IF(A168="cassette", "Cassette", IF(A168="gemheart", "Crystal Heart", IF(A168="strawberry", _xlfn.CONCAT("Strawberry ", D168+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B168)*(regions!$B$2:$B$27=C168), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 16 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F168" t="str">
         <f t="shared" si="2"/>
@@ -4417,12 +4420,12 @@
         <v>0</v>
       </c>
       <c r="D169">
-        <f>COUNTIFS($A$2:A169, A169, $B$2:B169, B169, $C$2:C169, C169) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A169, A169, $B$3:B169, B169, $C$3:C169, C169) - 1</f>
+        <v>16</v>
       </c>
       <c r="E169" t="str" cm="1">
         <f t="array" ref="E169">_xlfn.CONCAT(IF(A169="completion", "Completion", IF(A169="cassette", "Cassette", IF(A169="gemheart", "Crystal Heart", IF(A169="strawberry", _xlfn.CONCAT("Strawberry ", D169+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B169)*(regions!$B$2:$B$27=C169), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 17 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F169" t="str">
         <f t="shared" si="2"/>
@@ -4440,12 +4443,12 @@
         <v>0</v>
       </c>
       <c r="D170">
-        <f>COUNTIFS($A$2:A170, A170, $B$2:B170, B170, $C$2:C170, C170) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A170, A170, $B$3:B170, B170, $C$3:C170, C170) - 1</f>
+        <v>17</v>
       </c>
       <c r="E170" t="str" cm="1">
         <f t="array" ref="E170">_xlfn.CONCAT(IF(A170="completion", "Completion", IF(A170="cassette", "Cassette", IF(A170="gemheart", "Crystal Heart", IF(A170="strawberry", _xlfn.CONCAT("Strawberry ", D170+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B170)*(regions!$B$2:$B$27=C170), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 18 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F170" t="str">
         <f t="shared" si="2"/>
@@ -4463,12 +4466,12 @@
         <v>0</v>
       </c>
       <c r="D171">
-        <f>COUNTIFS($A$2:A171, A171, $B$2:B171, B171, $C$2:C171, C171) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A171, A171, $B$3:B171, B171, $C$3:C171, C171) - 1</f>
+        <v>18</v>
       </c>
       <c r="E171" t="str" cm="1">
         <f t="array" ref="E171">_xlfn.CONCAT(IF(A171="completion", "Completion", IF(A171="cassette", "Cassette", IF(A171="gemheart", "Crystal Heart", IF(A171="strawberry", _xlfn.CONCAT("Strawberry ", D171+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B171)*(regions!$B$2:$B$27=C171), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 19 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F171" t="str">
         <f t="shared" si="2"/>
@@ -4486,12 +4489,12 @@
         <v>0</v>
       </c>
       <c r="D172">
-        <f>COUNTIFS($A$2:A172, A172, $B$2:B172, B172, $C$2:C172, C172) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A172, A172, $B$3:B172, B172, $C$3:C172, C172) - 1</f>
+        <v>19</v>
       </c>
       <c r="E172" t="str" cm="1">
         <f t="array" ref="E172">_xlfn.CONCAT(IF(A172="completion", "Completion", IF(A172="cassette", "Cassette", IF(A172="gemheart", "Crystal Heart", IF(A172="strawberry", _xlfn.CONCAT("Strawberry ", D172+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B172)*(regions!$B$2:$B$27=C172), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 20 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F172" t="str">
         <f t="shared" si="2"/>
@@ -4509,12 +4512,12 @@
         <v>0</v>
       </c>
       <c r="D173">
-        <f>COUNTIFS($A$2:A173, A173, $B$2:B173, B173, $C$2:C173, C173) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A173, A173, $B$3:B173, B173, $C$3:C173, C173) - 1</f>
+        <v>20</v>
       </c>
       <c r="E173" t="str" cm="1">
         <f t="array" ref="E173">_xlfn.CONCAT(IF(A173="completion", "Completion", IF(A173="cassette", "Cassette", IF(A173="gemheart", "Crystal Heart", IF(A173="strawberry", _xlfn.CONCAT("Strawberry ", D173+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B173)*(regions!$B$2:$B$27=C173), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 21 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F173" t="str">
         <f t="shared" si="2"/>
@@ -4532,12 +4535,12 @@
         <v>0</v>
       </c>
       <c r="D174">
-        <f>COUNTIFS($A$2:A174, A174, $B$2:B174, B174, $C$2:C174, C174) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A174, A174, $B$3:B174, B174, $C$3:C174, C174) - 1</f>
+        <v>21</v>
       </c>
       <c r="E174" t="str" cm="1">
         <f t="array" ref="E174">_xlfn.CONCAT(IF(A174="completion", "Completion", IF(A174="cassette", "Cassette", IF(A174="gemheart", "Crystal Heart", IF(A174="strawberry", _xlfn.CONCAT("Strawberry ", D174+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B174)*(regions!$B$2:$B$27=C174), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 22 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F174" t="str">
         <f t="shared" si="2"/>
@@ -4555,12 +4558,12 @@
         <v>0</v>
       </c>
       <c r="D175">
-        <f>COUNTIFS($A$2:A175, A175, $B$2:B175, B175, $C$2:C175, C175) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A175, A175, $B$3:B175, B175, $C$3:C175, C175) - 1</f>
+        <v>22</v>
       </c>
       <c r="E175" t="str" cm="1">
         <f t="array" ref="E175">_xlfn.CONCAT(IF(A175="completion", "Completion", IF(A175="cassette", "Cassette", IF(A175="gemheart", "Crystal Heart", IF(A175="strawberry", _xlfn.CONCAT("Strawberry ", D175+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B175)*(regions!$B$2:$B$27=C175), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 23 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F175" t="str">
         <f t="shared" si="2"/>
@@ -4578,12 +4581,12 @@
         <v>0</v>
       </c>
       <c r="D176">
-        <f>COUNTIFS($A$2:A176, A176, $B$2:B176, B176, $C$2:C176, C176) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A176, A176, $B$3:B176, B176, $C$3:C176, C176) - 1</f>
+        <v>23</v>
       </c>
       <c r="E176" t="str" cm="1">
         <f t="array" ref="E176">_xlfn.CONCAT(IF(A176="completion", "Completion", IF(A176="cassette", "Cassette", IF(A176="gemheart", "Crystal Heart", IF(A176="strawberry", _xlfn.CONCAT("Strawberry ", D176+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B176)*(regions!$B$2:$B$27=C176), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 24 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F176" t="str">
         <f t="shared" si="2"/>
@@ -4601,12 +4604,12 @@
         <v>0</v>
       </c>
       <c r="D177">
-        <f>COUNTIFS($A$2:A177, A177, $B$2:B177, B177, $C$2:C177, C177) - 1</f>
-        <v>25</v>
+        <f>COUNTIFS($A$3:A177, A177, $B$3:B177, B177, $C$3:C177, C177) - 1</f>
+        <v>24</v>
       </c>
       <c r="E177" t="str" cm="1">
         <f t="array" ref="E177">_xlfn.CONCAT(IF(A177="completion", "Completion", IF(A177="cassette", "Cassette", IF(A177="gemheart", "Crystal Heart", IF(A177="strawberry", _xlfn.CONCAT("Strawberry ", D177+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B177)*(regions!$B$2:$B$27=C177), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 26 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 25 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="2"/>
@@ -4624,12 +4627,12 @@
         <v>0</v>
       </c>
       <c r="D178">
-        <f>COUNTIFS($A$2:A178, A178, $B$2:B178, B178, $C$2:C178, C178) - 1</f>
-        <v>26</v>
+        <f>COUNTIFS($A$3:A178, A178, $B$3:B178, B178, $C$3:C178, C178) - 1</f>
+        <v>25</v>
       </c>
       <c r="E178" t="str" cm="1">
         <f t="array" ref="E178">_xlfn.CONCAT(IF(A178="completion", "Completion", IF(A178="cassette", "Cassette", IF(A178="gemheart", "Crystal Heart", IF(A178="strawberry", _xlfn.CONCAT("Strawberry ", D178+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B178)*(regions!$B$2:$B$27=C178), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 27 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 26 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F178" t="str">
         <f t="shared" si="2"/>
@@ -4647,12 +4650,12 @@
         <v>0</v>
       </c>
       <c r="D179">
-        <f>COUNTIFS($A$2:A179, A179, $B$2:B179, B179, $C$2:C179, C179) - 1</f>
-        <v>27</v>
+        <f>COUNTIFS($A$3:A179, A179, $B$3:B179, B179, $C$3:C179, C179) - 1</f>
+        <v>26</v>
       </c>
       <c r="E179" t="str" cm="1">
         <f t="array" ref="E179">_xlfn.CONCAT(IF(A179="completion", "Completion", IF(A179="cassette", "Cassette", IF(A179="gemheart", "Crystal Heart", IF(A179="strawberry", _xlfn.CONCAT("Strawberry ", D179+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B179)*(regions!$B$2:$B$27=C179), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 28 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 27 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F179" t="str">
         <f t="shared" si="2"/>
@@ -4670,12 +4673,12 @@
         <v>0</v>
       </c>
       <c r="D180">
-        <f>COUNTIFS($A$2:A180, A180, $B$2:B180, B180, $C$2:C180, C180) - 1</f>
-        <v>28</v>
+        <f>COUNTIFS($A$3:A180, A180, $B$3:B180, B180, $C$3:C180, C180) - 1</f>
+        <v>27</v>
       </c>
       <c r="E180" t="str" cm="1">
         <f t="array" ref="E180">_xlfn.CONCAT(IF(A180="completion", "Completion", IF(A180="cassette", "Cassette", IF(A180="gemheart", "Crystal Heart", IF(A180="strawberry", _xlfn.CONCAT("Strawberry ", D180+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B180)*(regions!$B$2:$B$27=C180), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 29 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 28 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F180" t="str">
         <f t="shared" si="2"/>
@@ -4693,12 +4696,12 @@
         <v>0</v>
       </c>
       <c r="D181">
-        <f>COUNTIFS($A$2:A181, A181, $B$2:B181, B181, $C$2:C181, C181) - 1</f>
-        <v>29</v>
+        <f>COUNTIFS($A$3:A181, A181, $B$3:B181, B181, $C$3:C181, C181) - 1</f>
+        <v>28</v>
       </c>
       <c r="E181" t="str" cm="1">
         <f t="array" ref="E181">_xlfn.CONCAT(IF(A181="completion", "Completion", IF(A181="cassette", "Cassette", IF(A181="gemheart", "Crystal Heart", IF(A181="strawberry", _xlfn.CONCAT("Strawberry ", D181+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B181)*(regions!$B$2:$B$27=C181), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 30 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 29 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F181" t="str">
         <f t="shared" si="2"/>
@@ -4716,12 +4719,12 @@
         <v>0</v>
       </c>
       <c r="D182">
-        <f>COUNTIFS($A$2:A182, A182, $B$2:B182, B182, $C$2:C182, C182) - 1</f>
-        <v>30</v>
+        <f>COUNTIFS($A$3:A182, A182, $B$3:B182, B182, $C$3:C182, C182) - 1</f>
+        <v>29</v>
       </c>
       <c r="E182" t="str" cm="1">
         <f t="array" ref="E182">_xlfn.CONCAT(IF(A182="completion", "Completion", IF(A182="cassette", "Cassette", IF(A182="gemheart", "Crystal Heart", IF(A182="strawberry", _xlfn.CONCAT("Strawberry ", D182+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B182)*(regions!$B$2:$B$27=C182), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 31 (Chapter 5: Mirror Temple A-Side)</v>
+        <v>Strawberry 30 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F182" t="str">
         <f t="shared" si="2"/>
@@ -4733,18 +4736,18 @@
         <v>6</v>
       </c>
       <c r="B183">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C183">
         <v>0</v>
       </c>
       <c r="D183">
-        <f>COUNTIFS($A$2:A183, A183, $B$2:B183, B183, $C$2:C183, C183) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A183, A183, $B$3:B183, B183, $C$3:C183, C183) - 1</f>
+        <v>30</v>
       </c>
       <c r="E183" t="str" cm="1">
         <f t="array" ref="E183">_xlfn.CONCAT(IF(A183="completion", "Completion", IF(A183="cassette", "Cassette", IF(A183="gemheart", "Crystal Heart", IF(A183="strawberry", _xlfn.CONCAT("Strawberry ", D183+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B183)*(regions!$B$2:$B$27=C183), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 31 (Chapter 5: Mirror Temple A-Side)</v>
       </c>
       <c r="F183" t="str">
         <f t="shared" si="2"/>
@@ -4762,12 +4765,12 @@
         <v>0</v>
       </c>
       <c r="D184">
-        <f>COUNTIFS($A$2:A184, A184, $B$2:B184, B184, $C$2:C184, C184) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A184, A184, $B$3:B184, B184, $C$3:C184, C184) - 1</f>
+        <v>0</v>
       </c>
       <c r="E184" t="str" cm="1">
         <f t="array" ref="E184">_xlfn.CONCAT(IF(A184="completion", "Completion", IF(A184="cassette", "Cassette", IF(A184="gemheart", "Crystal Heart", IF(A184="strawberry", _xlfn.CONCAT("Strawberry ", D184+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B184)*(regions!$B$2:$B$27=C184), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 1 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F184" t="str">
         <f t="shared" si="2"/>
@@ -4785,12 +4788,12 @@
         <v>0</v>
       </c>
       <c r="D185">
-        <f>COUNTIFS($A$2:A185, A185, $B$2:B185, B185, $C$2:C185, C185) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A185, A185, $B$3:B185, B185, $C$3:C185, C185) - 1</f>
+        <v>1</v>
       </c>
       <c r="E185" t="str" cm="1">
         <f t="array" ref="E185">_xlfn.CONCAT(IF(A185="completion", "Completion", IF(A185="cassette", "Cassette", IF(A185="gemheart", "Crystal Heart", IF(A185="strawberry", _xlfn.CONCAT("Strawberry ", D185+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B185)*(regions!$B$2:$B$27=C185), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 2 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F185" t="str">
         <f t="shared" si="2"/>
@@ -4808,12 +4811,12 @@
         <v>0</v>
       </c>
       <c r="D186">
-        <f>COUNTIFS($A$2:A186, A186, $B$2:B186, B186, $C$2:C186, C186) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A186, A186, $B$3:B186, B186, $C$3:C186, C186) - 1</f>
+        <v>2</v>
       </c>
       <c r="E186" t="str" cm="1">
         <f t="array" ref="E186">_xlfn.CONCAT(IF(A186="completion", "Completion", IF(A186="cassette", "Cassette", IF(A186="gemheart", "Crystal Heart", IF(A186="strawberry", _xlfn.CONCAT("Strawberry ", D186+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B186)*(regions!$B$2:$B$27=C186), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 3 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F186" t="str">
         <f t="shared" si="2"/>
@@ -4831,12 +4834,12 @@
         <v>0</v>
       </c>
       <c r="D187">
-        <f>COUNTIFS($A$2:A187, A187, $B$2:B187, B187, $C$2:C187, C187) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A187, A187, $B$3:B187, B187, $C$3:C187, C187) - 1</f>
+        <v>3</v>
       </c>
       <c r="E187" t="str" cm="1">
         <f t="array" ref="E187">_xlfn.CONCAT(IF(A187="completion", "Completion", IF(A187="cassette", "Cassette", IF(A187="gemheart", "Crystal Heart", IF(A187="strawberry", _xlfn.CONCAT("Strawberry ", D187+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B187)*(regions!$B$2:$B$27=C187), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 5 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 4 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F187" t="str">
         <f t="shared" si="2"/>
@@ -4854,12 +4857,12 @@
         <v>0</v>
       </c>
       <c r="D188">
-        <f>COUNTIFS($A$2:A188, A188, $B$2:B188, B188, $C$2:C188, C188) - 1</f>
-        <v>5</v>
+        <f>COUNTIFS($A$3:A188, A188, $B$3:B188, B188, $C$3:C188, C188) - 1</f>
+        <v>4</v>
       </c>
       <c r="E188" t="str" cm="1">
         <f t="array" ref="E188">_xlfn.CONCAT(IF(A188="completion", "Completion", IF(A188="cassette", "Cassette", IF(A188="gemheart", "Crystal Heart", IF(A188="strawberry", _xlfn.CONCAT("Strawberry ", D188+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B188)*(regions!$B$2:$B$27=C188), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 6 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 5 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F188" t="str">
         <f t="shared" si="2"/>
@@ -4877,12 +4880,12 @@
         <v>0</v>
       </c>
       <c r="D189">
-        <f>COUNTIFS($A$2:A189, A189, $B$2:B189, B189, $C$2:C189, C189) - 1</f>
-        <v>6</v>
+        <f>COUNTIFS($A$3:A189, A189, $B$3:B189, B189, $C$3:C189, C189) - 1</f>
+        <v>5</v>
       </c>
       <c r="E189" t="str" cm="1">
         <f t="array" ref="E189">_xlfn.CONCAT(IF(A189="completion", "Completion", IF(A189="cassette", "Cassette", IF(A189="gemheart", "Crystal Heart", IF(A189="strawberry", _xlfn.CONCAT("Strawberry ", D189+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B189)*(regions!$B$2:$B$27=C189), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 7 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 6 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F189" t="str">
         <f t="shared" si="2"/>
@@ -4900,12 +4903,12 @@
         <v>0</v>
       </c>
       <c r="D190">
-        <f>COUNTIFS($A$2:A190, A190, $B$2:B190, B190, $C$2:C190, C190) - 1</f>
-        <v>7</v>
+        <f>COUNTIFS($A$3:A190, A190, $B$3:B190, B190, $C$3:C190, C190) - 1</f>
+        <v>6</v>
       </c>
       <c r="E190" t="str" cm="1">
         <f t="array" ref="E190">_xlfn.CONCAT(IF(A190="completion", "Completion", IF(A190="cassette", "Cassette", IF(A190="gemheart", "Crystal Heart", IF(A190="strawberry", _xlfn.CONCAT("Strawberry ", D190+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B190)*(regions!$B$2:$B$27=C190), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 8 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 7 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F190" t="str">
         <f t="shared" si="2"/>
@@ -4923,12 +4926,12 @@
         <v>0</v>
       </c>
       <c r="D191">
-        <f>COUNTIFS($A$2:A191, A191, $B$2:B191, B191, $C$2:C191, C191) - 1</f>
-        <v>8</v>
+        <f>COUNTIFS($A$3:A191, A191, $B$3:B191, B191, $C$3:C191, C191) - 1</f>
+        <v>7</v>
       </c>
       <c r="E191" t="str" cm="1">
         <f t="array" ref="E191">_xlfn.CONCAT(IF(A191="completion", "Completion", IF(A191="cassette", "Cassette", IF(A191="gemheart", "Crystal Heart", IF(A191="strawberry", _xlfn.CONCAT("Strawberry ", D191+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B191)*(regions!$B$2:$B$27=C191), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 9 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 8 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F191" t="str">
         <f t="shared" si="2"/>
@@ -4946,12 +4949,12 @@
         <v>0</v>
       </c>
       <c r="D192">
-        <f>COUNTIFS($A$2:A192, A192, $B$2:B192, B192, $C$2:C192, C192) - 1</f>
-        <v>9</v>
+        <f>COUNTIFS($A$3:A192, A192, $B$3:B192, B192, $C$3:C192, C192) - 1</f>
+        <v>8</v>
       </c>
       <c r="E192" t="str" cm="1">
         <f t="array" ref="E192">_xlfn.CONCAT(IF(A192="completion", "Completion", IF(A192="cassette", "Cassette", IF(A192="gemheart", "Crystal Heart", IF(A192="strawberry", _xlfn.CONCAT("Strawberry ", D192+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B192)*(regions!$B$2:$B$27=C192), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 10 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 9 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F192" t="str">
         <f t="shared" si="2"/>
@@ -4969,12 +4972,12 @@
         <v>0</v>
       </c>
       <c r="D193">
-        <f>COUNTIFS($A$2:A193, A193, $B$2:B193, B193, $C$2:C193, C193) - 1</f>
-        <v>10</v>
+        <f>COUNTIFS($A$3:A193, A193, $B$3:B193, B193, $C$3:C193, C193) - 1</f>
+        <v>9</v>
       </c>
       <c r="E193" t="str" cm="1">
         <f t="array" ref="E193">_xlfn.CONCAT(IF(A193="completion", "Completion", IF(A193="cassette", "Cassette", IF(A193="gemheart", "Crystal Heart", IF(A193="strawberry", _xlfn.CONCAT("Strawberry ", D193+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B193)*(regions!$B$2:$B$27=C193), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 11 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 10 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F193" t="str">
         <f t="shared" si="2"/>
@@ -4992,15 +4995,15 @@
         <v>0</v>
       </c>
       <c r="D194">
-        <f>COUNTIFS($A$2:A194, A194, $B$2:B194, B194, $C$2:C194, C194) - 1</f>
-        <v>11</v>
+        <f>COUNTIFS($A$3:A194, A194, $B$3:B194, B194, $C$3:C194, C194) - 1</f>
+        <v>10</v>
       </c>
       <c r="E194" t="str" cm="1">
         <f t="array" ref="E194">_xlfn.CONCAT(IF(A194="completion", "Completion", IF(A194="cassette", "Cassette", IF(A194="gemheart", "Crystal Heart", IF(A194="strawberry", _xlfn.CONCAT("Strawberry ", D194+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B194)*(regions!$B$2:$B$27=C194), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 12 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 11 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F194" t="str">
-        <f t="shared" ref="F194:F234" si="3">IF(A194="strawberry", "Strawberry", E194)</f>
+        <f t="shared" si="2"/>
         <v>Strawberry</v>
       </c>
     </row>
@@ -5015,15 +5018,15 @@
         <v>0</v>
       </c>
       <c r="D195">
-        <f>COUNTIFS($A$2:A195, A195, $B$2:B195, B195, $C$2:C195, C195) - 1</f>
-        <v>12</v>
+        <f>COUNTIFS($A$3:A195, A195, $B$3:B195, B195, $C$3:C195, C195) - 1</f>
+        <v>11</v>
       </c>
       <c r="E195" t="str" cm="1">
         <f t="array" ref="E195">_xlfn.CONCAT(IF(A195="completion", "Completion", IF(A195="cassette", "Cassette", IF(A195="gemheart", "Crystal Heart", IF(A195="strawberry", _xlfn.CONCAT("Strawberry ", D195+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B195)*(regions!$B$2:$B$27=C195), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 13 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 12 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F195" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F195:F235" si="3">IF(A195="strawberry", "Strawberry", E195)</f>
         <v>Strawberry</v>
       </c>
     </row>
@@ -5038,12 +5041,12 @@
         <v>0</v>
       </c>
       <c r="D196">
-        <f>COUNTIFS($A$2:A196, A196, $B$2:B196, B196, $C$2:C196, C196) - 1</f>
-        <v>13</v>
+        <f>COUNTIFS($A$3:A196, A196, $B$3:B196, B196, $C$3:C196, C196) - 1</f>
+        <v>12</v>
       </c>
       <c r="E196" t="str" cm="1">
         <f t="array" ref="E196">_xlfn.CONCAT(IF(A196="completion", "Completion", IF(A196="cassette", "Cassette", IF(A196="gemheart", "Crystal Heart", IF(A196="strawberry", _xlfn.CONCAT("Strawberry ", D196+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B196)*(regions!$B$2:$B$27=C196), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 14 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 13 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F196" t="str">
         <f t="shared" si="3"/>
@@ -5061,12 +5064,12 @@
         <v>0</v>
       </c>
       <c r="D197">
-        <f>COUNTIFS($A$2:A197, A197, $B$2:B197, B197, $C$2:C197, C197) - 1</f>
-        <v>14</v>
+        <f>COUNTIFS($A$3:A197, A197, $B$3:B197, B197, $C$3:C197, C197) - 1</f>
+        <v>13</v>
       </c>
       <c r="E197" t="str" cm="1">
         <f t="array" ref="E197">_xlfn.CONCAT(IF(A197="completion", "Completion", IF(A197="cassette", "Cassette", IF(A197="gemheart", "Crystal Heart", IF(A197="strawberry", _xlfn.CONCAT("Strawberry ", D197+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B197)*(regions!$B$2:$B$27=C197), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 15 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 14 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F197" t="str">
         <f t="shared" si="3"/>
@@ -5084,12 +5087,12 @@
         <v>0</v>
       </c>
       <c r="D198">
-        <f>COUNTIFS($A$2:A198, A198, $B$2:B198, B198, $C$2:C198, C198) - 1</f>
-        <v>15</v>
+        <f>COUNTIFS($A$3:A198, A198, $B$3:B198, B198, $C$3:C198, C198) - 1</f>
+        <v>14</v>
       </c>
       <c r="E198" t="str" cm="1">
         <f t="array" ref="E198">_xlfn.CONCAT(IF(A198="completion", "Completion", IF(A198="cassette", "Cassette", IF(A198="gemheart", "Crystal Heart", IF(A198="strawberry", _xlfn.CONCAT("Strawberry ", D198+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B198)*(regions!$B$2:$B$27=C198), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 16 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 15 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F198" t="str">
         <f t="shared" si="3"/>
@@ -5107,12 +5110,12 @@
         <v>0</v>
       </c>
       <c r="D199">
-        <f>COUNTIFS($A$2:A199, A199, $B$2:B199, B199, $C$2:C199, C199) - 1</f>
-        <v>16</v>
+        <f>COUNTIFS($A$3:A199, A199, $B$3:B199, B199, $C$3:C199, C199) - 1</f>
+        <v>15</v>
       </c>
       <c r="E199" t="str" cm="1">
         <f t="array" ref="E199">_xlfn.CONCAT(IF(A199="completion", "Completion", IF(A199="cassette", "Cassette", IF(A199="gemheart", "Crystal Heart", IF(A199="strawberry", _xlfn.CONCAT("Strawberry ", D199+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B199)*(regions!$B$2:$B$27=C199), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 17 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 16 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F199" t="str">
         <f t="shared" si="3"/>
@@ -5130,12 +5133,12 @@
         <v>0</v>
       </c>
       <c r="D200">
-        <f>COUNTIFS($A$2:A200, A200, $B$2:B200, B200, $C$2:C200, C200) - 1</f>
-        <v>17</v>
+        <f>COUNTIFS($A$3:A200, A200, $B$3:B200, B200, $C$3:C200, C200) - 1</f>
+        <v>16</v>
       </c>
       <c r="E200" t="str" cm="1">
         <f t="array" ref="E200">_xlfn.CONCAT(IF(A200="completion", "Completion", IF(A200="cassette", "Cassette", IF(A200="gemheart", "Crystal Heart", IF(A200="strawberry", _xlfn.CONCAT("Strawberry ", D200+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B200)*(regions!$B$2:$B$27=C200), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 18 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 17 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F200" t="str">
         <f t="shared" si="3"/>
@@ -5153,12 +5156,12 @@
         <v>0</v>
       </c>
       <c r="D201">
-        <f>COUNTIFS($A$2:A201, A201, $B$2:B201, B201, $C$2:C201, C201) - 1</f>
-        <v>18</v>
+        <f>COUNTIFS($A$3:A201, A201, $B$3:B201, B201, $C$3:C201, C201) - 1</f>
+        <v>17</v>
       </c>
       <c r="E201" t="str" cm="1">
         <f t="array" ref="E201">_xlfn.CONCAT(IF(A201="completion", "Completion", IF(A201="cassette", "Cassette", IF(A201="gemheart", "Crystal Heart", IF(A201="strawberry", _xlfn.CONCAT("Strawberry ", D201+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B201)*(regions!$B$2:$B$27=C201), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 19 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 18 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F201" t="str">
         <f t="shared" si="3"/>
@@ -5176,12 +5179,12 @@
         <v>0</v>
       </c>
       <c r="D202">
-        <f>COUNTIFS($A$2:A202, A202, $B$2:B202, B202, $C$2:C202, C202) - 1</f>
-        <v>19</v>
+        <f>COUNTIFS($A$3:A202, A202, $B$3:B202, B202, $C$3:C202, C202) - 1</f>
+        <v>18</v>
       </c>
       <c r="E202" t="str" cm="1">
         <f t="array" ref="E202">_xlfn.CONCAT(IF(A202="completion", "Completion", IF(A202="cassette", "Cassette", IF(A202="gemheart", "Crystal Heart", IF(A202="strawberry", _xlfn.CONCAT("Strawberry ", D202+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B202)*(regions!$B$2:$B$27=C202), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 20 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 19 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F202" t="str">
         <f t="shared" si="3"/>
@@ -5199,12 +5202,12 @@
         <v>0</v>
       </c>
       <c r="D203">
-        <f>COUNTIFS($A$2:A203, A203, $B$2:B203, B203, $C$2:C203, C203) - 1</f>
-        <v>20</v>
+        <f>COUNTIFS($A$3:A203, A203, $B$3:B203, B203, $C$3:C203, C203) - 1</f>
+        <v>19</v>
       </c>
       <c r="E203" t="str" cm="1">
         <f t="array" ref="E203">_xlfn.CONCAT(IF(A203="completion", "Completion", IF(A203="cassette", "Cassette", IF(A203="gemheart", "Crystal Heart", IF(A203="strawberry", _xlfn.CONCAT("Strawberry ", D203+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B203)*(regions!$B$2:$B$27=C203), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 21 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 20 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F203" t="str">
         <f t="shared" si="3"/>
@@ -5222,12 +5225,12 @@
         <v>0</v>
       </c>
       <c r="D204">
-        <f>COUNTIFS($A$2:A204, A204, $B$2:B204, B204, $C$2:C204, C204) - 1</f>
-        <v>21</v>
+        <f>COUNTIFS($A$3:A204, A204, $B$3:B204, B204, $C$3:C204, C204) - 1</f>
+        <v>20</v>
       </c>
       <c r="E204" t="str" cm="1">
         <f t="array" ref="E204">_xlfn.CONCAT(IF(A204="completion", "Completion", IF(A204="cassette", "Cassette", IF(A204="gemheart", "Crystal Heart", IF(A204="strawberry", _xlfn.CONCAT("Strawberry ", D204+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B204)*(regions!$B$2:$B$27=C204), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 22 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 21 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F204" t="str">
         <f t="shared" si="3"/>
@@ -5245,12 +5248,12 @@
         <v>0</v>
       </c>
       <c r="D205">
-        <f>COUNTIFS($A$2:A205, A205, $B$2:B205, B205, $C$2:C205, C205) - 1</f>
-        <v>22</v>
+        <f>COUNTIFS($A$3:A205, A205, $B$3:B205, B205, $C$3:C205, C205) - 1</f>
+        <v>21</v>
       </c>
       <c r="E205" t="str" cm="1">
         <f t="array" ref="E205">_xlfn.CONCAT(IF(A205="completion", "Completion", IF(A205="cassette", "Cassette", IF(A205="gemheart", "Crystal Heart", IF(A205="strawberry", _xlfn.CONCAT("Strawberry ", D205+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B205)*(regions!$B$2:$B$27=C205), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 23 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 22 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F205" t="str">
         <f t="shared" si="3"/>
@@ -5268,12 +5271,12 @@
         <v>0</v>
       </c>
       <c r="D206">
-        <f>COUNTIFS($A$2:A206, A206, $B$2:B206, B206, $C$2:C206, C206) - 1</f>
-        <v>23</v>
+        <f>COUNTIFS($A$3:A206, A206, $B$3:B206, B206, $C$3:C206, C206) - 1</f>
+        <v>22</v>
       </c>
       <c r="E206" t="str" cm="1">
         <f t="array" ref="E206">_xlfn.CONCAT(IF(A206="completion", "Completion", IF(A206="cassette", "Cassette", IF(A206="gemheart", "Crystal Heart", IF(A206="strawberry", _xlfn.CONCAT("Strawberry ", D206+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B206)*(regions!$B$2:$B$27=C206), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 24 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 23 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F206" t="str">
         <f t="shared" si="3"/>
@@ -5291,12 +5294,12 @@
         <v>0</v>
       </c>
       <c r="D207">
-        <f>COUNTIFS($A$2:A207, A207, $B$2:B207, B207, $C$2:C207, C207) - 1</f>
-        <v>24</v>
+        <f>COUNTIFS($A$3:A207, A207, $B$3:B207, B207, $C$3:C207, C207) - 1</f>
+        <v>23</v>
       </c>
       <c r="E207" t="str" cm="1">
         <f t="array" ref="E207">_xlfn.CONCAT(IF(A207="completion", "Completion", IF(A207="cassette", "Cassette", IF(A207="gemheart", "Crystal Heart", IF(A207="strawberry", _xlfn.CONCAT("Strawberry ", D207+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B207)*(regions!$B$2:$B$27=C207), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 25 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 24 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F207" t="str">
         <f t="shared" si="3"/>
@@ -5314,12 +5317,12 @@
         <v>0</v>
       </c>
       <c r="D208">
-        <f>COUNTIFS($A$2:A208, A208, $B$2:B208, B208, $C$2:C208, C208) - 1</f>
-        <v>25</v>
+        <f>COUNTIFS($A$3:A208, A208, $B$3:B208, B208, $C$3:C208, C208) - 1</f>
+        <v>24</v>
       </c>
       <c r="E208" t="str" cm="1">
         <f t="array" ref="E208">_xlfn.CONCAT(IF(A208="completion", "Completion", IF(A208="cassette", "Cassette", IF(A208="gemheart", "Crystal Heart", IF(A208="strawberry", _xlfn.CONCAT("Strawberry ", D208+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B208)*(regions!$B$2:$B$27=C208), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 26 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 25 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F208" t="str">
         <f t="shared" si="3"/>
@@ -5337,12 +5340,12 @@
         <v>0</v>
       </c>
       <c r="D209">
-        <f>COUNTIFS($A$2:A209, A209, $B$2:B209, B209, $C$2:C209, C209) - 1</f>
-        <v>26</v>
+        <f>COUNTIFS($A$3:A209, A209, $B$3:B209, B209, $C$3:C209, C209) - 1</f>
+        <v>25</v>
       </c>
       <c r="E209" t="str" cm="1">
         <f t="array" ref="E209">_xlfn.CONCAT(IF(A209="completion", "Completion", IF(A209="cassette", "Cassette", IF(A209="gemheart", "Crystal Heart", IF(A209="strawberry", _xlfn.CONCAT("Strawberry ", D209+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B209)*(regions!$B$2:$B$27=C209), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 27 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 26 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F209" t="str">
         <f t="shared" si="3"/>
@@ -5360,12 +5363,12 @@
         <v>0</v>
       </c>
       <c r="D210">
-        <f>COUNTIFS($A$2:A210, A210, $B$2:B210, B210, $C$2:C210, C210) - 1</f>
-        <v>27</v>
+        <f>COUNTIFS($A$3:A210, A210, $B$3:B210, B210, $C$3:C210, C210) - 1</f>
+        <v>26</v>
       </c>
       <c r="E210" t="str" cm="1">
         <f t="array" ref="E210">_xlfn.CONCAT(IF(A210="completion", "Completion", IF(A210="cassette", "Cassette", IF(A210="gemheart", "Crystal Heart", IF(A210="strawberry", _xlfn.CONCAT("Strawberry ", D210+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B210)*(regions!$B$2:$B$27=C210), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 28 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 27 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F210" t="str">
         <f t="shared" si="3"/>
@@ -5383,12 +5386,12 @@
         <v>0</v>
       </c>
       <c r="D211">
-        <f>COUNTIFS($A$2:A211, A211, $B$2:B211, B211, $C$2:C211, C211) - 1</f>
-        <v>28</v>
+        <f>COUNTIFS($A$3:A211, A211, $B$3:B211, B211, $C$3:C211, C211) - 1</f>
+        <v>27</v>
       </c>
       <c r="E211" t="str" cm="1">
         <f t="array" ref="E211">_xlfn.CONCAT(IF(A211="completion", "Completion", IF(A211="cassette", "Cassette", IF(A211="gemheart", "Crystal Heart", IF(A211="strawberry", _xlfn.CONCAT("Strawberry ", D211+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B211)*(regions!$B$2:$B$27=C211), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 29 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 28 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F211" t="str">
         <f t="shared" si="3"/>
@@ -5406,12 +5409,12 @@
         <v>0</v>
       </c>
       <c r="D212">
-        <f>COUNTIFS($A$2:A212, A212, $B$2:B212, B212, $C$2:C212, C212) - 1</f>
-        <v>29</v>
+        <f>COUNTIFS($A$3:A212, A212, $B$3:B212, B212, $C$3:C212, C212) - 1</f>
+        <v>28</v>
       </c>
       <c r="E212" t="str" cm="1">
         <f t="array" ref="E212">_xlfn.CONCAT(IF(A212="completion", "Completion", IF(A212="cassette", "Cassette", IF(A212="gemheart", "Crystal Heart", IF(A212="strawberry", _xlfn.CONCAT("Strawberry ", D212+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B212)*(regions!$B$2:$B$27=C212), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 30 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 29 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F212" t="str">
         <f t="shared" si="3"/>
@@ -5429,12 +5432,12 @@
         <v>0</v>
       </c>
       <c r="D213">
-        <f>COUNTIFS($A$2:A213, A213, $B$2:B213, B213, $C$2:C213, C213) - 1</f>
-        <v>30</v>
+        <f>COUNTIFS($A$3:A213, A213, $B$3:B213, B213, $C$3:C213, C213) - 1</f>
+        <v>29</v>
       </c>
       <c r="E213" t="str" cm="1">
         <f t="array" ref="E213">_xlfn.CONCAT(IF(A213="completion", "Completion", IF(A213="cassette", "Cassette", IF(A213="gemheart", "Crystal Heart", IF(A213="strawberry", _xlfn.CONCAT("Strawberry ", D213+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B213)*(regions!$B$2:$B$27=C213), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 31 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 30 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F213" t="str">
         <f t="shared" si="3"/>
@@ -5452,12 +5455,12 @@
         <v>0</v>
       </c>
       <c r="D214">
-        <f>COUNTIFS($A$2:A214, A214, $B$2:B214, B214, $C$2:C214, C214) - 1</f>
-        <v>31</v>
+        <f>COUNTIFS($A$3:A214, A214, $B$3:B214, B214, $C$3:C214, C214) - 1</f>
+        <v>30</v>
       </c>
       <c r="E214" t="str" cm="1">
         <f t="array" ref="E214">_xlfn.CONCAT(IF(A214="completion", "Completion", IF(A214="cassette", "Cassette", IF(A214="gemheart", "Crystal Heart", IF(A214="strawberry", _xlfn.CONCAT("Strawberry ", D214+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B214)*(regions!$B$2:$B$27=C214), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 32 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 31 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F214" t="str">
         <f t="shared" si="3"/>
@@ -5475,12 +5478,12 @@
         <v>0</v>
       </c>
       <c r="D215">
-        <f>COUNTIFS($A$2:A215, A215, $B$2:B215, B215, $C$2:C215, C215) - 1</f>
-        <v>32</v>
+        <f>COUNTIFS($A$3:A215, A215, $B$3:B215, B215, $C$3:C215, C215) - 1</f>
+        <v>31</v>
       </c>
       <c r="E215" t="str" cm="1">
         <f t="array" ref="E215">_xlfn.CONCAT(IF(A215="completion", "Completion", IF(A215="cassette", "Cassette", IF(A215="gemheart", "Crystal Heart", IF(A215="strawberry", _xlfn.CONCAT("Strawberry ", D215+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B215)*(regions!$B$2:$B$27=C215), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 33 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 32 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F215" t="str">
         <f t="shared" si="3"/>
@@ -5498,12 +5501,12 @@
         <v>0</v>
       </c>
       <c r="D216">
-        <f>COUNTIFS($A$2:A216, A216, $B$2:B216, B216, $C$2:C216, C216) - 1</f>
-        <v>33</v>
+        <f>COUNTIFS($A$3:A216, A216, $B$3:B216, B216, $C$3:C216, C216) - 1</f>
+        <v>32</v>
       </c>
       <c r="E216" t="str" cm="1">
         <f t="array" ref="E216">_xlfn.CONCAT(IF(A216="completion", "Completion", IF(A216="cassette", "Cassette", IF(A216="gemheart", "Crystal Heart", IF(A216="strawberry", _xlfn.CONCAT("Strawberry ", D216+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B216)*(regions!$B$2:$B$27=C216), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 34 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 33 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F216" t="str">
         <f t="shared" si="3"/>
@@ -5521,12 +5524,12 @@
         <v>0</v>
       </c>
       <c r="D217">
-        <f>COUNTIFS($A$2:A217, A217, $B$2:B217, B217, $C$2:C217, C217) - 1</f>
-        <v>34</v>
+        <f>COUNTIFS($A$3:A217, A217, $B$3:B217, B217, $C$3:C217, C217) - 1</f>
+        <v>33</v>
       </c>
       <c r="E217" t="str" cm="1">
         <f t="array" ref="E217">_xlfn.CONCAT(IF(A217="completion", "Completion", IF(A217="cassette", "Cassette", IF(A217="gemheart", "Crystal Heart", IF(A217="strawberry", _xlfn.CONCAT("Strawberry ", D217+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B217)*(regions!$B$2:$B$27=C217), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 35 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 34 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F217" t="str">
         <f t="shared" si="3"/>
@@ -5544,12 +5547,12 @@
         <v>0</v>
       </c>
       <c r="D218">
-        <f>COUNTIFS($A$2:A218, A218, $B$2:B218, B218, $C$2:C218, C218) - 1</f>
-        <v>35</v>
+        <f>COUNTIFS($A$3:A218, A218, $B$3:B218, B218, $C$3:C218, C218) - 1</f>
+        <v>34</v>
       </c>
       <c r="E218" t="str" cm="1">
         <f t="array" ref="E218">_xlfn.CONCAT(IF(A218="completion", "Completion", IF(A218="cassette", "Cassette", IF(A218="gemheart", "Crystal Heart", IF(A218="strawberry", _xlfn.CONCAT("Strawberry ", D218+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B218)*(regions!$B$2:$B$27=C218), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 36 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 35 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F218" t="str">
         <f t="shared" si="3"/>
@@ -5567,12 +5570,12 @@
         <v>0</v>
       </c>
       <c r="D219">
-        <f>COUNTIFS($A$2:A219, A219, $B$2:B219, B219, $C$2:C219, C219) - 1</f>
-        <v>36</v>
+        <f>COUNTIFS($A$3:A219, A219, $B$3:B219, B219, $C$3:C219, C219) - 1</f>
+        <v>35</v>
       </c>
       <c r="E219" t="str" cm="1">
         <f t="array" ref="E219">_xlfn.CONCAT(IF(A219="completion", "Completion", IF(A219="cassette", "Cassette", IF(A219="gemheart", "Crystal Heart", IF(A219="strawberry", _xlfn.CONCAT("Strawberry ", D219+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B219)*(regions!$B$2:$B$27=C219), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 37 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 36 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F219" t="str">
         <f t="shared" si="3"/>
@@ -5590,12 +5593,12 @@
         <v>0</v>
       </c>
       <c r="D220">
-        <f>COUNTIFS($A$2:A220, A220, $B$2:B220, B220, $C$2:C220, C220) - 1</f>
-        <v>37</v>
+        <f>COUNTIFS($A$3:A220, A220, $B$3:B220, B220, $C$3:C220, C220) - 1</f>
+        <v>36</v>
       </c>
       <c r="E220" t="str" cm="1">
         <f t="array" ref="E220">_xlfn.CONCAT(IF(A220="completion", "Completion", IF(A220="cassette", "Cassette", IF(A220="gemheart", "Crystal Heart", IF(A220="strawberry", _xlfn.CONCAT("Strawberry ", D220+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B220)*(regions!$B$2:$B$27=C220), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 38 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 37 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F220" t="str">
         <f t="shared" si="3"/>
@@ -5613,12 +5616,12 @@
         <v>0</v>
       </c>
       <c r="D221">
-        <f>COUNTIFS($A$2:A221, A221, $B$2:B221, B221, $C$2:C221, C221) - 1</f>
-        <v>38</v>
+        <f>COUNTIFS($A$3:A221, A221, $B$3:B221, B221, $C$3:C221, C221) - 1</f>
+        <v>37</v>
       </c>
       <c r="E221" t="str" cm="1">
         <f t="array" ref="E221">_xlfn.CONCAT(IF(A221="completion", "Completion", IF(A221="cassette", "Cassette", IF(A221="gemheart", "Crystal Heart", IF(A221="strawberry", _xlfn.CONCAT("Strawberry ", D221+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B221)*(regions!$B$2:$B$27=C221), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 39 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 38 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F221" t="str">
         <f t="shared" si="3"/>
@@ -5636,12 +5639,12 @@
         <v>0</v>
       </c>
       <c r="D222">
-        <f>COUNTIFS($A$2:A222, A222, $B$2:B222, B222, $C$2:C222, C222) - 1</f>
-        <v>39</v>
+        <f>COUNTIFS($A$3:A222, A222, $B$3:B222, B222, $C$3:C222, C222) - 1</f>
+        <v>38</v>
       </c>
       <c r="E222" t="str" cm="1">
         <f t="array" ref="E222">_xlfn.CONCAT(IF(A222="completion", "Completion", IF(A222="cassette", "Cassette", IF(A222="gemheart", "Crystal Heart", IF(A222="strawberry", _xlfn.CONCAT("Strawberry ", D222+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B222)*(regions!$B$2:$B$27=C222), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 40 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 39 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F222" t="str">
         <f t="shared" si="3"/>
@@ -5659,12 +5662,12 @@
         <v>0</v>
       </c>
       <c r="D223">
-        <f>COUNTIFS($A$2:A223, A223, $B$2:B223, B223, $C$2:C223, C223) - 1</f>
-        <v>40</v>
+        <f>COUNTIFS($A$3:A223, A223, $B$3:B223, B223, $C$3:C223, C223) - 1</f>
+        <v>39</v>
       </c>
       <c r="E223" t="str" cm="1">
         <f t="array" ref="E223">_xlfn.CONCAT(IF(A223="completion", "Completion", IF(A223="cassette", "Cassette", IF(A223="gemheart", "Crystal Heart", IF(A223="strawberry", _xlfn.CONCAT("Strawberry ", D223+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B223)*(regions!$B$2:$B$27=C223), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 41 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 40 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F223" t="str">
         <f t="shared" si="3"/>
@@ -5682,12 +5685,12 @@
         <v>0</v>
       </c>
       <c r="D224">
-        <f>COUNTIFS($A$2:A224, A224, $B$2:B224, B224, $C$2:C224, C224) - 1</f>
-        <v>41</v>
+        <f>COUNTIFS($A$3:A224, A224, $B$3:B224, B224, $C$3:C224, C224) - 1</f>
+        <v>40</v>
       </c>
       <c r="E224" t="str" cm="1">
         <f t="array" ref="E224">_xlfn.CONCAT(IF(A224="completion", "Completion", IF(A224="cassette", "Cassette", IF(A224="gemheart", "Crystal Heart", IF(A224="strawberry", _xlfn.CONCAT("Strawberry ", D224+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B224)*(regions!$B$2:$B$27=C224), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 42 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 41 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F224" t="str">
         <f t="shared" si="3"/>
@@ -5705,12 +5708,12 @@
         <v>0</v>
       </c>
       <c r="D225">
-        <f>COUNTIFS($A$2:A225, A225, $B$2:B225, B225, $C$2:C225, C225) - 1</f>
-        <v>42</v>
+        <f>COUNTIFS($A$3:A225, A225, $B$3:B225, B225, $C$3:C225, C225) - 1</f>
+        <v>41</v>
       </c>
       <c r="E225" t="str" cm="1">
         <f t="array" ref="E225">_xlfn.CONCAT(IF(A225="completion", "Completion", IF(A225="cassette", "Cassette", IF(A225="gemheart", "Crystal Heart", IF(A225="strawberry", _xlfn.CONCAT("Strawberry ", D225+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B225)*(regions!$B$2:$B$27=C225), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 43 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 42 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F225" t="str">
         <f t="shared" si="3"/>
@@ -5728,12 +5731,12 @@
         <v>0</v>
       </c>
       <c r="D226">
-        <f>COUNTIFS($A$2:A226, A226, $B$2:B226, B226, $C$2:C226, C226) - 1</f>
-        <v>43</v>
+        <f>COUNTIFS($A$3:A226, A226, $B$3:B226, B226, $C$3:C226, C226) - 1</f>
+        <v>42</v>
       </c>
       <c r="E226" t="str" cm="1">
         <f t="array" ref="E226">_xlfn.CONCAT(IF(A226="completion", "Completion", IF(A226="cassette", "Cassette", IF(A226="gemheart", "Crystal Heart", IF(A226="strawberry", _xlfn.CONCAT("Strawberry ", D226+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B226)*(regions!$B$2:$B$27=C226), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 44 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 43 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F226" t="str">
         <f t="shared" si="3"/>
@@ -5751,12 +5754,12 @@
         <v>0</v>
       </c>
       <c r="D227">
-        <f>COUNTIFS($A$2:A227, A227, $B$2:B227, B227, $C$2:C227, C227) - 1</f>
-        <v>44</v>
+        <f>COUNTIFS($A$3:A227, A227, $B$3:B227, B227, $C$3:C227, C227) - 1</f>
+        <v>43</v>
       </c>
       <c r="E227" t="str" cm="1">
         <f t="array" ref="E227">_xlfn.CONCAT(IF(A227="completion", "Completion", IF(A227="cassette", "Cassette", IF(A227="gemheart", "Crystal Heart", IF(A227="strawberry", _xlfn.CONCAT("Strawberry ", D227+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B227)*(regions!$B$2:$B$27=C227), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 45 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 44 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F227" t="str">
         <f t="shared" si="3"/>
@@ -5774,12 +5777,12 @@
         <v>0</v>
       </c>
       <c r="D228">
-        <f>COUNTIFS($A$2:A228, A228, $B$2:B228, B228, $C$2:C228, C228) - 1</f>
-        <v>45</v>
+        <f>COUNTIFS($A$3:A228, A228, $B$3:B228, B228, $C$3:C228, C228) - 1</f>
+        <v>44</v>
       </c>
       <c r="E228" t="str" cm="1">
         <f t="array" ref="E228">_xlfn.CONCAT(IF(A228="completion", "Completion", IF(A228="cassette", "Cassette", IF(A228="gemheart", "Crystal Heart", IF(A228="strawberry", _xlfn.CONCAT("Strawberry ", D228+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B228)*(regions!$B$2:$B$27=C228), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 46 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 45 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F228" t="str">
         <f t="shared" si="3"/>
@@ -5797,12 +5800,12 @@
         <v>0</v>
       </c>
       <c r="D229">
-        <f>COUNTIFS($A$2:A229, A229, $B$2:B229, B229, $C$2:C229, C229) - 1</f>
-        <v>46</v>
+        <f>COUNTIFS($A$3:A229, A229, $B$3:B229, B229, $C$3:C229, C229) - 1</f>
+        <v>45</v>
       </c>
       <c r="E229" t="str" cm="1">
         <f t="array" ref="E229">_xlfn.CONCAT(IF(A229="completion", "Completion", IF(A229="cassette", "Cassette", IF(A229="gemheart", "Crystal Heart", IF(A229="strawberry", _xlfn.CONCAT("Strawberry ", D229+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B229)*(regions!$B$2:$B$27=C229), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 47 (Chapter 7: The Summit A-Side)</v>
+        <v>Strawberry 46 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F229" t="str">
         <f t="shared" si="3"/>
@@ -5814,18 +5817,18 @@
         <v>6</v>
       </c>
       <c r="B230">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C230">
         <v>0</v>
       </c>
       <c r="D230">
-        <f>COUNTIFS($A$2:A230, A230, $B$2:B230, B230, $C$2:C230, C230) - 1</f>
-        <v>0</v>
+        <f>COUNTIFS($A$3:A230, A230, $B$3:B230, B230, $C$3:C230, C230) - 1</f>
+        <v>46</v>
       </c>
       <c r="E230" t="str" cm="1">
         <f t="array" ref="E230">_xlfn.CONCAT(IF(A230="completion", "Completion", IF(A230="cassette", "Cassette", IF(A230="gemheart", "Crystal Heart", IF(A230="strawberry", _xlfn.CONCAT("Strawberry ", D230+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B230)*(regions!$B$2:$B$27=C230), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 1 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 47 (Chapter 7: The Summit A-Side)</v>
       </c>
       <c r="F230" t="str">
         <f t="shared" si="3"/>
@@ -5843,12 +5846,12 @@
         <v>0</v>
       </c>
       <c r="D231">
-        <f>COUNTIFS($A$2:A231, A231, $B$2:B231, B231, $C$2:C231, C231) - 1</f>
-        <v>1</v>
+        <f>COUNTIFS($A$3:A231, A231, $B$3:B231, B231, $C$3:C231, C231) - 1</f>
+        <v>0</v>
       </c>
       <c r="E231" t="str" cm="1">
         <f t="array" ref="E231">_xlfn.CONCAT(IF(A231="completion", "Completion", IF(A231="cassette", "Cassette", IF(A231="gemheart", "Crystal Heart", IF(A231="strawberry", _xlfn.CONCAT("Strawberry ", D231+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B231)*(regions!$B$2:$B$27=C231), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 2 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 1 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F231" t="str">
         <f t="shared" si="3"/>
@@ -5866,12 +5869,12 @@
         <v>0</v>
       </c>
       <c r="D232">
-        <f>COUNTIFS($A$2:A232, A232, $B$2:B232, B232, $C$2:C232, C232) - 1</f>
-        <v>2</v>
+        <f>COUNTIFS($A$3:A232, A232, $B$3:B232, B232, $C$3:C232, C232) - 1</f>
+        <v>1</v>
       </c>
       <c r="E232" t="str" cm="1">
         <f t="array" ref="E232">_xlfn.CONCAT(IF(A232="completion", "Completion", IF(A232="cassette", "Cassette", IF(A232="gemheart", "Crystal Heart", IF(A232="strawberry", _xlfn.CONCAT("Strawberry ", D232+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B232)*(regions!$B$2:$B$27=C232), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 3 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 2 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F232" t="str">
         <f t="shared" si="3"/>
@@ -5889,12 +5892,12 @@
         <v>0</v>
       </c>
       <c r="D233">
-        <f>COUNTIFS($A$2:A233, A233, $B$2:B233, B233, $C$2:C233, C233) - 1</f>
-        <v>3</v>
+        <f>COUNTIFS($A$3:A233, A233, $B$3:B233, B233, $C$3:C233, C233) - 1</f>
+        <v>2</v>
       </c>
       <c r="E233" t="str" cm="1">
         <f t="array" ref="E233">_xlfn.CONCAT(IF(A233="completion", "Completion", IF(A233="cassette", "Cassette", IF(A233="gemheart", "Crystal Heart", IF(A233="strawberry", _xlfn.CONCAT("Strawberry ", D233+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B233)*(regions!$B$2:$B$27=C233), regions!$C$2:$C$27, "", 0, 1), ")")</f>
-        <v>Strawberry 4 (Chapter 8: Core A-Side)</v>
+        <v>Strawberry 3 (Chapter 8: Core A-Side)</v>
       </c>
       <c r="F233" t="str">
         <f t="shared" si="3"/>
@@ -5912,14 +5915,37 @@
         <v>0</v>
       </c>
       <c r="D234">
-        <f>COUNTIFS($A$2:A234, A234, $B$2:B234, B234, $C$2:C234, C234) - 1</f>
-        <v>4</v>
+        <f>COUNTIFS($A$3:A234, A234, $B$3:B234, B234, $C$3:C234, C234) - 1</f>
+        <v>3</v>
       </c>
       <c r="E234" t="str" cm="1">
         <f t="array" ref="E234">_xlfn.CONCAT(IF(A234="completion", "Completion", IF(A234="cassette", "Cassette", IF(A234="gemheart", "Crystal Heart", IF(A234="strawberry", _xlfn.CONCAT("Strawberry ", D234+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B234)*(regions!$B$2:$B$27=C234), regions!$C$2:$C$27, "", 0, 1), ")")</f>
+        <v>Strawberry 4 (Chapter 8: Core A-Side)</v>
+      </c>
+      <c r="F234" t="str">
+        <f t="shared" si="3"/>
+        <v>Strawberry</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>6</v>
+      </c>
+      <c r="B235">
+        <v>9</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235">
+        <f>COUNTIFS($A$3:A235, A235, $B$3:B235, B235, $C$3:C235, C235) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="E235" t="str" cm="1">
+        <f t="array" ref="E235">_xlfn.CONCAT(IF(A235="completion", "Completion", IF(A235="cassette", "Cassette", IF(A235="gemheart", "Crystal Heart", IF(A235="strawberry", _xlfn.CONCAT("Strawberry ", D235+1), "")))), " (", _xlfn.XLOOKUP(1, (regions!$A$2:$A$27=B235)*(regions!$B$2:$B$27=C235), regions!$C$2:$C$27, "", 0, 1), ")")</f>
         <v>Strawberry 5 (Chapter 8: Core A-Side)</v>
       </c>
-      <c r="F234" t="str">
+      <c r="F235" t="str">
         <f t="shared" si="3"/>
         <v>Strawberry</v>
       </c>
@@ -5934,7 +5960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1A1AF2-907D-41B3-B0A4-149E1E23A84D}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>

</xml_diff>